<commit_message>
Win10 -> Win11, 2021 -> 2022
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpsuzuki\Documents\2022_03\fresta2022\fresta2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63FB1A73-CCA7-44AC-87F0-8D5FE6622580}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE3D42C-D758-4B86-BB96-2840647BE9D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" tabRatio="782" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" tabRatio="782" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -1551,10 +1551,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>FRESTA-TEXT-2021 Win10 chap.0</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">自分のパソコンの基本的なスペックを確認しておきましょう。CPUの型式、OSのビット数、記憶容量など。
 なお、この章は広島大学の学生番号がわかる前に実施することができます。 </t>
     <rPh sb="56" eb="57">
@@ -4982,6 +4978,10 @@
     <rPh sb="17" eb="18">
       <t>サガ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2022 Win11 chap.0</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -5419,7 +5419,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5435,7 +5435,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -5443,7 +5443,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -5494,7 +5494,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5502,7 +5502,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5518,7 +5518,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5542,7 +5542,7 @@
     </row>
     <row r="8" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D8" t="s">
         <v>130</v>
@@ -5558,7 +5558,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -5602,7 +5602,7 @@
         <v>108</v>
       </c>
       <c r="D14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5616,7 +5616,7 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -5657,7 +5657,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5665,7 +5665,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5681,7 +5681,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -5689,7 +5689,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5703,7 +5703,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -5713,13 +5713,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5727,24 +5727,24 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -5752,13 +5752,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5766,24 +5766,24 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -5791,46 +5791,46 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C19" t="s">
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -5838,13 +5838,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -5852,24 +5852,24 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="92.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -5877,13 +5877,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -5891,35 +5891,35 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C24" t="s">
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C26" t="s">
         <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5927,13 +5927,13 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C27" t="s">
         <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -5941,13 +5941,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C28" t="s">
         <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -6055,8 +6055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.2"/>
@@ -6073,7 +6073,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s" ph="1">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6097,7 +6097,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s" ph="1">
-        <v>173</v>
+        <v>347</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="304.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -6105,7 +6105,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s" ph="1">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -6125,7 +6125,7 @@
         <v>9</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="81.599999999999994" ph="1" x14ac:dyDescent="0.2">
@@ -6133,13 +6133,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s" ph="1">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
@@ -6147,13 +6147,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s" ph="1">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C9" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
@@ -6161,7 +6161,7 @@
         <v>99</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
@@ -6175,7 +6175,7 @@
         <v>9</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="102" ph="1" x14ac:dyDescent="0.2">
@@ -6183,35 +6183,35 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s" ph="1">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s" ph="1">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="14" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s" ph="1">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C14" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="122.4" ph="1" x14ac:dyDescent="0.2">
@@ -6219,13 +6219,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s" ph="1">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C15" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
@@ -6233,13 +6233,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s" ph="1">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C16" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="81.599999999999994" ph="1" x14ac:dyDescent="0.2">
@@ -6247,24 +6247,24 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s" ph="1">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="122.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s" ph="1">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="19" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6272,271 +6272,271 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s" ph="1">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s" ph="1">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="122.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s" ph="1">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="22" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s" ph="1">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s" ph="1">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="24" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s" ph="1">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s" ph="1">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C25" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s" ph="1">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C26" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D26" t="s" ph="1">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s" ph="1">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C27" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D27" t="s" ph="1">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="81.599999999999994" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s" ph="1">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C28" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D28" t="s" ph="1">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s" ph="1">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C29" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D29" t="s" ph="1">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="102" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s" ph="1">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C30" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D30" t="s" ph="1">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s" ph="1">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C31" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D31" t="s" ph="1">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="81.599999999999994" ph="1" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s" ph="1">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C32" t="s" ph="1">
+        <v>307</v>
+      </c>
+      <c r="D32" t="s" ph="1">
         <v>308</v>
-      </c>
-      <c r="D32" t="s" ph="1">
-        <v>309</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s" ph="1">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D33" t="s" ph="1">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s" ph="1">
+        <v>320</v>
+      </c>
+      <c r="D34" t="s" ph="1">
         <v>321</v>
-      </c>
-      <c r="D34" t="s" ph="1">
-        <v>322</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D35" t="s" ph="1">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s" ph="1">
+        <v>325</v>
+      </c>
+      <c r="D36" t="s" ph="1">
         <v>326</v>
-      </c>
-      <c r="D36" t="s" ph="1">
-        <v>327</v>
       </c>
     </row>
     <row r="37" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s" ph="1">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C37" t="s" ph="1">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D37" t="s" ph="1">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="38" spans="2:4" customFormat="1" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D38" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="39" spans="2:4" customFormat="1" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D39" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="40" spans="2:4" customFormat="1" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D40" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s" ph="1">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D41" t="s" ph="1">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="81.599999999999994" ph="1" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s" ph="1">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D42" t="s" ph="1">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s" ph="1">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D43" t="s" ph="1">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s" ph="1">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D44" t="s" ph="1">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="45" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s" ph="1">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D45" t="s" ph="1">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="46" spans="2:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s" ph="1">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D46" t="s" ph="1">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -6550,7 +6550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
@@ -6567,7 +6567,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6591,48 +6591,48 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s" ph="1">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C7" t="s" ph="1">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="8" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s" ph="1">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C8" t="s" ph="1">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="9" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s" ph="1">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C9" t="s" ph="1">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="10" spans="1:4" customFormat="1" ht="81.599999999999994" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s" ph="1">
+        <v>312</v>
+      </c>
+      <c r="D10" t="s" ph="1">
         <v>313</v>
-      </c>
-      <c r="D10" t="s" ph="1">
-        <v>314</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="145.19999999999999" x14ac:dyDescent="0.2">
@@ -6771,17 +6771,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -6970,7 +6970,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -6978,7 +6978,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7179,7 +7179,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7187,7 +7187,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7203,7 +7203,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -7211,7 +7211,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7227,7 +7227,7 @@
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -7323,7 +7323,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7331,7 +7331,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7347,7 +7347,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7355,7 +7355,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7371,7 +7371,7 @@
     </row>
     <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -7379,7 +7379,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -7390,7 +7390,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -7398,7 +7398,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -7409,7 +7409,7 @@
     </row>
     <row r="12" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D12" t="s">
         <v>110</v>
@@ -7420,7 +7420,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -7440,7 +7440,7 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7448,13 +7448,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7537,7 +7537,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="264" x14ac:dyDescent="0.2">
@@ -7545,7 +7545,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7639,13 +7639,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7667,7 +7667,7 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7811,7 +7811,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -7881,7 +7881,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
@@ -8051,7 +8051,7 @@
         <v>144</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8075,7 +8075,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -8099,7 +8099,7 @@
     </row>
     <row r="8" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update how to fix wrong keymap
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpsuzuki\Documents\2022_03\fresta2022\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E32E789-F999-464C-8F4B-60E85F949A3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491841C9-10A9-492E-BEC0-8EE4DF8186F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" tabRatio="782" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="356">
   <si>
     <t>header1</t>
   </si>
@@ -56,22 +56,7 @@
     <t>chartn</t>
   </si>
   <si>
-    <t>win10-1-04.svg</t>
-  </si>
-  <si>
     <t>panel panel-warning</t>
-  </si>
-  <si>
-    <t>win10-1-11.svg</t>
-  </si>
-  <si>
-    <t>win10-1-12.svg</t>
-  </si>
-  <si>
-    <t>win10-1-13.svg</t>
-  </si>
-  <si>
-    <t>win10-1-14.svg</t>
   </si>
   <si>
     <t>&lt;h2&gt;この章を始める前に&lt;/h2&gt;</t>
@@ -318,14 +303,6 @@
 詳細はメディアセンターWebサイトの&lt;a href="https://www.media.hiroshima-u.ac.jp/services/print/webprint"&gt;「Webプリントサービス」&lt;/a&gt;
 で。
   </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">左メニューから「地域と言語」をクリックしてください。
- 真ん中の「優先する言語」から「日本語」をクリックしてください。 その後表示される「オプション」をクリックしてください。   </t>
-    <rPh sb="33" eb="35">
-      <t>ユウセン</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -417,17 +394,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">歯車のアイコン「設定」をクリックして、出てくるメニューの中から「時刻と言語」をクリックしてください。
-  </t>
-    <rPh sb="19" eb="20">
-      <t>デ</t>
-    </rPh>
-    <rPh sb="28" eb="29">
-      <t>ナカ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">キーボードレイアウトについての質問に答えます。「Microsoft IME」になっていることを確認して、「はい」をクリックしましょう。
   </t>
     <phoneticPr fontId="1"/>
@@ -519,59 +485,9 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">最後にバッテリー駆動時間を確認しましょう。
-画面下のタスクバーのバッテリーアイコンをクリックしてください。すると、バッテリー残量がパーセント表示され、およそあと何時間利用できるかの推定値が表示されます。
-100%充電時のここの残り時間表示が、あなたのPCのバッテリー駆動時間の推定値ということになります。（例：80%で「残り6時間」であれば、6÷0.8=7.5なので、バッテリー駆動時間は7.5時間）
-&lt;div class="spl"&gt;※ 残り時間は、システム起動後ある程度時間が経過し、しかも使用状況が安定した状態でないと表示されないようです。
-時間を置いて何度か試してみても表示されないようであれば、カタログなどで仕様を確認してください。
- &lt;/div&gt;
-  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;div class="panel-heading"&gt;&lt;span class="glyphicon glyphicon-warning-sign"&gt;&lt;/span&gt;&lt;a name="wrongkb"&gt;&lt;/a&gt; Surfaceを利用されているみなさん&lt;/div&gt;
 &lt;div class="panel-body" style="padding:10px"&gt;パソコンのスペック確認はここまでです。Surfaceをつかっている方は、タイプカバーキーボード設定に不具合があることがあるので、確認しておきましょう。不具合の内容は、キーボードが日本語用のものなのに、英語用になっているというものです。文字キーは同じですが、記号の配列が違うため、正常に入力できません。 &lt;/div&gt;
   </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">画面左下のWindowsアイコンをクリックした後Shiftキーを押しながら、「２」を押してみてください。
- そのときに「”」（ダブルクォーテーション）が出るならばキーボード設定は正常なので、この下の項目は飛ばして次の章に進んでください。「＠」が出るならばキーボードの設定が間違って英語になっていますので、次の項目に進んで変更しましょう。  </t>
-    <rPh sb="76" eb="77">
-      <t>デ</t>
-    </rPh>
-    <rPh sb="86" eb="88">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="89" eb="91">
-      <t>セイジョウ</t>
-    </rPh>
-    <rPh sb="97" eb="98">
-      <t>シタ</t>
-    </rPh>
-    <rPh sb="108" eb="109">
-      <t>ショウ</t>
-    </rPh>
-    <rPh sb="110" eb="111">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="152" eb="153">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="154" eb="156">
-      <t>コウモク</t>
-    </rPh>
-    <rPh sb="157" eb="158">
-      <t>スス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">左メニューの真ん中あたりにある「レイアウトを変更する」をクリックしてください。
- すると青い画面がでますので，「英語キーボード(101/102キー）」となっているのを「日本語キーボード(106/109キー）」に変更し、「サインアウト」をクリックしてください。 これでキーボードが日本語の設定になりました。 一度サインアウトしてから、このパソコンのユーザ名とパスワードでもう一度入り直してください。   </t>
-    <rPh sb="176" eb="177">
-      <t>メイ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -5072,12 +4988,173 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>「優先する言語」の下に「日本語」がある筈です。その右側の「…」をクリックし、オプションメニューを展開します。その中から「言語オプション」を選択します。</t>
+    <rPh sb="1" eb="3">
+      <t>ユウセン</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ゲンゴ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>シタ</t>
+    </rPh>
+    <rPh sb="12" eb="15">
+      <t>ニホンゴ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>ハズ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>ミギガワ</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>テンカイ</t>
+    </rPh>
+    <rPh sb="56" eb="57">
+      <t>ナカ</t>
+    </rPh>
+    <rPh sb="60" eb="62">
+      <t>ゲンゴ</t>
+    </rPh>
+    <rPh sb="69" eb="71">
+      <t>センタク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「言語オプション」の中に「キーボードレイアウト」のサブメニューがあります。もしキートップに平仮名が印字されているのに「日本語キーボード」になっていない場合は、「レイアウトを変更する」をクリックします。</t>
+    <rPh sb="1" eb="3">
+      <t>ゲンゴ</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>ナカ</t>
+    </rPh>
+    <rPh sb="45" eb="48">
+      <t>ヒラガナ</t>
+    </rPh>
+    <rPh sb="49" eb="51">
+      <t>インジ</t>
+    </rPh>
+    <rPh sb="59" eb="62">
+      <t>ニホンゴ</t>
+    </rPh>
+    <rPh sb="75" eb="77">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="86" eb="88">
+      <t>ヘンコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>選択可能なキー配列から日本語キーボードを選び、OKで完了した後に再起動します。</t>
+    <rPh sb="0" eb="2">
+      <t>センタク</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>カノウ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ハイレツ</t>
+    </rPh>
+    <rPh sb="11" eb="14">
+      <t>ニホンゴ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>エラ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>カンリョウ</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>アト</t>
+    </rPh>
+    <rPh sb="32" eb="35">
+      <t>サイキドウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">スタートメニューの検索フォームを一度クリックし、Shiftキーを押しながら、「２」を押してみてください。
+ そのときに「”」（ダブルクォーテーション）が出るならばキーボード設定は正常なので、この下の項目は飛ばして次の章に進んでください。「＠」が出るならばキーボードの設定が間違って英語になっていますので、次の項目に進んで変更しましょう。  </t>
+    <rPh sb="9" eb="11">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>イチド</t>
+    </rPh>
+    <rPh sb="76" eb="77">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="86" eb="88">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="89" eb="91">
+      <t>セイジョウ</t>
+    </rPh>
+    <rPh sb="97" eb="98">
+      <t>シタ</t>
+    </rPh>
+    <rPh sb="108" eb="109">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="110" eb="111">
+      <t>スス</t>
+    </rPh>
+    <rPh sb="152" eb="153">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="154" eb="156">
+      <t>コウモク</t>
+    </rPh>
+    <rPh sb="157" eb="158">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-test-keyboard.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-setting-lang.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-setting-jpn.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-setting-keyboard.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-setting-keyboard-change.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スタートメニューから「設定」アプリを起動し、「時刻と言語」のメニューリストから「言語と地域」をクリックします。</t>
+    <rPh sb="23" eb="25">
+      <t>ジコク</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>ゲンゴ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>ゲンゴ</t>
+    </rPh>
+    <rPh sb="43" eb="45">
+      <t>チイキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5098,13 +5175,6 @@
       <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -5134,7 +5204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -5143,9 +5213,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -5507,7 +5574,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5523,7 +5590,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -5531,7 +5598,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -5545,7 +5612,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5582,7 +5649,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5590,7 +5657,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5606,7 +5673,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5614,7 +5681,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5625,20 +5692,20 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="D8" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -5646,13 +5713,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -5660,37 +5727,37 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="D12" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="D13" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D14" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5698,23 +5765,23 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -5745,7 +5812,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5753,7 +5820,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5769,7 +5836,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -5777,7 +5844,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5791,7 +5858,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -5801,13 +5868,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5815,24 +5882,24 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -5840,13 +5907,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5854,24 +5921,24 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -5879,46 +5946,46 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -5926,13 +5993,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -5940,24 +6007,24 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
       </c>
       <c r="D21" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="92.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="C22" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D22" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -5965,13 +6032,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -5979,35 +6046,35 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="C24" t="s">
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="C25" t="s">
         <v>7</v>
       </c>
       <c r="D25" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="C26" t="s">
         <v>7</v>
       </c>
       <c r="D26" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6015,13 +6082,13 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="C27" t="s">
         <v>7</v>
       </c>
       <c r="D27" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -6029,13 +6096,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="C28" t="s">
         <v>7</v>
       </c>
       <c r="D28" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -6107,9 +6174,9 @@
       <c r="A46" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="6"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
@@ -6161,7 +6228,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s" ph="1">
-        <v>255</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6169,7 +6236,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s" ph="1">
-        <v>350</v>
+        <v>340</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6185,7 +6252,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s" ph="1">
-        <v>310</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="304.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -6193,7 +6260,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s" ph="1">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -6207,13 +6274,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s" ph="1">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="C7" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>257</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="81.599999999999994" ph="1" x14ac:dyDescent="0.2">
@@ -6221,21 +6288,21 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s" ph="1">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>258</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s" ph="1">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>259</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
@@ -6243,13 +6310,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s" ph="1">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C10" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="122.4" ph="1" x14ac:dyDescent="0.2">
@@ -6257,24 +6324,24 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s" ph="1">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>261</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s" ph="1">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>262</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="122.4" ph="1" x14ac:dyDescent="0.2">
@@ -6282,13 +6349,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s" ph="1">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>264</v>
+        <v>254</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
@@ -6296,13 +6363,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s" ph="1">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="C14" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>266</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="81.599999999999994" ph="1" x14ac:dyDescent="0.2">
@@ -6310,24 +6377,24 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s" ph="1">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="C15" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>267</v>
+        <v>257</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="122.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s" ph="1">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="C16" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>270</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6335,343 +6402,343 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s" ph="1">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>272</v>
+        <v>262</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s" ph="1">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>274</v>
+        <v>264</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="122.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s" ph="1">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>275</v>
+        <v>265</v>
       </c>
     </row>
     <row r="20" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s" ph="1">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>277</v>
+        <v>267</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s" ph="1">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>279</v>
+        <v>269</v>
       </c>
     </row>
     <row r="22" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s" ph="1">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>282</v>
+        <v>272</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s" ph="1">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>283</v>
+        <v>273</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s" ph="1">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>297</v>
+        <v>287</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s" ph="1">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="C25" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>287</v>
+        <v>277</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="81.599999999999994" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s" ph="1">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="C26" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D26" t="s" ph="1">
-        <v>288</v>
+        <v>278</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s" ph="1">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="C27" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D27" t="s" ph="1">
-        <v>291</v>
+        <v>281</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="102" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s" ph="1">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="C28" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D28" t="s" ph="1">
-        <v>292</v>
+        <v>282</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s" ph="1">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="C29" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D29" t="s" ph="1">
-        <v>294</v>
+        <v>284</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="81.599999999999994" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s" ph="1">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="C30" t="s" ph="1">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="D30" t="s" ph="1">
-        <v>299</v>
+        <v>289</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s" ph="1">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="C31" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D31" t="s" ph="1">
-        <v>325</v>
+        <v>315</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s" ph="1">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="C32" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D32" t="s" ph="1">
-        <v>326</v>
+        <v>316</v>
       </c>
     </row>
     <row r="33" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="C33" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D33" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
     </row>
     <row r="34" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s" ph="1">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="C34" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D34" t="s" ph="1">
-        <v>311</v>
+        <v>301</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s" ph="1">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="C35" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D35" t="s" ph="1">
-        <v>312</v>
+        <v>302</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="C36" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D36" t="s" ph="1">
-        <v>313</v>
+        <v>303</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="C37" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
     </row>
     <row r="38" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s" ph="1">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="C38" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D38" t="s" ph="1">
-        <v>315</v>
+        <v>305</v>
       </c>
     </row>
     <row r="39" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s" ph="1">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="C39" t="s" ph="1">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="D39" t="s" ph="1">
-        <v>344</v>
+        <v>334</v>
       </c>
     </row>
     <row r="40" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s" ph="1">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="C40" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D40" t="s" ph="1">
-        <v>316</v>
+        <v>306</v>
       </c>
     </row>
     <row r="41" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s" ph="1">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="C41" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D41" t="s" ph="1">
-        <v>317</v>
+        <v>307</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s" ph="1">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="C42" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D42" t="s" ph="1">
-        <v>319</v>
+        <v>309</v>
       </c>
     </row>
     <row r="43" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s" ph="1">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="C43" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D43" t="s" ph="1">
-        <v>320</v>
+        <v>310</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s" ph="1">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="C44" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D44" t="s" ph="1">
-        <v>321</v>
+        <v>311</v>
       </c>
     </row>
     <row r="45" spans="2:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s" ph="1">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="C45" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D45" t="s" ph="1">
-        <v>347</v>
+        <v>337</v>
       </c>
     </row>
     <row r="46" spans="2:4" ht="81.599999999999994" ph="1" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s" ph="1">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="C46" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D46" t="s" ph="1">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s" ph="1">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="C47" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D47" t="s" ph="1">
-        <v>349</v>
+        <v>339</v>
       </c>
     </row>
     <row r="48" spans="2:4" ph="1" x14ac:dyDescent="0.2">
@@ -6688,8 +6755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -6705,7 +6772,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6713,7 +6780,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6729,148 +6796,130 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s" ph="1">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="C7" t="s" ph="1">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>300</v>
+        <v>290</v>
       </c>
     </row>
     <row r="8" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s" ph="1">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="C8" t="s" ph="1">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>301</v>
+        <v>291</v>
       </c>
     </row>
     <row r="9" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s" ph="1">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="C9" t="s" ph="1">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>302</v>
+        <v>292</v>
       </c>
     </row>
     <row r="10" spans="1:4" customFormat="1" ht="61.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s" ph="1">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>304</v>
+        <v>294</v>
       </c>
     </row>
     <row r="11" spans="1:4" customFormat="1" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s" ph="1">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>353</v>
+        <v>343</v>
       </c>
     </row>
     <row r="12" spans="1:4" customFormat="1" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s" ph="1">
+        <v>345</v>
+      </c>
+      <c r="D12" t="s" ph="1">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="D12" t="s" ph="1">
+      <c r="D15" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="D16" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="D17" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
         <v>354</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="145.19999999999999" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -6884,7 +6933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -6901,7 +6950,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6909,7 +6958,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6925,17 +6974,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -6943,13 +6992,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -6957,13 +7006,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -6971,13 +7020,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -6985,13 +7034,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6999,13 +7048,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -7013,13 +7062,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7027,29 +7076,29 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D15" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -7063,13 +7112,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -7100,7 +7149,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7108,7 +7157,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7124,7 +7173,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -7132,7 +7181,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7143,7 +7192,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7151,13 +7200,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7165,13 +7214,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7179,13 +7228,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7193,13 +7242,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -7207,18 +7256,18 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7226,13 +7275,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -7240,13 +7289,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="145.19999999999999" x14ac:dyDescent="0.2">
@@ -7254,13 +7303,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7268,13 +7317,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7282,13 +7331,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -7296,13 +7345,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -7333,7 +7382,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7341,7 +7390,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7357,7 +7406,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -7365,7 +7414,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7376,49 +7425,49 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="D10" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="D11" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="D12" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="D13" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7426,13 +7475,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7440,13 +7489,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -7477,7 +7526,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7485,7 +7534,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7501,7 +7550,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7509,7 +7558,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7520,12 +7569,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -7533,18 +7582,18 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -7552,21 +7601,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="D12" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7574,13 +7623,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7588,13 +7637,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7602,13 +7651,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7616,27 +7665,27 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="5" customFormat="1" ht="92.4" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>103</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="4" customFormat="1" ht="92.4" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -7667,7 +7716,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7675,7 +7724,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7691,7 +7740,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="264" x14ac:dyDescent="0.2">
@@ -7699,7 +7748,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7710,7 +7759,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -7732,13 +7781,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7746,18 +7795,18 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -7779,13 +7828,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7793,21 +7842,21 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D15" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7815,13 +7864,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7829,13 +7878,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D17" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -7843,13 +7892,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7857,13 +7906,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -7871,18 +7920,18 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -7904,13 +7953,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7918,13 +7967,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7932,18 +7981,18 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -7965,13 +8014,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7979,13 +8028,13 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -7993,13 +8042,13 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8007,13 +8056,13 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="184.8" x14ac:dyDescent="0.2">
@@ -8021,13 +8070,13 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8035,13 +8084,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8049,13 +8098,13 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8063,13 +8112,13 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8077,13 +8126,13 @@
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="158.4" x14ac:dyDescent="0.2">
@@ -8091,26 +8140,26 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="D38" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8118,7 +8167,7 @@
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C40" t="s">
         <v>4</v>
@@ -8132,13 +8181,13 @@
         <v>4</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C41" t="s">
         <v>7</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -8146,21 +8195,21 @@
         <v>4</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C42" t="s">
         <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D43" t="s" ph="1">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -8168,13 +8217,13 @@
         <v>4</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C44" t="s">
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -8202,10 +8251,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8213,7 +8262,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8229,7 +8278,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -8237,7 +8286,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8248,17 +8297,17 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -8266,7 +8315,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
fix keymap change for win11ja
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpsuzuki\Documents\2022_03\fresta2022\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491841C9-10A9-492E-BEC0-8EE4DF8186F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B169FF71-E6A5-49F8-9F87-3129F823507A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" tabRatio="782" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4097,10 +4097,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-setting-system.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>win11ja-setting-version-info.png</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -5118,10 +5114,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-setting-lang.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>win11ja-setting-jpn.png</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -5147,6 +5139,14 @@
     <rPh sb="43" eb="45">
       <t>チイキ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-setting-system-only.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-setting-timezone.png</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -6236,7 +6236,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s" ph="1">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6252,7 +6252,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s" ph="1">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="304.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -6260,7 +6260,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s" ph="1">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -6274,7 +6274,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s" ph="1">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C7" t="s" ph="1">
         <v>7</v>
@@ -6288,7 +6288,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s" ph="1">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>7</v>
@@ -6324,7 +6324,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s" ph="1">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>7</v>
@@ -6545,7 +6545,7 @@
     </row>
     <row r="30" spans="1:4" ht="81.599999999999994" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s" ph="1">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C30" t="s" ph="1">
         <v>288</v>
@@ -6556,189 +6556,189 @@
     </row>
     <row r="31" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s" ph="1">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C31" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D31" t="s" ph="1">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s" ph="1">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C32" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D32" t="s" ph="1">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="33" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C33" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D33" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="34" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s" ph="1">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C34" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D34" t="s" ph="1">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s" ph="1">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C35" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D35" t="s" ph="1">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C36" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D36" t="s" ph="1">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C37" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="38" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s" ph="1">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C38" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D38" t="s" ph="1">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="39" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s" ph="1">
+        <v>331</v>
+      </c>
+      <c r="C39" t="s" ph="1">
         <v>332</v>
       </c>
-      <c r="C39" t="s" ph="1">
+      <c r="D39" t="s" ph="1">
         <v>333</v>
-      </c>
-      <c r="D39" t="s" ph="1">
-        <v>334</v>
       </c>
     </row>
     <row r="40" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s" ph="1">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C40" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D40" t="s" ph="1">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="41" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s" ph="1">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C41" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D41" t="s" ph="1">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s" ph="1">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C42" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D42" t="s" ph="1">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="43" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s" ph="1">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C43" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D43" t="s" ph="1">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s" ph="1">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C44" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D44" t="s" ph="1">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="45" spans="2:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s" ph="1">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C45" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D45" t="s" ph="1">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="46" spans="2:4" ht="81.599999999999994" ph="1" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s" ph="1">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C46" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D46" t="s" ph="1">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s" ph="1">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C47" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D47" t="s" ph="1">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="48" spans="2:4" ph="1" x14ac:dyDescent="0.2">
@@ -6755,8 +6755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -6780,7 +6780,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6796,12 +6796,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s" ph="1">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C7" t="s" ph="1">
         <v>288</v>
@@ -6812,48 +6812,48 @@
     </row>
     <row r="8" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s" ph="1">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>288</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>291</v>
+        <v>354</v>
       </c>
     </row>
     <row r="9" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s" ph="1">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C9" t="s" ph="1">
         <v>288</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="10" spans="1:4" customFormat="1" ht="61.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s" ph="1">
+        <v>292</v>
+      </c>
+      <c r="D10" t="s" ph="1">
         <v>293</v>
-      </c>
-      <c r="D10" t="s" ph="1">
-        <v>294</v>
       </c>
     </row>
     <row r="11" spans="1:4" customFormat="1" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s" ph="1">
+        <v>341</v>
+      </c>
+      <c r="D11" t="s" ph="1">
         <v>342</v>
-      </c>
-      <c r="D11" t="s" ph="1">
-        <v>343</v>
       </c>
     </row>
     <row r="12" spans="1:4" customFormat="1" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s" ph="1">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -6875,37 +6875,37 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
         <v>349</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="D15" t="s">
         <v>355</v>
-      </c>
-      <c r="D15" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D16" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D17" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -6913,13 +6913,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wifi chapter updated (win11ja)
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpsuzuki\Documents\2022_03\fresta2022\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BD1448-99E0-45A7-B433-FAF22FCDDE0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A026150A-BDE4-4B9E-B469-04A334B4A7E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" tabRatio="782" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" tabRatio="782" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="349">
   <si>
     <t>header1</t>
   </si>
@@ -74,30 +74,7 @@
     <t>win10-4-01.svg</t>
   </si>
   <si>
-    <t>win10-4-02.svg</t>
-  </si>
-  <si>
-    <t>win10-4-03.svg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">「接続」をクリックしてください。
-このときに「自動的に接続」にチェックを入れておくと，次回から同じWi-Fiには自動的に接続され，手間が省けます。 
-  </t>
-  </si>
-  <si>
-    <t>win10-4-04.svg</t>
-  </si>
-  <si>
-    <t>win10-4-05.svg</t>
-  </si>
-  <si>
-    <t>win10-4-06.svg</t>
-  </si>
-  <si>
     <t>win10-4-07.svg</t>
-  </si>
-  <si>
-    <t>win10-4-10.png</t>
   </si>
   <si>
     <t>&lt;h2&gt;&lt;a name="windows_update"&gt;&lt;/a&gt;Windows Updateの設定&lt;/h2&gt;</t>
@@ -306,46 +283,11 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <r>
-      <t>この画面になったら「接続」をクリックしてください。
-これで接続の設定が完了しました。
-接続が完了すると「接続済み」と表示されます。&lt;span class="check"&gt;check-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">&lt;span&gt;&lt;/span&gt;
-&lt;/span&gt;
-   </t>
-    </r>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">ウィルス対策ソフトのDefenderを含めて、Windows基本システムは定期的に自動更新されます。
 このウィンドウの上の方で更新状況が確認できます。&lt;span class="check"&gt;check-4&lt;span&gt;&lt;/span&gt;
 &lt;/span&gt;
 さらに、Officeも自動更新するように設定しましょう。「詳細オプション」をクリックしてください。
   </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win10-4-11.jpg</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -498,42 +440,6 @@
     <rPh sb="185" eb="186">
       <t>シメ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">PCをHINET Wi-Fiに接続する設定をおこないます。
-画面右下のWi-Fiアイコンをみてください。Wi-Fi機能をオフにしている場合には、&lt;img height="30px" src="image/win10-wifi-indicator_3.png" /&gt;のようなアイコンになっています。その場合は、まずこれをクリックして&amp;quot;Wi-Fi&amp;quot;のボタンをクリック、Wi-Fi機能をオンにしましょう
-Wi-Fi機能がオンになるとタスクバーのアイコンが&lt;img height="30px" src="image/win10-wifi-indicator_1.png" /&gt;となります。次の項目に進みましょう
-  </t>
-    <rPh sb="150" eb="152">
-      <t>バアイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Wi-Fiの一覧が出ますので，「HU-CUPXX」(XXは数字) を選択します。数字の部分はエリアで異なります。 総合科学部付近では「HU-CUP30」に接続できます。霞は「HU-CUP40」、東千田は「HU-CUP50」です。 
-&lt;p class="spl"&gt;※ 教室（講義室）で「HU-CUPXX」が表示されない場合は、あなたのパソコンが教室の無線LANに対応していないのかもしれません。その場合は、メディアセンターに相談してください。&lt;/p&gt;
-  </t>
-    <rPh sb="133" eb="135">
-      <t>キョウシツ</t>
-    </rPh>
-    <rPh sb="136" eb="139">
-      <t>コウギシツ</t>
-    </rPh>
-    <rPh sb="198" eb="200">
-      <t>バアイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ネットワークに接続した時点で、「Windowsをよりいっそう活用できるようになります」という画面が出ることがあります。これはパソコンの初期設定のときにスキップした設定をするところですが、ここでは左下の「今はスキップ」をクリックしてください。ここにある設定は後でできます。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;div class="panel-heading"&gt;&lt;span class="glyphicon glyphicon-warning-sign"&gt;&lt;/span&gt;
-パスワードを変更したら...&lt;/div&gt;
-&lt;div class="panel-body" style="padding:10px"&gt;この章の最初に「一度設定したら次回からは（同じエリアでは）設定不要です」と書かれていますが、パスワードを変更した場合には再設定が必要になります。 &lt;/div&gt;
-  </t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1226,15 +1132,6 @@
 履修登録をしたり、成績を確認することができます。
 また「掲示」では、授業や学部からの連絡が表示されます。
   </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">「ユーザ名」のところにアカウント名を入力します。
-&lt;p class="spl"&gt;※ アカウント名は学生番号の最初のアルファベットが小文字のものになります&lt;/p&gt;
-「パスワード」には広大パスワードを記入します。
-&lt;p class="spl"&gt;※ 大文字を入力するときは、SHIFTキーを押しながら文字キーを押します。&lt;/p&gt;
-両方を入力したら「OK」をクリックしてください。
-   </t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -5150,12 +5047,139 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>通知領域の地球儀マークをクリックし、さらにWiFiのサブメニューを展開します。電波が出ているWiFi基地局の一覧が出ますので、その中からHU-CUPxx (xxには数字2つが入ります)となっているものを選びます。</t>
+    <rPh sb="0" eb="2">
+      <t>ツウチ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>リョウイキ</t>
+    </rPh>
+    <rPh sb="5" eb="8">
+      <t>チキュウギ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>テンカイ</t>
+    </rPh>
+    <rPh sb="39" eb="41">
+      <t>デンパ</t>
+    </rPh>
+    <rPh sb="42" eb="43">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="50" eb="53">
+      <t>キチキョク</t>
+    </rPh>
+    <rPh sb="54" eb="56">
+      <t>イチラン</t>
+    </rPh>
+    <rPh sb="57" eb="58">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="65" eb="66">
+      <t>ナカ</t>
+    </rPh>
+    <rPh sb="82" eb="84">
+      <t>スウジ</t>
+    </rPh>
+    <rPh sb="87" eb="88">
+      <t>ハイ</t>
+    </rPh>
+    <rPh sb="101" eb="102">
+      <t>エラ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-wifi-select.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>HU-CUPxxの基地局を選び、接続ボタンを押すと、認証が求められます。IMCアカウントとパスワードを入力し、OKボタンで進めます。初めて接続する基地局では本当に接続するか再確認を求められます。</t>
+    <rPh sb="9" eb="12">
+      <t>キチキョク</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>エラ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>オ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>ニンショウ</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>モト</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="61" eb="62">
+      <t>スス</t>
+    </rPh>
+    <rPh sb="66" eb="67">
+      <t>ハジ</t>
+    </rPh>
+    <rPh sb="69" eb="71">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="73" eb="76">
+      <t>キチキョク</t>
+    </rPh>
+    <rPh sb="78" eb="80">
+      <t>ホントウ</t>
+    </rPh>
+    <rPh sb="81" eb="83">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="86" eb="89">
+      <t>サイカクニン</t>
+    </rPh>
+    <rPh sb="90" eb="91">
+      <t>モト</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-wifi-auth.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-wifi-delete.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>基地局に対するボタンが「切断」になったら接続が完了しています。</t>
+    <rPh sb="0" eb="3">
+      <t>キチキョク</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>タイ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>セツダン</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>カンリョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-wifi-connected.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5165,14 +5189,6 @@
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
@@ -5578,7 +5594,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5594,7 +5610,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -5602,7 +5618,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -5616,7 +5632,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5653,7 +5669,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5661,7 +5677,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5677,7 +5693,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5685,7 +5701,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5701,15 +5717,15 @@
     </row>
     <row r="8" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="D8" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -5717,13 +5733,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -5731,37 +5747,37 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="D12" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="D13" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D14" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5769,23 +5785,23 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -5816,7 +5832,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5824,7 +5840,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5840,7 +5856,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -5848,7 +5864,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5862,7 +5878,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -5872,13 +5888,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5886,24 +5902,24 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -5911,13 +5927,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5925,24 +5941,24 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -5950,46 +5966,46 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -5997,13 +6013,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6011,24 +6027,24 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
       </c>
       <c r="D21" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="92.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="C22" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="D22" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -6036,13 +6052,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6050,35 +6066,35 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="C24" t="s">
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="C25" t="s">
         <v>7</v>
       </c>
       <c r="D25" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="C26" t="s">
         <v>7</v>
       </c>
       <c r="D26" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6086,13 +6102,13 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="C27" t="s">
         <v>7</v>
       </c>
       <c r="D27" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -6100,13 +6116,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="C28" t="s">
         <v>7</v>
       </c>
       <c r="D28" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -6214,7 +6230,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -6232,7 +6248,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>350</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6240,7 +6256,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6256,7 +6272,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>351</v>
+        <v>337</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="304.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -6264,7 +6280,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -6278,13 +6294,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
       <c r="C7" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>245</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -6292,21 +6308,21 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>352</v>
+        <v>338</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>246</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>353</v>
+        <v>339</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>247</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
@@ -6314,13 +6330,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C10" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>248</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
@@ -6328,24 +6344,24 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>249</v>
+        <v>235</v>
       </c>
     </row>
     <row r="12" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>250</v>
+        <v>236</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
@@ -6353,13 +6369,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>354</v>
+        <v>340</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>252</v>
+        <v>238</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
@@ -6367,13 +6383,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="C14" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>253</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -6381,24 +6397,24 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="C15" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>254</v>
+        <v>240</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="C16" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>257</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6406,345 +6422,345 @@
         <v>4</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>259</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B18" s="6" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>261</v>
+        <v>247</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>262</v>
+        <v>248</v>
       </c>
     </row>
     <row r="20" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>264</v>
+        <v>250</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>266</v>
+        <v>252</v>
       </c>
     </row>
     <row r="22" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>269</v>
+        <v>255</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>270</v>
+        <v>256</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>284</v>
+        <v>270</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="C25" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>274</v>
+        <v>260</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="C26" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D26" t="s" ph="1">
-        <v>275</v>
+        <v>261</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="C27" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D27" t="s" ph="1">
-        <v>278</v>
+        <v>264</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="C28" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D28" t="s" ph="1">
-        <v>279</v>
+        <v>265</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="C29" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D29" t="s" ph="1">
-        <v>281</v>
+        <v>267</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="C30" t="s" ph="1">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="D30" t="s" ph="1">
-        <v>286</v>
+        <v>272</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
       <c r="C31" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D31" t="s" ph="1">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="C32" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D32" t="s" ph="1">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="33" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
       <c r="C33" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D33" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="E33"/>
     </row>
     <row r="34" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="C34" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D34" t="s" ph="1">
-        <v>296</v>
+        <v>282</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
       <c r="C35" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D35" t="s" ph="1">
-        <v>297</v>
+        <v>283</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="C36" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D36" t="s" ph="1">
-        <v>298</v>
+        <v>284</v>
       </c>
     </row>
     <row r="37" spans="2:5" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
       <c r="C37" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="E37"/>
     </row>
     <row r="38" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
       <c r="C38" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D38" t="s" ph="1">
-        <v>300</v>
+        <v>286</v>
       </c>
     </row>
     <row r="39" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
       <c r="C39" t="s" ph="1">
-        <v>326</v>
+        <v>312</v>
       </c>
       <c r="D39" t="s" ph="1">
-        <v>327</v>
+        <v>313</v>
       </c>
     </row>
     <row r="40" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B40" s="6" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
       <c r="C40" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D40" t="s" ph="1">
-        <v>301</v>
+        <v>287</v>
       </c>
     </row>
     <row r="41" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B41" s="6" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="C41" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D41" t="s" ph="1">
-        <v>302</v>
+        <v>288</v>
       </c>
     </row>
     <row r="42" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B42" s="6" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="C42" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D42" t="s" ph="1">
-        <v>304</v>
+        <v>290</v>
       </c>
     </row>
     <row r="43" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B43" s="6" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="C43" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D43" t="s" ph="1">
-        <v>305</v>
+        <v>291</v>
       </c>
     </row>
     <row r="44" spans="2:5" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B44" s="6" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
       <c r="C44" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D44" t="s" ph="1">
-        <v>306</v>
+        <v>292</v>
       </c>
     </row>
     <row r="45" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B45" s="6" t="s">
-        <v>329</v>
+        <v>315</v>
       </c>
       <c r="C45" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D45" t="s" ph="1">
-        <v>330</v>
+        <v>316</v>
       </c>
     </row>
     <row r="46" spans="2:5" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B46" s="6" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
       <c r="C46" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D46" t="s" ph="1">
-        <v>307</v>
+        <v>293</v>
       </c>
     </row>
     <row r="47" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B47" s="6" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
       <c r="C47" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D47" t="s" ph="1">
-        <v>332</v>
+        <v>318</v>
       </c>
     </row>
     <row r="48" spans="2:5" ph="1" x14ac:dyDescent="0.2">
@@ -6779,7 +6795,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6787,7 +6803,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>334</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6803,64 +6819,64 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s" ph="1">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="C7" t="s" ph="1">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>287</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s" ph="1">
-        <v>294</v>
+        <v>280</v>
       </c>
       <c r="C8" t="s" ph="1">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>348</v>
+        <v>334</v>
       </c>
     </row>
     <row r="9" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s" ph="1">
-        <v>295</v>
+        <v>281</v>
       </c>
       <c r="C9" t="s" ph="1">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>288</v>
+        <v>274</v>
       </c>
     </row>
     <row r="10" spans="1:4" customFormat="1" ht="61.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s" ph="1">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>290</v>
+        <v>276</v>
       </c>
     </row>
     <row r="11" spans="1:4" customFormat="1" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s" ph="1">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>336</v>
+        <v>322</v>
       </c>
     </row>
     <row r="12" spans="1:4" customFormat="1" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s" ph="1">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>337</v>
+        <v>323</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -6868,7 +6884,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -6882,37 +6898,37 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
       <c r="D15" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>339</v>
+        <v>325</v>
       </c>
       <c r="D16" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="D17" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -6920,13 +6936,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>341</v>
+        <v>327</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -6938,10 +6954,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="B9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -6981,17 +6997,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -6999,13 +7015,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -7013,7 +7029,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -7022,110 +7038,54 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>103</v>
+        <v>342</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>104</v>
+        <v>344</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
+        <v>345</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
+        <v>347</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="145.19999999999999" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>145</v>
+        <v>94</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="66" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="145.19999999999999" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" t="s">
-        <v>21</v>
+        <v>346</v>
       </c>
     </row>
   </sheetData>
@@ -7156,7 +7116,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7164,7 +7124,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7180,7 +7140,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -7188,7 +7148,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7199,7 +7159,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7207,13 +7167,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7221,13 +7181,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7235,13 +7195,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7249,13 +7209,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -7263,18 +7223,18 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7282,13 +7242,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -7296,13 +7256,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="145.19999999999999" x14ac:dyDescent="0.2">
@@ -7310,13 +7270,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7324,13 +7284,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7338,13 +7298,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -7352,13 +7312,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -7389,7 +7349,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7397,7 +7357,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7413,7 +7373,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -7421,7 +7381,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7437,44 +7397,44 @@
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D10" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="D11" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="D12" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="D13" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7482,13 +7442,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7496,7 +7456,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -7533,7 +7493,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7541,7 +7501,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7557,7 +7517,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7565,7 +7525,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7581,7 +7541,7 @@
     </row>
     <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -7589,7 +7549,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -7600,7 +7560,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -7608,21 +7568,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="D12" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7630,13 +7590,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7644,13 +7604,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7658,13 +7618,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7672,13 +7632,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="4" customFormat="1" ht="92.4" x14ac:dyDescent="0.2">
@@ -7686,13 +7646,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -7723,7 +7683,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7731,7 +7691,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7747,7 +7707,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="264" x14ac:dyDescent="0.2">
@@ -7755,7 +7715,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7766,7 +7726,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -7788,13 +7748,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7802,18 +7762,18 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -7835,13 +7795,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7849,21 +7809,21 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D15" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7871,13 +7831,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7885,13 +7845,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -7899,13 +7859,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7913,13 +7873,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -7927,18 +7887,18 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -7960,13 +7920,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7974,13 +7934,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7988,18 +7948,18 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -8021,13 +7981,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8035,13 +7995,13 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8049,13 +8009,13 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8063,13 +8023,13 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="184.8" x14ac:dyDescent="0.2">
@@ -8077,13 +8037,13 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8091,13 +8051,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8105,13 +8065,13 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8119,13 +8079,13 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8133,13 +8093,13 @@
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="158.4" x14ac:dyDescent="0.2">
@@ -8147,26 +8107,26 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="D38" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8174,7 +8134,7 @@
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C40" t="s">
         <v>4</v>
@@ -8188,13 +8148,13 @@
         <v>4</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C41" t="s">
         <v>7</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -8202,21 +8162,21 @@
         <v>4</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C42" t="s">
         <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D43" t="s" ph="1">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -8224,13 +8184,13 @@
         <v>4</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C44" t="s">
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -8258,10 +8218,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8269,7 +8229,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8285,7 +8245,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -8293,7 +8253,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8304,17 +8264,17 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -8322,7 +8282,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
win11ja: windows update + virus scan
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpsuzuki\Documents\2022_03\fresta2022\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCC3744-3E05-4903-93F2-F4A7A8B01FBD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DD0C3F-7196-41E7-9260-F42F2F51C22B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" tabRatio="782" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" tabRatio="782" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -422,12 +422,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">&lt;div class="panel-heading"&gt;&lt;span class="glyphicon glyphicon-warning-sign"&gt;&lt;/span&gt;&lt;a name="wrongkb"&gt;&lt;/a&gt; Surfaceを利用されているみなさん&lt;/div&gt;
-&lt;div class="panel-body" style="padding:10px"&gt;パソコンのスペック確認はここまでです。Surfaceをつかっている方は、タイプカバーキーボード設定に不具合があることがあるので、確認しておきましょう。不具合の内容は、キーボードが日本語用のものなのに、英語用になっているというものです。文字キーは同じですが、記号の配列が違うため、正常に入力できません。 &lt;/div&gt;
-  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">広島大学では、図書館、講義室、福利施設など学内の多くの共用スペースで、「HiNET Wi-Fi」が利用できます。ここでは、HiNET Wi-Fiを通して、あなたのPCで学内ネットワークとインターネットを利用できるようにする方法を説明します。一度設定すると、次回からは（同じエリアでは）設定不要です。
 右の図では、どのエリアでどんな名前のアクセスポイントが使われているかを示します。
  </t>
@@ -4043,10 +4037,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>FRESTA-TEXT-2022 Win11 chap.1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>スタートメニューの中の「設定」アプリを探します。歯車のアイコンをクリックして起動します。</t>
     <rPh sb="9" eb="10">
       <t>ナカ</t>
@@ -5185,6 +5175,14 @@
       <t>サクジョ</t>
     </rPh>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2022 Win11 chap.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;div class="panel-heading"&gt;&lt;span class="glyphicon glyphicon-warning-sign"&gt;&lt;/span&gt;&lt;a name="wrongkb"&gt;&lt;/a&gt; Surfaceを利用されているみなさん&lt;/div&gt;
+&lt;div class="panel-body" style="padding:10px"&gt;パソコンのスペック確認はここまでです。Surfaceをつかっている方は、タイプカバーキーボード設定に不具合があることがあるので、確認しておきましょう。不具合の内容は、キーボードが日本語用のものなのに、英語用になっているというものです。文字キーは同じですが、記号の配列が違うため、正常に入力できません。 &lt;/div&gt;
+  </t>
   </si>
 </sst>
 </file>
@@ -5606,7 +5604,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5622,7 +5620,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -5630,7 +5628,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -5644,7 +5642,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5681,7 +5679,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5689,7 +5687,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5705,7 +5703,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5713,7 +5711,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5729,15 +5727,15 @@
     </row>
     <row r="8" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -5745,13 +5743,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -5759,29 +5757,29 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13" t="s">
         <v>119</v>
-      </c>
-      <c r="D13" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5789,7 +5787,7 @@
         <v>88</v>
       </c>
       <c r="D14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5803,17 +5801,17 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -5844,7 +5842,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5852,7 +5850,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5868,7 +5866,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -5876,7 +5874,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5890,7 +5888,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -5900,13 +5898,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5914,24 +5912,24 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -5939,13 +5937,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5953,24 +5951,24 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -5978,46 +5976,46 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -6025,13 +6023,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6039,24 +6037,24 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
       </c>
       <c r="D21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="92.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C22" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -6064,13 +6062,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6078,35 +6076,35 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C24" t="s">
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C25" t="s">
         <v>7</v>
       </c>
       <c r="D25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C26" t="s">
         <v>7</v>
       </c>
       <c r="D26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6114,13 +6112,13 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C27" t="s">
         <v>7</v>
       </c>
       <c r="D27" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -6128,13 +6126,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C28" t="s">
         <v>7</v>
       </c>
       <c r="D28" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -6260,7 +6258,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6268,7 +6266,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6284,7 +6282,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="304.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -6292,7 +6290,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -6306,13 +6304,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C7" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -6320,21 +6318,21 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
@@ -6348,7 +6346,7 @@
         <v>7</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
@@ -6356,24 +6354,24 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
@@ -6381,13 +6379,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
@@ -6395,13 +6393,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C14" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -6409,24 +6407,24 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C15" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C16" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="17" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6434,345 +6432,345 @@
         <v>4</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B18" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="20" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="22" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C25" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C26" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D26" t="s" ph="1">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C27" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D27" t="s" ph="1">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C28" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D28" t="s" ph="1">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C29" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D29" t="s" ph="1">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C30" t="s" ph="1">
+        <v>269</v>
+      </c>
+      <c r="D30" t="s" ph="1">
         <v>270</v>
-      </c>
-      <c r="D30" t="s" ph="1">
-        <v>271</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C31" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D31" t="s" ph="1">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C32" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D32" t="s" ph="1">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="33" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C33" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D33" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E33"/>
     </row>
     <row r="34" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C34" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D34" t="s" ph="1">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C35" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D35" t="s" ph="1">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C36" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D36" t="s" ph="1">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="37" spans="2:5" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C37" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E37"/>
     </row>
     <row r="38" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C38" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D38" t="s" ph="1">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="39" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="C39" t="s" ph="1">
+        <v>309</v>
+      </c>
+      <c r="D39" t="s" ph="1">
         <v>310</v>
-      </c>
-      <c r="C39" t="s" ph="1">
-        <v>311</v>
-      </c>
-      <c r="D39" t="s" ph="1">
-        <v>312</v>
       </c>
     </row>
     <row r="40" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B40" s="6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C40" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D40" t="s" ph="1">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="41" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B41" s="6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C41" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D41" t="s" ph="1">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="42" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B42" s="6" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C42" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D42" t="s" ph="1">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="43" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B43" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C43" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D43" t="s" ph="1">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="44" spans="2:5" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B44" s="6" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C44" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D44" t="s" ph="1">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="45" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B45" s="6" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C45" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D45" t="s" ph="1">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="46" spans="2:5" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B46" s="6" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C46" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D46" t="s" ph="1">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="47" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B47" s="6" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C47" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D47" t="s" ph="1">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="48" spans="2:5" ph="1" x14ac:dyDescent="0.2">
@@ -6788,115 +6786,116 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.21875" style="6" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B2" s="6" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="6" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B7" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="C7" t="s" ph="1">
+        <v>269</v>
+      </c>
+      <c r="D7" t="s" ph="1">
+        <v>271</v>
+      </c>
+      <c r="E7" ph="1"/>
+    </row>
+    <row r="8" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="6" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s" ph="1">
+      <c r="C8" t="s" ph="1">
+        <v>269</v>
+      </c>
+      <c r="D8" t="s" ph="1">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="C7" t="s" ph="1">
-        <v>270</v>
-      </c>
-      <c r="D7" t="s" ph="1">
+      <c r="C9" t="s" ph="1">
+        <v>269</v>
+      </c>
+      <c r="D9" t="s" ph="1">
         <v>272</v>
       </c>
     </row>
-    <row r="8" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s" ph="1">
-        <v>279</v>
-      </c>
-      <c r="C8" t="s" ph="1">
-        <v>270</v>
-      </c>
-      <c r="D8" t="s" ph="1">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s" ph="1">
-        <v>280</v>
-      </c>
-      <c r="C9" t="s" ph="1">
-        <v>270</v>
-      </c>
-      <c r="D9" t="s" ph="1">
+    <row r="10" spans="1:5" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="6" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" customFormat="1" ht="61.2" ph="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s" ph="1">
+      <c r="D10" t="s" ph="1">
         <v>274</v>
       </c>
-      <c r="D10" t="s" ph="1">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" customFormat="1" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s" ph="1">
+    </row>
+    <row r="11" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="D11" t="s" ph="1">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="D12" t="s" ph="1">
         <v>320</v>
       </c>
-      <c r="D11" t="s" ph="1">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" customFormat="1" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s" ph="1">
-        <v>323</v>
-      </c>
-      <c r="D12" t="s" ph="1">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:5" ht="132" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>92</v>
+      <c r="B13" s="6" t="s">
+        <v>347</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -6905,56 +6904,56 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="79.2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B15" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="D15" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B16" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="D16" t="s">
         <v>327</v>
       </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B17" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="D17" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="D15" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B16" s="1" t="s">
+    <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="D16" t="s">
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
         <v>329</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B17" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="D17" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -6968,7 +6967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B9" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -7009,17 +7008,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7027,7 +7026,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -7041,7 +7040,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -7055,13 +7054,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7069,21 +7068,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D12" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7091,7 +7090,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -7122,7 +7121,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7130,7 +7129,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7146,7 +7145,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -7154,7 +7153,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7262,7 +7261,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -7276,7 +7275,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -7304,7 +7303,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -7318,13 +7317,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -7355,7 +7354,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7363,7 +7362,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7379,7 +7378,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -7387,7 +7386,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7403,44 +7402,44 @@
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7448,13 +7447,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7499,7 +7498,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7507,7 +7506,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7523,7 +7522,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7531,7 +7530,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7547,7 +7546,7 @@
     </row>
     <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -7555,7 +7554,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -7566,7 +7565,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -7574,7 +7573,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -7585,7 +7584,7 @@
     </row>
     <row r="12" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D12" t="s">
         <v>90</v>
@@ -7596,7 +7595,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -7616,7 +7615,7 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7624,13 +7623,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7652,7 +7651,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>4</v>
@@ -7697,7 +7696,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7713,7 +7712,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="264" x14ac:dyDescent="0.2">
@@ -7721,7 +7720,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7815,13 +7814,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7829,7 +7828,7 @@
         <v>88</v>
       </c>
       <c r="D15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7843,7 +7842,7 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7865,7 +7864,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -7940,7 +7939,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -7987,7 +7986,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -8043,7 +8042,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -8057,13 +8056,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8071,13 +8070,13 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8085,13 +8084,13 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8099,13 +8098,13 @@
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="158.4" x14ac:dyDescent="0.2">
@@ -8113,21 +8112,21 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -8224,10 +8223,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8251,7 +8250,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -8275,7 +8274,7 @@
     </row>
     <row r="8" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update win11ja for Google Chrome installation.
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpsuzuki\Documents\2022_03\fresta2022\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECE2168-75EA-4D23-81CB-022B1E8E8AD5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF9520C-B8CB-4506-9A72-C447E6B6F396}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" tabRatio="782" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" tabRatio="782" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
     <sheet name="ch0" sheetId="2" r:id="rId2"/>
     <sheet name="ch1" sheetId="3" r:id="rId3"/>
     <sheet name="ch2" sheetId="6" r:id="rId4"/>
-    <sheet name="ch3" sheetId="5" r:id="rId5"/>
-    <sheet name="ch4" sheetId="12" r:id="rId6"/>
+    <sheet name="ch3" sheetId="12" r:id="rId5"/>
+    <sheet name="ch4" sheetId="5" r:id="rId6"/>
     <sheet name="ch5" sheetId="4" r:id="rId7"/>
     <sheet name="ch6" sheetId="7" r:id="rId8"/>
     <sheet name="ch7" sheetId="8" r:id="rId9"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="352">
   <si>
     <t>header1</t>
   </si>
@@ -60,9 +60,6 @@
   </si>
   <si>
     <t>&lt;h2&gt;この章を始める前に&lt;/h2&gt;</t>
-  </si>
-  <si>
-    <t>win10-2-11.svg</t>
   </si>
   <si>
     <t>無線LANで学内ネットワークに接続できるように設定しましょう。</t>
@@ -258,15 +255,6 @@
   </si>
   <si>
     <t>win10-5-14a.jpg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Chromeのインストールはあっという間に終わります。自動的にChromeが起動して初期設定を行うよう促してきますが、ここでは右上の×をクリックして閉じてください。
-&lt;p class="spl"&gt;※ Windows10にはEdgeというWebブラウザが標準的なものとして付属してきますが、うまく表示できないWebページがときどきあります。そういうときに、「もう一つのブラウザ」としてこのChromeを使ってみてください。&lt;/p&gt;
-  </t>
-    <rPh sb="63" eb="65">
-      <t>ミギウエ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -360,46 +348,6 @@
     <rPh sb="185" eb="186">
       <t>シメ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">「このアプリがデバイスに変更を加えることを許可しますか」と聞かれるので「はい」と答えてください。
-  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">まずGoogle Chromeを入れます。Web上の配布サイトから直接ダウンロードしましょう。
-&lt;a href="https://www.google.com/chrome/"&gt;https://www.google.com/chrome/&lt;/a&gt;
-（または「Chrome インストール」を検索して出てくるChromeダウンロードページ）
-で、「Chromeをダウンロード」をクリックしてください。
-</t>
-    <rPh sb="144" eb="146">
-      <t>ケンサク</t>
-    </rPh>
-    <rPh sb="148" eb="149">
-      <t>デ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Google Chrome 利用規約が表示されるので、「同意してインストール」をクリックします。
-</t>
-    <rPh sb="14" eb="16">
-      <t>リヨウ</t>
-    </rPh>
-    <rPh sb="16" eb="18">
-      <t>キヤク</t>
-    </rPh>
-    <rPh sb="19" eb="21">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="28" eb="30">
-      <t>ドウイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win10-2-42.png</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -536,67 +484,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>&lt;h2&gt;&lt;a name="chrome"&gt;&lt;/a&gt;Google Chromeを入れる&lt;/h2&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win10-2-41.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win10-2-43.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win10-2-44.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>しばらくすると画面の下のところでアイコンが黄色く点滅するので、それをクリックします。
-&lt;p class="spl"&gt;※自動的に画面が切り替わることもありますので、その場合は下の項目に進んでください。&lt;/p&gt;</t>
-    <rPh sb="7" eb="9">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="10" eb="11">
-      <t>シタ</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>キイロ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>テンメツ</t>
-    </rPh>
-    <rPh sb="59" eb="62">
-      <t>ジドウテキ</t>
-    </rPh>
-    <rPh sb="63" eb="65">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="66" eb="67">
-      <t>キ</t>
-    </rPh>
-    <rPh sb="68" eb="69">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="83" eb="85">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="86" eb="87">
-      <t>シタ</t>
-    </rPh>
-    <rPh sb="88" eb="90">
-      <t>コウモク</t>
-    </rPh>
-    <rPh sb="91" eb="92">
-      <t>スス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win10-2-10a.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>win10-4-24.svg</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -610,53 +497,6 @@
   </si>
   <si>
     <t>description</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ダウンロードしたファイルを実行します。
-&lt;p class="spl"&gt;※右の図はWebブラウザにMicrosoft Edgeを使った場合の表示です。他のブラウザを使った場合、表示が少し違うものになりますが「ダウンロードしたファイルを実行する」ことは同じです。</t>
-    <rPh sb="13" eb="15">
-      <t>ジッコウ</t>
-    </rPh>
-    <rPh sb="36" eb="37">
-      <t>ミギ</t>
-    </rPh>
-    <rPh sb="38" eb="39">
-      <t>ズ</t>
-    </rPh>
-    <rPh sb="63" eb="64">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="66" eb="68">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="69" eb="71">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="74" eb="75">
-      <t>タ</t>
-    </rPh>
-    <rPh sb="81" eb="82">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="84" eb="86">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="87" eb="89">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="90" eb="91">
-      <t>スコ</t>
-    </rPh>
-    <rPh sb="92" eb="93">
-      <t>チガ</t>
-    </rPh>
-    <rPh sb="116" eb="118">
-      <t>ジッコウ</t>
-    </rPh>
-    <rPh sb="124" eb="125">
-      <t>オナ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1105,18 +945,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>FRESTA-TEXT-2021 Win10 chap.4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Microsoft Office を使えるようにしましょう。</t>
     <rPh sb="18" eb="19">
       <t>ツカ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Google Chromeのインストール</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1258,24 +1090,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">Windows Update を使って、WindowsとOfficeがつねに最新版で使えるように設定します。
-さらに、Defenderでのフルスキャン（全てのファイルに対するウィルスチェック）のやり方を確認しておきます。
-&lt;ul&gt;&lt;li&gt;&lt;a href="#windows_update"&gt;Windows Updateの設定&lt;/a&gt;
-&lt;/li&gt;
-&lt;li&gt;&lt;a href="#defender"&gt;Defenderの手動更新とフルスキャン&lt;/a&gt;
-&lt;/li&gt;
- &lt;/ul&gt;
-この章は、インターネットに接続していれば、広島大学の学生証をもらう前に実施することができます。 
- </t>
-    <rPh sb="240" eb="242">
-      <t>ジタク</t>
-    </rPh>
-    <rPh sb="251" eb="253">
-      <t>セツゾク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">Bb9で配布されている教材をダウンロードできることを確認するため、「ノートパソコン点検届」のコースをみてみましょう。
 まず、コース一覧から「ノートパソコン点検届2021」をクリックしてコースを開きましょう。
   </t>
@@ -1353,16 +1167,6 @@
   </si>
   <si>
     <t>FRESTA-TEXT-2021 Win10 App.A</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">ここでは、Google Chrome のインストールを行います。
-&lt;ul&gt;
-&lt;li&gt;
-&lt;a href="#chrome"&gt;Google Chromeのインストール&lt;/a&gt;
-&lt;/li&gt;
-&lt;/ul&gt;
- </t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -5118,6 +4922,475 @@
   </si>
   <si>
     <t>初期設定 (学生番号が無くても可能です)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Windows Update を使って、WindowsとOfficeがつねに最新版で使えるように設定します。
+さらに、Defenderでのフルスキャン（全てのファイルに対するウィルスチェック）のやり方を確認しておきます。
+&lt;ul&gt;&lt;li&gt;&lt;a href="#windows_update"&gt;Windows Updateの設定&lt;/a&gt;
+&lt;/li&gt;
+&lt;li&gt;&lt;a href="#defender"&gt;Defenderでのフルスキャン&lt;/a&gt;
+&lt;/li&gt;
+ &lt;/ul&gt;
+この章は、インターネットに接続していれば、広島大学の学生証をもらう前に実施することができます。 
+ </t>
+    <rPh sb="236" eb="238">
+      <t>ジタク</t>
+    </rPh>
+    <rPh sb="247" eb="249">
+      <t>セツゾク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2021 Win11 chap.4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Google Chromeのインストール (学生番号が無くても可能です)</t>
+    <rPh sb="22" eb="24">
+      <t>ガクセイ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>バンゴウ</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>ナ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>カノウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ここでは、Microsoft Edgeの初期設定とGoogle Chrome のインストールを行います。
+&lt;ul&gt;
+&lt;li&gt;
+&lt;a href="#chrome"&gt;Google Chromeのインストール&lt;/a&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+ </t>
+    <rPh sb="20" eb="22">
+      <t>ショキ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>セッテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>まず画面の最下部のタスクバーに「e」を模した青緑のアイコンがありますので、これをクリックしてMicrosoft Edgeを起動します。</t>
+    <rPh sb="2" eb="4">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="5" eb="8">
+      <t>サイカブ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>アオミドリ</t>
+    </rPh>
+    <rPh sb="61" eb="63">
+      <t>キドウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>起動すると他のブラウザの情報を取り込もうとしますが、まだ無いので、チェックを外し、ユーザデータを使用せずに開始をクリックします。</t>
+    <rPh sb="0" eb="2">
+      <t>キドウ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ホカ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>コ</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>ナ</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>ハズ</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="53" eb="55">
+      <t>カイシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ターゲット広告を行う「Webエクスペリエンスのカスタマイズ」のチェックも外した上で開始します。</t>
+    <rPh sb="5" eb="7">
+      <t>コウコク</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>ハズ</t>
+    </rPh>
+    <rPh sb="39" eb="40">
+      <t>ウエ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>カイシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ブラウザの配色設定をしようとしますが、かまっている時間がないので、上段の「+」ボタンを押して新規のタブを開きます。</t>
+    <rPh sb="5" eb="7">
+      <t>ハイショク</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>ジカン</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>ジョウダン</t>
+    </rPh>
+    <rPh sb="43" eb="44">
+      <t>オ</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>シンキ</t>
+    </rPh>
+    <rPh sb="52" eb="53">
+      <t>ヒラ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Edgeの規定の新規タブには大量の広告が入ってくるので、オンライン授業などで画面共有の際に憚られるような画面になる場合があります。右上の歯車アイコンを押して、画面レイアウトを「シンプル」にしましょう。これでEdgeの基本的な設定は終わります。</t>
+    <rPh sb="5" eb="7">
+      <t>キテイ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>シンキ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>タイリョウ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>コウコク</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>ハイ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>ジュギョウ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>キョウユウ</t>
+    </rPh>
+    <rPh sb="43" eb="44">
+      <t>サイ</t>
+    </rPh>
+    <rPh sb="45" eb="46">
+      <t>ハバカ</t>
+    </rPh>
+    <rPh sb="52" eb="54">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="57" eb="59">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="65" eb="66">
+      <t>ミギ</t>
+    </rPh>
+    <rPh sb="66" eb="67">
+      <t>ウエ</t>
+    </rPh>
+    <rPh sb="68" eb="70">
+      <t>ハグルマ</t>
+    </rPh>
+    <rPh sb="75" eb="76">
+      <t>オ</t>
+    </rPh>
+    <rPh sb="79" eb="81">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="108" eb="111">
+      <t>キホンテキ</t>
+    </rPh>
+    <rPh sb="112" eb="114">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="115" eb="116">
+      <t>オ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ブラウザの最上部は本来はwww.microsoft.comなどのURL(ホームページアドレスなどと呼ばれることがあります)を入れるものですが、多くのブラウザが検索フォームも兼ねています。ここにGoogle Chrome downloadと入れてみましょう。Microsoftが入れてほしくなさそうな広告を入れてきますが、無視してGoogleからダウンロードします。
+ここで注意しないといけないのは、「Google Chromeのダウンロード」と称してウイルスをダウンロードさせるようなサイトが検索の上位に来る可能性があるということです。URLがwww.google.comになっていることを確認した上でジャンプしましょう。</t>
+    <rPh sb="5" eb="6">
+      <t>サイ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ジョウブ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ホンライ</t>
+    </rPh>
+    <rPh sb="49" eb="50">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="62" eb="63">
+      <t>イ</t>
+    </rPh>
+    <rPh sb="71" eb="72">
+      <t>オオ</t>
+    </rPh>
+    <rPh sb="79" eb="81">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="86" eb="87">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="119" eb="120">
+      <t>イ</t>
+    </rPh>
+    <rPh sb="138" eb="139">
+      <t>イ</t>
+    </rPh>
+    <rPh sb="149" eb="151">
+      <t>コウコク</t>
+    </rPh>
+    <rPh sb="152" eb="153">
+      <t>イ</t>
+    </rPh>
+    <rPh sb="160" eb="162">
+      <t>ムシ</t>
+    </rPh>
+    <rPh sb="186" eb="188">
+      <t>チュウイ</t>
+    </rPh>
+    <rPh sb="222" eb="223">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="246" eb="248">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="249" eb="251">
+      <t>ジョウイ</t>
+    </rPh>
+    <rPh sb="252" eb="253">
+      <t>ク</t>
+    </rPh>
+    <rPh sb="254" eb="257">
+      <t>カノウセイ</t>
+    </rPh>
+    <rPh sb="295" eb="297">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="299" eb="300">
+      <t>ウエ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Googleのダウンロードページにジャンプしました。Google Chromeのブラウザ内部のデータをGoogleに送信しても良いかという許可チェックボックスがありますが、このチェックを外してダウンロードを行います。</t>
+    <rPh sb="44" eb="46">
+      <t>ナイブ</t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t>ソウシン</t>
+    </rPh>
+    <rPh sb="63" eb="64">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="69" eb="71">
+      <t>キョカ</t>
+    </rPh>
+    <rPh sb="93" eb="94">
+      <t>ハズ</t>
+    </rPh>
+    <rPh sb="103" eb="104">
+      <t>オコナ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ダウンロードが終わるとEdgeの右上に「↓」マークが現れます。これに緑のマークがついていたらダウンロードが完了しています。「↓」をクリックしてダウンロードしたファイルのリストを出し、右横のフォルダアイコンをクリックします。マウスポインタを持っていかないとフォルダアイコンが出ないので気をつけてください。</t>
+    <rPh sb="7" eb="8">
+      <t>オ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>ミギウエ</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>アラワ</t>
+    </rPh>
+    <rPh sb="34" eb="35">
+      <t>ミドリ</t>
+    </rPh>
+    <rPh sb="53" eb="55">
+      <t>カンリョウ</t>
+    </rPh>
+    <rPh sb="88" eb="89">
+      <t>ダ</t>
+    </rPh>
+    <rPh sb="91" eb="93">
+      <t>ミギヨコ</t>
+    </rPh>
+    <rPh sb="119" eb="120">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="136" eb="137">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="141" eb="142">
+      <t>キ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ファイル操作のためのウィンドウ(エクスプローラ）が開きます。ダウンロードしたGoogleChromeファイルを左側のクイックアクセスにあるデスクトップフォルダに移動しましょう。</t>
+    <rPh sb="4" eb="6">
+      <t>ソウサ</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="55" eb="57">
+      <t>ヒダリガワ</t>
+    </rPh>
+    <rPh sb="80" eb="82">
+      <t>イドウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Edgeやエクスプローラのウィンドウを閉じてデスクトップを出すとGoogleChromeファイルがデスクトップにあります。これをクリックしてインストールを開始します。</t>
+    <rPh sb="19" eb="20">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>ダ</t>
+    </rPh>
+    <rPh sb="77" eb="79">
+      <t>カイシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「このアプリがデバイスに変更を加えることを許可しますか?」と確認を求められます。「確認済みの発行先: Google LLC」となっていることを確認し、「はい」で進めます。Google Chrome本体のダウンロードが開始されます。</t>
+    <rPh sb="12" eb="14">
+      <t>ヘンコウ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>クワ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>キョカ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>モト</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="43" eb="44">
+      <t>ズ</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>ハッコウ</t>
+    </rPh>
+    <rPh sb="48" eb="49">
+      <t>サキ</t>
+    </rPh>
+    <rPh sb="71" eb="73">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="80" eb="81">
+      <t>スス</t>
+    </rPh>
+    <rPh sb="98" eb="100">
+      <t>ホンタイ</t>
+    </rPh>
+    <rPh sb="108" eb="110">
+      <t>カイシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>完了するとGoogle Chromeが自動的に起動します。</t>
+    <rPh sb="0" eb="2">
+      <t>カンリョウ</t>
+    </rPh>
+    <rPh sb="19" eb="22">
+      <t>ジドウテキ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>キドウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-start-edge-taskbar.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-edge-prep1.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-edge-prep2.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-edge-prep3.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-edge-layout.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-edge-search-chrome.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-google-chrome-download-page.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-edge-download-file.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-explorer.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-google-chrome-desktop.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-chrome-install-check.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-chrome-hello.png</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -5540,7 +5813,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5556,7 +5829,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -5564,7 +5837,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>201</v>
+        <v>184</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -5578,7 +5851,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5615,7 +5888,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5623,7 +5896,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5639,7 +5912,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5647,7 +5920,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5663,15 +5936,15 @@
     </row>
     <row r="8" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="D8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -5679,13 +5952,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -5693,37 +5966,37 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="D12" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="D13" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D14" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5731,23 +6004,23 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -5778,7 +6051,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5786,7 +6059,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5802,7 +6075,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -5810,7 +6083,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5824,7 +6097,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -5834,13 +6107,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5848,24 +6121,24 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -5873,13 +6146,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5887,24 +6160,24 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -5912,46 +6185,46 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -5959,13 +6232,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -5973,24 +6246,24 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
       </c>
       <c r="D21" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="92.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
       <c r="C22" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="D22" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -5998,13 +6271,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6012,35 +6285,35 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="C24" t="s">
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="C25" t="s">
         <v>7</v>
       </c>
       <c r="D25" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
       <c r="C26" t="s">
         <v>7</v>
       </c>
       <c r="D26" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6048,13 +6321,13 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="C27" t="s">
         <v>7</v>
       </c>
       <c r="D27" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -6062,13 +6335,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="C28" t="s">
         <v>7</v>
       </c>
       <c r="D28" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -6176,7 +6449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -6194,7 +6467,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>304</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6202,7 +6475,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>340</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6218,7 +6491,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="304.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -6226,7 +6499,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -6240,13 +6513,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>309</v>
+        <v>292</v>
       </c>
       <c r="C7" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>202</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -6254,21 +6527,21 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>306</v>
+        <v>289</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>203</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>204</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
@@ -6276,13 +6549,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C10" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>205</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
@@ -6290,24 +6563,24 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>206</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>207</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
@@ -6315,13 +6588,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>209</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
@@ -6329,13 +6602,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
       <c r="C14" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>210</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -6343,24 +6616,24 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
       <c r="C15" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>211</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="C16" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>214</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6368,345 +6641,345 @@
         <v>4</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>216</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B18" s="6" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>218</v>
+        <v>201</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>219</v>
+        <v>202</v>
       </c>
     </row>
     <row r="20" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>222</v>
+        <v>205</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>221</v>
+        <v>204</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>223</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>226</v>
+        <v>209</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>227</v>
+        <v>210</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>241</v>
+        <v>224</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
       <c r="C25" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>231</v>
+        <v>214</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="C26" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D26" t="s" ph="1">
-        <v>232</v>
+        <v>215</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
       <c r="C27" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D27" t="s" ph="1">
-        <v>235</v>
+        <v>218</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="C28" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D28" t="s" ph="1">
-        <v>236</v>
+        <v>219</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="C29" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D29" t="s" ph="1">
-        <v>238</v>
+        <v>221</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>248</v>
+        <v>231</v>
       </c>
       <c r="C30" t="s" ph="1">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="D30" t="s" ph="1">
-        <v>243</v>
+        <v>226</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
       <c r="C31" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D31" t="s" ph="1">
-        <v>266</v>
+        <v>249</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
-        <v>265</v>
+        <v>248</v>
       </c>
       <c r="C32" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D32" t="s" ph="1">
-        <v>267</v>
+        <v>250</v>
       </c>
     </row>
     <row r="33" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="C33" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D33" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="E33"/>
     </row>
     <row r="34" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="C34" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D34" t="s" ph="1">
-        <v>252</v>
+        <v>235</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
       <c r="C35" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D35" t="s" ph="1">
-        <v>253</v>
+        <v>236</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
       <c r="C36" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D36" t="s" ph="1">
-        <v>254</v>
+        <v>237</v>
       </c>
     </row>
     <row r="37" spans="2:5" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
       <c r="C37" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="E37"/>
     </row>
     <row r="38" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
       <c r="C38" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D38" t="s" ph="1">
-        <v>256</v>
+        <v>239</v>
       </c>
     </row>
     <row r="39" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="C39" t="s" ph="1">
-        <v>282</v>
+        <v>265</v>
       </c>
       <c r="D39" t="s" ph="1">
-        <v>283</v>
+        <v>266</v>
       </c>
     </row>
     <row r="40" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B40" s="6" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="C40" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D40" t="s" ph="1">
-        <v>257</v>
+        <v>240</v>
       </c>
     </row>
     <row r="41" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B41" s="6" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
       <c r="C41" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D41" t="s" ph="1">
-        <v>258</v>
+        <v>241</v>
       </c>
     </row>
     <row r="42" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B42" s="6" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="C42" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D42" t="s" ph="1">
-        <v>260</v>
+        <v>243</v>
       </c>
     </row>
     <row r="43" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B43" s="6" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="C43" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D43" t="s" ph="1">
-        <v>261</v>
+        <v>244</v>
       </c>
     </row>
     <row r="44" spans="2:5" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B44" s="6" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
       <c r="C44" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D44" t="s" ph="1">
-        <v>262</v>
+        <v>245</v>
       </c>
     </row>
     <row r="45" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B45" s="6" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
       <c r="C45" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D45" t="s" ph="1">
-        <v>286</v>
+        <v>269</v>
       </c>
     </row>
     <row r="46" spans="2:5" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B46" s="6" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="C46" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D46" t="s" ph="1">
-        <v>263</v>
+        <v>246</v>
       </c>
     </row>
     <row r="47" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B47" s="6" t="s">
-        <v>287</v>
+        <v>270</v>
       </c>
       <c r="C47" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D47" t="s" ph="1">
-        <v>288</v>
+        <v>271</v>
       </c>
     </row>
     <row r="48" spans="2:5" ph="1" x14ac:dyDescent="0.2">
@@ -6741,7 +7014,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -6749,7 +7022,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>339</v>
+        <v>322</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -6765,65 +7038,65 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>317</v>
+        <v>300</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="C7" t="s" ph="1">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>244</v>
+        <v>227</v>
       </c>
       <c r="E7" ph="1"/>
     </row>
     <row r="8" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="C8" t="s" ph="1">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>302</v>
+        <v>285</v>
       </c>
     </row>
     <row r="9" spans="1:5" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
       <c r="C9" t="s" ph="1">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>245</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:5" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>247</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>289</v>
+        <v>272</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>290</v>
+        <v>273</v>
       </c>
     </row>
     <row r="12" spans="1:5" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>292</v>
+        <v>275</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>291</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="132" x14ac:dyDescent="0.2">
@@ -6831,7 +7104,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>318</v>
+        <v>301</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -6845,37 +7118,37 @@
         <v>4</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>296</v>
+        <v>279</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>297</v>
+        <v>280</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>301</v>
+        <v>284</v>
       </c>
       <c r="D15" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>293</v>
+        <v>276</v>
       </c>
       <c r="D16" t="s">
-        <v>298</v>
+        <v>281</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>294</v>
+        <v>277</v>
       </c>
       <c r="D17" t="s">
-        <v>299</v>
+        <v>282</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6883,13 +7156,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>295</v>
+        <v>278</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>300</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -6903,8 +7176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView zoomScale="112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A4" zoomScale="112" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -6920,7 +7193,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>320</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6928,7 +7201,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>338</v>
+        <v>321</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6944,7 +7217,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>337</v>
+        <v>320</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -6952,7 +7225,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>129</v>
+        <v>324</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6963,7 +7236,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6971,13 +7244,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>322</v>
+        <v>305</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>321</v>
+        <v>304</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6985,13 +7258,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>323</v>
+        <v>306</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>324</v>
+        <v>307</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -6999,7 +7272,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>325</v>
+        <v>308</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -7010,7 +7283,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>326</v>
+        <v>309</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -7021,21 +7294,21 @@
         <v>4</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>327</v>
+        <v>310</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>328</v>
+        <v>311</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>329</v>
+        <v>312</v>
       </c>
       <c r="D13" t="s">
-        <v>330</v>
+        <v>313</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -7043,13 +7316,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>331</v>
+        <v>314</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>332</v>
+        <v>315</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7057,13 +7330,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>333</v>
+        <v>316</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>335</v>
+        <v>318</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -7071,13 +7344,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>334</v>
+        <v>317</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>336</v>
+        <v>319</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -7112,11 +7385,192 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C43F54BA-B356-43A4-B76F-707ED0C70724}">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="82.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="30.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D9" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D10" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="D11" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="D12" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="D13" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="D14" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="D15" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D16" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D17" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D18" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="D19" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="D20" t="s">
+        <v>351</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -7132,7 +7586,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7140,7 +7594,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7156,17 +7610,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7174,13 +7628,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -7188,13 +7642,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7202,13 +7656,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>310</v>
+        <v>293</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>311</v>
+        <v>294</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7216,21 +7670,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>312</v>
+        <v>295</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>313</v>
+        <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>314</v>
+        <v>297</v>
       </c>
       <c r="D12" t="s">
-        <v>315</v>
+        <v>298</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7238,151 +7692,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>316</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C43F54BA-B356-43A4-B76F-707ED0C70724}">
-  <dimension ref="A1:D15"/>
-  <sheetViews>
-    <sheetView zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="66" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D10" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D13" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="66" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>10</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -7413,7 +7723,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7421,7 +7731,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7437,7 +7747,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7445,7 +7755,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7461,7 +7771,7 @@
     </row>
     <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -7469,18 +7779,18 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -7488,21 +7798,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="D12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7510,13 +7820,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7524,13 +7834,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7538,13 +7848,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7552,13 +7862,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="4" customFormat="1" ht="92.4" x14ac:dyDescent="0.2">
@@ -7566,13 +7876,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -7603,7 +7913,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7611,7 +7921,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7627,7 +7937,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="264" x14ac:dyDescent="0.2">
@@ -7635,7 +7945,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7646,7 +7956,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -7668,13 +7978,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
         <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7682,18 +7992,18 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -7715,13 +8025,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7729,21 +8039,21 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D15" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7751,13 +8061,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7765,13 +8075,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
         <v>27</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>28</v>
-      </c>
-      <c r="D17" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -7779,13 +8089,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7793,13 +8103,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
         <v>31</v>
-      </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -7807,18 +8117,18 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
         <v>33</v>
-      </c>
-      <c r="C20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -7840,13 +8150,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
         <v>36</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7854,13 +8164,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7868,18 +8178,18 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
         <v>39</v>
-      </c>
-      <c r="C25" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -7901,13 +8211,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7915,13 +8225,13 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
         <v>43</v>
-      </c>
-      <c r="C29" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -7929,13 +8239,13 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
         <v>45</v>
-      </c>
-      <c r="C30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7943,13 +8253,13 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
         <v>47</v>
-      </c>
-      <c r="C31" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="184.8" x14ac:dyDescent="0.2">
@@ -7957,13 +8267,13 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7971,13 +8281,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -7985,13 +8295,13 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7999,13 +8309,13 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8013,13 +8323,13 @@
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="158.4" x14ac:dyDescent="0.2">
@@ -8027,26 +8337,26 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="D38" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8054,7 +8364,7 @@
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C40" t="s">
         <v>4</v>
@@ -8068,13 +8378,13 @@
         <v>4</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C41" t="s">
         <v>7</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -8082,21 +8392,21 @@
         <v>4</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C42" t="s">
         <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D43" t="s" ph="1">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -8104,13 +8414,13 @@
         <v>4</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C44" t="s">
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -8138,10 +8448,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8149,7 +8459,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8165,7 +8475,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -8173,7 +8483,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8184,17 +8494,17 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -8202,7 +8512,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
win11ja: update for Teams
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpsuzuki\Documents\2022_03\fresta2022\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89397D4-E97B-4780-BF69-97DEF637516E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA9D3F9-7640-43F3-8739-753A28082C41}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" tabRatio="782" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="351">
   <si>
     <t>header1</t>
   </si>
@@ -806,25 +806,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>このPCを組織が管理できるようにしますか、と質問されますが、このチェックを外し、「このアプリのみにサインインする」を選びましょう。</t>
-    <rPh sb="5" eb="7">
-      <t>ソシキ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>カンリ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>シツモン</t>
-    </rPh>
-    <rPh sb="37" eb="38">
-      <t>ハズ</t>
-    </rPh>
-    <rPh sb="58" eb="59">
-      <t>エラ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>サインインしたアカウントには、そのアカウントのネット接続状態が表示されます。「会議」に出席している場合は、この接続状態が「会議中」になります。</t>
     <rPh sb="26" eb="28">
       <t>セツゾク</t>
@@ -987,27 +968,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ch7-teams-start0.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ch7-teams-account.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ch7-teams-password.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ch7-teams-signin-limited.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>ch7-teams-signined0.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ch7-teams-lookup-teams.png</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1230,89 +1191,6 @@
     </rPh>
     <rPh sb="107" eb="108">
       <t>ツク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ch7-teams-firewall.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>場合によっては、Teamsの通信についてWindows内蔵のファイヤーウォールが許可して大丈夫か確認を求められます。大学の無線LANやネットカフェなど様々な人が使うネットワークに接続している場合、なぜか「非推奨」となっているパブリックネットワークにチェックが入っていて、そうしないといけないかのような雰囲気を出しますが、「キャンセル」で許可しない状態を維持しても大きな問題は起きません。</t>
-    <rPh sb="0" eb="2">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>ツウシン</t>
-    </rPh>
-    <rPh sb="27" eb="29">
-      <t>ナイゾウ</t>
-    </rPh>
-    <rPh sb="40" eb="42">
-      <t>キョカ</t>
-    </rPh>
-    <rPh sb="44" eb="47">
-      <t>ダイジョウブ</t>
-    </rPh>
-    <rPh sb="48" eb="50">
-      <t>カクニン</t>
-    </rPh>
-    <rPh sb="51" eb="52">
-      <t>モト</t>
-    </rPh>
-    <rPh sb="58" eb="60">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="61" eb="63">
-      <t>ムセン</t>
-    </rPh>
-    <rPh sb="75" eb="77">
-      <t>サマザマ</t>
-    </rPh>
-    <rPh sb="78" eb="79">
-      <t>ヒト</t>
-    </rPh>
-    <rPh sb="80" eb="81">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="89" eb="91">
-      <t>セツゾク</t>
-    </rPh>
-    <rPh sb="95" eb="97">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="102" eb="103">
-      <t>ヒ</t>
-    </rPh>
-    <rPh sb="103" eb="105">
-      <t>スイショウ</t>
-    </rPh>
-    <rPh sb="129" eb="130">
-      <t>ハイ</t>
-    </rPh>
-    <rPh sb="150" eb="153">
-      <t>フンイキ</t>
-    </rPh>
-    <rPh sb="154" eb="155">
-      <t>ダ</t>
-    </rPh>
-    <rPh sb="168" eb="170">
-      <t>キョカ</t>
-    </rPh>
-    <rPh sb="173" eb="175">
-      <t>ジョウタイ</t>
-    </rPh>
-    <rPh sb="176" eb="178">
-      <t>イジ</t>
-    </rPh>
-    <rPh sb="181" eb="182">
-      <t>オオ</t>
-    </rPh>
-    <rPh sb="184" eb="186">
-      <t>モンダイ</t>
-    </rPh>
-    <rPh sb="187" eb="188">
-      <t>オ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -2074,51 +1952,6 @@
     </rPh>
     <rPh sb="181" eb="183">
       <t>サンショウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>はじめてTeamsを起動すると、Microsoft Officeのアクティベーションと同様のサインインを促されます。広島大学のオンライン授業を受けるには、アカウント名でサインインが必要です。</t>
-    <rPh sb="10" eb="12">
-      <t>キドウ</t>
-    </rPh>
-    <rPh sb="43" eb="45">
-      <t>ドウヨウ</t>
-    </rPh>
-    <rPh sb="52" eb="53">
-      <t>ウナガ</t>
-    </rPh>
-    <rPh sb="58" eb="60">
-      <t>ヒロシマ</t>
-    </rPh>
-    <rPh sb="68" eb="70">
-      <t>ジュギョウ</t>
-    </rPh>
-    <rPh sb="71" eb="72">
-      <t>ウ</t>
-    </rPh>
-    <rPh sb="90" eb="92">
-      <t>ヒツヨウダイガク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>まずアカウント名(@hiroshima-u.ac.jpを含め)を入力します。</t>
-    <rPh sb="28" eb="29">
-      <t>フク</t>
-    </rPh>
-    <rPh sb="32" eb="34">
-      <t>ニュウリョク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>次にアカウント名のパスワードを入力します。</t>
-    <rPh sb="0" eb="1">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>ニュウリョク</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -5422,80 +5255,138 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>包括ライセンスでMicrosoft Office365をインストールした場合は、Microsoft Teamsは既にインストールされている筈です。タスクバーの検索フォームで「Teams」を検索すれば出てくる筈です。
-もし別途Officeを購入したため、Microsoft Teamsがまだ入っていないという場合は、https://www.microsoft.com/ja-jp/microsoft-teams/download-app からダウンロードしてインストールしてください(Office365と違ってアカウントにサインインしなくてもダウンロードできます)。また、iOS機器(iPhone, iPad)やAndroid機器でも動きますが、ここではPCでの確認手順を説明します。</t>
-    <rPh sb="0" eb="2">
-      <t>ホウカツ</t>
-    </rPh>
-    <rPh sb="36" eb="38">
+    <t>win11-teams-variants.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Microsoft Teamsには「職場または学校用」のものと、「小企業用」のものの2つがあります。自分のPCのタスクバーの検索フォームから「Teams」を検索すると、「学校用Teamsだけが有る」「学校用と小企業用Teamsがある」「小企業用Teamsだけがある」の3つの可能性があります。アイコンが少し違います。</t>
+    <rPh sb="50" eb="52">
+      <t>ジブン</t>
+    </rPh>
+    <rPh sb="62" eb="64">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="78" eb="80">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="85" eb="87">
+      <t>ガッコウ</t>
+    </rPh>
+    <rPh sb="87" eb="88">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="96" eb="97">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="100" eb="102">
+      <t>ガッコウ</t>
+    </rPh>
+    <rPh sb="102" eb="103">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="104" eb="107">
+      <t>ショウキギョウ</t>
+    </rPh>
+    <rPh sb="107" eb="108">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="118" eb="121">
+      <t>ショウキギョウ</t>
+    </rPh>
+    <rPh sb="121" eb="122">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="137" eb="140">
+      <t>カノウセイ</t>
+    </rPh>
+    <rPh sb="151" eb="152">
+      <t>スコ</t>
+    </rPh>
+    <rPh sb="153" eb="154">
+      <t>チガ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-teams-first-dialog.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Teamsを起動します。学校用Teamsの場合には「職場または…」とメッセージが出ますが、小企業用Teamsはサインインのメニューがあり、「職場学校用Teamsのダウンロード」リンクがあります。お使いのPCに学校用Teamsが無い場合には、このリンクからダウンロードしてインストールし、学校用Teamsを起動しなおしてください。
+学校用Teamsの「開始する」で進めます。</t>
+    <rPh sb="6" eb="8">
+      <t>キドウ</t>
+    </rPh>
+    <rPh sb="12" eb="15">
+      <t>ガッコウヨウ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
       <t>バアイ</t>
     </rPh>
-    <rPh sb="56" eb="57">
-      <t>スデ</t>
-    </rPh>
-    <rPh sb="69" eb="70">
-      <t>ハズ</t>
-    </rPh>
-    <rPh sb="79" eb="81">
-      <t>ケンサク</t>
-    </rPh>
-    <rPh sb="94" eb="96">
-      <t>ケンサク</t>
-    </rPh>
-    <rPh sb="99" eb="100">
+    <rPh sb="26" eb="28">
+      <t>ショクバ</t>
+    </rPh>
+    <rPh sb="40" eb="41">
       <t>デ</t>
     </rPh>
-    <rPh sb="103" eb="104">
-      <t>ハズ</t>
-    </rPh>
-    <rPh sb="110" eb="112">
-      <t>ベット</t>
-    </rPh>
-    <rPh sb="119" eb="121">
-      <t>コウニュウ</t>
-    </rPh>
-    <rPh sb="144" eb="145">
-      <t>ハイ</t>
-    </rPh>
-    <rPh sb="153" eb="155">
+    <rPh sb="45" eb="48">
+      <t>ショウキギョウ</t>
+    </rPh>
+    <rPh sb="48" eb="49">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="70" eb="72">
+      <t>ショクバ</t>
+    </rPh>
+    <rPh sb="72" eb="74">
+      <t>ガッコウ</t>
+    </rPh>
+    <rPh sb="74" eb="75">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="98" eb="99">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="104" eb="107">
+      <t>ガッコウヨウ</t>
+    </rPh>
+    <rPh sb="113" eb="114">
+      <t>ナ</t>
+    </rPh>
+    <rPh sb="115" eb="117">
       <t>バアイ</t>
     </rPh>
-    <rPh sb="251" eb="252">
-      <t>チガ</t>
-    </rPh>
-    <rPh sb="288" eb="290">
-      <t>キキ</t>
-    </rPh>
-    <rPh sb="312" eb="314">
-      <t>キキ</t>
-    </rPh>
-    <rPh sb="316" eb="317">
-      <t>ウゴ</t>
-    </rPh>
-    <rPh sb="330" eb="332">
-      <t>カクニン</t>
-    </rPh>
-    <rPh sb="332" eb="334">
-      <t>テジュン</t>
-    </rPh>
-    <rPh sb="335" eb="337">
-      <t>セツメイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Teamsのアイコンがスタートメニューにない場合は、検索フォームから「t」または「te」と入力して検索してください。</t>
-    <rPh sb="22" eb="24">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>ケンサク</t>
+    <rPh sb="143" eb="146">
+      <t>ガッコウヨウ</t>
+    </rPh>
+    <rPh sb="152" eb="154">
+      <t>キドウ</t>
+    </rPh>
+    <rPh sb="165" eb="168">
+      <t>ガッコウヨウ</t>
+    </rPh>
+    <rPh sb="175" eb="177">
+      <t>カイシ</t>
+    </rPh>
+    <rPh sb="181" eb="182">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-teams-signin.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IMCアカウント(@hiroshima-u.ac.jpを含む)を入力し、さらにパスワードも入力してサインインします。</t>
+    <rPh sb="28" eb="29">
+      <t>フク</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>ニュウリョク</t>
     </rPh>
     <rPh sb="45" eb="47">
       <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="49" eb="51">
-      <t>ケンサク</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -5919,7 +5810,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5935,7 +5826,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -5943,7 +5834,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -5994,7 +5885,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6002,7 +5893,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6018,7 +5909,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6042,7 +5933,7 @@
     </row>
     <row r="8" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D8" t="s">
         <v>65</v>
@@ -6050,7 +5941,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6058,10 +5949,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="D10" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6069,50 +5960,50 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="D11" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="D12" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
       <c r="D13" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
       <c r="D14" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="D15" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="D16" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6120,26 +6011,26 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="D17" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="D18" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="D19" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -6151,16 +6042,16 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DB449D4-AFC1-462F-B851-41C4675E501D}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="75.77734375" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
     <col min="4" max="4" width="38.33203125" customWidth="1"/>
   </cols>
@@ -6170,7 +6061,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6178,7 +6069,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6194,7 +6085,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -6202,7 +6093,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6211,28 +6102,31 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
+    <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>346</v>
+      </c>
+      <c r="D8" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="D9" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
+        <v>350</v>
       </c>
       <c r="D10" t="s">
-        <v>105</v>
+        <v>349</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6240,44 +6134,41 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>142</v>
+        <v>341</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>100</v>
+        <v>340</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
       <c r="B12" s="1" t="s">
-        <v>143</v>
+        <v>115</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
       <c r="B14" s="1" t="s">
         <v>93</v>
       </c>
@@ -6285,182 +6176,150 @@
         <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
       <c r="B17" s="1" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="92.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>94</v>
+        <v>134</v>
       </c>
       <c r="C18" t="s">
-        <v>7</v>
+        <v>118</v>
       </c>
       <c r="D18" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
       <c r="B19" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>4</v>
-      </c>
       <c r="B21" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
       </c>
       <c r="D21" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="92.4" customHeight="1" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="C22" t="s">
-        <v>126</v>
+        <v>7</v>
       </c>
       <c r="D22" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C24" t="s">
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C25" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="66" x14ac:dyDescent="0.2">
-      <c r="B26" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C27" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>4</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C28" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" t="s">
-        <v>124</v>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -6468,6 +6327,11 @@
         <v>4</v>
       </c>
     </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>4</v>
@@ -6503,16 +6367,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>4</v>
-      </c>
-    </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>4</v>
@@ -6522,40 +6376,36 @@
       <c r="A42" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>4</v>
-      </c>
+      <c r="B42" s="5"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="D45" ph="1"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="5"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="D49" ph="1"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="D52" ph="1"/>
+    </row>
+    <row r="48" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="D48" ph="1"/>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D51" ph="1"/>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D54" ph="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -6586,7 +6436,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6594,7 +6444,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6610,7 +6460,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="304.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -6618,7 +6468,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -6632,13 +6482,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="C7" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>150</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -6646,21 +6496,21 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>152</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
@@ -6674,7 +6524,7 @@
         <v>7</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
@@ -6682,24 +6532,24 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>154</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>155</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
@@ -6707,13 +6557,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>157</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
@@ -6721,13 +6571,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="C14" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>158</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -6735,24 +6585,24 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="C15" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>159</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C16" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>162</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6760,345 +6610,345 @@
         <v>4</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>164</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B18" s="6" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>166</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>167</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>171</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>174</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>175</v>
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>189</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="C25" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>179</v>
+        <v>168</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="C26" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D26" t="s" ph="1">
-        <v>180</v>
+        <v>169</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="C27" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D27" t="s" ph="1">
-        <v>183</v>
+        <v>172</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="C28" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D28" t="s" ph="1">
-        <v>184</v>
+        <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="C29" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D29" t="s" ph="1">
-        <v>186</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="C30" t="s" ph="1">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="D30" t="s" ph="1">
-        <v>191</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="C31" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D31" t="s" ph="1">
-        <v>214</v>
+        <v>203</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="C32" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D32" t="s" ph="1">
-        <v>215</v>
+        <v>204</v>
       </c>
     </row>
     <row r="33" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="C33" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D33" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="E33"/>
     </row>
     <row r="34" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="C34" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D34" t="s" ph="1">
-        <v>200</v>
+        <v>189</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="C35" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D35" t="s" ph="1">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="C36" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D36" t="s" ph="1">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="37" spans="2:5" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="C37" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="E37"/>
     </row>
     <row r="38" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="C38" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D38" t="s" ph="1">
-        <v>204</v>
+        <v>193</v>
       </c>
     </row>
     <row r="39" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="C39" t="s" ph="1">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="D39" t="s" ph="1">
-        <v>231</v>
+        <v>220</v>
       </c>
     </row>
     <row r="40" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B40" s="6" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="C40" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D40" t="s" ph="1">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="41" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B41" s="6" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="C41" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D41" t="s" ph="1">
-        <v>206</v>
+        <v>195</v>
       </c>
     </row>
     <row r="42" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B42" s="6" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="C42" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D42" t="s" ph="1">
-        <v>208</v>
+        <v>197</v>
       </c>
     </row>
     <row r="43" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B43" s="6" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="C43" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D43" t="s" ph="1">
-        <v>209</v>
+        <v>198</v>
       </c>
     </row>
     <row r="44" spans="2:5" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B44" s="6" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="C44" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D44" t="s" ph="1">
-        <v>210</v>
+        <v>199</v>
       </c>
     </row>
     <row r="45" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B45" s="6" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="C45" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D45" t="s" ph="1">
-        <v>234</v>
+        <v>223</v>
       </c>
     </row>
     <row r="46" spans="2:5" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B46" s="6" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C46" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D46" t="s" ph="1">
-        <v>211</v>
+        <v>200</v>
       </c>
     </row>
     <row r="47" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B47" s="6" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="C47" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D47" t="s" ph="1">
-        <v>236</v>
+        <v>225</v>
       </c>
     </row>
     <row r="48" spans="2:5" ph="1" x14ac:dyDescent="0.2">
@@ -7141,7 +6991,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -7157,65 +7007,65 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="C7" t="s" ph="1">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="E7" ph="1"/>
     </row>
     <row r="8" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="C8" t="s" ph="1">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>250</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:5" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="C9" t="s" ph="1">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>193</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:5" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>238</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:5" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>239</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="132" x14ac:dyDescent="0.2">
@@ -7223,7 +7073,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -7237,37 +7087,37 @@
         <v>4</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="D15" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="D16" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="D17" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7275,13 +7125,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -7312,7 +7162,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7320,7 +7170,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7336,7 +7186,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -7344,7 +7194,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7363,13 +7213,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7377,13 +7227,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -7391,7 +7241,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -7402,7 +7252,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -7413,21 +7263,21 @@
         <v>4</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="D13" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -7435,13 +7285,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7449,13 +7299,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -7463,13 +7313,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -7532,7 +7382,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7548,7 +7398,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -7556,7 +7406,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7572,47 +7422,47 @@
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="D9" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="D10" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="D11" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="D12" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="D13" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7620,10 +7470,10 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="D14" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7631,50 +7481,50 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="D15" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="D16" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="D17" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="D18" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="D19" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="D20" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -7688,8 +7538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:B16"/>
+    <sheetView topLeftCell="A10" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -7713,7 +7563,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7729,7 +7579,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7737,7 +7587,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7772,7 +7622,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7780,21 +7630,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
       <c r="D12" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -7802,13 +7652,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7816,13 +7666,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -7830,13 +7680,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -7892,7 +7742,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8010,13 +7860,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8038,7 +7888,7 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8182,7 +8032,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -8430,7 +8280,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8446,17 +8296,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -8492,13 +8342,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8506,21 +8356,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="D12" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -8528,7 +8378,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -8559,7 +8409,7 @@
         <v>67</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8583,7 +8433,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -8607,7 +8457,7 @@
     </row>
     <row r="8" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
remove windows update from the chapter for spec checking
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpsuzuki\Documents\2022_03\fresta2022\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA9D3F9-7640-43F3-8739-753A28082C41}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80383B39-E6BE-4E11-AFDC-0634A8B8E6D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" tabRatio="782" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" tabRatio="782" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="347">
   <si>
     <t>header1</t>
   </si>
@@ -3504,70 +3504,6 @@
   </si>
   <si>
     <t>win11ja-desktop-no-annot.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「設定」アプリの「Windows Update」メニューを選び、更新プログラムをチェックします。再起動を求められる場合があります。</t>
-    <rPh sb="1" eb="3">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="29" eb="30">
-      <t>エラ</t>
-    </rPh>
-    <rPh sb="32" eb="34">
-      <t>コウシン</t>
-    </rPh>
-    <rPh sb="48" eb="51">
-      <t>サイキドウ</t>
-    </rPh>
-    <rPh sb="52" eb="53">
-      <t>モト</t>
-    </rPh>
-    <rPh sb="57" eb="59">
-      <t>バアイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11ja-windows-update.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11ja-windows-update-option.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「最新の状態です」となった場合には、「詳細オプション」から「その他のMicrosoft製品…」もオンにし、改めて「最新の状態です」になるまで更新しましょう。</t>
-    <rPh sb="1" eb="3">
-      <t>サイシン</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>ジョウタイ</t>
-    </rPh>
-    <rPh sb="13" eb="15">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="19" eb="21">
-      <t>ショウサイ</t>
-    </rPh>
-    <rPh sb="32" eb="33">
-      <t>ホカ</t>
-    </rPh>
-    <rPh sb="43" eb="45">
-      <t>セイヒン</t>
-    </rPh>
-    <rPh sb="53" eb="54">
-      <t>アラタ</t>
-    </rPh>
-    <rPh sb="57" eb="59">
-      <t>サイシン</t>
-    </rPh>
-    <rPh sb="60" eb="62">
-      <t>ジョウタイ</t>
-    </rPh>
-    <rPh sb="70" eb="72">
-      <t>コウシン</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -5909,7 +5845,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5941,7 +5877,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -5949,10 +5885,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D10" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -5960,50 +5896,50 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D11" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D12" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="D13" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="D14" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D15" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D16" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6011,26 +5947,26 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D17" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D18" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="D19" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -6044,8 +5980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DB449D4-AFC1-462F-B851-41C4675E501D}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -6085,7 +6021,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -6104,10 +6040,10 @@
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="D8" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -6115,18 +6051,18 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="D9" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="D10" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6134,13 +6070,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -6436,7 +6372,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6444,7 +6380,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6460,7 +6396,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="304.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -6482,7 +6418,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C7" t="s" ph="1">
         <v>7</v>
@@ -6496,7 +6432,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>7</v>
@@ -6507,7 +6443,7 @@
     </row>
     <row r="9" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D9" t="s" ph="1">
         <v>141</v>
@@ -6557,7 +6493,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>7</v>
@@ -6964,10 +6900,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -6991,7 +6927,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -7007,7 +6943,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
@@ -7030,7 +6966,7 @@
         <v>179</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:5" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -7052,86 +6988,70 @@
         <v>184</v>
       </c>
     </row>
-    <row r="11" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="132" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
       <c r="B11" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="D11" t="s" ph="1">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
+        <v>251</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="79.2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
       <c r="B12" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="D12" t="s" ph="1">
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B13" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="D13" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B14" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D14" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B15" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="D15" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="132" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="79.2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="6" t="s">
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
         <v>233</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B15" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="D15" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B16" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="D16" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B17" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="D17" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -7162,7 +7082,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7170,7 +7090,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7186,7 +7106,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -7194,7 +7114,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7213,13 +7133,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7227,13 +7147,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -7241,7 +7161,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -7252,7 +7172,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -7263,21 +7183,21 @@
         <v>4</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D13" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -7285,13 +7205,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7299,13 +7219,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -7313,13 +7233,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -7382,7 +7302,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7398,7 +7318,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -7406,7 +7326,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7427,42 +7347,42 @@
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="D9" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D10" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D11" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D12" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D13" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7470,10 +7390,10 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D14" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7481,50 +7401,50 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D15" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D16" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D17" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D18" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D19" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D20" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -7563,7 +7483,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7579,7 +7499,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7587,7 +7507,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7630,21 +7550,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="D12" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -7652,13 +7572,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7666,13 +7586,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -7680,13 +7600,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -7742,7 +7662,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8280,7 +8200,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8296,7 +8216,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8342,13 +8262,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8356,21 +8276,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D12" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -8378,7 +8298,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -8433,7 +8353,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix MyMomiji login process.
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpsuzuki\Documents\2022_03\fresta2022\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED4951A4-97D6-499E-823D-4BAF3666245F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B026AFE-6746-4CAA-AEFB-6F28EB629CA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" tabRatio="694" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" tabRatio="694" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="365">
   <si>
     <t>header1</t>
   </si>
@@ -137,11 +137,6 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;h2&gt;&lt;a name="mymomiji"&gt;&lt;/a&gt;MYもみじ (履修登録や掲示板など)&lt;/h2&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">広島大学では履修登録、成績確認、各種通知は「MYもみじ」を利用して行います。「MYもみじ」へログインしてみましょう。
-広大ID（学生番号）、広大パスワードを入力し、「Myもみじへログイン」をクリックしてください。
-   </t>
   </si>
   <si>
     <t>win10-6-10.svg</t>
@@ -5730,6 +5725,26 @@
     </rPh>
     <rPh sb="33" eb="35">
       <t>ヒツヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">広島大学では履修登録、成績確認、各種通知は「MYもみじ」を利用して行います。「MYもみじ」へログインしてみましょう。
+まず「Myもみじへログイン」をクリックしてください。
+   </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>hirodaiID-login.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>広大IDとパスワードを入力し、「ログイン」をクリックします。</t>
+    <rPh sb="0" eb="2">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ニュウリョク</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -6153,7 +6168,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6169,7 +6184,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -6177,7 +6192,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -6191,7 +6206,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6225,10 +6240,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6236,7 +6251,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6252,7 +6267,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -6260,7 +6275,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6271,17 +6286,17 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -6289,7 +6304,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -6326,7 +6341,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6334,7 +6349,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6350,7 +6365,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6358,7 +6373,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6374,15 +6389,15 @@
     </row>
     <row r="8" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6390,10 +6405,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="D10" t="s">
         <v>307</v>
-      </c>
-      <c r="D10" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6401,50 +6416,50 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D12" t="s">
         <v>311</v>
-      </c>
-      <c r="D12" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D14" t="s">
         <v>315</v>
-      </c>
-      <c r="D14" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D15" t="s">
         <v>317</v>
-      </c>
-      <c r="D15" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="D16" t="s">
         <v>319</v>
-      </c>
-      <c r="D16" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6452,26 +6467,26 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D17" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D18" t="s">
         <v>322</v>
-      </c>
-      <c r="D18" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D19" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -6502,7 +6517,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6510,7 +6525,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6526,7 +6541,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -6534,7 +6549,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6545,10 +6560,10 @@
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -6556,18 +6571,18 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D9" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D10" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6575,13 +6590,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -6589,46 +6604,46 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -6636,13 +6651,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6650,24 +6665,24 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="92.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -6675,13 +6690,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -6689,35 +6704,35 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
       </c>
       <c r="D21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C22" t="s">
         <v>7</v>
       </c>
       <c r="D22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6725,13 +6740,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -6739,13 +6754,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C24" t="s">
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -6877,7 +6892,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6885,7 +6900,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6901,7 +6916,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="304.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -6909,7 +6924,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -6923,13 +6938,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C7" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -6937,21 +6952,21 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
@@ -6959,13 +6974,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
@@ -6973,24 +6988,24 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
@@ -6998,13 +7013,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
@@ -7012,13 +7027,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C14" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -7026,24 +7041,24 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C15" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C16" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -7051,345 +7066,345 @@
         <v>4</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B18" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C25" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C26" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D26" t="s" ph="1">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C27" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D27" t="s" ph="1">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C28" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D28" t="s" ph="1">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C29" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D29" t="s" ph="1">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C30" t="s" ph="1">
+        <v>177</v>
+      </c>
+      <c r="D30" t="s" ph="1">
         <v>178</v>
-      </c>
-      <c r="D30" t="s" ph="1">
-        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C31" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D31" t="s" ph="1">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C32" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D32" t="s" ph="1">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="33" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C33" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D33" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E33"/>
     </row>
     <row r="34" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C34" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D34" t="s" ph="1">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C35" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D35" t="s" ph="1">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C36" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D36" t="s" ph="1">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="37" spans="2:5" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C37" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E37"/>
     </row>
     <row r="38" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C38" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D38" t="s" ph="1">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="39" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C39" t="s" ph="1">
         <v>217</v>
       </c>
-      <c r="C39" t="s" ph="1">
+      <c r="D39" t="s" ph="1">
         <v>218</v>
-      </c>
-      <c r="D39" t="s" ph="1">
-        <v>219</v>
       </c>
     </row>
     <row r="40" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B40" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C40" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D40" t="s" ph="1">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="41" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B41" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C41" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D41" t="s" ph="1">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="42" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B42" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C42" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D42" t="s" ph="1">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="43" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B43" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C43" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D43" t="s" ph="1">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="44" spans="2:5" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B44" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C44" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D44" t="s" ph="1">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="45" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B45" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C45" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D45" t="s" ph="1">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="46" spans="2:5" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B46" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C46" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D46" t="s" ph="1">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="47" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B47" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C47" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D47" t="s" ph="1">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="48" spans="2:5" ph="1" x14ac:dyDescent="0.2">
@@ -7425,7 +7440,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -7433,7 +7448,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -7449,49 +7464,49 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C7" t="s" ph="1">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E7" ph="1"/>
     </row>
     <row r="8" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C8" t="s" ph="1">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:5" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C9" t="s" ph="1">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:5" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="D10" t="s" ph="1">
         <v>182</v>
-      </c>
-      <c r="D10" t="s" ph="1">
-        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="132" x14ac:dyDescent="0.2">
@@ -7499,7 +7514,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -7513,37 +7528,37 @@
         <v>4</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
         <v>228</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D13" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
@@ -7551,13 +7566,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -7588,7 +7603,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7596,7 +7611,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7612,7 +7627,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -7620,7 +7635,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7639,13 +7654,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7653,13 +7668,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
         <v>255</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -7667,7 +7682,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -7678,7 +7693,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -7689,21 +7704,21 @@
         <v>4</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
         <v>259</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="D13" t="s">
         <v>261</v>
-      </c>
-      <c r="D13" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -7711,13 +7726,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
         <v>263</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7725,13 +7740,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -7739,13 +7754,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -7800,7 +7815,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7808,7 +7823,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7824,7 +7839,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -7832,7 +7847,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7848,47 +7863,47 @@
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D10" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D11" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D12" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -7896,10 +7911,10 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D14" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7907,50 +7922,50 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D16" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D18" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D19" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D20" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -7964,7 +7979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D6E33FB-2290-439B-854D-9A45A4600EF5}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -7981,7 +7996,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7989,7 +8004,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8005,7 +8020,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -8016,7 +8031,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8027,7 +8042,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8035,7 +8050,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -8043,10 +8058,10 @@
     </row>
     <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="D9" t="s">
         <v>351</v>
-      </c>
-      <c r="D9" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -8054,13 +8069,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>353</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="198" x14ac:dyDescent="0.2">
@@ -8068,18 +8083,18 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
         <v>355</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8087,7 +8102,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -8098,7 +8113,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -8109,7 +8124,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -8125,7 +8140,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -8142,7 +8157,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8150,7 +8165,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8166,7 +8181,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -8174,7 +8189,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8190,7 +8205,7 @@
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -8198,7 +8213,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -8209,7 +8224,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -8217,21 +8232,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
         <v>328</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -8239,13 +8254,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>331</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8253,13 +8268,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -8267,13 +8282,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -8302,10 +8317,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8329,7 +8344,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8345,7 +8360,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="264" x14ac:dyDescent="0.2">
@@ -8353,7 +8368,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8447,21 +8462,21 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8469,13 +8484,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8497,7 +8512,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -8553,282 +8568,290 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
         <v>32</v>
       </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" t="s">
+    </row>
+    <row r="24" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="D24" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="66" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="1" t="s">
+    <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="184.8" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B26" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C28" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="184.8" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="158.4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B39" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C33" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C34" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C36" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="158.4" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>4</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C37" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B38" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D38" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B39" s="1" t="s">
+    <row r="41" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>4</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C40" t="s">
-        <v>4</v>
-      </c>
-      <c r="D40" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="C41" t="s">
-        <v>7</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="D41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>4</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C42" t="s">
         <v>7</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
+      <c r="B44" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D44" t="s" ph="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
-      <c r="B43" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D43" t="s" ph="1">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>4</v>
-      </c>
-      <c r="B44" s="1" t="s">
+      <c r="C45" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" t="s">
         <v>49</v>
-      </c>
-      <c r="C44" t="s">
-        <v>7</v>
-      </c>
-      <c r="D44" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -8867,7 +8890,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8883,17 +8906,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -8901,7 +8924,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -8915,7 +8938,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -8929,13 +8952,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>242</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8943,21 +8966,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
         <v>244</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D12" t="s">
         <v>246</v>
-      </c>
-      <c r="D12" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -8965,7 +8988,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update momiji login process.
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpsuzuki\Documents\2022_03\fresta2022\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B026AFE-6746-4CAA-AEFB-6F28EB629CA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D79CC9B-D169-495A-8A76-FECF6311036A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" tabRatio="694" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -139,9 +139,6 @@
     <t xml:space="preserve">&lt;h2&gt;&lt;a name="mymomiji"&gt;&lt;/a&gt;MYもみじ (履修登録や掲示板など)&lt;/h2&gt; </t>
   </si>
   <si>
-    <t>win10-6-10.svg</t>
-  </si>
-  <si>
     <t>win10-6-11.svg</t>
   </si>
   <si>
@@ -5732,6 +5729,10 @@
     <t xml:space="preserve">広島大学では履修登録、成績確認、各種通知は「MYもみじ」を利用して行います。「MYもみじ」へログインしてみましょう。
 まず「Myもみじへログイン」をクリックしてください。
    </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-momiji-before-login.png</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -6168,7 +6169,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6184,7 +6185,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -6192,7 +6193,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -6206,7 +6207,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6240,10 +6241,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6251,7 +6252,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6267,7 +6268,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -6275,7 +6276,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6286,17 +6287,17 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -6304,7 +6305,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -6341,7 +6342,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6349,7 +6350,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6365,7 +6366,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6373,7 +6374,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6389,15 +6390,15 @@
     </row>
     <row r="8" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6405,10 +6406,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="D10" t="s">
         <v>306</v>
-      </c>
-      <c r="D10" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6416,50 +6417,50 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="D12" t="s">
         <v>310</v>
-      </c>
-      <c r="D12" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D14" t="s">
         <v>314</v>
-      </c>
-      <c r="D14" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="D15" t="s">
         <v>316</v>
-      </c>
-      <c r="D15" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D16" t="s">
         <v>318</v>
-      </c>
-      <c r="D16" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6467,26 +6468,26 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D17" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D18" t="s">
         <v>321</v>
-      </c>
-      <c r="D18" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D19" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -6517,7 +6518,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6525,7 +6526,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6541,7 +6542,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -6549,7 +6550,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6560,10 +6561,10 @@
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D8" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -6571,18 +6572,18 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D10" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6590,13 +6591,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -6604,46 +6605,46 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -6651,13 +6652,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6665,24 +6666,24 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="92.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -6690,13 +6691,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -6704,35 +6705,35 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
       </c>
       <c r="D21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C22" t="s">
         <v>7</v>
       </c>
       <c r="D22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6740,13 +6741,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -6754,13 +6755,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C24" t="s">
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -6892,7 +6893,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6900,7 +6901,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6916,7 +6917,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="304.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -6924,7 +6925,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -6938,13 +6939,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C7" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -6952,21 +6953,21 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
@@ -6974,13 +6975,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
@@ -6988,24 +6989,24 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
@@ -7013,13 +7014,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
@@ -7027,13 +7028,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C14" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -7041,24 +7042,24 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C15" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C16" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -7066,345 +7067,345 @@
         <v>4</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B18" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C25" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C26" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D26" t="s" ph="1">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C27" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D27" t="s" ph="1">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C28" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D28" t="s" ph="1">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C29" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D29" t="s" ph="1">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C30" t="s" ph="1">
+        <v>176</v>
+      </c>
+      <c r="D30" t="s" ph="1">
         <v>177</v>
-      </c>
-      <c r="D30" t="s" ph="1">
-        <v>178</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C31" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D31" t="s" ph="1">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C32" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D32" t="s" ph="1">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="33" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C33" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D33" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E33"/>
     </row>
     <row r="34" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C34" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D34" t="s" ph="1">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C35" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D35" t="s" ph="1">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C36" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D36" t="s" ph="1">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="37" spans="2:5" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C37" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E37"/>
     </row>
     <row r="38" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C38" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D38" t="s" ph="1">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="39" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="C39" t="s" ph="1">
         <v>216</v>
       </c>
-      <c r="C39" t="s" ph="1">
+      <c r="D39" t="s" ph="1">
         <v>217</v>
-      </c>
-      <c r="D39" t="s" ph="1">
-        <v>218</v>
       </c>
     </row>
     <row r="40" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B40" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C40" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D40" t="s" ph="1">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="41" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B41" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C41" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D41" t="s" ph="1">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="42" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B42" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C42" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D42" t="s" ph="1">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="43" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B43" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C43" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D43" t="s" ph="1">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="44" spans="2:5" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B44" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C44" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D44" t="s" ph="1">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="45" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B45" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C45" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D45" t="s" ph="1">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="46" spans="2:5" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B46" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C46" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D46" t="s" ph="1">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="47" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B47" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C47" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D47" t="s" ph="1">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="48" spans="2:5" ph="1" x14ac:dyDescent="0.2">
@@ -7440,7 +7441,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -7448,7 +7449,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -7464,49 +7465,49 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C7" t="s" ph="1">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E7" ph="1"/>
     </row>
     <row r="8" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C8" t="s" ph="1">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:5" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C9" t="s" ph="1">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:5" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="D10" t="s" ph="1">
         <v>181</v>
-      </c>
-      <c r="D10" t="s" ph="1">
-        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="132" x14ac:dyDescent="0.2">
@@ -7514,7 +7515,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -7528,37 +7529,37 @@
         <v>4</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
         <v>227</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D13" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
@@ -7566,13 +7567,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -7603,7 +7604,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7611,7 +7612,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7627,7 +7628,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -7635,7 +7636,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7654,13 +7655,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7668,13 +7669,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
         <v>254</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -7682,7 +7683,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -7693,7 +7694,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -7704,21 +7705,21 @@
         <v>4</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
         <v>258</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="D13" t="s">
         <v>260</v>
-      </c>
-      <c r="D13" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -7726,13 +7727,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
         <v>262</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7740,13 +7741,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -7754,13 +7755,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -7815,7 +7816,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7823,7 +7824,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7839,7 +7840,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -7847,7 +7848,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7863,47 +7864,47 @@
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D10" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D12" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D13" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -7911,10 +7912,10 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D14" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7922,50 +7923,50 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D15" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D16" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D20" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -7996,7 +7997,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8004,7 +8005,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8020,7 +8021,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -8031,7 +8032,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8042,7 +8043,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8050,7 +8051,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -8058,10 +8059,10 @@
     </row>
     <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="D9" t="s">
         <v>350</v>
-      </c>
-      <c r="D9" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -8069,13 +8070,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>352</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="198" x14ac:dyDescent="0.2">
@@ -8083,18 +8084,18 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
         <v>354</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8102,7 +8103,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -8113,7 +8114,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -8124,7 +8125,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -8157,7 +8158,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8165,7 +8166,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8181,7 +8182,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -8189,7 +8190,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8205,7 +8206,7 @@
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -8213,7 +8214,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -8224,7 +8225,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -8232,21 +8233,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
         <v>327</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D12" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -8254,13 +8255,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>330</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8268,13 +8269,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -8282,13 +8283,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -8320,7 +8321,7 @@
   <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8344,7 +8345,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8360,7 +8361,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="264" x14ac:dyDescent="0.2">
@@ -8368,7 +8369,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8462,21 +8463,21 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8484,13 +8485,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8512,7 +8513,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -8573,13 +8574,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="6" t="s">
+        <v>361</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
         <v>362</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.2">
@@ -8595,13 +8596,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8609,18 +8610,18 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
         <v>34</v>
-      </c>
-      <c r="C26" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -8642,13 +8643,13 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8656,13 +8657,13 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
         <v>38</v>
-      </c>
-      <c r="C30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8670,13 +8671,13 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
         <v>40</v>
-      </c>
-      <c r="C31" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8684,13 +8685,13 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" t="s">
         <v>42</v>
-      </c>
-      <c r="C32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="184.8" x14ac:dyDescent="0.2">
@@ -8698,13 +8699,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8712,13 +8713,13 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8726,13 +8727,13 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8740,13 +8741,13 @@
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8754,13 +8755,13 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="158.4" x14ac:dyDescent="0.2">
@@ -8768,26 +8769,26 @@
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C38" t="s">
         <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8795,7 +8796,7 @@
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
@@ -8809,13 +8810,13 @@
         <v>4</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C42" t="s">
         <v>7</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -8823,21 +8824,21 @@
         <v>4</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C43" t="s">
         <v>7</v>
       </c>
       <c r="D43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D44" t="s" ph="1">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -8845,13 +8846,13 @@
         <v>4</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C45" t="s">
         <v>7</v>
       </c>
       <c r="D45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -8890,7 +8891,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8906,17 +8907,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -8924,7 +8925,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -8938,7 +8939,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -8952,13 +8953,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>241</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8966,21 +8967,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
         <v>243</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D12" t="s">
         <v>245</v>
-      </c>
-      <c r="D12" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -8988,7 +8989,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update momiji login procedure
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpsuzuki\Documents\2022_03\fresta2022\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421A8CF6-BC3F-488D-9DD5-05F236CA81D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BFE9A0-235A-4D45-8A1D-F507455B3FCF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" tabRatio="694" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,9 +93,6 @@
   </t>
   </si>
   <si>
-    <t>win10-6-02.svg</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;h2&gt;&lt;a name="mail"&gt;&lt;/a&gt;Office365 (Webメールとオンラインストレージ)&lt;/h2&gt; </t>
   </si>
   <si>
@@ -5549,6 +5546,10 @@
     <rPh sb="98" eb="100">
       <t>キョウザイ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-momiji-before-login0.png</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -5971,7 +5972,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5987,7 +5988,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -5995,7 +5996,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -6009,7 +6010,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6043,10 +6044,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6054,7 +6055,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6070,7 +6071,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -6078,7 +6079,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6089,17 +6090,17 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -6107,7 +6108,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -6144,7 +6145,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6152,7 +6153,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6168,7 +6169,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6176,7 +6177,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6192,15 +6193,15 @@
     </row>
     <row r="8" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6208,10 +6209,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D10" t="s">
         <v>291</v>
-      </c>
-      <c r="D10" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6219,50 +6220,50 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D11" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="D12" t="s">
         <v>295</v>
-      </c>
-      <c r="D12" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D13" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D14" t="s">
         <v>299</v>
-      </c>
-      <c r="D14" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D15" t="s">
         <v>301</v>
-      </c>
-      <c r="D15" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="D16" t="s">
         <v>303</v>
-      </c>
-      <c r="D16" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6270,26 +6271,26 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="D18" t="s">
         <v>306</v>
-      </c>
-      <c r="D18" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D19" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -6320,7 +6321,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6328,7 +6329,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6344,7 +6345,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -6352,7 +6353,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6363,10 +6364,10 @@
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -6374,18 +6375,18 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D10" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6393,13 +6394,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -6407,46 +6408,46 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -6454,13 +6455,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6468,24 +6469,24 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="92.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -6493,13 +6494,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -6507,35 +6508,35 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
       </c>
       <c r="D21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C22" t="s">
         <v>7</v>
       </c>
       <c r="D22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6543,13 +6544,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -6557,13 +6558,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C24" t="s">
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -6695,7 +6696,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6703,7 +6704,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6719,7 +6720,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="304.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -6727,7 +6728,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -6741,13 +6742,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C7" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -6755,21 +6756,21 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
@@ -6777,13 +6778,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
@@ -6791,24 +6792,24 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
@@ -6816,13 +6817,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
@@ -6830,13 +6831,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C14" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -6844,24 +6845,24 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C15" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C16" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6869,345 +6870,345 @@
         <v>4</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B18" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C25" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C26" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D26" t="s" ph="1">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C27" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D27" t="s" ph="1">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C28" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D28" t="s" ph="1">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C29" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D29" t="s" ph="1">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C30" t="s" ph="1">
+        <v>161</v>
+      </c>
+      <c r="D30" t="s" ph="1">
         <v>162</v>
-      </c>
-      <c r="D30" t="s" ph="1">
-        <v>163</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C31" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D31" t="s" ph="1">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C32" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D32" t="s" ph="1">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="33" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C33" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D33" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E33"/>
     </row>
     <row r="34" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C34" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D34" t="s" ph="1">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C35" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D35" t="s" ph="1">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C36" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D36" t="s" ph="1">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="37" spans="2:5" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C37" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E37"/>
     </row>
     <row r="38" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C38" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D38" t="s" ph="1">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="39" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="C39" t="s" ph="1">
         <v>201</v>
       </c>
-      <c r="C39" t="s" ph="1">
+      <c r="D39" t="s" ph="1">
         <v>202</v>
-      </c>
-      <c r="D39" t="s" ph="1">
-        <v>203</v>
       </c>
     </row>
     <row r="40" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B40" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C40" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D40" t="s" ph="1">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="41" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B41" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C41" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D41" t="s" ph="1">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="42" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B42" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C42" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D42" t="s" ph="1">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="43" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B43" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C43" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D43" t="s" ph="1">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="44" spans="2:5" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B44" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C44" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D44" t="s" ph="1">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="45" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B45" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C45" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D45" t="s" ph="1">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="46" spans="2:5" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B46" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C46" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D46" t="s" ph="1">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="47" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B47" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C47" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D47" t="s" ph="1">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="48" spans="2:5" ph="1" x14ac:dyDescent="0.2">
@@ -7243,7 +7244,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -7251,7 +7252,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -7267,49 +7268,49 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C7" t="s" ph="1">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E7" ph="1"/>
     </row>
     <row r="8" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C8" t="s" ph="1">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:5" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C9" t="s" ph="1">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:5" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="D10" t="s" ph="1">
         <v>166</v>
-      </c>
-      <c r="D10" t="s" ph="1">
-        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="132" x14ac:dyDescent="0.2">
@@ -7317,7 +7318,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -7331,37 +7332,37 @@
         <v>4</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
         <v>212</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
@@ -7369,13 +7370,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -7406,7 +7407,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7414,7 +7415,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7430,7 +7431,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -7438,7 +7439,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7457,13 +7458,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7471,13 +7472,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
         <v>239</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -7485,7 +7486,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -7496,7 +7497,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -7507,21 +7508,21 @@
         <v>4</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
         <v>243</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="D13" t="s">
         <v>245</v>
-      </c>
-      <c r="D13" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -7529,13 +7530,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
         <v>247</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7543,13 +7544,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -7557,13 +7558,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -7618,7 +7619,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7626,7 +7627,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7642,7 +7643,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -7650,7 +7651,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7666,47 +7667,47 @@
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -7714,10 +7715,10 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7725,50 +7726,50 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D16" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D20" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -7799,7 +7800,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7807,7 +7808,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7823,7 +7824,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -7834,7 +7835,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7845,7 +7846,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -7853,7 +7854,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -7861,10 +7862,10 @@
     </row>
     <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="D9" t="s">
         <v>335</v>
-      </c>
-      <c r="D9" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7872,13 +7873,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>337</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="198" x14ac:dyDescent="0.2">
@@ -7886,18 +7887,18 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
         <v>339</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7905,7 +7906,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -7916,7 +7917,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -7927,7 +7928,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -7960,7 +7961,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7968,7 +7969,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7984,7 +7985,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7992,7 +7993,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8008,7 +8009,7 @@
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -8016,7 +8017,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -8027,7 +8028,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -8035,21 +8036,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
         <v>312</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D12" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -8057,13 +8058,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>315</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8071,13 +8072,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -8085,13 +8086,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -8122,8 +8123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:XFD40"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8147,7 +8148,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8163,7 +8164,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="264" x14ac:dyDescent="0.2">
@@ -8171,7 +8172,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8224,12 +8225,12 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>351</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -8251,13 +8252,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>21</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8265,21 +8266,21 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8287,13 +8288,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8301,13 +8302,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
         <v>23</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>24</v>
-      </c>
-      <c r="D17" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -8315,13 +8316,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8329,13 +8330,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
         <v>27</v>
-      </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8343,18 +8344,18 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
         <v>29</v>
-      </c>
-      <c r="C20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -8376,21 +8377,21 @@
         <v>4</v>
       </c>
       <c r="B23" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
         <v>347</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D24" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -8398,13 +8399,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8412,18 +8413,18 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
         <v>33</v>
-      </c>
-      <c r="C26" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -8445,13 +8446,13 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8459,13 +8460,13 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
         <v>37</v>
-      </c>
-      <c r="C30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8473,13 +8474,13 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
         <v>39</v>
-      </c>
-      <c r="C31" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8487,13 +8488,13 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" t="s">
         <v>41</v>
-      </c>
-      <c r="C32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8501,13 +8502,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8515,7 +8516,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
@@ -8529,13 +8530,13 @@
         <v>4</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C35" t="s">
         <v>7</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -8543,21 +8544,21 @@
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C36" t="s">
         <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D37" t="s" ph="1">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -8565,13 +8566,13 @@
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C38" t="s">
         <v>7</v>
       </c>
       <c r="D38" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -8610,7 +8611,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8626,17 +8627,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -8644,7 +8645,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -8658,7 +8659,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -8672,13 +8673,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>226</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8686,21 +8687,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
         <v>228</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D12" t="s">
         <v>230</v>
-      </c>
-      <c r="D12" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -8708,7 +8709,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Outlook login process updated.
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpsuzuki\Documents\2022_03\fresta2022\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BFE9A0-235A-4D45-8A1D-F507455B3FCF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79445AE8-A622-4CBB-8CBA-B81855C40A47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" tabRatio="694" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="343">
   <si>
     <t>header1</t>
   </si>
@@ -94,26 +94,6 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;h2&gt;&lt;a name="mail"&gt;&lt;/a&gt;Office365 (Webメールとオンラインストレージ)&lt;/h2&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">「もみじ」で「Webメール」のバナーをクリックしましょう。
-  </t>
-  </si>
-  <si>
-    <t>win10-6-03.svg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Office365で使えるアプリの一覧が表示されます。「Outlook」をクリック。 
-  </t>
-  </si>
-  <si>
-    <t>chart flame</t>
-  </si>
-  <si>
-    <t>win10-6-27.svg</t>
-  </si>
-  <si>
-    <t>win10-6-07.svg</t>
   </si>
   <si>
     <t xml:space="preserve">次に、Office365のオンラインストレージのOneDriveを見て見ましょう。画面左上のつぶつぶをクリックします。
@@ -240,16 +220,6 @@
   </si>
   <si>
     <t>win10-6-24a.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Office365にサインインする画面になります。まず「IMCアカウント名@hiroshima-u.ac.jp」を記入し「次へ」をクリックします。
-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Hiroshima Universityと書かれた画面に移動しますので、広大パスワードを入力し「サインイン」をクリックします。
-</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -368,22 +338,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">メールの画面が開きます。
-大学からの電子メールでの連絡は、広大メールで来ます。
-常にメールチェックするようにしてください。&lt;span class="check"&gt;check-9&lt;/span&gt;
-スマホのOutlookアプリでも、複雑な設定は必要なくメールの送受信が可能です。ここは必携PC設定の手順を示していますので、Web版をお知らせしましたが、スマホ版の方が使いやすく、新規メールが届いた時の通知もありますので、おすすめです。
-&lt;img alt="*outlook icon*" src="image/win10-outlook-app.png" width="64" /&gt;  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">するとこのような画面になります。&lt;span class="check"&gt;check-10&lt;/span&gt;
 履修登録をしたり、成績を確認することができます。
 また「掲示」では、授業や学部からの連絡が表示されます。
   </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win10-6-41.svg</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -620,10 +578,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ch5-signin-password.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>&lt;p class="spl"&gt;※学生番号と、学生番号と一緒にもらえる「広大パスワード」が必要です。&lt;/p&gt;</t>
     <rPh sb="16" eb="18">
       <t>ガクセイ</t>
@@ -1640,14 +1594,6 @@
   </si>
   <si>
     <t>（付録A）Officeのインストール</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>office365-portal.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">portal.office.comへのリンクをクリックしてください。
-  </t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -5551,6 +5497,60 @@
   <si>
     <t>win11-momiji-before-login0.png</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Office365のページの左側にブラウザ内で使用できるアプリのアイコンが並びます。「O」の文字があるOutlook for Webをクリックします。</t>
+    <rPh sb="14" eb="16">
+      <t>ヒダリガワ</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>ナイ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="37" eb="38">
+      <t>ナラ</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>モジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Outlook for Webのページが開き、新着メールを確認することができます。大学からのメール連絡は広大メールに来ますので、常にメールチェックするようにしてください。</t>
+    <rPh sb="20" eb="21">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>シンチャク</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="49" eb="51">
+      <t>レンラク</t>
+    </rPh>
+    <rPh sb="52" eb="54">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="58" eb="59">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="64" eb="65">
+      <t>ツネ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-office365-outlook-start.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-outlook-for-web.png</t>
   </si>
 </sst>
 </file>
@@ -5972,7 +5972,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5988,7 +5988,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -5996,7 +5996,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -6010,7 +6010,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6044,10 +6044,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6055,7 +6055,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6071,7 +6071,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -6079,7 +6079,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6090,17 +6090,17 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -6108,7 +6108,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -6128,8 +6128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392D1BFF-FF5C-4A7E-8C9C-E750AF0FFFAF}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -6145,7 +6145,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6153,7 +6153,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6169,7 +6169,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6177,7 +6177,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6193,15 +6193,15 @@
     </row>
     <row r="8" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6209,10 +6209,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
       <c r="D10" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6220,50 +6220,50 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="D11" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="D12" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="D13" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="D14" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
       <c r="D15" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="D16" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6271,26 +6271,26 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="D17" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
       <c r="D18" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="D19" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -6321,7 +6321,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6329,7 +6329,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6345,7 +6345,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -6353,7 +6353,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6364,10 +6364,10 @@
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
       <c r="D8" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -6375,18 +6375,18 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
       <c r="D9" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>325</v>
+        <v>312</v>
       </c>
       <c r="D10" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6394,13 +6394,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -6408,46 +6408,46 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -6455,13 +6455,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6469,24 +6469,24 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="92.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C18" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="D18" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -6494,13 +6494,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -6508,35 +6508,35 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
       </c>
       <c r="D21" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="C22" t="s">
         <v>7</v>
       </c>
       <c r="D22" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6544,13 +6544,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -6558,13 +6558,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="C24" t="s">
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -6696,7 +6696,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6704,7 +6704,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6720,7 +6720,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="304.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -6728,7 +6728,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -6742,13 +6742,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="C7" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>121</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -6756,21 +6756,21 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>122</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>123</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
@@ -6778,13 +6778,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
@@ -6792,24 +6792,24 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
@@ -6817,13 +6817,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>128</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
@@ -6831,13 +6831,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="C14" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>129</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -6845,24 +6845,24 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="C15" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>130</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="C16" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>133</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6870,345 +6870,345 @@
         <v>4</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>135</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B18" s="6" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>137</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>138</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>140</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>145</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>146</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>160</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="C25" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>150</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="C26" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D26" t="s" ph="1">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="C27" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D27" t="s" ph="1">
-        <v>154</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="C28" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D28" t="s" ph="1">
-        <v>155</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="C29" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D29" t="s" ph="1">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="C30" t="s" ph="1">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="D30" t="s" ph="1">
-        <v>162</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="C31" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D31" t="s" ph="1">
-        <v>185</v>
+        <v>172</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="C32" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D32" t="s" ph="1">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="33" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="C33" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D33" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="E33"/>
     </row>
     <row r="34" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="C34" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D34" t="s" ph="1">
-        <v>171</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="C35" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D35" t="s" ph="1">
-        <v>172</v>
+        <v>159</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="C36" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D36" t="s" ph="1">
-        <v>173</v>
+        <v>160</v>
       </c>
     </row>
     <row r="37" spans="2:5" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="C37" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="E37"/>
     </row>
     <row r="38" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="C38" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D38" t="s" ph="1">
-        <v>175</v>
+        <v>162</v>
       </c>
     </row>
     <row r="39" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="C39" t="s" ph="1">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="D39" t="s" ph="1">
-        <v>202</v>
+        <v>189</v>
       </c>
     </row>
     <row r="40" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B40" s="6" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="C40" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D40" t="s" ph="1">
-        <v>176</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B41" s="6" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="C41" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D41" t="s" ph="1">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B42" s="6" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="C42" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D42" t="s" ph="1">
-        <v>179</v>
+        <v>166</v>
       </c>
     </row>
     <row r="43" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B43" s="6" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="C43" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D43" t="s" ph="1">
-        <v>180</v>
+        <v>167</v>
       </c>
     </row>
     <row r="44" spans="2:5" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B44" s="6" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="C44" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D44" t="s" ph="1">
-        <v>181</v>
+        <v>168</v>
       </c>
     </row>
     <row r="45" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B45" s="6" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="C45" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D45" t="s" ph="1">
-        <v>205</v>
+        <v>192</v>
       </c>
     </row>
     <row r="46" spans="2:5" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B46" s="6" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="C46" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D46" t="s" ph="1">
-        <v>182</v>
+        <v>169</v>
       </c>
     </row>
     <row r="47" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B47" s="6" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="C47" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D47" t="s" ph="1">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
     <row r="48" spans="2:5" ph="1" x14ac:dyDescent="0.2">
@@ -7244,7 +7244,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -7252,7 +7252,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -7268,49 +7268,49 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="C7" t="s" ph="1">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="E7" ph="1"/>
     </row>
     <row r="8" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="C8" t="s" ph="1">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>217</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:5" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="C9" t="s" ph="1">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>164</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:5" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>166</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="132" x14ac:dyDescent="0.2">
@@ -7318,7 +7318,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -7332,37 +7332,37 @@
         <v>4</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="D13" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="D14" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="D15" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
@@ -7370,13 +7370,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -7407,7 +7407,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7415,7 +7415,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7431,7 +7431,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -7439,7 +7439,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7458,13 +7458,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7472,13 +7472,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -7486,7 +7486,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -7497,7 +7497,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -7508,21 +7508,21 @@
         <v>4</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="D13" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -7530,13 +7530,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7544,13 +7544,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -7558,13 +7558,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -7619,7 +7619,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7627,7 +7627,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7643,7 +7643,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -7651,7 +7651,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7667,47 +7667,47 @@
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="D9" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="D10" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="D11" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="D12" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="D13" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -7715,10 +7715,10 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="D14" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7726,50 +7726,50 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="D15" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="D16" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="D17" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="D18" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="D19" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="D20" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -7800,7 +7800,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7808,7 +7808,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>345</v>
+        <v>332</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7824,7 +7824,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>344</v>
+        <v>331</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -7835,7 +7835,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7846,7 +7846,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -7854,7 +7854,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -7862,10 +7862,10 @@
     </row>
     <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
       <c r="D9" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7873,13 +7873,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>337</v>
+        <v>324</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="198" x14ac:dyDescent="0.2">
@@ -7887,18 +7887,18 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>338</v>
+        <v>325</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7906,7 +7906,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -7917,7 +7917,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -7928,7 +7928,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>343</v>
+        <v>330</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -7961,7 +7961,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7969,7 +7969,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7985,7 +7985,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>327</v>
+        <v>314</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7993,7 +7993,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8009,7 +8009,7 @@
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -8017,7 +8017,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -8028,7 +8028,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -8036,21 +8036,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>312</v>
+        <v>299</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>319</v>
+        <v>306</v>
       </c>
       <c r="D12" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -8058,13 +8058,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8072,13 +8072,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -8086,13 +8086,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -8121,10 +8121,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8148,7 +8148,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8164,7 +8164,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="264" x14ac:dyDescent="0.2">
@@ -8172,7 +8172,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8225,7 +8225,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>351</v>
+        <v>338</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -8247,40 +8247,34 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
+        <v>277</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
+        <v>280</v>
       </c>
       <c r="D14" t="s">
-        <v>112</v>
+        <v>279</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>57</v>
+        <v>281</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>282</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8288,13 +8282,10 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" t="s">
-        <v>4</v>
+        <v>284</v>
       </c>
       <c r="D16" t="s">
-        <v>77</v>
+        <v>283</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8302,199 +8293,187 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D17" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="D18" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D19" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
         <v>23</v>
       </c>
-      <c r="D17" t="s">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="D25" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="1" t="s">
+    <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="1" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" t="s">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
+    <row r="31" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="6" t="s">
-        <v>349</v>
-      </c>
-      <c r="D24" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="66" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C25" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" s="1" t="s">
+    <row r="32" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C26" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C29" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C31" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8502,77 +8481,91 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>350</v>
+        <v>34</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>43</v>
+        <v>337</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>52</v>
+      <c r="B35" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="C35" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>51</v>
+      <c r="B36" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="C36" t="s">
         <v>7</v>
       </c>
-      <c r="D36" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
+      <c r="D36" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
       <c r="B37" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D37" t="s" ph="1">
-        <v>54</v>
+        <v>45</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>4</v>
-      </c>
       <c r="B38" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C38" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" t="s" ph="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" t="s">
         <v>7</v>
       </c>
-      <c r="D38" t="s">
-        <v>46</v>
+      <c r="D39" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -8611,7 +8604,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8627,17 +8620,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -8645,7 +8638,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -8659,7 +8652,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -8673,13 +8666,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8687,21 +8680,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="D12" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -8709,7 +8702,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update onedrive in web browser
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpsuzuki\Documents\2022_03\fresta2022\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79445AE8-A622-4CBB-8CBA-B81855C40A47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3164EBE7-8408-4514-AAE0-960A4B309A40}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" tabRatio="694" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,21 +96,10 @@
     <t xml:space="preserve">&lt;h2&gt;&lt;a name="mail"&gt;&lt;/a&gt;Office365 (Webメールとオンラインストレージ)&lt;/h2&gt; </t>
   </si>
   <si>
-    <t xml:space="preserve">次に、Office365のオンラインストレージのOneDriveを見て見ましょう。画面左上のつぶつぶをクリックします。
-するとOffice365で使用できるアプリケーション一覧が表示されます。その中にある「OneDrive」をクリックしましょう
-  </t>
-  </si>
-  <si>
-    <t>win10-6-08.svg</t>
-  </si>
-  <si>
     <t xml:space="preserve">ここにはひとりあたり１TBまで、データを置いておくことができます。
 データのバックアップをとっておいたり、外出先でもデータを取り出したりできるようになるので、活用しましょう。
 OneDriveにもアプリがありますので、スマホでも活用できます。
   </t>
-  </si>
-  <si>
-    <t>win10-6-09.svg</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;h2&gt;&lt;a name="mymomiji"&gt;&lt;/a&gt;MYもみじ (履修登録や掲示板など)&lt;/h2&gt; </t>
@@ -5551,6 +5540,19 @@
   </si>
   <si>
     <t>win11-outlook-for-web.png</t>
+  </si>
+  <si>
+    <t>win11-office365-from-outlook-to-onedrive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">次に、Office365のオンラインストレージのOneDriveを見て見ましょう。画面左上のつぶつぶをクリックします。
+するとOffice365で使用できるアプリケーション一覧が表示されます。その中にある「OneDrive」をクリックしましょう
+  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-onedrive-in-browser.png</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -5972,7 +5974,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5988,7 +5990,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -5996,7 +5998,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -6010,7 +6012,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6044,10 +6046,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6055,7 +6057,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6071,7 +6073,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -6079,7 +6081,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6090,17 +6092,17 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -6108,7 +6110,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -6145,7 +6147,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6153,7 +6155,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6169,7 +6171,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6177,7 +6179,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6193,15 +6195,15 @@
     </row>
     <row r="8" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6209,10 +6211,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D10" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6220,50 +6222,50 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D11" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D12" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D13" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D14" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D15" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D16" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6271,26 +6273,26 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D17" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D18" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D19" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -6321,7 +6323,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6329,7 +6331,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6345,7 +6347,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -6353,7 +6355,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6364,10 +6366,10 @@
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D8" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -6375,18 +6377,18 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D9" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D10" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6394,13 +6396,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -6408,46 +6410,46 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -6455,13 +6457,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6469,24 +6471,24 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="92.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C18" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D18" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -6494,13 +6496,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -6508,35 +6510,35 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
       </c>
       <c r="D21" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C22" t="s">
         <v>7</v>
       </c>
       <c r="D22" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6544,13 +6546,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -6558,13 +6560,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C24" t="s">
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -6696,7 +6698,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6704,7 +6706,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6720,7 +6722,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="304.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -6728,7 +6730,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -6742,13 +6744,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C7" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -6756,21 +6758,21 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
@@ -6778,13 +6780,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
@@ -6792,24 +6794,24 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
@@ -6817,13 +6819,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
@@ -6831,13 +6833,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C14" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -6845,24 +6847,24 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C15" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C16" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6870,345 +6872,345 @@
         <v>4</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B18" s="6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C25" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C26" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D26" t="s" ph="1">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C27" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D27" t="s" ph="1">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C28" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D28" t="s" ph="1">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C29" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D29" t="s" ph="1">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C30" t="s" ph="1">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D30" t="s" ph="1">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C31" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D31" t="s" ph="1">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C32" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D32" t="s" ph="1">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="33" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C33" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D33" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E33"/>
     </row>
     <row r="34" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C34" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D34" t="s" ph="1">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C35" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D35" t="s" ph="1">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C36" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D36" t="s" ph="1">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" spans="2:5" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C37" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E37"/>
     </row>
     <row r="38" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C38" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D38" t="s" ph="1">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C39" t="s" ph="1">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D39" t="s" ph="1">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="40" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B40" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C40" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D40" t="s" ph="1">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B41" s="6" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C41" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D41" t="s" ph="1">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="42" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B42" s="6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C42" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D42" t="s" ph="1">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="43" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B43" s="6" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C43" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D43" t="s" ph="1">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="44" spans="2:5" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B44" s="6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C44" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D44" t="s" ph="1">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="45" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B45" s="6" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C45" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D45" t="s" ph="1">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="46" spans="2:5" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B46" s="6" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C46" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D46" t="s" ph="1">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="47" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B47" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C47" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D47" t="s" ph="1">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="48" spans="2:5" ph="1" x14ac:dyDescent="0.2">
@@ -7244,7 +7246,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -7252,7 +7254,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -7268,49 +7270,49 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C7" t="s" ph="1">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E7" ph="1"/>
     </row>
     <row r="8" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C8" t="s" ph="1">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:5" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C9" t="s" ph="1">
+        <v>145</v>
+      </c>
+      <c r="D9" t="s" ph="1">
         <v>148</v>
-      </c>
-      <c r="D9" t="s" ph="1">
-        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:5" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="132" x14ac:dyDescent="0.2">
@@ -7318,7 +7320,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -7332,37 +7334,37 @@
         <v>4</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D13" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D14" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D15" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
@@ -7370,13 +7372,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -7407,7 +7409,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7415,7 +7417,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7431,7 +7433,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -7439,7 +7441,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7458,13 +7460,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7472,13 +7474,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -7486,7 +7488,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -7497,7 +7499,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -7508,21 +7510,21 @@
         <v>4</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D13" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -7530,13 +7532,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7544,13 +7546,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -7558,13 +7560,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -7619,7 +7621,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7627,7 +7629,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7643,7 +7645,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -7651,7 +7653,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7667,47 +7669,47 @@
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D10" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D11" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D12" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D13" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -7715,10 +7717,10 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D14" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7726,50 +7728,50 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D16" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D17" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D18" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D19" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D20" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -7800,7 +7802,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7808,7 +7810,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7824,7 +7826,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -7835,7 +7837,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7846,7 +7848,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -7854,7 +7856,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -7862,10 +7864,10 @@
     </row>
     <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D9" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7873,13 +7875,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="198" x14ac:dyDescent="0.2">
@@ -7887,18 +7889,18 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7906,7 +7908,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -7917,7 +7919,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -7928,7 +7930,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -7961,7 +7963,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7969,7 +7971,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7985,7 +7987,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7993,7 +7995,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8009,7 +8011,7 @@
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -8017,7 +8019,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -8028,7 +8030,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -8036,21 +8038,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D12" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -8058,13 +8060,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8072,13 +8074,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -8086,13 +8088,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -8124,7 +8126,7 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8148,7 +8150,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8164,7 +8166,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="264" x14ac:dyDescent="0.2">
@@ -8172,7 +8174,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8225,7 +8227,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -8252,10 +8254,10 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D13" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8263,18 +8265,18 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D14" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D15" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8282,10 +8284,10 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D16" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8293,10 +8295,10 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D17" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8304,18 +8306,18 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D18" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D19" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8323,13 +8325,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>20</v>
+        <v>341</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>21</v>
+        <v>340</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8337,18 +8339,18 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>23</v>
+        <v>342</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -8370,21 +8372,21 @@
         <v>4</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D25" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -8392,13 +8394,13 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8406,18 +8408,18 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -8439,13 +8441,13 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8453,13 +8455,13 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8467,13 +8469,13 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8481,13 +8483,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8495,13 +8497,13 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8509,7 +8511,7 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
@@ -8523,13 +8525,13 @@
         <v>4</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C36" t="s">
         <v>7</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -8537,21 +8539,21 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C37" t="s">
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D38" t="s" ph="1">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -8559,13 +8561,13 @@
         <v>4</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C39" t="s">
         <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -8604,7 +8606,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8620,17 +8622,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -8638,7 +8640,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -8652,7 +8654,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -8666,13 +8668,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8680,21 +8682,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D12" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -8702,7 +8704,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ch10 does not work well.
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpsuzuki\Documents\2022_03\fresta2022\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E74CC27-5647-487A-8291-991CD0083E4C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD151C2-F1B0-43D8-93EE-4599F0B2EBE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" tabRatio="694" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" tabRatio="817" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="ch7" sheetId="5" r:id="rId9"/>
     <sheet name="ch8" sheetId="8" r:id="rId10"/>
     <sheet name="ch9" sheetId="9" r:id="rId11"/>
-    <sheet name="ch10" sheetId="14" r:id="rId12"/>
+    <sheet name="chA" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
@@ -6307,8 +6307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DB449D4-AFC1-462F-B851-41C4675E501D}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8126,7 +8126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
image rename, win11 -> win11ja
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpsuzuki\Documents\2022_03\fresta2022\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62BF207-C6B3-4CB6-B2BA-D6B562249E02}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B31142D-93C4-405B-92C1-9A32EF4527D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" tabRatio="856" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" tabRatio="856" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -3395,10 +3395,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11-wifi-select.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>HU-CUPxxの基地局を選び、接続ボタンを押すと、認証が求められます。IMCアカウントとパスワードを入力し、OKボタンで進めます。初めて接続する基地局では本当に接続するか再確認を求められます。</t>
     <rPh sb="9" eb="12">
       <t>キチキョク</t>
@@ -3448,10 +3444,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11-wifi-auth.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>基地局に対するボタンが「切断」になったら接続が完了しています。</t>
     <rPh sb="0" eb="3">
       <t>キチキョク</t>
@@ -3468,10 +3460,6 @@
     <rPh sb="23" eb="25">
       <t>カンリョウ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11-wifi-connected.png</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -3521,10 +3509,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11-windows-update.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>まず、Windows Updateを設定しましょう。「設定」アプリを起動し、「Windows Update」を選んで、「更新プログラムのチェック」をクリックします。更新データがあると「今すぐダウンロード」に変わるので、クリックして更新を進めます。</t>
     <rPh sb="27" eb="29">
       <t>セッテイ</t>
@@ -3602,10 +3586,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11-windows-update-option.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>&lt;h2&gt;ウイルススキャン&lt;/h2&gt;</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -3657,10 +3637,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11-setting-security.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>さらに「Windowsセキュリティを開く」をクリックします。</t>
     <rPh sb="18" eb="19">
       <t>ヒラ</t>
@@ -3668,10 +3644,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11-setting-security2.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>「Windowsセキュリティ」のウィンドウが開きます。「ウイルスと脅威の防止」をクリックします。</t>
     <rPh sb="22" eb="23">
       <t>ヒラ</t>
@@ -3685,10 +3657,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11-windows-security.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>まず「スキャンのオプション」をクリックし、「フルスキャン」を選びます。スクロールして「今すぐスキャン」をクリックし、フルスキャンを開始します。</t>
     <rPh sb="30" eb="31">
       <t>エラ</t>
@@ -3709,14 +3677,6 @@
     <rPh sb="19" eb="21">
       <t>デンゲン</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11-start-full-scan.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11-scan-progress.png</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -4301,14 +4261,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11-ms-signin.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11-ms-signin2.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>IMCアカウントを「@hiroshima-u.ac.jp」つきで入力し、さらにパスワードも入力します。このサイトはMicrosoftのサイトなので、「@hiroshima-u.ac.jp」がついていないと貴方の学生番号がどの大学のものか判らないため、「@hiroshima-u.ac.jp」を加える必要があります。</t>
     <rPh sb="32" eb="34">
       <t>ニュウリョク</t>
@@ -4368,14 +4320,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11-ms-signin3.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11-ms-myaccount.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>サインインが完了すると、右上の人型のマークが社員証のマークに変わっています。これをクリックしてサブメニューを表示させ、さらに「アカウントを表示」に進みます。「マイアカウント」というページに移動します。</t>
     <rPh sb="6" eb="8">
       <t>カンリョウ</t>
@@ -4432,10 +4376,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11-ms-office365.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>右上にある「Officeのインストール」をクリックし、さらに「Office365アプリ」を選択して、ダウンロードします。</t>
     <rPh sb="0" eb="2">
       <t>ミギウエ</t>
@@ -4446,10 +4386,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11-office365-download.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>ダウンロードが終わったら、GoogleChromeのインストールと同様にフォルダアイコンをクリックしてOfficeSetupをデスクトップに移動します。</t>
     <rPh sb="7" eb="8">
       <t>オ</t>
@@ -4463,14 +4399,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11-officesetup.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11-office365-install.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>インストールが完了したらOfficeSetupは削除しましょう。</t>
     <rPh sb="7" eb="9">
       <t>カンリョウ</t>
@@ -4478,14 +4406,6 @@
     <rPh sb="24" eb="26">
       <t>サクジョ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11-officesetup-delete.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11-lookup-msoffice-app.png</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -4605,14 +4525,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11-search-excel.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11-office-license0a.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>IMCアカウント(@hiroshima-u.ac.jpを含む)を入力し、パスワードも入力します。</t>
     <rPh sb="28" eb="29">
       <t>フク</t>
@@ -4626,14 +4538,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11-office-license2.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11-office-signin-limited.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>「組織がデバイスを管理できるようにする」のチェックを外し、「いいえ、このアプリのみにサインインします」をクリックします。</t>
     <rPh sb="1" eb="3">
       <t>ソシキ</t>
@@ -4644,10 +4548,6 @@
     <rPh sb="26" eb="27">
       <t>ハズ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11-office-license-agreement.png</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -4817,10 +4717,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11-teams-variants.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Microsoft Teamsには「職場または学校用」のものと、「小企業用」のものの2つがあります。自分のPCのタスクバーの検索フォームから「Teams」を検索すると、「学校用Teamsだけが有る」「学校用と小企業用Teamsがある」「小企業用Teamsだけがある」の3つの可能性があります。アイコンが少し違います。</t>
     <rPh sb="50" eb="52">
       <t>ジブン</t>
@@ -4867,14 +4763,6 @@
     <rPh sb="153" eb="154">
       <t>チガ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11-teams-first-dialog.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11-teams-signin.png</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -5373,10 +5261,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11-momiji-before-login.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>hirodaiID-login.png</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -5424,10 +5308,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11-momiji-before-login0.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Office365のページの左側にブラウザ内で使用できるアプリのアイコンが並びます。「O」の文字があるOutlook for Webをクリックします。</t>
     <rPh sb="14" eb="16">
       <t>ヒダリガワ</t>
@@ -5475,27 +5355,12 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11-office365-outlook-start.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11-outlook-for-web.png</t>
-  </si>
-  <si>
     <t xml:space="preserve">次に、Office365のオンラインストレージのOneDriveを見て見ましょう。画面左上のつぶつぶをクリックします。
 するとOffice365で使用できるアプリケーション一覧が表示されます。その中にある「OneDrive」をクリックしましょう
   </t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11-onedrive-in-browser.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11-office365-from-outlook-to-onedrive.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>FRESTA-TEXT-2021 Win11 chap.8</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -5545,6 +5410,108 @@
       <t>カタ</t>
     </rPh>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-wifi-select.png</t>
+  </si>
+  <si>
+    <t>win11ja-wifi-auth.png</t>
+  </si>
+  <si>
+    <t>win11ja-wifi-connected.png</t>
+  </si>
+  <si>
+    <t>win11ja-windows-update.png</t>
+  </si>
+  <si>
+    <t>win11ja-windows-update-option.png</t>
+  </si>
+  <si>
+    <t>win11ja-setting-security.png</t>
+  </si>
+  <si>
+    <t>win11ja-setting-security2.png</t>
+  </si>
+  <si>
+    <t>win11ja-windows-security.png</t>
+  </si>
+  <si>
+    <t>win11ja-start-full-scan.png</t>
+  </si>
+  <si>
+    <t>win11ja-scan-progress.png</t>
+  </si>
+  <si>
+    <t>win11ja-search-excel.png</t>
+  </si>
+  <si>
+    <t>win11ja-office-license0a.png</t>
+  </si>
+  <si>
+    <t>win11ja-office-license2.png</t>
+  </si>
+  <si>
+    <t>win11ja-office-signin-limited.png</t>
+  </si>
+  <si>
+    <t>win11ja-office-license-agreement.png</t>
+  </si>
+  <si>
+    <t>win11ja-momiji-before-login0.png</t>
+  </si>
+  <si>
+    <t>win11ja-ms-signin.png</t>
+  </si>
+  <si>
+    <t>win11ja-ms-signin2.png</t>
+  </si>
+  <si>
+    <t>win11ja-ms-signin3.png</t>
+  </si>
+  <si>
+    <t>win11ja-ms-myaccount.png</t>
+  </si>
+  <si>
+    <t>win11ja-ms-office365.png</t>
+  </si>
+  <si>
+    <t>win11ja-office365-outlook-start.png</t>
+  </si>
+  <si>
+    <t>win11ja-outlook-for-web.png</t>
+  </si>
+  <si>
+    <t>win11ja-office365-from-outlook-to-onedrive.png</t>
+  </si>
+  <si>
+    <t>win11ja-onedrive-in-browser.png</t>
+  </si>
+  <si>
+    <t>win11ja-momiji-before-login.png</t>
+  </si>
+  <si>
+    <t>win11ja-office365-download.png</t>
+  </si>
+  <si>
+    <t>win11ja-officesetup.png</t>
+  </si>
+  <si>
+    <t>win11ja-office365-install.png</t>
+  </si>
+  <si>
+    <t>win11ja-officesetup-delete.png</t>
+  </si>
+  <si>
+    <t>win11ja-lookup-msoffice-app.png</t>
+  </si>
+  <si>
+    <t>win11ja-teams-variants.png</t>
+  </si>
+  <si>
+    <t>win11ja-teams-first-dialog.png</t>
+  </si>
+  <si>
+    <t>win11ja-teams-signin.png</t>
   </si>
 </sst>
 </file>
@@ -6025,7 +5992,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -6065,7 +6032,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>333</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -6122,8 +6089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392D1BFF-FF5C-4A7E-8C9C-E750AF0FFFAF}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D37" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -6139,7 +6106,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>340</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6147,7 +6114,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>335</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6163,17 +6130,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>334</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>340</v>
+        <v>306</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>339</v>
+        <v>305</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6205,7 +6172,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6213,10 +6180,10 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="D12" t="s">
-        <v>266</v>
+        <v>324</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6224,50 +6191,50 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="D13" t="s">
-        <v>267</v>
+        <v>325</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="D14" t="s">
-        <v>270</v>
+        <v>326</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="D15" t="s">
-        <v>271</v>
+        <v>327</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="D16" t="s">
-        <v>274</v>
+        <v>328</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="D17" t="s">
-        <v>276</v>
+        <v>334</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>277</v>
+        <v>261</v>
       </c>
       <c r="D18" t="s">
-        <v>278</v>
+        <v>335</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6275,31 +6242,31 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>284</v>
+        <v>264</v>
       </c>
       <c r="D19" t="s">
-        <v>279</v>
+        <v>336</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
       <c r="D20" t="s">
-        <v>281</v>
+        <v>337</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>283</v>
+        <v>263</v>
       </c>
       <c r="D21" t="s">
-        <v>282</v>
+        <v>338</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>341</v>
+        <v>307</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -6315,37 +6282,37 @@
     </row>
     <row r="25" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>297</v>
+        <v>271</v>
       </c>
       <c r="D25" t="s">
-        <v>296</v>
+        <v>339</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>301</v>
+        <v>273</v>
       </c>
       <c r="D26" t="s">
-        <v>298</v>
+        <v>340</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>300</v>
+        <v>272</v>
       </c>
       <c r="D27" t="s">
-        <v>299</v>
+        <v>341</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>292</v>
+        <v>268</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>291</v>
+        <v>321</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -6503,7 +6470,7 @@
   <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:D47"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.2"/>
@@ -6528,7 +6495,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6544,7 +6511,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>338</v>
+        <v>304</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="304.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -7052,7 +7019,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -7076,7 +7043,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -7092,7 +7059,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>337</v>
+        <v>303</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
@@ -7142,7 +7109,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -7215,13 +7182,13 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView zoomScale="112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="100.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="87.88671875" style="6" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
@@ -7231,7 +7198,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7239,7 +7206,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7255,7 +7222,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -7263,7 +7230,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7282,13 +7249,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>214</v>
+        <v>311</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7296,13 +7263,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>217</v>
+        <v>312</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -7310,7 +7277,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -7321,7 +7288,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -7332,21 +7299,21 @@
         <v>4</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>221</v>
+        <v>313</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="D13" t="s">
-        <v>223</v>
+        <v>314</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -7354,13 +7321,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>225</v>
+        <v>315</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7368,13 +7335,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>228</v>
+        <v>316</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -7382,13 +7349,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>229</v>
+        <v>317</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -7427,7 +7394,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -7451,7 +7418,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7467,7 +7434,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -7475,7 +7442,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7496,42 +7463,42 @@
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="D9" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="D10" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="D11" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="D12" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="D13" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -7539,10 +7506,10 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="D14" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7550,50 +7517,50 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="D15" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="D16" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="D17" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="D18" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="D19" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="D20" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -7608,7 +7575,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -7624,7 +7591,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>304</v>
+        <v>276</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7632,7 +7599,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>319</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7648,7 +7615,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>318</v>
+        <v>290</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -7659,7 +7626,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>305</v>
+        <v>277</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7670,7 +7637,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>306</v>
+        <v>278</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -7678,7 +7645,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>307</v>
+        <v>279</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -7686,10 +7653,10 @@
     </row>
     <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>308</v>
+        <v>280</v>
       </c>
       <c r="D9" t="s">
-        <v>309</v>
+        <v>281</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7697,13 +7664,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>310</v>
+        <v>282</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>311</v>
+        <v>283</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="198" x14ac:dyDescent="0.2">
@@ -7711,18 +7678,18 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>312</v>
+        <v>284</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>313</v>
+        <v>285</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>314</v>
+        <v>286</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7730,7 +7697,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>315</v>
+        <v>287</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -7741,7 +7708,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>316</v>
+        <v>288</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -7752,7 +7719,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>317</v>
+        <v>289</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -7769,7 +7736,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -7793,7 +7760,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7809,7 +7776,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>302</v>
+        <v>274</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7817,7 +7784,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7860,21 +7827,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>286</v>
+        <v>266</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>287</v>
+        <v>318</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>294</v>
+        <v>269</v>
       </c>
       <c r="D12" t="s">
-        <v>288</v>
+        <v>319</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -7882,13 +7849,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>289</v>
+        <v>267</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>290</v>
+        <v>320</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7896,13 +7863,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>292</v>
+        <v>268</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>291</v>
+        <v>321</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -7910,13 +7877,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>295</v>
+        <v>270</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>293</v>
+        <v>322</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -7948,7 +7915,7 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -7972,7 +7939,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7988,7 +7955,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>336</v>
+        <v>302</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="264" x14ac:dyDescent="0.2">
@@ -8049,7 +8016,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -8076,10 +8043,10 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="D13" t="s">
-        <v>266</v>
+        <v>324</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8087,18 +8054,18 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="D14" t="s">
-        <v>267</v>
+        <v>325</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="D15" t="s">
-        <v>270</v>
+        <v>326</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8106,10 +8073,10 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="D16" t="s">
-        <v>271</v>
+        <v>327</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8117,10 +8084,10 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="D17" t="s">
-        <v>274</v>
+        <v>328</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8128,18 +8095,18 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>326</v>
+        <v>296</v>
       </c>
       <c r="D18" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>327</v>
+        <v>297</v>
       </c>
       <c r="D19" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8147,13 +8114,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>330</v>
+        <v>298</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8167,7 +8134,7 @@
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -8194,21 +8161,21 @@
         <v>4</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>320</v>
+        <v>292</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>321</v>
+        <v>333</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>323</v>
+        <v>294</v>
       </c>
       <c r="D25" t="s">
-        <v>322</v>
+        <v>293</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -8319,7 +8286,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>324</v>
+        <v>295</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
@@ -8403,8 +8370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8428,7 +8395,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8444,7 +8411,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>303</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8496,7 +8463,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>205</v>
+        <v>308</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8504,21 +8471,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>207</v>
+        <v>309</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D12" t="s">
-        <v>209</v>
+        <v>310</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -8526,7 +8493,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
win11ja: update how to access Office365 portal.
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpsuzuki\Documents\2022_03\fresta2022\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CB8D7A-C254-44B8-AFA4-44F104BF2131}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6AE30E-A543-40A5-A02B-5C2DFC7D0FFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" tabRatio="856" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="337">
   <si>
     <t>header1</t>
   </si>
@@ -3318,22 +3318,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">ここでは、Microsoft Edgeの初期設定とGoogle Chrome のインストールを行います。
-&lt;ul&gt;
-&lt;li&gt;
-&lt;a href="#chrome"&gt;Google Chromeのインストール&lt;/a&gt;
-&lt;/li&gt;
-&lt;/ul&gt;
- </t>
-    <rPh sb="20" eb="22">
-      <t>ショキ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>セッテイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>まず画面の最下部のタスクバーに「e」を模した青緑のアイコンがありますので、これをクリックしてMicrosoft Edgeを起動します。</t>
     <rPh sb="2" eb="4">
       <t>ガメン</t>
@@ -3428,138 +3412,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Edgeの規定の新規タブには大量の広告が入ってくるので、オンライン授業などで画面共有の際に憚られるような画面になる場合があります。右上の歯車アイコンを押して、画面レイアウトを「シンプル」にしましょう。これでEdgeの基本的な設定は終わります。</t>
-    <rPh sb="5" eb="7">
-      <t>キテイ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>シンキ</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>タイリョウ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>コウコク</t>
-    </rPh>
-    <rPh sb="20" eb="21">
-      <t>ハイ</t>
-    </rPh>
-    <rPh sb="33" eb="35">
-      <t>ジュギョウ</t>
-    </rPh>
-    <rPh sb="38" eb="40">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="40" eb="42">
-      <t>キョウユウ</t>
-    </rPh>
-    <rPh sb="43" eb="44">
-      <t>サイ</t>
-    </rPh>
-    <rPh sb="45" eb="46">
-      <t>ハバカ</t>
-    </rPh>
-    <rPh sb="52" eb="54">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="57" eb="59">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="65" eb="66">
-      <t>ミギ</t>
-    </rPh>
-    <rPh sb="66" eb="67">
-      <t>ウエ</t>
-    </rPh>
-    <rPh sb="68" eb="70">
-      <t>ハグルマ</t>
-    </rPh>
-    <rPh sb="75" eb="76">
-      <t>オ</t>
-    </rPh>
-    <rPh sb="79" eb="81">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="108" eb="111">
-      <t>キホンテキ</t>
-    </rPh>
-    <rPh sb="112" eb="114">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="115" eb="116">
-      <t>オ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ブラウザの最上部は本来はwww.microsoft.comなどのURL(ホームページアドレスなどと呼ばれることがあります)を入れるものですが、多くのブラウザが検索フォームも兼ねています。ここにGoogle Chrome downloadと入れてみましょう。Microsoftが入れてほしくなさそうな広告を入れてきますが、無視してGoogleからダウンロードします。
-ここで注意しないといけないのは、「Google Chromeのダウンロード」と称してウイルスをダウンロードさせるようなサイトが検索の上位に来る可能性があるということです。URLがwww.google.comになっていることを確認した上でジャンプしましょう。</t>
-    <rPh sb="5" eb="6">
-      <t>サイ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>ジョウブ</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>ホンライ</t>
-    </rPh>
-    <rPh sb="49" eb="50">
-      <t>ヨ</t>
-    </rPh>
-    <rPh sb="62" eb="63">
-      <t>イ</t>
-    </rPh>
-    <rPh sb="71" eb="72">
-      <t>オオ</t>
-    </rPh>
-    <rPh sb="79" eb="81">
-      <t>ケンサク</t>
-    </rPh>
-    <rPh sb="86" eb="87">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="119" eb="120">
-      <t>イ</t>
-    </rPh>
-    <rPh sb="138" eb="139">
-      <t>イ</t>
-    </rPh>
-    <rPh sb="149" eb="151">
-      <t>コウコク</t>
-    </rPh>
-    <rPh sb="152" eb="153">
-      <t>イ</t>
-    </rPh>
-    <rPh sb="160" eb="162">
-      <t>ムシ</t>
-    </rPh>
-    <rPh sb="186" eb="188">
-      <t>チュウイ</t>
-    </rPh>
-    <rPh sb="222" eb="223">
-      <t>ショウ</t>
-    </rPh>
-    <rPh sb="246" eb="248">
-      <t>ケンサク</t>
-    </rPh>
-    <rPh sb="249" eb="251">
-      <t>ジョウイ</t>
-    </rPh>
-    <rPh sb="252" eb="253">
-      <t>ク</t>
-    </rPh>
-    <rPh sb="254" eb="257">
-      <t>カノウセイ</t>
-    </rPh>
-    <rPh sb="295" eb="297">
-      <t>カクニン</t>
-    </rPh>
-    <rPh sb="299" eb="300">
-      <t>ウエ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Googleのダウンロードページにジャンプしました。Google Chromeのブラウザ内部のデータをGoogleに送信しても良いかという許可チェックボックスがありますが、このチェックを外してダウンロードを行います。</t>
     <rPh sb="44" eb="46">
       <t>ナイブ</t>
@@ -3718,10 +3570,6 @@
   </si>
   <si>
     <t>win11ja-edge-layout.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11ja-edge-search-chrome.png</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -3790,34 +3638,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>microsoft.comにアクセスします。画面の一番上に広告が出てくることがありますが、「結構です」で消しておきましょう。右上に「サインイン」と注された人型アイコンがあるので、クリックします。URLフォームの横にある人型アイコンではないことに注意してください。</t>
-    <rPh sb="22" eb="24">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="25" eb="27">
-      <t>イチバン</t>
-    </rPh>
-    <rPh sb="27" eb="28">
-      <t>ウエ</t>
-    </rPh>
-    <rPh sb="29" eb="31">
-      <t>コウコク</t>
-    </rPh>
-    <rPh sb="32" eb="33">
-      <t>デ</t>
-    </rPh>
-    <rPh sb="46" eb="48">
-      <t>ケッコウ</t>
-    </rPh>
-    <rPh sb="52" eb="53">
-      <t>ケ</t>
-    </rPh>
-    <rPh sb="62" eb="64">
-      <t>ミギウエ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>IMCアカウントを「@hiroshima-u.ac.jp」つきで入力し、さらにパスワードも入力します。このサイトはMicrosoftのサイトなので、「@hiroshima-u.ac.jp」がついていないと貴方の学生番号がどの大学のものか判らないため、「@hiroshima-u.ac.jp」を加える必要があります。</t>
     <rPh sb="32" eb="34">
       <t>ニュウリョク</t>
@@ -3873,62 +3693,6 @@
     </rPh>
     <rPh sb="76" eb="77">
       <t>カマ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>サインインが完了すると、右上の人型のマークが社員証のマークに変わっています。これをクリックしてサブメニューを表示させ、さらに「アカウントを表示」に進みます。「マイアカウント」というページに移動します。</t>
-    <rPh sb="6" eb="8">
-      <t>カンリョウ</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>ミギウエ</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>ヒトガタ</t>
-    </rPh>
-    <rPh sb="22" eb="25">
-      <t>シャインショウ</t>
-    </rPh>
-    <rPh sb="30" eb="31">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="54" eb="56">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="69" eb="71">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="73" eb="74">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="94" eb="96">
-      <t>イドウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「マイアカウント」のページの左上に3x3個の点が並んでいるアイコンがあるので、これをクリックしてサブメニューを表示させます。その中の「Office」をクリックすると、「マイアカウント」から「Office365」のページに移動します。</t>
-    <rPh sb="14" eb="16">
-      <t>ヒダリウエ</t>
-    </rPh>
-    <rPh sb="20" eb="21">
-      <t>コ</t>
-    </rPh>
-    <rPh sb="22" eb="23">
-      <t>テン</t>
-    </rPh>
-    <rPh sb="24" eb="25">
-      <t>ナラ</t>
-    </rPh>
-    <rPh sb="55" eb="57">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="64" eb="65">
-      <t>ナカ</t>
-    </rPh>
-    <rPh sb="110" eb="112">
-      <t>イドウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -4432,24 +4196,6 @@
     </rPh>
     <rPh sb="65" eb="67">
       <t>リヨウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>次のリンクから広島大学オンライン学習支援システム（Moodle）にアクセスしてください。
-&lt;a href="https://moodle.vle.hiroshima-u.ac.jp/local/hulogin/"&gt;https://moodle.vle.hiroshima-u.ac.jp/local/hulogin/&lt;/a&gt;
-「広大IDでログイン」をクリックしましょう。</t>
-    <rPh sb="0" eb="1">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="7" eb="11">
-      <t>ヒロシマダイガク</t>
-    </rPh>
-    <rPh sb="16" eb="20">
-      <t>ガクシュウシエン</t>
-    </rPh>
-    <rPh sb="164" eb="166">
-      <t>ヒロダイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -4920,19 +4666,10 @@
     <t>win11ja-momiji-before-login0.png</t>
   </si>
   <si>
-    <t>win11ja-ms-signin.png</t>
-  </si>
-  <si>
     <t>win11ja-ms-signin2.png</t>
   </si>
   <si>
     <t>win11ja-ms-signin3.png</t>
-  </si>
-  <si>
-    <t>win11ja-ms-myaccount.png</t>
-  </si>
-  <si>
-    <t>win11ja-ms-office365.png</t>
   </si>
   <si>
     <t>win11ja-office365-outlook-start.png</t>
@@ -5655,6 +5392,178 @@
     </rPh>
     <rPh sb="28" eb="29">
       <t>カタ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Edgeの規定の新規タブには大量の広告が入ってくるので、オンライン授業などで画面共有の際に憚られるような画面になる場合があります。右上の歯車アイコンを押して、画面レイアウトを「シンプル」にしましょう。これでEdgeの基本的な設定は終わります。
+このwebテキストをスマートフォンなどで見ている方は、これ以降では、様々なwebページにアクセスするため、この初期設定テキストを設定対象のPCの上のEdgeで見ながら作業すると簡単です。</t>
+    <rPh sb="5" eb="7">
+      <t>キテイ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>シンキ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>タイリョウ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>コウコク</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>ハイ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>ジュギョウ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>キョウユウ</t>
+    </rPh>
+    <rPh sb="43" eb="44">
+      <t>サイ</t>
+    </rPh>
+    <rPh sb="45" eb="46">
+      <t>ハバカ</t>
+    </rPh>
+    <rPh sb="52" eb="54">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="57" eb="59">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="65" eb="66">
+      <t>ミギ</t>
+    </rPh>
+    <rPh sb="66" eb="67">
+      <t>ウエ</t>
+    </rPh>
+    <rPh sb="68" eb="70">
+      <t>ハグルマ</t>
+    </rPh>
+    <rPh sb="75" eb="76">
+      <t>オ</t>
+    </rPh>
+    <rPh sb="79" eb="81">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="108" eb="111">
+      <t>キホンテキ</t>
+    </rPh>
+    <rPh sb="112" eb="114">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="115" eb="116">
+      <t>オ</t>
+    </rPh>
+    <rPh sb="142" eb="143">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="146" eb="147">
+      <t>カタ</t>
+    </rPh>
+    <rPh sb="151" eb="153">
+      <t>イコウ</t>
+    </rPh>
+    <rPh sb="156" eb="158">
+      <t>サマザマ</t>
+    </rPh>
+    <rPh sb="177" eb="179">
+      <t>ショキ</t>
+    </rPh>
+    <rPh sb="179" eb="181">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="186" eb="188">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="188" eb="190">
+      <t>タイショウ</t>
+    </rPh>
+    <rPh sb="194" eb="195">
+      <t>ウエ</t>
+    </rPh>
+    <rPh sb="201" eb="202">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="205" eb="207">
+      <t>サギョウ</t>
+    </rPh>
+    <rPh sb="210" eb="212">
+      <t>カンタン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>それでは&lt;a href="https://www.google.com/chrome/" target="_blank" rel="noreferrer"&gt;https://www.google.com/chrome/&lt;/a&gt;からGoogle Chromeをダウンロードしましょう。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ここでは、Microsoft Edgeの初期設定とGoogle Chrome のインストールを行います。Microsoft Edgeの初期設定が終わったら、このwebテキストをMicrosoft Edgeで表示させて作業を進めるのが簡単です。
+ </t>
+    <rPh sb="20" eb="22">
+      <t>ショキ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="67" eb="69">
+      <t>ショキ</t>
+    </rPh>
+    <rPh sb="69" eb="71">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="72" eb="73">
+      <t>オ</t>
+    </rPh>
+    <rPh sb="103" eb="105">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="108" eb="110">
+      <t>サギョウ</t>
+    </rPh>
+    <rPh sb="111" eb="112">
+      <t>スス</t>
+    </rPh>
+    <rPh sb="116" eb="118">
+      <t>カンタン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>次のリンクから広島大学オンライン学習支援システム（Moodle）にアクセスしてください。
+&lt;a href="https://moodle.vle.hiroshima-u.ac.jp/local/hulogin/" target="_blank" rel="noreferrer"&gt;https://moodle.vle.hiroshima-u.ac.jp/local/hulogin/&lt;/a&gt;
+「広大IDでログイン」をクリックしましょう。</t>
+    <rPh sb="0" eb="1">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="7" eb="11">
+      <t>ヒロシマダイガク</t>
+    </rPh>
+    <rPh sb="16" eb="20">
+      <t>ガクシュウシエン</t>
+    </rPh>
+    <rPh sb="197" eb="199">
+      <t>ヒロダイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-imc-office365-portal.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メディアセンタのMicrosoft 365ポータルサイト&lt;a href="https://www.media.hiroshima-u.ac.jp/services/webmail-portal/" target="_blank" rel="noreferrer"&gt;https://www.media.hiroshima-u.ac.jp/services/webmail-portal/&lt;/a&gt;にジャンプします。水色の「Microsoft365ポータル」を押すと&lt;a href="https://portal.office.com/" target="_blank" rel="noreferrer"&gt;https://portal.office.com/&lt;/a&gt;に移動します。</t>
+    <rPh sb="205" eb="207">
+      <t>ミズイロ</t>
+    </rPh>
+    <rPh sb="227" eb="228">
+      <t>オ</t>
+    </rPh>
+    <rPh sb="331" eb="333">
+      <t>イドウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -6134,10 +6043,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392D1BFF-FF5C-4A7E-8C9C-E750AF0FFFAF}">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -6153,7 +6062,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6161,7 +6070,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6177,22 +6086,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6224,18 +6133,18 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>236</v>
+        <v>336</v>
       </c>
       <c r="D16" t="s">
-        <v>295</v>
+        <v>335</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6243,270 +6152,254 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="D17" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D18" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D19" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D20" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D21" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D22" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D23" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D29" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="D21" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B22" s="1" t="s">
+    <row r="30" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D30" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D31" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="D22" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D23" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="D24" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="D25" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C29" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B31" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="D31" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="B32" s="1" t="s">
-        <v>254</v>
+      <c r="C32" t="s">
+        <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>311</v>
+        <v>284</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>253</v>
+        <v>74</v>
+      </c>
+      <c r="C33" t="s">
+        <v>7</v>
       </c>
       <c r="D33" t="s">
-        <v>312</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>249</v>
+        <v>81</v>
       </c>
       <c r="C34" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="C35" t="s">
         <v>7</v>
       </c>
       <c r="D35" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="C36" t="s">
         <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="C37" t="s">
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C38" t="s">
         <v>7</v>
       </c>
       <c r="D38" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="C39" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="D39" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C40" t="s">
         <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" ht="105.6" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C41" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="D41" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" ht="79.2" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C42" t="s">
         <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C43" t="s">
         <v>7</v>
       </c>
       <c r="D43" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C44" t="s">
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="2:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C45" t="s">
         <v>7</v>
       </c>
       <c r="D45" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B46" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C46" t="s">
-        <v>7</v>
-      </c>
-      <c r="D46" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" ht="66" x14ac:dyDescent="0.2">
-      <c r="B47" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C47" t="s">
-        <v>7</v>
-      </c>
-      <c r="D47" t="s">
         <v>75</v>
       </c>
     </row>
@@ -6563,7 +6456,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="304.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -6571,7 +6464,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -6635,7 +6528,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>7</v>
@@ -6660,7 +6553,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>7</v>
@@ -6985,7 +6878,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -6993,7 +6886,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
     </row>
     <row r="3" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -7009,7 +6902,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -7017,36 +6910,36 @@
     </row>
     <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="D7" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="D8" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="D9" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -7054,13 +6947,13 @@
     </row>
     <row r="12" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -7250,7 +7143,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -7291,7 +7184,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
@@ -7413,7 +7306,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView zoomScale="112" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="112" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
@@ -7487,7 +7380,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7501,7 +7394,7 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -7537,7 +7430,7 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -7545,7 +7438,7 @@
         <v>199</v>
       </c>
       <c r="D17" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -7559,7 +7452,7 @@
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7573,7 +7466,7 @@
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -7587,7 +7480,7 @@
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -7625,8 +7518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C43F54BA-B356-43A4-B76F-707ED0C70724}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="A8:XFD8"/>
+    <sheetView zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -7666,15 +7559,15 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>208</v>
+        <v>333</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7695,53 +7588,50 @@
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D10" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D11" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D12" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D13" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>213</v>
+        <v>331</v>
       </c>
       <c r="D14" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D15" t="s">
-        <v>226</v>
+        <v>332</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7749,50 +7639,50 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D16" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D17" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D18" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D19" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D20" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D21" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -7804,10 +7694,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D6E33FB-2290-439B-854D-9A45A4600EF5}">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D42" sqref="B40:D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -7823,7 +7713,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7831,7 +7721,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7847,7 +7737,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -7858,7 +7748,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7872,7 +7762,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -7883,18 +7773,18 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>258</v>
+        <v>334</v>
       </c>
       <c r="D11" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7902,13 +7792,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="198" x14ac:dyDescent="0.2">
@@ -7916,18 +7806,18 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -7938,7 +7828,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -7949,7 +7839,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -7960,7 +7850,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -7998,13 +7888,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -8025,21 +7915,21 @@
     </row>
     <row r="26" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="D27" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -8126,7 +8016,7 @@
     </row>
     <row r="36" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
@@ -8140,7 +8030,7 @@
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
@@ -8154,155 +8044,139 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>236</v>
+        <v>336</v>
       </c>
       <c r="D40" t="s">
-        <v>295</v>
+        <v>335</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="D41" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D42" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>239</v>
+        <v>263</v>
       </c>
       <c r="D43" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
-        <v>240</v>
+        <v>264</v>
       </c>
       <c r="D44" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
+      </c>
+      <c r="C45" t="s">
+        <v>4</v>
       </c>
       <c r="D45" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
-        <v>272</v>
+        <v>17</v>
+      </c>
+      <c r="C46" t="s">
+        <v>4</v>
       </c>
       <c r="D46" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B47" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="C47" t="s">
-        <v>4</v>
-      </c>
-      <c r="D47" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C48" t="s">
-        <v>4</v>
-      </c>
-      <c r="D48" t="s">
-        <v>303</v>
+        <v>326</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B49" s="1"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B51" s="1"/>
-    </row>
-    <row r="52" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>325</v>
+      </c>
+      <c r="C50" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" ht="118.8" x14ac:dyDescent="0.2">
+      <c r="B51" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C51" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="B52" s="1" t="s">
-        <v>336</v>
+        <v>36</v>
       </c>
       <c r="C52" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D52" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" ht="118.8" x14ac:dyDescent="0.2">
-      <c r="B53" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C53" t="s">
-        <v>7</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" ht="105.6" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" ht="92.4" x14ac:dyDescent="0.2">
+      <c r="B53" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D53" t="s" ph="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B54" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C54" t="s">
         <v>7</v>
       </c>
       <c r="D54" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" ht="92.4" x14ac:dyDescent="0.2">
-      <c r="B55" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D55" t="s" ph="1">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" ht="92.4" x14ac:dyDescent="0.2">
-      <c r="B56" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C56" t="s">
-        <v>7</v>
-      </c>
-      <c r="D56" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="57" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="D57" ph="1"/>
+    <row r="55" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="D55" ph="1"/>
+    </row>
+    <row r="66" spans="4:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="D66" ph="1"/>
     </row>
     <row r="68" spans="4:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="D68" ph="1"/>
-    </row>
-    <row r="70" spans="4:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="D70" ph="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -8340,7 +8214,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8356,7 +8230,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -8364,7 +8238,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8388,7 +8262,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -8407,21 +8281,21 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="D15" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -8429,13 +8303,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8443,13 +8317,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -8457,13 +8331,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -8519,7 +8393,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8535,7 +8409,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8587,7 +8461,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8601,7 +8475,7 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -8609,7 +8483,7 @@
         <v>189</v>
       </c>
       <c r="D12" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
win11ja: update for 1st login to MyMomiji
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20383"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20384"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpsuzuki\Documents\2022_03\fresta2022\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6AE30E-A543-40A5-A02B-5C2DFC7D0FFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349E4500-EC14-4618-A018-A92E12451EF1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" tabRatio="856" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" tabRatio="856" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="339">
   <si>
     <t>header1</t>
   </si>
@@ -5565,6 +5565,76 @@
     <rPh sb="331" eb="333">
       <t>イドウ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>初めてMyもみじにログインするときだけ、この画面が出ます。画面の説明をよく読んで、「同意する」「同意しない」のどちらかを選んで「次へ」をクリックしてください。
+※ 図中でも説明していますが、どちらを選んでも後で変更はできます。また、どちらを選んでもMyもみじは使えます。
+さらに詳しいことは画面中にあるFAQへのリンクを参照してください。</t>
+    <rPh sb="0" eb="1">
+      <t>ハジ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>セツメイ</t>
+    </rPh>
+    <rPh sb="37" eb="38">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>ドウイ</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>ドウイ</t>
+    </rPh>
+    <rPh sb="60" eb="61">
+      <t>エラ</t>
+    </rPh>
+    <rPh sb="64" eb="65">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="82" eb="84">
+      <t>ズチュウ</t>
+    </rPh>
+    <rPh sb="86" eb="88">
+      <t>セツメイ</t>
+    </rPh>
+    <rPh sb="99" eb="100">
+      <t>エラ</t>
+    </rPh>
+    <rPh sb="103" eb="104">
+      <t>アト</t>
+    </rPh>
+    <rPh sb="105" eb="107">
+      <t>ヘンコウ</t>
+    </rPh>
+    <rPh sb="120" eb="121">
+      <t>エラ</t>
+    </rPh>
+    <rPh sb="130" eb="131">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="139" eb="140">
+      <t>クワ</t>
+    </rPh>
+    <rPh sb="145" eb="148">
+      <t>ガメンチュウ</t>
+    </rPh>
+    <rPh sb="160" eb="162">
+      <t>サンショウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mymomiji-1stlogin.png</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -6045,7 +6115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392D1BFF-FF5C-4A7E-8C9C-E750AF0FFFAF}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD20"/>
     </sheetView>
   </sheetViews>
@@ -7694,10 +7764,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D6E33FB-2290-439B-854D-9A45A4600EF5}">
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D42" sqref="B40:D42"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -7932,251 +8002,259 @@
         <v>253</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D28" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C28" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
+    <row r="30" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C29" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B33" s="1" t="s">
+    <row r="34" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C33" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="B34" s="1" t="s">
+    <row r="35" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C34" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B35" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C35" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C36" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="C37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B37" s="1"/>
-    </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B38" s="1" t="s">
-        <v>302</v>
-      </c>
+      <c r="B38" s="1"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C39" t="s">
-        <v>4</v>
-      </c>
-      <c r="D39" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="41" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B41" s="1" t="s">
+    <row r="42" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D42" t="s">
         <v>287</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B42" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="D42" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>263</v>
+        <v>233</v>
       </c>
       <c r="D43" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="D44" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B45" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="45" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B45" s="1" t="s">
+    <row r="46" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B46" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="C45" t="s">
-        <v>4</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="C46" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="46" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="B46" s="1" t="s">
+    <row r="47" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B47" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C46" t="s">
-        <v>4</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="C47" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B47" s="1"/>
-    </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B49" s="1" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B49" s="1"/>
-    </row>
-    <row r="50" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B50" s="1" t="s">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B50" s="1"/>
+    </row>
+    <row r="51" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B51" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="C50" t="s">
-        <v>4</v>
-      </c>
-      <c r="D50" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" ht="118.8" x14ac:dyDescent="0.2">
-      <c r="B51" s="2" t="s">
+      <c r="C51" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" ht="118.8" x14ac:dyDescent="0.2">
+      <c r="B52" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C51" t="s">
-        <v>7</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" ht="105.6" x14ac:dyDescent="0.2">
-      <c r="B52" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="C52" t="s">
         <v>7</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" ht="105.6" x14ac:dyDescent="0.2">
+      <c r="B53" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C53" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" ht="92.4" x14ac:dyDescent="0.2">
-      <c r="B53" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D53" t="s" ph="1">
-        <v>39</v>
       </c>
     </row>
     <row r="54" spans="2:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B54" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D54" t="s" ph="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" ht="92.4" x14ac:dyDescent="0.2">
+      <c r="B55" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>7</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D55" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="D55" ph="1"/>
-    </row>
-    <row r="66" spans="4:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="D66" ph="1"/>
-    </row>
-    <row r="68" spans="4:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="D68" ph="1"/>
+    <row r="56" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="D56" ph="1"/>
+    </row>
+    <row r="67" spans="4:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="D67" ph="1"/>
+    </row>
+    <row r="69" spans="4:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="D69" ph="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -8189,7 +8267,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix link win11 ch7
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/kishiba_hiroshima-u_ac_jp/Documents/Documents/fresta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{82F8F6E8-2E19-4DC2-BAA5-9DE285F40007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC89A13B-ECDE-47F6-9972-76AC6F4E3F2C}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{82F8F6E8-2E19-4DC2-BAA5-9DE285F40007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FE0B895-6E8F-4815-AA1D-2DD5E4799964}"/>
   <bookViews>
     <workbookView xWindow="2655" yWindow="-14565" windowWidth="18225" windowHeight="11880" tabRatio="856" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5666,20 +5666,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>&lt;h2&gt;&lt;a name="helpdesk"&gt;&lt;/a&gt;点検届の提出&lt;/h2&gt;</t>
-    <rPh sb="27" eb="30">
-      <t>テンケントドケ</t>
-    </rPh>
-    <rPh sb="31" eb="33">
-      <t>テイシュツ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&lt;h3&gt;&lt;a name="helpdesk"&gt;&lt;/a&gt;問い合わせ&lt;/h3&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">この章では、Wi-Fiで広島大学の学内ネットワークに接続するための設定を行います。以下の手順はアカウントに関連したサービスが全て利用可能になる4/1 以降に実施してください。
 この章まで進めば、この実習の目標である「点検届の提出」ができるはずです！
 &lt;ul&gt;
@@ -5774,6 +5760,20 @@
   </si>
   <si>
     <t>無線LANで学内ネットワークに接続できるように設定しましょう。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2&gt;&lt;a name="checklist"&gt;&lt;/a&gt;点検届の提出&lt;/h2&gt;</t>
+    <rPh sb="28" eb="31">
+      <t>テンケントドケ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>テイシュツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2&gt;&lt;a name="helpdesk"&gt;&lt;/a&gt;問い合わせ&lt;/h2&gt;</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -8613,8 +8613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -8630,7 +8630,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -8638,7 +8638,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -8659,7 +8659,7 @@
     </row>
     <row r="6" spans="1:4" ht="153" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -8746,7 +8746,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -8772,7 +8772,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="165.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix "広大moodle" etc. win11
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/kishiba_hiroshima-u_ac_jp/Documents/Documents/fresta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{82F8F6E8-2E19-4DC2-BAA5-9DE285F40007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FE0B895-6E8F-4815-AA1D-2DD5E4799964}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{82F8F6E8-2E19-4DC2-BAA5-9DE285F40007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBA4B8B8-9ABC-48F8-944B-8FFE245902BF}"/>
   <bookViews>
-    <workbookView xWindow="2655" yWindow="-14565" windowWidth="18225" windowHeight="11880" tabRatio="856" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10275" yWindow="-13845" windowWidth="18225" windowHeight="11880" tabRatio="856" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -4034,27 +4034,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">「Moodle」は、オープンソースで提供されているオンライン学習支援システムです。広島大学ではMoodleを広大IDでログインして利用できるようにしています。
-ここに授業で使う資料が掲載されたり、テストを受けたり、課題を提出したりすることがあります。
-</t>
-    <rPh sb="18" eb="20">
-      <t>テイキョウ</t>
-    </rPh>
-    <rPh sb="30" eb="32">
-      <t>ガクシュウ</t>
-    </rPh>
-    <rPh sb="32" eb="34">
-      <t>シエン</t>
-    </rPh>
-    <rPh sb="54" eb="56">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="65" eb="67">
-      <t>リヨウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>moodle-login.png</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -4572,31 +4551,6 @@
     </rPh>
     <rPh sb="34" eb="36">
       <t>ヒツヨウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>広島大学の学習支援システム群にログインし、多要素認証（MFA）の設定を行いましょう。またその他の</t>
-    <rPh sb="0" eb="4">
-      <t>ヒロシマダイガク</t>
-    </rPh>
-    <rPh sb="5" eb="9">
-      <t>ガクシュウシエン</t>
-    </rPh>
-    <rPh sb="13" eb="14">
-      <t>グン</t>
-    </rPh>
-    <rPh sb="21" eb="26">
-      <t>タヨウソニンショウ</t>
-    </rPh>
-    <rPh sb="32" eb="34">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="35" eb="36">
-      <t>オコナ</t>
-    </rPh>
-    <rPh sb="46" eb="47">
-      <t>ホカ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -5497,31 +5451,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>大学で提供されているオンラインサービスはいくつもありますが、まずオンライン学習支援システムのMoodleにログインしてみましょう。
- &lt;ul&gt;
-&lt;li&gt;&lt;a href="#moodle"&gt;広大moodleにログインする&lt;/a&gt;
-&lt;/li&gt;
-&lt;li&gt;&lt;a href="#mfa"&gt;多要素認証(MFA)の設定&lt;/a&gt;
-&lt;/li&gt;
-&lt;li&gt;&lt;a href="#momiji"&gt;MyMOMIJIにログインする&lt;/a&gt;
-&lt;/li&gt;
-&lt;li&gt;&lt;a href="#bb9"&gt;Bb9にログインする&lt;/a&gt;
-&lt;/li&gt;
-&lt;li&gt;&lt;a href="#office365"&gt;Office365にログインする&lt;/a&gt;
-&lt;/li&gt;
- &lt;/ul&gt;</t>
-    <rPh sb="94" eb="96">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="139" eb="144">
-      <t>タヨウソニンショウ</t>
-    </rPh>
-    <rPh sb="150" eb="152">
-      <t>セッテイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;h2&gt;&lt;a name="moodle"&gt;&lt;/a&gt;広大moodle (オンライン学習支援システム)&lt;/h2&gt; </t>
     <rPh sb="25" eb="27">
       <t>ヒロダイ</t>
@@ -5774,6 +5703,83 @@
   </si>
   <si>
     <t>&lt;h2&gt;&lt;a name="helpdesk"&gt;&lt;/a&gt;問い合わせ&lt;/h2&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>広島大学の学習支援システム群にログインし、多要素認証（MFA）の設定を行いましょう。</t>
+    <rPh sb="0" eb="4">
+      <t>ヒロシマダイガク</t>
+    </rPh>
+    <rPh sb="5" eb="9">
+      <t>ガクシュウシエン</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>グン</t>
+    </rPh>
+    <rPh sb="21" eb="26">
+      <t>タヨウソニンショウ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>オコナ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>大学で提供されているオンラインサービスはいくつもありますが、まずオンライン学習支援システムの広大moodleにログインしてみましょう。
+ &lt;ul&gt;
+&lt;li&gt;&lt;a href="#moodle"&gt;広大moodleにログインする&lt;/a&gt;
+&lt;/li&gt;
+&lt;li&gt;&lt;a href="#mfa"&gt;多要素認証(MFA)の設定&lt;/a&gt;
+&lt;/li&gt;
+&lt;li&gt;&lt;a href="#momiji"&gt;MyMOMIJIにログインする&lt;/a&gt;
+&lt;/li&gt;
+&lt;li&gt;&lt;a href="#bb9"&gt;Bb9にログインする&lt;/a&gt;
+&lt;/li&gt;
+&lt;li&gt;&lt;a href="#office365"&gt;Office365にログインする&lt;/a&gt;
+&lt;/li&gt;
+ &lt;/ul&gt;</t>
+    <rPh sb="46" eb="48">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="96" eb="98">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="141" eb="146">
+      <t>タヨウソニンショウ</t>
+    </rPh>
+    <rPh sb="152" eb="154">
+      <t>セッテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">「Moodle」は、オープンソースで提供されているオンライン学習支援システムです。広島大学ではMoodleを広大IDでログインして利用できるようにしており、これを「広大moodle」と呼んでいます。
+ここに授業で使う資料が掲載されたり、テストを受けたり、課題を提出したりすることがあります。
+</t>
+    <rPh sb="18" eb="20">
+      <t>テイキョウ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>ガクシュウ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>シエン</t>
+    </rPh>
+    <rPh sb="54" eb="56">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="65" eb="67">
+      <t>リヨウ</t>
+    </rPh>
+    <rPh sb="82" eb="84">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="92" eb="93">
+      <t>ヨ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -6206,7 +6212,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6244,7 +6250,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6281,7 +6287,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6289,7 +6295,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6305,22 +6311,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6360,10 +6366,10 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D16" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -6374,12 +6380,12 @@
         <v>223</v>
       </c>
       <c r="D17" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6387,7 +6393,7 @@
         <v>224</v>
       </c>
       <c r="D19" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -6395,7 +6401,7 @@
         <v>225</v>
       </c>
       <c r="D20" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6403,7 +6409,7 @@
         <v>226</v>
       </c>
       <c r="D21" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6414,7 +6420,7 @@
         <v>229</v>
       </c>
       <c r="D22" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -6422,7 +6428,7 @@
         <v>227</v>
       </c>
       <c r="D23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6430,12 +6436,12 @@
         <v>228</v>
       </c>
       <c r="D24" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -6454,7 +6460,7 @@
         <v>236</v>
       </c>
       <c r="D30" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -6462,7 +6468,7 @@
         <v>238</v>
       </c>
       <c r="D31" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -6470,7 +6476,7 @@
         <v>237</v>
       </c>
       <c r="D32" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
@@ -6481,7 +6487,7 @@
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
@@ -6680,7 +6686,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="304.25" customHeight="1" ph="1" x14ac:dyDescent="0.25">
@@ -6688,7 +6694,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -6752,7 +6758,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>7</v>
@@ -6777,7 +6783,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>7</v>
@@ -7102,7 +7108,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="2" spans="1:4" customFormat="1" ht="19.149999999999999" ph="1" x14ac:dyDescent="0.25">
@@ -7110,7 +7116,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="1:4" customFormat="1" ht="19.149999999999999" ph="1" x14ac:dyDescent="0.25">
@@ -7126,7 +7132,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:4" customFormat="1" ht="19.149999999999999" ph="1" x14ac:dyDescent="0.25">
@@ -7134,36 +7140,36 @@
     </row>
     <row r="6" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D7" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D8" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D9" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -7171,13 +7177,13 @@
     </row>
     <row r="12" spans="1:4" ht="19.149999999999999" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="19.149999999999999" x14ac:dyDescent="0.25">
@@ -7408,7 +7414,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -7455,10 +7461,10 @@
     </row>
     <row r="11" spans="1:5" customFormat="1" ht="19.149999999999999" ph="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="127.5" x14ac:dyDescent="0.25">
@@ -7612,7 +7618,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -7626,7 +7632,7 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -7662,7 +7668,7 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -7670,7 +7676,7 @@
         <v>191</v>
       </c>
       <c r="D17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -7684,7 +7690,7 @@
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7698,7 +7704,7 @@
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -7712,7 +7718,7 @@
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -7791,7 +7797,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -7799,7 +7805,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7852,7 +7858,7 @@
     </row>
     <row r="14" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D14" t="s">
         <v>214</v>
@@ -7863,7 +7869,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -7928,8 +7934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D6E33FB-2290-439B-854D-9A45A4600EF5}">
   <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -7945,7 +7951,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>293</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7953,7 +7959,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7969,7 +7975,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -7980,7 +7986,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>332</v>
+        <v>343</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7994,7 +8000,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -8005,7 +8011,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>240</v>
+        <v>344</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -8013,10 +8019,10 @@
     </row>
     <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D11" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -8024,13 +8030,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
         <v>242</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="191.25" x14ac:dyDescent="0.25">
@@ -8038,18 +8044,18 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>244</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -8060,7 +8066,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -8071,7 +8077,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -8082,7 +8088,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -8120,13 +8126,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -8147,29 +8153,29 @@
     </row>
     <row r="26" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D27" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D28" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -8256,7 +8262,7 @@
     </row>
     <row r="37" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
@@ -8270,7 +8276,7 @@
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
@@ -8286,10 +8292,10 @@
     </row>
     <row r="41" spans="2:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D41" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -8297,12 +8303,12 @@
         <v>223</v>
       </c>
       <c r="D42" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -8310,34 +8316,34 @@
         <v>224</v>
       </c>
       <c r="D44" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="45" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D45" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="46" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D46" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C47" t="s">
         <v>4</v>
       </c>
       <c r="D47" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="48" spans="2:4" ht="51" x14ac:dyDescent="0.25">
@@ -8348,7 +8354,7 @@
         <v>4</v>
       </c>
       <c r="D48" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
@@ -8356,7 +8362,7 @@
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
@@ -8364,7 +8370,7 @@
     </row>
     <row r="52" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C52" t="s">
         <v>4</v>
@@ -8475,7 +8481,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -8507,7 +8513,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -8532,7 +8538,7 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -8540,7 +8546,7 @@
         <v>234</v>
       </c>
       <c r="D15" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -8554,7 +8560,7 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -8568,7 +8574,7 @@
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
@@ -8582,7 +8588,7 @@
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -8613,7 +8619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -8630,7 +8636,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -8638,7 +8644,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -8659,12 +8665,12 @@
     </row>
     <row r="6" spans="1:4" ht="153" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -8711,7 +8717,7 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -8725,7 +8731,7 @@
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -8733,7 +8739,7 @@
         <v>181</v>
       </c>
       <c r="D13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -8746,7 +8752,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -8754,30 +8760,30 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="165.75" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
win11: chapter 0 - not eduroam but HU-CUP.
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D79960-8E8C-4D80-9219-177B5628728B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11EB3FE4-7BFA-4164-B584-17ABC391F869}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -4424,85 +4424,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Windows11Homeは、ネット環境が無いとここから進めることができません(Windows11Proも皆さんが買った時期によっては同じかもしれません)。一度ネット環境に接続してください。接続するとWindowsの更新データをネットからダウンロードしますので、遅いネット環境である場合や、通信データ量に応じて課金されるネット環境しか無い場合は、大学のネット環境を使ってください。ネット環境に接続されると、「次へ」のボタンが押せるようになるので、押しましょう。</t>
-    <rPh sb="18" eb="20">
-      <t>カンキョウ</t>
-    </rPh>
-    <rPh sb="21" eb="22">
-      <t>ナ</t>
-    </rPh>
-    <rPh sb="28" eb="29">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="53" eb="54">
-      <t>ミナ</t>
-    </rPh>
-    <rPh sb="57" eb="58">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="60" eb="62">
-      <t>ジキ</t>
-    </rPh>
-    <rPh sb="67" eb="68">
-      <t>オナ</t>
-    </rPh>
-    <rPh sb="78" eb="80">
-      <t>イチド</t>
-    </rPh>
-    <rPh sb="83" eb="85">
-      <t>カンキョウ</t>
-    </rPh>
-    <rPh sb="86" eb="88">
-      <t>セツゾク</t>
-    </rPh>
-    <rPh sb="95" eb="97">
-      <t>セツゾク</t>
-    </rPh>
-    <rPh sb="108" eb="110">
-      <t>コウシン</t>
-    </rPh>
-    <rPh sb="131" eb="132">
-      <t>オソ</t>
-    </rPh>
-    <rPh sb="136" eb="138">
-      <t>カンキョウ</t>
-    </rPh>
-    <rPh sb="141" eb="143">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="145" eb="147">
-      <t>ツウシン</t>
-    </rPh>
-    <rPh sb="150" eb="151">
-      <t>リョウ</t>
-    </rPh>
-    <rPh sb="152" eb="153">
-      <t>オウ</t>
-    </rPh>
-    <rPh sb="155" eb="157">
-      <t>カキン</t>
-    </rPh>
-    <rPh sb="163" eb="165">
-      <t>カンキョウ</t>
-    </rPh>
-    <rPh sb="167" eb="168">
-      <t>ナ</t>
-    </rPh>
-    <rPh sb="169" eb="171">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="173" eb="175">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="179" eb="181">
-      <t>カンキョウ</t>
-    </rPh>
-    <rPh sb="182" eb="183">
-      <t>ツカ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">必携PC初期実習では、みなさんのパソコンを広島大学のキャンパスで使用するための準備をおこないます。ここでおこなうことを以下にあげます。おおむね６０分程度かかると思います。頑張ってください。
   </t>
     <rPh sb="4" eb="6">
@@ -5961,55 +5882,6 @@
   </si>
   <si>
     <t>FRESTA-TEXT-2023 Win11 chap.8</t>
-  </si>
-  <si>
-    <t>HU-CUPの基地局を選び、接続ボタンを押すと、認証が求められます。IMCアカウントとパスワードを入力し、OKボタンで進めます。初めて接続する基地局では本当に接続するか再確認を求められます。</t>
-    <rPh sb="7" eb="10">
-      <t>キチキョク</t>
-    </rPh>
-    <rPh sb="11" eb="12">
-      <t>エラ</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>セツゾク</t>
-    </rPh>
-    <rPh sb="20" eb="21">
-      <t>オ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>ニンショウ</t>
-    </rPh>
-    <rPh sb="27" eb="28">
-      <t>モト</t>
-    </rPh>
-    <rPh sb="49" eb="51">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="59" eb="60">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="64" eb="65">
-      <t>ハジ</t>
-    </rPh>
-    <rPh sb="67" eb="69">
-      <t>セツゾク</t>
-    </rPh>
-    <rPh sb="71" eb="74">
-      <t>キチキョク</t>
-    </rPh>
-    <rPh sb="76" eb="78">
-      <t>ホントウ</t>
-    </rPh>
-    <rPh sb="79" eb="81">
-      <t>セツゾク</t>
-    </rPh>
-    <rPh sb="84" eb="87">
-      <t>サイカクニン</t>
-    </rPh>
-    <rPh sb="88" eb="89">
-      <t>モト</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t xml:space="preserve">広島大学では、図書館、講義室、福利施設など学内の多くの共用スペースで、「HiNET Wi-Fi」が利用できます。ここでは、HiNET Wi-Fiを通して、あなたのPCで学内ネットワークとインターネットを利用できるようにする方法を説明します。一度設定すると、次回からは（同じ基地局に対しては）設定不要です。 </t>
@@ -6735,6 +6607,153 @@
     </rPh>
     <rPh sb="63" eb="64">
       <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;a id="choose_wifi_api"&gt;&lt;/a&gt;HU-CUPの基地局を選び、接続ボタンを押すと、認証が求められます。IMCアカウントとパスワードを入力し、OKボタンで進めます。初めて接続する基地局では本当に接続するか再確認を求められます。</t>
+    <rPh sb="35" eb="38">
+      <t>キチキョク</t>
+    </rPh>
+    <rPh sb="39" eb="40">
+      <t>エラ</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="48" eb="49">
+      <t>オ</t>
+    </rPh>
+    <rPh sb="52" eb="54">
+      <t>ニンショウ</t>
+    </rPh>
+    <rPh sb="55" eb="56">
+      <t>モト</t>
+    </rPh>
+    <rPh sb="77" eb="79">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="87" eb="88">
+      <t>スス</t>
+    </rPh>
+    <rPh sb="92" eb="93">
+      <t>ハジ</t>
+    </rPh>
+    <rPh sb="95" eb="97">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="99" eb="102">
+      <t>キチキョク</t>
+    </rPh>
+    <rPh sb="104" eb="106">
+      <t>ホントウ</t>
+    </rPh>
+    <rPh sb="107" eb="109">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="112" eb="115">
+      <t>サイカクニン</t>
+    </rPh>
+    <rPh sb="116" eb="117">
+      <t>モト</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Windows11Homeは、ネット環境が無いとここから進めることができません(Windows11Proも皆さんが買った時期によっては同じかもしれません)。一度ネット環境に接続してください。このスクリーンショットは大学のネット環境のHU-CUPに接続していますが、自宅のネット環境でも問題ありません。ネット環境に接続されると、「次へ」のボタンが押せるようになるので、押しましょう。
+どうしても自宅にネット環境が無いという人は大学に来て&lt;a href="../ch7.html"&gt;HU-CUPへの接続手順&lt;/a&gt;を参考にして接続しましょう(基地局リストを出すところまでの手順が済んでいる状態です)。</t>
+    <rPh sb="18" eb="20">
+      <t>カンキョウ</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>ナ</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>スス</t>
+    </rPh>
+    <rPh sb="53" eb="54">
+      <t>ミナ</t>
+    </rPh>
+    <rPh sb="57" eb="58">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="60" eb="62">
+      <t>ジキ</t>
+    </rPh>
+    <rPh sb="67" eb="68">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="78" eb="80">
+      <t>イチド</t>
+    </rPh>
+    <rPh sb="83" eb="85">
+      <t>カンキョウ</t>
+    </rPh>
+    <rPh sb="86" eb="88">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="107" eb="109">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="113" eb="115">
+      <t>カンキョウ</t>
+    </rPh>
+    <rPh sb="123" eb="125">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="132" eb="134">
+      <t>ジタク</t>
+    </rPh>
+    <rPh sb="138" eb="140">
+      <t>カンキョウ</t>
+    </rPh>
+    <rPh sb="142" eb="144">
+      <t>モンダイ</t>
+    </rPh>
+    <rPh sb="196" eb="198">
+      <t>ジタク</t>
+    </rPh>
+    <rPh sb="202" eb="204">
+      <t>カンキョウ</t>
+    </rPh>
+    <rPh sb="205" eb="206">
+      <t>ナ</t>
+    </rPh>
+    <rPh sb="210" eb="211">
+      <t>ヒト</t>
+    </rPh>
+    <rPh sb="212" eb="214">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="215" eb="216">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="247" eb="249">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="249" eb="251">
+      <t>テジュン</t>
+    </rPh>
+    <rPh sb="256" eb="258">
+      <t>サンコウ</t>
+    </rPh>
+    <rPh sb="261" eb="263">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="269" eb="272">
+      <t>キチキョク</t>
+    </rPh>
+    <rPh sb="276" eb="277">
+      <t>ダ</t>
+    </rPh>
+    <rPh sb="284" eb="286">
+      <t>テジュン</t>
+    </rPh>
+    <rPh sb="287" eb="288">
+      <t>ス</t>
+    </rPh>
+    <rPh sb="292" eb="294">
+      <t>ジョウタイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -7174,7 +7193,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7190,7 +7209,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7198,7 +7217,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -7212,7 +7231,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7273,7 +7292,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -7320,7 +7339,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.2">
@@ -7360,7 +7379,7 @@
     </row>
     <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>232</v>
@@ -7368,7 +7387,7 @@
     </row>
     <row r="21" spans="1:4" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>233</v>
@@ -7395,7 +7414,7 @@
     </row>
     <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D24" t="s">
         <v>236</v>
@@ -7606,8 +7625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.2"/>
@@ -7648,7 +7667,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="304.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -7715,12 +7734,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="118.8" ph="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>268</v>
+        <v>384</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>7</v>
@@ -7784,10 +7803,10 @@
     </row>
     <row r="16" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
@@ -7883,10 +7902,10 @@
     </row>
     <row r="25" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
@@ -7935,18 +7954,18 @@
     </row>
     <row r="30" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D30" t="s" ph="1">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D31" t="s" ph="1">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="66" ph="1" x14ac:dyDescent="0.2">
@@ -8126,7 +8145,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="5" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -8163,7 +8182,7 @@
     </row>
     <row r="10" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -8182,13 +8201,13 @@
     </row>
     <row r="13" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -8408,7 +8427,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
@@ -8447,7 +8466,7 @@
     </row>
     <row r="10" spans="1:5" customFormat="1" ht="79.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D10" t="s" ph="1">
         <v>106</v>
@@ -8538,7 +8557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -8555,7 +8574,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8563,7 +8582,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8579,7 +8598,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -8587,7 +8606,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8620,7 +8639,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -8692,7 +8711,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -8706,7 +8725,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -8725,140 +8744,140 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="82.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="49.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D25" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D26" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D27" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D28" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D29" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D31" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="46.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D32" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="131.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D33" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="25.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D38" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="D40" t="s">
         <v>323</v>
-      </c>
-      <c r="D40" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B41" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D41" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="D42" t="s">
         <v>327</v>
-      </c>
-      <c r="D42" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B43" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="D43" t="s">
         <v>329</v>
-      </c>
-      <c r="D43" t="s">
-        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -8913,7 +8932,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9067,7 +9086,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -9075,7 +9094,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9091,7 +9110,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -9102,7 +9121,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -9121,7 +9140,7 @@
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -9134,7 +9153,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -9145,7 +9164,7 @@
     </row>
     <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -9156,7 +9175,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9164,7 +9183,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -9172,15 +9191,15 @@
     </row>
     <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D15" t="s">
         <v>285</v>
-      </c>
-      <c r="D15" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D16" t="s">
         <v>201</v>
@@ -9205,13 +9224,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -9224,21 +9243,21 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
         <v>289</v>
-      </c>
-      <c r="C20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D21" t="s">
         <v>291</v>
-      </c>
-      <c r="D21" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9246,21 +9265,21 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D23" t="s">
         <v>294</v>
-      </c>
-      <c r="D23" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9268,13 +9287,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -9282,7 +9301,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -9298,7 +9317,7 @@
     </row>
     <row r="28" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -9309,7 +9328,7 @@
     </row>
     <row r="29" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D29" t="s">
         <v>203</v>
@@ -9325,13 +9344,13 @@
     </row>
     <row r="31" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -9339,7 +9358,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -9358,13 +9377,13 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
         <v>300</v>
-      </c>
-      <c r="C35" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9406,7 +9425,7 @@
     </row>
     <row r="41" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D41" t="s">
         <v>228</v>
@@ -9488,7 +9507,7 @@
     </row>
     <row r="51" spans="2:4" ht="132" x14ac:dyDescent="0.2">
       <c r="B51" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C51" t="s">
         <v>7</v>
@@ -9579,7 +9598,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -9680,7 +9699,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -9717,8 +9736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="B7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B7" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -9734,7 +9753,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -9742,7 +9761,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9758,17 +9777,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -9781,7 +9800,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -9806,7 +9825,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -9820,7 +9839,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>359</v>
+        <v>383</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -9847,7 +9866,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9855,12 +9874,12 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D18" t="s">
         <v>201</v>
@@ -9868,20 +9887,20 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D19" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ch0: password should be different from the passwords of the services provided by Hiroshima University.
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3186B84-F494-4C99-8160-388DC2BFEAF6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534F454B-C8BE-4083-9C61-E7E7781E4D32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1647,19 +1647,6 @@
   </si>
   <si>
     <t>win11ja-msaccount-mail-passwd.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>今作ったメールアドレスのパスワードを設定します。</t>
-    <rPh sb="0" eb="1">
-      <t>イマ</t>
-    </rPh>
-    <rPh sb="1" eb="2">
-      <t>ツク</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>セッテイ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -6754,6 +6741,34 @@
     </rPh>
     <rPh sb="289" eb="291">
       <t>ジョウタイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>今作ったメールアドレスのパスワードを設定します。大学から提供されるアカウント類と同じパスワードにしないように注意してください。</t>
+    <rPh sb="0" eb="1">
+      <t>イマ</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>ツク</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>テイキョウ</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>ルイ</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="54" eb="56">
+      <t>チュウイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -7193,7 +7208,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7209,7 +7224,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7217,7 +7232,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -7231,7 +7246,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7268,7 +7283,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7276,7 +7291,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7292,22 +7307,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7339,7 +7354,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.2">
@@ -7347,10 +7362,10 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7358,39 +7373,39 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7398,31 +7413,31 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D23" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D24" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7438,37 +7453,37 @@
     </row>
     <row r="30" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D30" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D31" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D32" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
@@ -7625,8 +7640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.2"/>
@@ -7643,7 +7658,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -7651,7 +7666,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -7667,7 +7682,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="304.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -7675,7 +7690,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -7689,7 +7704,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C7" t="s" ph="1">
         <v>7</v>
@@ -7703,7 +7718,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>7</v>
@@ -7714,7 +7729,7 @@
     </row>
     <row r="9" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D9" t="s" ph="1">
         <v>64</v>
@@ -7739,7 +7754,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>7</v>
@@ -7764,7 +7779,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>7</v>
@@ -7803,10 +7818,10 @@
     </row>
     <row r="16" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="D16" t="s" ph="1">
         <v>370</v>
-      </c>
-      <c r="D16" t="s" ph="1">
-        <v>371</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
@@ -7836,7 +7851,7 @@
     </row>
     <row r="19" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>7</v>
@@ -7856,9 +7871,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ph="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
-        <v>82</v>
+        <v>384</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>7</v>
@@ -7869,136 +7884,136 @@
     </row>
     <row r="22" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C26" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D26" t="s" ph="1">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C27" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D27" t="s" ph="1">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C28" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D28" t="s" ph="1">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C29" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D29" t="s" ph="1">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D30" t="s" ph="1">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D31" t="s" ph="1">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C32" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D32" t="s" ph="1">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C33" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D33" t="s" ph="1">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="2:5" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C34" t="s" ph="1">
+        <v>101</v>
+      </c>
+      <c r="D34" t="s" ph="1">
         <v>102</v>
-      </c>
-      <c r="D34" t="s" ph="1">
-        <v>103</v>
       </c>
     </row>
     <row r="35" spans="2:5" ph="1" x14ac:dyDescent="0.2">
@@ -8121,7 +8136,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -8129,7 +8144,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -8145,7 +8160,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -8153,36 +8168,36 @@
     </row>
     <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="D8" t="s">
         <v>250</v>
-      </c>
-      <c r="D8" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -8190,178 +8205,178 @@
     </row>
     <row r="12" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C14" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C15" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C16" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B18" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C19" t="s" ph="1">
         <v>132</v>
       </c>
-      <c r="C19" t="s" ph="1">
+      <c r="D19" t="s" ph="1">
         <v>133</v>
-      </c>
-      <c r="D19" t="s" ph="1">
-        <v>134</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C25" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C26" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D26" t="s" ph="1">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C27" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D27" t="s" ph="1">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -8411,7 +8426,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -8427,57 +8442,57 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C7" t="s" ph="1">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E7" ph="1"/>
     </row>
     <row r="8" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" t="s" ph="1">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:5" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C9" t="s" ph="1">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:5" customFormat="1" ht="79.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:5" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="132" x14ac:dyDescent="0.2">
@@ -8485,7 +8500,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -8499,37 +8514,37 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>143</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8537,13 +8552,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -8574,7 +8589,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8582,7 +8597,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8598,7 +8613,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -8606,7 +8621,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8625,13 +8640,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -8639,13 +8654,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -8653,7 +8668,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -8664,7 +8679,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -8675,21 +8690,21 @@
         <v>4</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -8697,13 +8712,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8711,13 +8726,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8725,13 +8740,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -8744,140 +8759,140 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="82.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="49.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D25" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D27" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D28" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="D29" t="s">
         <v>377</v>
-      </c>
-      <c r="D29" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D30" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D31" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="46.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D32" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="131.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D33" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="25.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D38" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="D40" t="s">
         <v>322</v>
-      </c>
-      <c r="D40" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B41" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D41" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="D42" t="s">
         <v>326</v>
-      </c>
-      <c r="D42" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B43" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="D43" t="s">
         <v>328</v>
-      </c>
-      <c r="D43" t="s">
-        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -8916,7 +8931,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8932,7 +8947,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8940,7 +8955,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8961,42 +8976,42 @@
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9004,7 +9019,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9012,50 +9027,50 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D21" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -9086,7 +9101,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -9094,7 +9109,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9110,7 +9125,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -9121,7 +9136,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -9140,7 +9155,7 @@
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -9153,7 +9168,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -9164,18 +9179,18 @@
     </row>
     <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9183,7 +9198,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -9191,18 +9206,18 @@
     </row>
     <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D15" t="s">
         <v>284</v>
-      </c>
-      <c r="D15" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -9210,13 +9225,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
         <v>202</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="198" x14ac:dyDescent="0.2">
@@ -9224,18 +9239,18 @@
         <v>4</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9243,21 +9258,21 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
         <v>288</v>
-      </c>
-      <c r="C20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D21" t="s">
         <v>290</v>
-      </c>
-      <c r="D21" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9265,21 +9280,21 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D23" t="s">
         <v>293</v>
-      </c>
-      <c r="D23" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9287,13 +9302,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -9301,7 +9316,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -9317,40 +9332,40 @@
     </row>
     <row r="28" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D30" t="s">
         <v>263</v>
-      </c>
-      <c r="D30" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -9358,7 +9373,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -9377,69 +9392,69 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
         <v>299</v>
-      </c>
-      <c r="C35" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D36" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D37" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D39" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D40" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D41" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C42" t="s">
         <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9450,7 +9465,7 @@
         <v>4</v>
       </c>
       <c r="D43" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -9458,7 +9473,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -9466,7 +9481,7 @@
     </row>
     <row r="47" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C47" t="s">
         <v>4</v>
@@ -9507,7 +9522,7 @@
     </row>
     <row r="51" spans="2:4" ht="132" x14ac:dyDescent="0.2">
       <c r="B51" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C51" t="s">
         <v>7</v>
@@ -9582,7 +9597,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9598,7 +9613,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -9606,7 +9621,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -9630,7 +9645,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -9649,21 +9664,21 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -9671,13 +9686,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9685,13 +9700,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -9699,13 +9714,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -9753,7 +9768,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -9761,7 +9776,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9777,17 +9792,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -9800,7 +9815,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -9825,13 +9840,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9839,21 +9854,21 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -9861,12 +9876,12 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9874,33 +9889,33 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D19" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
win11ja: use new images to check storage size
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\fresta2024\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F1955F-3DDA-4D19-9BAE-E23C17CCA45E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09374112-A1BA-4143-8F56-69E9728311EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="395">
   <si>
     <t>header1</t>
   </si>
@@ -3612,23 +3612,6 @@
   </si>
   <si>
     <t>学外からのアクセスのときは、ここで多要素認証（MFA）の認証手続きが入る場合があります。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11ja-check-storage-size.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>さらに内蔵ストレージ(HDDやSSDなど)の容量も調べます。</t>
-    <rPh sb="3" eb="5">
-      <t>ナイゾウ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>ヨウリョウ</t>
-    </rPh>
-    <rPh sb="25" eb="26">
-      <t>シラ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -4714,45 +4697,6 @@
     </rPh>
     <rPh sb="134" eb="135">
       <t>ヨ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>バージョン情報が表示されます。「デバイスの仕様」に、パソコンのプロセッサ(CPU)やRAMの情報、またオペレーティングシステムの分類が書かれています。「Windowsの仕様」に貴方が使っているWindowsの細かいバージョンが書かれています。
-&lt;span class="check"&gt;check 1&lt;/span&gt;
-&lt;span class="check"&gt;check 2&lt;/span&gt;</t>
-    <rPh sb="5" eb="7">
-      <t>ジョウホウ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>シヨウ</t>
-    </rPh>
-    <rPh sb="46" eb="48">
-      <t>ジョウホウ</t>
-    </rPh>
-    <rPh sb="64" eb="66">
-      <t>ブンルイ</t>
-    </rPh>
-    <rPh sb="67" eb="68">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="84" eb="86">
-      <t>シヨウ</t>
-    </rPh>
-    <rPh sb="88" eb="90">
-      <t>アナタ</t>
-    </rPh>
-    <rPh sb="91" eb="92">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="104" eb="105">
-      <t>コマ</t>
-    </rPh>
-    <rPh sb="113" eb="114">
-      <t>カ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -7090,6 +7034,102 @@
   </si>
   <si>
     <t>win11ja-onedrive-unlink-warning.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>バージョン情報が表示されます。「デバイスの仕様」に、パソコンのプロセッサ(CPU)やRAMの情報、またオペレーティングシステムの分類が書かれています。「Windowsの仕様」に貴方が使っているWindowsの細かいバージョンが書かれています。
+&lt;span class="check"&gt;check 1&lt;/span&gt;
+&lt;span class="check"&gt;check 2&lt;/span&gt;
+終わったら「システム」に戻ります。</t>
+    <rPh sb="5" eb="7">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="64" eb="66">
+      <t>ブンルイ</t>
+    </rPh>
+    <rPh sb="67" eb="68">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="84" eb="86">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="88" eb="90">
+      <t>アナタ</t>
+    </rPh>
+    <rPh sb="91" eb="92">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="104" eb="105">
+      <t>コマ</t>
+    </rPh>
+    <rPh sb="113" eb="114">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="192" eb="193">
+      <t>オ</t>
+    </rPh>
+    <rPh sb="204" eb="205">
+      <t>モド</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>さらに内蔵ストレージ(HDDやSSDなど)の容量も調べます。
+「システム」(①)、のメニューから「ストレージ」(②)を選び展開します。</t>
+    <rPh sb="3" eb="5">
+      <t>ナイゾウ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>ヨウリョウ</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>シラ</t>
+    </rPh>
+    <rPh sb="59" eb="60">
+      <t>エラ</t>
+    </rPh>
+    <rPh sb="61" eb="63">
+      <t>テンカイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-setting-storage-menu.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-setting-storage-detail.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Windowsがインストールされているストレージの総容量、使用量、空き容量が示されます。</t>
+    <rPh sb="25" eb="26">
+      <t>ソウ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>ヨウリョウ</t>
+    </rPh>
+    <rPh sb="29" eb="32">
+      <t>シヨウリョウ</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>ヨウリョウ</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>シメ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -7531,7 +7571,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7547,7 +7587,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7555,7 +7595,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -7569,7 +7609,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7630,7 +7670,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -7677,7 +7717,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.2">
@@ -7717,7 +7757,7 @@
     </row>
     <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>195</v>
@@ -7725,7 +7765,7 @@
     </row>
     <row r="21" spans="1:4" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>196</v>
@@ -7752,7 +7792,7 @@
     </row>
     <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D24" t="s">
         <v>199</v>
@@ -7963,8 +8003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView topLeftCell="A16" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.2"/>
@@ -8005,7 +8045,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="304.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -8013,7 +8053,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -8077,7 +8117,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>7</v>
@@ -8141,10 +8181,10 @@
     </row>
     <row r="16" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
@@ -8196,7 +8236,7 @@
     </row>
     <row r="21" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>7</v>
@@ -8240,51 +8280,51 @@
     </row>
     <row r="25" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C25" t="s" ph="1">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="26" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C26" t="s" ph="1">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D26" t="s" ph="1">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C27" t="s" ph="1">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D27" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C28" t="s" ph="1">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D28" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C29" t="s" ph="1">
         <v>7</v>
@@ -8295,13 +8335,13 @@
     </row>
     <row r="30" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C30" t="s" ph="1">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D30" t="s" ph="1">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
@@ -8339,34 +8379,34 @@
     </row>
     <row r="34" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D34" t="s" ph="1">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C35" t="s" ph="1">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D35" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D36" t="s" ph="1">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="37" spans="2:5" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C37" t="s" ph="1">
         <v>7</v>
@@ -8498,10 +8538,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8541,7 +8581,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
@@ -8578,234 +8618,242 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:5" customFormat="1" ht="79.2" ph="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" customFormat="1" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>291</v>
+        <v>390</v>
       </c>
       <c r="D10" t="s" ph="1">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:5" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>220</v>
+        <v>391</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>219</v>
+        <v>392</v>
       </c>
     </row>
     <row r="12" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="D12" t="s" ph="1">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="D13" t="s" ph="1">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="6" t="s">
         <v>370</v>
       </c>
-      <c r="D12" t="s" ph="1">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="6" t="s">
-        <v>373</v>
-      </c>
-      <c r="D13" t="s" ph="1">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" customFormat="1" ht="66" ph="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="6" t="s">
-        <v>384</v>
-      </c>
       <c r="D14" t="s" ph="1">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" customFormat="1" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>343</v>
+        <v>381</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>359</v>
-      </c>
-      <c r="D16" t="s">
-        <v>385</v>
+        <v>340</v>
+      </c>
+      <c r="D16" t="s" ph="1">
+        <v>346</v>
       </c>
     </row>
     <row r="17" spans="1:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="D17" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="D18" t="s" ph="1">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="6" t="s">
+        <v>385</v>
+      </c>
+      <c r="D19" t="s" ph="1">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="6" t="s">
         <v>387</v>
       </c>
-      <c r="D17" t="s" ph="1">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="6" t="s">
+      <c r="D20" t="s" ph="1">
         <v>388</v>
       </c>
-      <c r="D18" t="s" ph="1">
+    </row>
+    <row r="21" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="D21" t="s" ph="1">
         <v>389</v>
       </c>
     </row>
-    <row r="19" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="6" t="s">
-        <v>390</v>
-      </c>
-      <c r="D19" t="s" ph="1">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="D20" t="s" ph="1">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="D21" t="s" ph="1">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+        <v>342</v>
+      </c>
+      <c r="D22" t="s" ph="1">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="8" t="s">
-        <v>342</v>
-      </c>
-      <c r="C24" s="3" ph="1"/>
-      <c r="D24" s="3" t="s" ph="1">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="8" t="s">
-        <v>357</v>
+        <v>339</v>
       </c>
       <c r="C25" s="3" ph="1"/>
       <c r="D25" s="3" t="s" ph="1">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="2" t="s">
-        <v>358</v>
+        <v>347</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="8" t="s">
+        <v>354</v>
       </c>
       <c r="C26" s="3" ph="1"/>
       <c r="D26" s="3" t="s" ph="1">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
-        <v>344</v>
+        <v>355</v>
       </c>
       <c r="C27" s="3" ph="1"/>
       <c r="D27" s="3" t="s" ph="1">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
       <c r="C28" s="3" ph="1"/>
       <c r="D28" s="3" t="s" ph="1">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="132" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="C29" s="3" ph="1"/>
+      <c r="D29" s="3" t="s" ph="1">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="132" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>348</v>
-      </c>
-      <c r="C29" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>4</v>
-      </c>
       <c r="B30" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="C30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B31" s="6" t="s">
+    <row r="32" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B32" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D32" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B32" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D32" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B34" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D34" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" s="6" t="s">
+    <row r="35" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C34" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="6"/>
     </row>
     <row r="36" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6"/>
     </row>
-    <row r="39" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="6"/>
+    <row r="37" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="6"/>
     </row>
     <row r="40" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B40" s="6"/>
+    </row>
+    <row r="41" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -8835,7 +8883,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8843,7 +8891,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8859,7 +8907,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -8867,7 +8915,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8900,7 +8948,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -8972,7 +9020,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -8986,7 +9034,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -9005,124 +9053,124 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="82.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="82.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D25" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="55.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D26" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D27" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D28" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D29" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D30" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="50.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D32" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D33" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D34" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D35" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="46.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D36" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="131.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="6" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D41" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9162,7 +9210,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -9178,7 +9226,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="5" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -9186,32 +9234,32 @@
     </row>
     <row r="6" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -9220,14 +9268,14 @@
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C13" ph="1"/>
       <c r="D13" ph="1"/>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C14" ph="1"/>
       <c r="D14" ph="1"/>
@@ -9239,13 +9287,13 @@
     </row>
     <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C16" ph="1"/>
     </row>
     <row r="17" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C17" ph="1"/>
       <c r="D17" ph="1"/>
@@ -9395,7 +9443,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9549,7 +9597,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -9557,7 +9605,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9573,7 +9621,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -9584,7 +9632,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -9603,7 +9651,7 @@
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -9616,7 +9664,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -9627,7 +9675,7 @@
     </row>
     <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -9638,7 +9686,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9646,7 +9694,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -9654,15 +9702,15 @@
     </row>
     <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D15" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D16" t="s">
         <v>164</v>
@@ -9687,13 +9735,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -9706,21 +9754,21 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D21" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9728,21 +9776,21 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D23" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9750,13 +9798,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -9764,7 +9812,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -9780,7 +9828,7 @@
     </row>
     <row r="28" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -9791,7 +9839,7 @@
     </row>
     <row r="29" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D29" t="s">
         <v>166</v>
@@ -9807,13 +9855,13 @@
     </row>
     <row r="31" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -9821,7 +9869,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -9840,13 +9888,13 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9888,7 +9936,7 @@
     </row>
     <row r="41" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D41" t="s">
         <v>191</v>
@@ -9907,7 +9955,7 @@
     </row>
     <row r="43" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C43" t="s">
         <v>4</v>
@@ -9940,7 +9988,7 @@
     </row>
     <row r="48" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C48" t="s">
         <v>7</v>
@@ -9968,7 +10016,7 @@
     </row>
     <row r="51" spans="2:4" ht="132" x14ac:dyDescent="0.2">
       <c r="B51" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C51" t="s">
         <v>7</v>
@@ -10059,7 +10107,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -10067,7 +10115,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -10097,7 +10145,7 @@
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -10160,7 +10208,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -10214,7 +10262,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -10222,7 +10270,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -10238,17 +10286,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -10261,7 +10309,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -10286,7 +10334,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -10300,7 +10348,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -10327,7 +10375,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -10335,12 +10383,12 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D18" t="s">
         <v>164</v>
@@ -10348,20 +10396,20 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D19" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
win11ja: update onedrive handling
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\fresta2024\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09374112-A1BA-4143-8F56-69E9728311EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AB34C7-DB83-4575-AA28-4F5B1E31DEBC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="390">
   <si>
     <t>header1</t>
   </si>
@@ -1471,64 +1471,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>「Microsoftアカウントを追加しましょう」と尋ねられます。これは、このパソコンに対してMicrosoftアカウントを追加するという意味です。もし貴方が@outlook.comや@outlook.jpといったMicrosoftのメールアドレスを既に持っていたら、既にMicrosoftアカウントを持っています。gmail.comやyahoo.co.jpやdocomo.ne.jpのようなMicrosoftが提供していないメールアドレスしかなければ、新たに作ることになります。以降では、新たに作る手順を示します。</t>
-    <rPh sb="16" eb="18">
-      <t>ツイカ</t>
-    </rPh>
-    <rPh sb="25" eb="26">
-      <t>タズ</t>
-    </rPh>
-    <rPh sb="43" eb="44">
-      <t>タイ</t>
-    </rPh>
-    <rPh sb="61" eb="63">
-      <t>ツイカ</t>
-    </rPh>
-    <rPh sb="68" eb="70">
-      <t>イミ</t>
-    </rPh>
-    <rPh sb="75" eb="77">
-      <t>アナタ</t>
-    </rPh>
-    <rPh sb="124" eb="125">
-      <t>スデ</t>
-    </rPh>
-    <rPh sb="126" eb="127">
-      <t>モ</t>
-    </rPh>
-    <rPh sb="133" eb="134">
-      <t>スデ</t>
-    </rPh>
-    <rPh sb="150" eb="151">
-      <t>モ</t>
-    </rPh>
-    <rPh sb="205" eb="207">
-      <t>テイキョウ</t>
-    </rPh>
-    <rPh sb="226" eb="227">
-      <t>アラ</t>
-    </rPh>
-    <rPh sb="229" eb="230">
-      <t>ツク</t>
-    </rPh>
-    <rPh sb="239" eb="241">
-      <t>イコウ</t>
-    </rPh>
-    <rPh sb="244" eb="245">
-      <t>アラ</t>
-    </rPh>
-    <rPh sb="247" eb="248">
-      <t>ツク</t>
-    </rPh>
-    <rPh sb="249" eb="251">
-      <t>テジュン</t>
-    </rPh>
-    <rPh sb="252" eb="253">
-      <t>シメ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>win11ja-msaccount-create.png</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1889,37 +1831,6 @@
     </rPh>
     <rPh sb="31" eb="32">
       <t>マ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>既に持っているメールアドレスでMicrosoftアカウントを作るように案内されますが、混乱を避けるため、「新しいメールアドレスを取得」を選びます。</t>
-    <rPh sb="0" eb="1">
-      <t>スデ</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>モ</t>
-    </rPh>
-    <rPh sb="30" eb="31">
-      <t>ツク</t>
-    </rPh>
-    <rPh sb="35" eb="37">
-      <t>アンナイ</t>
-    </rPh>
-    <rPh sb="43" eb="45">
-      <t>コンラン</t>
-    </rPh>
-    <rPh sb="46" eb="47">
-      <t>サ</t>
-    </rPh>
-    <rPh sb="53" eb="54">
-      <t>アタラ</t>
-    </rPh>
-    <rPh sb="64" eb="66">
-      <t>シュトク</t>
-    </rPh>
-    <rPh sb="68" eb="69">
-      <t>エラ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -4635,68 +4546,6 @@
     </rPh>
     <rPh sb="140" eb="141">
       <t>タイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「ライセンス契約に同意します」で「同意する」をクリックします。
-&lt;p class="spl"&gt;※本来は「利用許諾契約書を読む」で契約事項を読んでから同意するものです。「ファイル」→「アカウント」→「Excelのバージョン情報」と辿ればいつでも読めるので、時間のある時に読んでおいてください。&lt;/p&gt;
-これでOfficeを使用するための準備が完了しました。&lt;span class="check"&gt;check 13&lt;span&gt;&lt;/span&gt;
-&lt;strong&gt;広島大学のOffice365アカウントは卒業などで学籍を失うと無くなってしまうので、Office365がインストールされたままでも卒業後は使えなくなります。&lt;/strong&gt;
-以上でこの章の作業は終了です。</t>
-    <rPh sb="6" eb="8">
-      <t>ケイヤク</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>ドウイ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>ドウイ</t>
-    </rPh>
-    <rPh sb="48" eb="50">
-      <t>ホンライ</t>
-    </rPh>
-    <rPh sb="52" eb="54">
-      <t>リヨウ</t>
-    </rPh>
-    <rPh sb="54" eb="56">
-      <t>キョダク</t>
-    </rPh>
-    <rPh sb="56" eb="59">
-      <t>ケイヤクショ</t>
-    </rPh>
-    <rPh sb="60" eb="61">
-      <t>ヨ</t>
-    </rPh>
-    <rPh sb="64" eb="66">
-      <t>ケイヤク</t>
-    </rPh>
-    <rPh sb="66" eb="68">
-      <t>ジコウ</t>
-    </rPh>
-    <rPh sb="69" eb="70">
-      <t>ヨ</t>
-    </rPh>
-    <rPh sb="74" eb="76">
-      <t>ドウイ</t>
-    </rPh>
-    <rPh sb="110" eb="112">
-      <t>ジョウホウ</t>
-    </rPh>
-    <rPh sb="114" eb="115">
-      <t>タド</t>
-    </rPh>
-    <rPh sb="121" eb="122">
-      <t>ヨ</t>
-    </rPh>
-    <rPh sb="127" eb="129">
-      <t>ジカン</t>
-    </rPh>
-    <rPh sb="132" eb="133">
-      <t>トキ</t>
-    </rPh>
-    <rPh sb="134" eb="135">
-      <t>ヨ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -6263,34 +6112,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>エクスプローラの左サイドバーにはOneDriveに連携された雲アイコンがある筈です。これを右クリックして「OneDrive」を選択し、さらに「設定」に進みます。</t>
-    <rPh sb="8" eb="9">
-      <t>ヒダリ</t>
-    </rPh>
-    <rPh sb="25" eb="27">
-      <t>レンケイ</t>
-    </rPh>
-    <rPh sb="30" eb="31">
-      <t>クモ</t>
-    </rPh>
-    <rPh sb="38" eb="39">
-      <t>ハズ</t>
-    </rPh>
-    <rPh sb="45" eb="46">
-      <t>ミギ</t>
-    </rPh>
-    <rPh sb="63" eb="65">
-      <t>センタク</t>
-    </rPh>
-    <rPh sb="71" eb="73">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="75" eb="76">
-      <t>スス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>OneDriveを使うためのアカウントでサインインするよう促すウィンドウが開きますが、「X」ボタンで閉じます。</t>
     <rPh sb="9" eb="10">
       <t>ツカ</t>
@@ -6307,53 +6128,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>念のため、エクスプローラの左サイドバーの「ホーム」をクリックし、「クイックアクセス」の下のフォルダに雲マークや「OneDrive」などの文字が見えないことを確認してください。</t>
-    <rPh sb="0" eb="1">
-      <t>ネン</t>
-    </rPh>
-    <rPh sb="13" eb="14">
-      <t>ヒダリ</t>
-    </rPh>
-    <rPh sb="43" eb="44">
-      <t>シタ</t>
-    </rPh>
-    <rPh sb="50" eb="51">
-      <t>クモ</t>
-    </rPh>
-    <rPh sb="68" eb="70">
-      <t>モジ</t>
-    </rPh>
-    <rPh sb="71" eb="72">
-      <t>ミ</t>
-    </rPh>
-    <rPh sb="78" eb="80">
-      <t>カクニン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>OneDriveと連携していないことを確認した上で、次の章に進みましょう。</t>
-    <rPh sb="9" eb="11">
-      <t>レンケイ</t>
-    </rPh>
-    <rPh sb="19" eb="21">
-      <t>カクニン</t>
-    </rPh>
-    <rPh sb="23" eb="24">
-      <t>ウエ</t>
-    </rPh>
-    <rPh sb="26" eb="27">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="28" eb="29">
-      <t>ショウ</t>
-    </rPh>
-    <rPh sb="30" eb="31">
-      <t>スス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;div class="panel-heading"&gt;&lt;span class="glyphicon glyphicon-warning-sign"&gt;&lt;/span&gt;&lt;a name="wrongkb"&gt;&lt;/a&gt; Surfaceを利用されているみなさん&lt;/div&gt;
 &lt;div class="panel-body" style="padding:10px"&gt;パソコンのスペック確認はここまでです。Surfaceをつかっている方は、タイプカバーキーボード設定に不具合があることがあるので、確認しておきましょう。不具合の内容は、キーボードが日本語用のものなのに、英語用になっているというものです。文字キーは同じですが、記号の配列が違うため、正常に入力できません。 &lt;/div&gt;
   </t>
@@ -6372,31 +6146,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-explorer-onedrive-folder.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11ja-explorer-onedrive-sideber-setting.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11ja-onedrive-setting-unlink.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>開いたOneDrive設定ウィンドウから、「このPCのリンクを解除する」をクリックします。</t>
-    <rPh sb="0" eb="1">
-      <t>ヒラ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="31" eb="33">
-      <t>カイジョ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>「オンラインのみのファイルは削除されます」という警告が出ますが、これは手元のエクスプローラでアクセスできなくなるという意味です。Webブラウザ経由でOneDriveにアクセスする形では残っていますので、解除しましょう。</t>
     <rPh sb="14" eb="16">
       <t>サクジョ</t>
@@ -6428,62 +6177,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>これをクリックした時、ログインしたMicrosoftアカウントとお使いのPCのOneDriveアプリがリンクがされていなければ、アカウントを入力するウィンドウが開きます。その場合はウィンドウを「X」ボタンで閉じ、次の章に進んで下さい。</t>
-    <rPh sb="9" eb="10">
-      <t>トキ</t>
-    </rPh>
-    <rPh sb="33" eb="34">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="70" eb="72">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="80" eb="81">
-      <t>ヒラ</t>
-    </rPh>
-    <rPh sb="87" eb="89">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="103" eb="104">
-      <t>ト</t>
-    </rPh>
-    <rPh sb="106" eb="107">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="108" eb="109">
-      <t>ショウ</t>
-    </rPh>
-    <rPh sb="110" eb="111">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="113" eb="114">
-      <t>クダ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>もしエクスプローラが開き、「個人用Vault」などのフォルダが見えた場合、既にアカウントと連携されています。これを解除しましょう。</t>
-    <rPh sb="10" eb="11">
-      <t>ヒラ</t>
-    </rPh>
-    <rPh sb="14" eb="17">
-      <t>コジンヨウ</t>
-    </rPh>
-    <rPh sb="31" eb="32">
-      <t>ミ</t>
-    </rPh>
-    <rPh sb="34" eb="36">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="37" eb="38">
-      <t>スデ</t>
-    </rPh>
-    <rPh sb="57" eb="59">
-      <t>カイジョ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>まず、タスクバーの右側の通知欄に雲のアイコンが無いかを確認します。「＾」も展開して確認してください。雲のアイコンがあれば、お使いのPCにはOneDriveアプリがインストールされています。</t>
     <rPh sb="37" eb="39">
       <t>テンカイ</t>
@@ -6581,25 +6274,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Webブラウザの履歴をMicrosoftアカウントに保存するかどうか尋ねられることがありますが、「今はしない」で進めましょう。</t>
-    <rPh sb="8" eb="10">
-      <t>リレキ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>ホゾン</t>
-    </rPh>
-    <rPh sb="34" eb="35">
-      <t>タズ</t>
-    </rPh>
-    <rPh sb="49" eb="50">
-      <t>イマ</t>
-    </rPh>
-    <rPh sb="56" eb="57">
-      <t>スス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>OneDriveでのバックアップについて聞かれることがありますが、ここでOneDriveを使うと皆さんのデータはお使いのパソコンではなく、先に作ったMicrosoftアカウントに保存されるようになります。先に作ったMicrosoftアカウントは無料アカウントであるため5GBしかなく、すぐいっぱいになってしまうので、ここでは「このPCにのみファイルを保存する」を選びましょう。</t>
     <rPh sb="20" eb="21">
       <t>キ</t>
@@ -7006,10 +6680,6 @@
     <rPh sb="117" eb="118">
       <t>スス</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11ja-onedrive-noaccount.png</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -7129,6 +6799,334 @@
     </rPh>
     <rPh sb="38" eb="39">
       <t>シメ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-onedrive-withaccount.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>念のため、エクスプローラの左サイドバーの「ホーム」をクリックし、「クイックアクセス」の下のフォルダに雲マークや「OneDrive」などの文字が見えないことを確認してください。エクスプローラは再起動しないと最新の状況を反映しない場合があります。</t>
+    <rPh sb="0" eb="1">
+      <t>ネン</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>ヒダリ</t>
+    </rPh>
+    <rPh sb="43" eb="44">
+      <t>シタ</t>
+    </rPh>
+    <rPh sb="50" eb="51">
+      <t>クモ</t>
+    </rPh>
+    <rPh sb="68" eb="70">
+      <t>モジ</t>
+    </rPh>
+    <rPh sb="71" eb="72">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="78" eb="80">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="95" eb="98">
+      <t>サイキドウ</t>
+    </rPh>
+    <rPh sb="102" eb="104">
+      <t>サイシン</t>
+    </rPh>
+    <rPh sb="105" eb="107">
+      <t>ジョウキョウ</t>
+    </rPh>
+    <rPh sb="108" eb="110">
+      <t>ハンエイ</t>
+    </rPh>
+    <rPh sb="113" eb="115">
+      <t>バアイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>あらためてOneDriveアプリを開きなおし、アカウントが無い状態になっていたらこの部分の設定は成功です。</t>
+    <rPh sb="17" eb="18">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>ナ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>ジョウタイ</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>ブブン</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>セイコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-onedrive-noaccount.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「ライセンス契約に同意します」で「同意する」をクリックします。
+&lt;p class="spl"&gt;※本来は「利用許諾契約書を読む」で契約事項を読んでから同意するものです。「ファイル」→「アカウント」→「Excelのバージョン情報」と辿ればいつでも読めるので、時間のある時に読んでおいてください。&lt;/p&gt;
+これでOfficeを使用するための準備が完了しました。&lt;span class="check"&gt;check 13&lt;span&gt;&lt;/span&gt;
+&lt;strong&gt;広島大学のOffice365アカウントは卒業などで学籍を失うと無くなってしまうので、Office365がインストールされたままでも卒業後は使えなくなります。&lt;/strong&gt;</t>
+    <rPh sb="6" eb="8">
+      <t>ケイヤク</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ドウイ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ドウイ</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>ホンライ</t>
+    </rPh>
+    <rPh sb="52" eb="54">
+      <t>リヨウ</t>
+    </rPh>
+    <rPh sb="54" eb="56">
+      <t>キョダク</t>
+    </rPh>
+    <rPh sb="56" eb="59">
+      <t>ケイヤクショ</t>
+    </rPh>
+    <rPh sb="60" eb="61">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="64" eb="66">
+      <t>ケイヤク</t>
+    </rPh>
+    <rPh sb="66" eb="68">
+      <t>ジコウ</t>
+    </rPh>
+    <rPh sb="69" eb="70">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="74" eb="76">
+      <t>ドウイ</t>
+    </rPh>
+    <rPh sb="110" eb="112">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="114" eb="115">
+      <t>タド</t>
+    </rPh>
+    <rPh sb="121" eb="122">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="127" eb="129">
+      <t>ジカン</t>
+    </rPh>
+    <rPh sb="132" eb="133">
+      <t>トキ</t>
+    </rPh>
+    <rPh sb="134" eb="135">
+      <t>ヨ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「Microsoftアカウントを追加しましょう」と尋ねられます。これは、このパソコンに対してMicrosoftアカウント（以降、MSアカウント）を追加するという意味です。もし貴方が@outlook.comや@outlook.jpといったMicrosoftのメールアドレスを既に持っていたら、既にMSアカウントを持っています。gmail.comやyahoo.co.jpやdocomo.ne.jpのようなMicrosoftが提供していないメールアドレスしかなければ、新たに作ることになります。以降では、新たに作る手順を示します。</t>
+    <rPh sb="16" eb="18">
+      <t>ツイカ</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>タズ</t>
+    </rPh>
+    <rPh sb="43" eb="44">
+      <t>タイ</t>
+    </rPh>
+    <rPh sb="61" eb="63">
+      <t>イコウ</t>
+    </rPh>
+    <rPh sb="73" eb="75">
+      <t>ツイカ</t>
+    </rPh>
+    <rPh sb="80" eb="82">
+      <t>イミ</t>
+    </rPh>
+    <rPh sb="87" eb="89">
+      <t>アナタ</t>
+    </rPh>
+    <rPh sb="136" eb="137">
+      <t>スデ</t>
+    </rPh>
+    <rPh sb="138" eb="139">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="145" eb="146">
+      <t>スデ</t>
+    </rPh>
+    <rPh sb="155" eb="156">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="210" eb="212">
+      <t>テイキョウ</t>
+    </rPh>
+    <rPh sb="231" eb="232">
+      <t>アラ</t>
+    </rPh>
+    <rPh sb="234" eb="235">
+      <t>ツク</t>
+    </rPh>
+    <rPh sb="244" eb="246">
+      <t>イコウ</t>
+    </rPh>
+    <rPh sb="249" eb="250">
+      <t>アラ</t>
+    </rPh>
+    <rPh sb="252" eb="253">
+      <t>ツク</t>
+    </rPh>
+    <rPh sb="254" eb="256">
+      <t>テジュン</t>
+    </rPh>
+    <rPh sb="257" eb="258">
+      <t>シメ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>既に持っているメールアドレスでMSアカウントを作るように案内されますが、混乱を避けるため、「新しいメールアドレスを取得」を選びます。以降では、ここで新規に作るものを「個人MSアカウント」あるいは「無料MSアカウント」と呼びます。
+これとは別に大学在籍期間中に大学が有償契約したMSアカウントもありますが、卒業、あるいは大学院進学で学籍番号が無効になると使えなくなります。</t>
+    <rPh sb="0" eb="1">
+      <t>スデ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>ツク</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>アンナイ</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>コンラン</t>
+    </rPh>
+    <rPh sb="39" eb="40">
+      <t>サ</t>
+    </rPh>
+    <rPh sb="46" eb="47">
+      <t>アタラ</t>
+    </rPh>
+    <rPh sb="57" eb="59">
+      <t>シュトク</t>
+    </rPh>
+    <rPh sb="61" eb="62">
+      <t>エラ</t>
+    </rPh>
+    <rPh sb="66" eb="68">
+      <t>イコウ</t>
+    </rPh>
+    <rPh sb="74" eb="76">
+      <t>シンキ</t>
+    </rPh>
+    <rPh sb="77" eb="78">
+      <t>ツク</t>
+    </rPh>
+    <rPh sb="83" eb="85">
+      <t>コジン</t>
+    </rPh>
+    <rPh sb="98" eb="100">
+      <t>ムリョウ</t>
+    </rPh>
+    <rPh sb="109" eb="110">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="119" eb="120">
+      <t>ベツ</t>
+    </rPh>
+    <rPh sb="121" eb="123">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="123" eb="125">
+      <t>ザイセキ</t>
+    </rPh>
+    <rPh sb="125" eb="128">
+      <t>キカンチュウ</t>
+    </rPh>
+    <rPh sb="129" eb="131">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="132" eb="134">
+      <t>ユウショウ</t>
+    </rPh>
+    <rPh sb="134" eb="136">
+      <t>ケイヤク</t>
+    </rPh>
+    <rPh sb="152" eb="154">
+      <t>ソツギョウ</t>
+    </rPh>
+    <rPh sb="159" eb="162">
+      <t>ダイガクイン</t>
+    </rPh>
+    <rPh sb="162" eb="164">
+      <t>シンガク</t>
+    </rPh>
+    <rPh sb="165" eb="167">
+      <t>ガクセキ</t>
+    </rPh>
+    <rPh sb="167" eb="169">
+      <t>バンゴウ</t>
+    </rPh>
+    <rPh sb="170" eb="172">
+      <t>ムコウ</t>
+    </rPh>
+    <rPh sb="176" eb="177">
+      <t>ツカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Webブラウザの履歴を個人MSアカウントに保存するかどうか尋ねられることがありますが、「今はしない」で進めましょう。</t>
+    <rPh sb="8" eb="10">
+      <t>リレキ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>コジン</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>タズ</t>
+    </rPh>
+    <rPh sb="44" eb="45">
+      <t>イマ</t>
+    </rPh>
+    <rPh sb="51" eb="52">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OneDriveと無料MSアカウントが連携していないことを確認できたら、次の章に進みましょう。</t>
+    <rPh sb="9" eb="11">
+      <t>ムリョウ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>レンケイ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>スス</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -7211,7 +7209,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -7571,7 +7569,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7587,7 +7585,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7595,7 +7593,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -7609,7 +7607,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7646,7 +7644,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7654,7 +7652,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7670,22 +7668,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7717,7 +7715,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.2">
@@ -7725,10 +7723,10 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D16" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7736,39 +7734,39 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D17" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D19" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7776,31 +7774,31 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D23" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D24" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7816,37 +7814,37 @@
     </row>
     <row r="30" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D30" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D31" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D32" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
@@ -8003,8 +8001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A35" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.2"/>
@@ -8021,7 +8019,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -8029,7 +8027,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -8045,7 +8043,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="304.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -8053,7 +8051,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -8067,7 +8065,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C7" t="s" ph="1">
         <v>7</v>
@@ -8081,7 +8079,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>7</v>
@@ -8092,7 +8090,7 @@
     </row>
     <row r="9" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D9" t="s" ph="1">
         <v>61</v>
@@ -8117,7 +8115,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>7</v>
@@ -8142,7 +8140,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>7</v>
@@ -8181,15 +8179,15 @@
     </row>
     <row r="16" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>358</v>
+        <v>346</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>72</v>
+        <v>386</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>7</v>
@@ -8203,238 +8201,238 @@
         <v>4</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>94</v>
+        <v>387</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C25" t="s" ph="1">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>360</v>
+        <v>348</v>
       </c>
     </row>
     <row r="26" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>375</v>
+        <v>362</v>
       </c>
       <c r="C26" t="s" ph="1">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="D26" t="s" ph="1">
-        <v>371</v>
+        <v>358</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>377</v>
+        <v>364</v>
       </c>
       <c r="C27" t="s" ph="1">
+        <v>351</v>
+      </c>
+      <c r="D27" t="s">
         <v>363</v>
-      </c>
-      <c r="D27" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
       <c r="C28" t="s" ph="1">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="D28" t="s">
-        <v>379</v>
+        <v>366</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>372</v>
+        <v>359</v>
       </c>
       <c r="C29" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D29" t="s" ph="1">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>373</v>
+        <v>360</v>
       </c>
       <c r="C30" t="s" ph="1">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="D30" t="s" ph="1">
-        <v>374</v>
+        <v>361</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C31" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D31" t="s" ph="1">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C32" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D32" t="s" ph="1">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C33" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D33" t="s" ph="1">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D34" t="s" ph="1">
-        <v>361</v>
+        <v>349</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>364</v>
+        <v>388</v>
       </c>
       <c r="C35" t="s" ph="1">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="D35" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>366</v>
+        <v>353</v>
       </c>
       <c r="D36" t="s" ph="1">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="37" spans="2:5" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>365</v>
+        <v>352</v>
       </c>
       <c r="C37" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D37" t="s" ph="1">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C38" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D38" t="s" ph="1">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="2:5" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C39" t="s" ph="1">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D39" t="s" ph="1">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="2:5" ph="1" x14ac:dyDescent="0.2">
@@ -8538,10 +8536,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8565,7 +8563,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -8581,279 +8579,250 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C7" t="s" ph="1">
+        <v>94</v>
+      </c>
+      <c r="D7" t="s" ph="1">
         <v>96</v>
-      </c>
-      <c r="D7" t="s" ph="1">
-        <v>98</v>
       </c>
       <c r="E7" ph="1"/>
     </row>
     <row r="8" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C8" t="s" ph="1">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:5" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C9" t="s" ph="1">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:5" customFormat="1" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>390</v>
+        <v>376</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>391</v>
+        <v>377</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>392</v>
+        <v>378</v>
       </c>
     </row>
     <row r="12" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>394</v>
+        <v>380</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>393</v>
+        <v>379</v>
       </c>
     </row>
     <row r="13" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>367</v>
+        <v>354</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>368</v>
+        <v>355</v>
       </c>
     </row>
     <row r="14" spans="1:5" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>369</v>
+        <v>356</v>
       </c>
     </row>
     <row r="15" spans="1:5" customFormat="1" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>380</v>
+        <v>367</v>
       </c>
     </row>
     <row r="16" spans="1:5" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="D16" t="s" ph="1">
         <v>340</v>
-      </c>
-      <c r="D16" t="s" ph="1">
-        <v>346</v>
       </c>
     </row>
     <row r="17" spans="1:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D17" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
     </row>
     <row r="18" spans="1:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B18" s="6" t="s">
-        <v>384</v>
+        <v>371</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>383</v>
+        <v>370</v>
       </c>
     </row>
     <row r="19" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>385</v>
+        <v>372</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>386</v>
+        <v>381</v>
       </c>
     </row>
     <row r="20" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>387</v>
+        <v>373</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>388</v>
+        <v>374</v>
       </c>
     </row>
     <row r="21" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>389</v>
+        <v>375</v>
       </c>
     </row>
     <row r="22" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="D22" t="s" ph="1">
         <v>342</v>
       </c>
-      <c r="D22" t="s" ph="1">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+        <v>383</v>
+      </c>
+      <c r="D23" t="s" ph="1">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>344</v>
+        <v>382</v>
+      </c>
+      <c r="D24" t="s" ph="1">
+        <v>340</v>
       </c>
     </row>
     <row r="25" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="6"/>
+      <c r="C26"/>
+      <c r="D26"/>
+    </row>
+    <row r="27" spans="1:4" ht="132" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="C25" s="3" ph="1"/>
-      <c r="D25" s="3" t="s" ph="1">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="8" t="s">
-        <v>354</v>
-      </c>
-      <c r="C26" s="3" ph="1"/>
-      <c r="D26" s="3" t="s" ph="1">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="C27" s="3" ph="1"/>
-      <c r="D27" s="3" t="s" ph="1">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="C28" s="3" ph="1"/>
-      <c r="D28" s="3" t="s" ph="1">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="C29" s="3" ph="1"/>
-      <c r="D29" s="3" t="s" ph="1">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="132" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>8</v>
-      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B29" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="C30" t="s">
-        <v>4</v>
+        <v>103</v>
       </c>
       <c r="D30" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>4</v>
-      </c>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C31" t="s">
-        <v>4</v>
+        <v>104</v>
       </c>
       <c r="D31" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
       <c r="B32" s="6" t="s">
-        <v>113</v>
+        <v>105</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B33" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D33" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B34" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D34" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C35" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="6"/>
-    </row>
-    <row r="37" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="6"/>
+    </row>
+    <row r="34" spans="2:2" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="6"/>
+    </row>
+    <row r="37" spans="2:2" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6"/>
     </row>
-    <row r="40" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="6"/>
-    </row>
-    <row r="41" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="6"/>
+    <row r="38" spans="2:2" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -8883,7 +8852,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8891,7 +8860,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8907,7 +8876,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -8915,7 +8884,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8934,13 +8903,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -8948,13 +8917,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -8962,7 +8931,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -8973,7 +8942,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -8984,21 +8953,21 @@
         <v>4</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -9006,13 +8975,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9020,13 +8989,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9034,13 +9003,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -9053,124 +9022,124 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="82.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="82.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D25" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="55.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="D26" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D27" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D28" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D29" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D30" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="50.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D32" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D33" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D34" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D35" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="46.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D36" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="131.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="6" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D41" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9185,7 +9154,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4600B07F-730C-4FC5-BA07-70D58F12A670}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -9202,7 +9171,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
@@ -9210,7 +9179,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -9226,7 +9195,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="5" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -9234,32 +9203,32 @@
     </row>
     <row r="6" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -9268,14 +9237,14 @@
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C13" ph="1"/>
       <c r="D13" ph="1"/>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C14" ph="1"/>
       <c r="D14" ph="1"/>
@@ -9287,68 +9256,68 @@
     </row>
     <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C16" ph="1"/>
     </row>
     <row r="17" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C17" ph="1"/>
       <c r="D17" ph="1"/>
     </row>
     <row r="18" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D19" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D20" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D21" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D22" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D23" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D24" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -9402,7 +9371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C43F54BA-B356-43A4-B76F-707ED0C70724}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView topLeftCell="B22" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -9427,7 +9396,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9443,7 +9412,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9451,7 +9420,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -9472,42 +9441,42 @@
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9515,7 +9484,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9523,50 +9492,50 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D16" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D19" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D20" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D21" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -9580,8 +9549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D6E33FB-2290-439B-854D-9A45A4600EF5}">
   <dimension ref="A1:D87"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A34" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:XFD44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -9597,7 +9566,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -9605,7 +9574,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9621,7 +9590,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -9632,7 +9601,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -9651,7 +9620,7 @@
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -9664,7 +9633,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -9675,18 +9644,18 @@
     </row>
     <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9694,7 +9663,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -9702,18 +9671,18 @@
     </row>
     <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D15" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D16" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -9721,13 +9690,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="198" x14ac:dyDescent="0.2">
@@ -9735,18 +9704,18 @@
         <v>4</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9754,21 +9723,21 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D21" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9776,21 +9745,21 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D23" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9798,13 +9767,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -9812,7 +9781,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -9828,40 +9797,40 @@
     </row>
     <row r="28" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D29" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D30" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -9869,7 +9838,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -9888,80 +9857,80 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D36" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D37" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D39" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D40" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D41" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C42" t="s">
         <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C43" t="s">
         <v>4</v>
       </c>
       <c r="D43" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -9969,7 +9938,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -9977,7 +9946,7 @@
     </row>
     <row r="47" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C47" t="s">
         <v>4</v>
@@ -9988,7 +9957,7 @@
     </row>
     <row r="48" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C48" t="s">
         <v>7</v>
@@ -10016,7 +9985,7 @@
     </row>
     <row r="51" spans="2:4" ht="132" x14ac:dyDescent="0.2">
       <c r="B51" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C51" t="s">
         <v>7</v>
@@ -10066,8 +10035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="A16" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -10091,7 +10060,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -10107,7 +10076,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -10115,7 +10084,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -10139,13 +10108,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -10158,21 +10127,21 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -10180,13 +10149,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -10194,27 +10163,27 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="132" x14ac:dyDescent="0.2">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>4</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>288</v>
+        <v>385</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -10225,13 +10194,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" s="4" customFormat="1" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="4" t="s">
-        <v>4</v>
+      <c r="B20" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="C20" s="4" ph="1"/>
+      <c r="D20" s="4" t="s" ph="1">
+        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -10245,7 +10217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -10262,7 +10234,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -10270,7 +10242,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -10286,17 +10258,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -10309,7 +10281,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -10334,13 +10306,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -10348,21 +10320,21 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -10370,12 +10342,12 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -10383,33 +10355,33 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D18" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D19" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
win11ja: update windows-update instruction
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\fresta2024\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AB34C7-DB83-4575-AA28-4F5B1E31DEBC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861792CF-E0ED-474C-96DE-B37BE43DA1F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="394">
   <si>
     <t>header1</t>
   </si>
@@ -2186,37 +2186,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>まず、Windows Updateを設定しましょう。「設定」アプリを起動し、「Windows Update」を選んで、「更新プログラムのチェック」をクリックします。更新データがあると「今すぐダウンロード」に変わるので、クリックして更新を進めます。</t>
-    <rPh sb="27" eb="29">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="34" eb="36">
-      <t>キドウ</t>
-    </rPh>
-    <rPh sb="55" eb="56">
-      <t>エラ</t>
-    </rPh>
-    <rPh sb="60" eb="62">
-      <t>コウシン</t>
-    </rPh>
-    <rPh sb="82" eb="84">
-      <t>コウシン</t>
-    </rPh>
-    <rPh sb="92" eb="93">
-      <t>イマ</t>
-    </rPh>
-    <rPh sb="103" eb="104">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="115" eb="117">
-      <t>コウシン</t>
-    </rPh>
-    <rPh sb="118" eb="119">
-      <t>スス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>&lt;h2&gt;ウイルススキャン&lt;/h2&gt;</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -3124,12 +3093,6 @@
   </si>
   <si>
     <t>win11ja-wifi-connected.png</t>
-  </si>
-  <si>
-    <t>win11ja-windows-update.png</t>
-  </si>
-  <si>
-    <t>win11ja-windows-update-option.png</t>
   </si>
   <si>
     <t>win11ja-setting-security.png</t>
@@ -4560,67 +4523,6 @@
     </rPh>
     <rPh sb="66" eb="68">
       <t>カイシ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「最新の状態です」と表示されるようになったら、「詳細オプション」をクリックして「その他のMicrosoft製品の更新プログラムを受け取る」も有効にします。これにより、Microsoft Officeをインストールした後にその更新も自動化されます。
-&lt;span class="check"&gt;check 3&lt;/span&gt;
-Microsoft Defenderのウイルス検出パターンファイルはこの更新の一環で実施されます。
-&lt;span class="check"&gt;check 5&lt;/span&gt;</t>
-    <rPh sb="1" eb="3">
-      <t>サイシン</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>ジョウタイ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>ショウサイ</t>
-    </rPh>
-    <rPh sb="42" eb="43">
-      <t>ホカ</t>
-    </rPh>
-    <rPh sb="53" eb="55">
-      <t>セイヒン</t>
-    </rPh>
-    <rPh sb="56" eb="58">
-      <t>コウシン</t>
-    </rPh>
-    <rPh sb="64" eb="65">
-      <t>ウ</t>
-    </rPh>
-    <rPh sb="66" eb="67">
-      <t>ト</t>
-    </rPh>
-    <rPh sb="70" eb="72">
-      <t>ユウコウ</t>
-    </rPh>
-    <rPh sb="108" eb="109">
-      <t>アト</t>
-    </rPh>
-    <rPh sb="112" eb="114">
-      <t>コウシン</t>
-    </rPh>
-    <rPh sb="115" eb="117">
-      <t>ジドウ</t>
-    </rPh>
-    <rPh sb="117" eb="118">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="182" eb="184">
-      <t>ケンシュツ</t>
-    </rPh>
-    <rPh sb="195" eb="197">
-      <t>コウシン</t>
-    </rPh>
-    <rPh sb="198" eb="200">
-      <t>イッカン</t>
-    </rPh>
-    <rPh sb="201" eb="203">
-      <t>ジッシ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -7127,6 +7029,119 @@
     </rPh>
     <rPh sb="40" eb="41">
       <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>まず、Windows Updateを設定しましょう。「設定」アプリを起動し、「Windows Update」(①)を選んで、まず「詳細オプション」(②)に進みます。</t>
+    <rPh sb="27" eb="29">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t>キドウ</t>
+    </rPh>
+    <rPh sb="58" eb="59">
+      <t>エラ</t>
+    </rPh>
+    <rPh sb="65" eb="67">
+      <t>ショウサイ</t>
+    </rPh>
+    <rPh sb="77" eb="78">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-winupdate-option1.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-winupdate-option2.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「Windows Update」のトップメニューにある「更新プログラムのチェック」をクリックします。</t>
+    <rPh sb="28" eb="30">
+      <t>コウシン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-update-start.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-update-auto-install.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「その他のMicrosoft製品の更新プログラムを受け取る」のトグルスイッチ(①)をオンにします。その後、「Windows Update」のトップメニューに戻ります(②をクリック)。これはMicrosoft Officeなどの更新も反映させるためです。</t>
+    <rPh sb="3" eb="4">
+      <t>ホカ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>セイヒン</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>コウシン</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>ウ</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="51" eb="52">
+      <t>アト</t>
+    </rPh>
+    <rPh sb="78" eb="79">
+      <t>モド</t>
+    </rPh>
+    <rPh sb="113" eb="115">
+      <t>コウシン</t>
+    </rPh>
+    <rPh sb="116" eb="118">
+      <t>ハンエイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>現在のWindows Updateは更新データがあり、推奨のものは自動的にダウンロードしインストールされます。再起動を求められる場合があります。
+&lt;span class="check"&gt;check 3&lt;/span&gt;
+Microsoft Defenderのウイルス検出パターンファイルはこの更新の一環で実施されます。
+&lt;span class="check"&gt;check 5&lt;/span&gt;</t>
+    <rPh sb="0" eb="2">
+      <t>ゲンザイ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>コウシン</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>スイショウ</t>
+    </rPh>
+    <rPh sb="33" eb="36">
+      <t>ジドウテキ</t>
+    </rPh>
+    <rPh sb="55" eb="58">
+      <t>サイキドウ</t>
+    </rPh>
+    <rPh sb="59" eb="60">
+      <t>モト</t>
+    </rPh>
+    <rPh sb="64" eb="66">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="131" eb="133">
+      <t>ケンシュツ</t>
+    </rPh>
+    <rPh sb="144" eb="146">
+      <t>コウシン</t>
+    </rPh>
+    <rPh sb="147" eb="149">
+      <t>イッカン</t>
+    </rPh>
+    <rPh sb="150" eb="152">
+      <t>ジッシ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -7569,7 +7584,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7585,7 +7600,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7593,7 +7608,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -7607,7 +7622,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7644,7 +7659,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7652,7 +7667,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7668,22 +7683,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7715,7 +7730,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.2">
@@ -7723,10 +7738,10 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D16" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7734,39 +7749,39 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D17" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D19" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7774,31 +7789,31 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D23" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D24" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7814,37 +7829,37 @@
     </row>
     <row r="30" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D30" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D31" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D32" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
@@ -8027,7 +8042,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -8043,7 +8058,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="304.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -8051,7 +8066,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -8115,7 +8130,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>7</v>
@@ -8140,7 +8155,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>7</v>
@@ -8179,15 +8194,15 @@
     </row>
     <row r="16" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>7</v>
@@ -8212,7 +8227,7 @@
     </row>
     <row r="19" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>7</v>
@@ -8234,7 +8249,7 @@
     </row>
     <row r="21" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>7</v>
@@ -8278,51 +8293,51 @@
     </row>
     <row r="25" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C25" t="s" ph="1">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="26" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C26" t="s" ph="1">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D26" t="s" ph="1">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C27" t="s" ph="1">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D27" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="C28" t="s" ph="1">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D28" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C29" t="s" ph="1">
         <v>7</v>
@@ -8333,13 +8348,13 @@
     </row>
     <row r="30" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C30" t="s" ph="1">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D30" t="s" ph="1">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
@@ -8377,34 +8392,34 @@
     </row>
     <row r="34" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D34" t="s" ph="1">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="C35" t="s" ph="1">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D35" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D36" t="s" ph="1">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="37" spans="2:5" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C37" t="s" ph="1">
         <v>7</v>
@@ -8538,7 +8553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -8563,7 +8578,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -8579,7 +8594,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
@@ -8618,7 +8633,7 @@
     </row>
     <row r="10" spans="1:5" customFormat="1" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="D10" t="s" ph="1">
         <v>98</v>
@@ -8626,119 +8641,119 @@
     </row>
     <row r="11" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="12" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="13" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="14" spans="1:5" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="15" spans="1:5" customFormat="1" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="16" spans="1:5" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="17" spans="1:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="D17" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="18" spans="1:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B18" s="6" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="19" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="20" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="21" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="22" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="D22" t="s" ph="1">
         <v>338</v>
-      </c>
-      <c r="D22" t="s" ph="1">
-        <v>342</v>
       </c>
     </row>
     <row r="23" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="24" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="25" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="26" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -8751,7 +8766,7 @@
         <v>8</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -8833,10 +8848,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8852,7 +8867,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8860,7 +8875,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8876,7 +8891,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -8884,7 +8899,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8898,251 +8913,267 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B11" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="D11" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="D12" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D19" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" t="s">
+    <row r="21" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B17" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="D17" t="s">
+    <row r="22" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="C20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="6" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="82.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="82.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="6" t="s">
-        <v>320</v>
-      </c>
-      <c r="D25" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="55.2" customHeight="1" x14ac:dyDescent="0.2">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="82.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="D26" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="82.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
       <c r="D27" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="55.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>307</v>
+        <v>341</v>
       </c>
       <c r="D28" t="s">
-        <v>308</v>
+        <v>257</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="D29" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="D30" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="D31" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="D29" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="D30" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="50.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="6" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="6" t="s">
+      <c r="D32" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="50.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="6" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="D34" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="D35" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="D36" t="s">
         <v>258</v>
       </c>
-      <c r="D32" t="s">
+    </row>
+    <row r="37" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="D37" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" ht="46.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="D38" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" ht="131.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="6" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B41" s="6" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="D43" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="33" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="6" t="s">
-        <v>296</v>
-      </c>
-      <c r="D33" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="D34" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="D35" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" ht="46.8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="D36" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" ht="131.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="6" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B39" s="6" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="6" t="s">
-        <v>325</v>
-      </c>
-      <c r="D41" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="2:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9171,7 +9202,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
@@ -9179,7 +9210,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="3" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -9195,7 +9226,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="5" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -9203,32 +9234,32 @@
     </row>
     <row r="6" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -9237,14 +9268,14 @@
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C13" ph="1"/>
       <c r="D13" ph="1"/>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="C14" ph="1"/>
       <c r="D14" ph="1"/>
@@ -9256,68 +9287,68 @@
     </row>
     <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C16" ph="1"/>
     </row>
     <row r="17" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C17" ph="1"/>
       <c r="D17" ph="1"/>
     </row>
     <row r="18" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -9396,7 +9427,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9412,7 +9443,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9420,7 +9451,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -9441,42 +9472,42 @@
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9484,7 +9515,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9492,50 +9523,50 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -9566,7 +9597,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -9574,7 +9605,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9590,7 +9621,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -9601,7 +9632,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -9620,7 +9651,7 @@
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -9633,7 +9664,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -9644,18 +9675,18 @@
     </row>
     <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9663,7 +9694,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -9671,18 +9702,18 @@
     </row>
     <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D15" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -9690,13 +9721,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
         <v>163</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="198" x14ac:dyDescent="0.2">
@@ -9704,18 +9735,18 @@
         <v>4</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9723,21 +9754,21 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D21" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9745,21 +9776,21 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D23" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9767,13 +9798,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -9781,7 +9812,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -9797,40 +9828,40 @@
     </row>
     <row r="28" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D29" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D30" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -9838,7 +9869,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -9857,80 +9888,80 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D36" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D37" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D39" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D40" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D41" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C42" t="s">
         <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C43" t="s">
         <v>4</v>
       </c>
       <c r="D43" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -9938,7 +9969,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -9946,7 +9977,7 @@
     </row>
     <row r="47" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C47" t="s">
         <v>4</v>
@@ -9957,7 +9988,7 @@
     </row>
     <row r="48" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C48" t="s">
         <v>7</v>
@@ -9985,7 +10016,7 @@
     </row>
     <row r="51" spans="2:4" ht="132" x14ac:dyDescent="0.2">
       <c r="B51" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C51" t="s">
         <v>7</v>
@@ -10060,7 +10091,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -10076,7 +10107,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -10084,7 +10115,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -10108,13 +10139,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -10127,21 +10158,21 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D15" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -10149,13 +10180,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -10163,13 +10194,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -10177,13 +10208,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -10199,11 +10230,11 @@
         <v>4</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C20" s="4" ph="1"/>
       <c r="D20" s="4" t="s" ph="1">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -10234,7 +10265,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -10242,7 +10273,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -10258,17 +10289,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -10281,7 +10312,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -10306,13 +10337,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -10320,13 +10351,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -10334,7 +10365,7 @@
         <v>118</v>
       </c>
       <c r="D13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -10347,7 +10378,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -10355,33 +10386,33 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D19" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
win11ja: update bitlocker instruction
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\fresta2024\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861792CF-E0ED-474C-96DE-B37BE43DA1F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B06919-D552-4556-A1F2-B797AF6F7309}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="398">
   <si>
     <t>header1</t>
   </si>
@@ -5495,53 +5495,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>まず、「設定」アプリを開き、「プライバシーとセキュリティ」に進みます。そこに「デバイスの暗号化」があれば、お使いのPCはBitLocker保護が使える機種です。古いWindows10用をアップデートした場合は、そのメニューはありません。また、メニューは存在するが、トグルスイッチがOFFになっている場合もあります。</t>
-    <rPh sb="4" eb="6">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="11" eb="12">
-      <t>ヒラ</t>
-    </rPh>
-    <rPh sb="30" eb="31">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="44" eb="47">
-      <t>アンゴウカ</t>
-    </rPh>
-    <rPh sb="54" eb="55">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="69" eb="71">
-      <t>ホゴ</t>
-    </rPh>
-    <rPh sb="72" eb="73">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="75" eb="77">
-      <t>キシュ</t>
-    </rPh>
-    <rPh sb="80" eb="81">
-      <t>フル</t>
-    </rPh>
-    <rPh sb="91" eb="92">
-      <t>ヨウ</t>
-    </rPh>
-    <rPh sb="101" eb="103">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="126" eb="128">
-      <t>ソンザイ</t>
-    </rPh>
-    <rPh sb="149" eb="151">
-      <t>バアイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bitlocker-setting-priv-sec.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>印刷したPDFファイルを保存する場所を尋ねられますので、まずはデスクトップに保存しましょう。ファイル名は「BitLocker鍵_202403xx」のように日付を含めたファイル名にしておくとまぎれが無いでしょう。</t>
     <rPh sb="0" eb="2">
       <t>インサツ</t>
@@ -6091,55 +6044,6 @@
     </rPh>
     <rPh sb="62" eb="63">
       <t>ツカ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>もしメニューがそもそもない場合はそのPCではBitLockerが有効になることは通常は無い筈なので、次の章に進んでください。メニューはあるがオフになっている場合も、次の章に進んで構いませんが、「いつ勝手に有効にされるかわからない」ことには十分注意し、気づいたらすぐこの手順に従ってBitLocker鍵を保存するようにしてください。</t>
-    <rPh sb="13" eb="15">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="32" eb="34">
-      <t>ユウコウ</t>
-    </rPh>
-    <rPh sb="40" eb="42">
-      <t>ツウジョウ</t>
-    </rPh>
-    <rPh sb="43" eb="44">
-      <t>ナ</t>
-    </rPh>
-    <rPh sb="45" eb="46">
-      <t>ハズ</t>
-    </rPh>
-    <rPh sb="50" eb="51">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="52" eb="53">
-      <t>ショウ</t>
-    </rPh>
-    <rPh sb="54" eb="55">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="78" eb="80">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="82" eb="83">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="84" eb="85">
-      <t>ショウ</t>
-    </rPh>
-    <rPh sb="86" eb="87">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="89" eb="90">
-      <t>カマ</t>
-    </rPh>
-    <rPh sb="134" eb="136">
-      <t>テジュン</t>
-    </rPh>
-    <rPh sb="137" eb="138">
-      <t>シタガ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -7142,6 +7046,217 @@
     </rPh>
     <rPh sb="150" eb="152">
       <t>ジッシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>まず、「設定」アプリを開き、「プライバシーとセキュリティ」(①)に進みます。そこに「デバイスの暗号化」(②)があれば、お使いのPCはBitLocker保護が使える機種です。また、メニューは存在しても、トグルスイッチがOFFになっている場合もあります。</t>
+    <rPh sb="4" eb="6">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>スス</t>
+    </rPh>
+    <rPh sb="47" eb="50">
+      <t>アンゴウカ</t>
+    </rPh>
+    <rPh sb="60" eb="61">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="75" eb="77">
+      <t>ホゴ</t>
+    </rPh>
+    <rPh sb="78" eb="79">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="81" eb="83">
+      <t>キシュ</t>
+    </rPh>
+    <rPh sb="94" eb="96">
+      <t>ソンザイ</t>
+    </rPh>
+    <rPh sb="117" eb="119">
+      <t>バアイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>古いWindows10 Homeをアップデートした場合は、このメニューがない場合もあります。もしメニューがそもそもない場合はそのPCではBitLockerが有効になることは通常は無い筈なので、次の章に進んでください。</t>
+    <rPh sb="59" eb="61">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="78" eb="80">
+      <t>ユウコウ</t>
+    </rPh>
+    <rPh sb="86" eb="88">
+      <t>ツウジョウ</t>
+    </rPh>
+    <rPh sb="89" eb="90">
+      <t>ナ</t>
+    </rPh>
+    <rPh sb="91" eb="92">
+      <t>ハズ</t>
+    </rPh>
+    <rPh sb="96" eb="97">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="98" eb="99">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="100" eb="101">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11ja-setting-bitlocker-able.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11ja-setting-bitlocker-unable.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-setting-bitlocker-incomplete.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「デバイスの暗号化」のメニューを開くと、サインインしていないのでBitLockerが完了できないと言われる場合がありますが、個人MSアカウントを作ったのにサインインしていないと言われた場合は、ネットワークに接続されていることを確認してボタンを押し、サインインしてみてください。どうしても解消しない場合はBitLockerのトグルスイッチをOFFにしてください。この警告が出ている状態のWindows11では、以降の手順での鍵の保存ができません。</t>
+    <rPh sb="6" eb="9">
+      <t>アンゴウカ</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>カンリョウ</t>
+    </rPh>
+    <rPh sb="49" eb="50">
+      <t>イ</t>
+    </rPh>
+    <rPh sb="53" eb="55">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="62" eb="64">
+      <t>コジン</t>
+    </rPh>
+    <rPh sb="72" eb="73">
+      <t>ツク</t>
+    </rPh>
+    <rPh sb="88" eb="89">
+      <t>イ</t>
+    </rPh>
+    <rPh sb="92" eb="94">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="103" eb="105">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="113" eb="115">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="121" eb="122">
+      <t>オ</t>
+    </rPh>
+    <rPh sb="143" eb="145">
+      <t>カイショウ</t>
+    </rPh>
+    <rPh sb="148" eb="150">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="182" eb="184">
+      <t>ケイコク</t>
+    </rPh>
+    <rPh sb="185" eb="186">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="189" eb="191">
+      <t>ジョウタイ</t>
+    </rPh>
+    <rPh sb="204" eb="206">
+      <t>イコウ</t>
+    </rPh>
+    <rPh sb="207" eb="209">
+      <t>テジュン</t>
+    </rPh>
+    <rPh sb="211" eb="212">
+      <t>カギ</t>
+    </rPh>
+    <rPh sb="213" eb="215">
+      <t>ホゾン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メニューはあるがオフになっている場合、次の章に進んで構いませんが、「いつ勝手に有効にされるかわからない」ことには十分注意し、気づいたらすぐこの手順に従ってBitLocker鍵を保存するようにしてください。エクスプローラで「PC」をクリックした場合に出てくるシステムドライブのアイコンに南京錠マークがついていれば、BitLockerが有効になっています。南京錠マークが解錠されている状態が「アクセス権を得ている状態」で、施錠されている状態が「アクセス権が無くドライブの内容は見えない状態」です。</t>
+    <rPh sb="16" eb="18">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>スス</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>カマ</t>
+    </rPh>
+    <rPh sb="71" eb="73">
+      <t>テジュン</t>
+    </rPh>
+    <rPh sb="74" eb="75">
+      <t>シタガ</t>
+    </rPh>
+    <rPh sb="121" eb="123">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="124" eb="125">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="142" eb="145">
+      <t>ナンキンジョウ</t>
+    </rPh>
+    <rPh sb="166" eb="168">
+      <t>ユウコウ</t>
+    </rPh>
+    <rPh sb="176" eb="179">
+      <t>ナンキンジョウ</t>
+    </rPh>
+    <rPh sb="183" eb="185">
+      <t>カイジョウ</t>
+    </rPh>
+    <rPh sb="190" eb="192">
+      <t>ジョウタイ</t>
+    </rPh>
+    <rPh sb="200" eb="201">
+      <t>エ</t>
+    </rPh>
+    <rPh sb="204" eb="206">
+      <t>ジョウタイ</t>
+    </rPh>
+    <rPh sb="209" eb="211">
+      <t>セジョウ</t>
+    </rPh>
+    <rPh sb="216" eb="218">
+      <t>ジョウタイ</t>
+    </rPh>
+    <rPh sb="226" eb="227">
+      <t>ナ</t>
+    </rPh>
+    <rPh sb="233" eb="235">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="236" eb="237">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="240" eb="242">
+      <t>ジョウタイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -8194,15 +8309,15 @@
     </row>
     <row r="16" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>7</v>
@@ -8227,7 +8342,7 @@
     </row>
     <row r="19" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>7</v>
@@ -8296,48 +8411,48 @@
         <v>290</v>
       </c>
       <c r="C25" t="s" ph="1">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="26" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C26" t="s" ph="1">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D26" t="s" ph="1">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C27" t="s" ph="1">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D27" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C28" t="s" ph="1">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D28" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C29" t="s" ph="1">
         <v>7</v>
@@ -8348,13 +8463,13 @@
     </row>
     <row r="30" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C30" t="s" ph="1">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D30" t="s" ph="1">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
@@ -8395,23 +8510,23 @@
         <v>291</v>
       </c>
       <c r="D34" t="s" ph="1">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C35" t="s" ph="1">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D35" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D36" t="s" ph="1">
         <v>294</v>
@@ -8419,7 +8534,7 @@
     </row>
     <row r="37" spans="2:5" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C37" t="s" ph="1">
         <v>7</v>
@@ -8633,7 +8748,7 @@
     </row>
     <row r="10" spans="1:5" customFormat="1" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D10" t="s" ph="1">
         <v>98</v>
@@ -8641,119 +8756,119 @@
     </row>
     <row r="11" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="12" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="13" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="14" spans="1:5" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="15" spans="1:5" customFormat="1" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="16" spans="1:5" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="17" spans="1:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D17" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="18" spans="1:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B18" s="6" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="19" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="20" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="21" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="22" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="23" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="24" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="25" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="26" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -8766,7 +8881,7 @@
         <v>8</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -8848,10 +8963,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8918,29 +9033,29 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D11" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D12" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -8948,13 +9063,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -9061,119 +9176,136 @@
         <v>270</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="82.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>316</v>
+        <v>391</v>
       </c>
       <c r="D27" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="55.2" customHeight="1" x14ac:dyDescent="0.2">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>341</v>
+        <v>392</v>
       </c>
       <c r="D28" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="67.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="D29" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="D30" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="6" t="s">
+    <row r="31" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D32" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="6" t="s">
+    <row r="33" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D33" t="s">
         <v>304</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="6" t="s">
-        <v>306</v>
-      </c>
-      <c r="D31" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="6" t="s">
-        <v>310</v>
-      </c>
-      <c r="D32" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" ht="50.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="6" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="D34" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="D35" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="50.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="6" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D37" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="35" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="6" t="s">
+    <row r="38" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D38" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="36" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="6" t="s">
+    <row r="39" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D39" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="37" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="6" t="s">
+    <row r="40" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D40" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="38" spans="2:4" ht="46.8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="D38" t="s">
+    <row r="41" spans="2:4" ht="46.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="D41" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="39" spans="2:4" ht="131.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="6" t="s">
+    <row r="42" spans="2:4" ht="131.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="6" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B44" s="6" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="6" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="40" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B41" s="6" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="6" t="s">
-        <v>321</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="D46" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="44" spans="2:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="2:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9226,7 +9358,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="5" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -9234,32 +9366,32 @@
     </row>
     <row r="6" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -9268,14 +9400,14 @@
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C13" ph="1"/>
       <c r="D13" ph="1"/>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C14" ph="1"/>
       <c r="D14" ph="1"/>
@@ -9287,13 +9419,13 @@
     </row>
     <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C16" ph="1"/>
     </row>
     <row r="17" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C17" ph="1"/>
       <c r="D17" ph="1"/>
@@ -10208,7 +10340,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -10230,11 +10362,11 @@
         <v>4</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C20" s="4" ph="1"/>
       <c r="D20" s="4" t="s" ph="1">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
win11ja: update instruction for bitlocker
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\fresta2024\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B06919-D552-4556-A1F2-B797AF6F7309}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4845A2F1-076E-4FDC-9D41-51CEE748BA65}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="400">
   <si>
     <t>header1</t>
   </si>
@@ -7050,7 +7050,19 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>まず、「設定」アプリを開き、「プライバシーとセキュリティ」(①)に進みます。そこに「デバイスの暗号化」(②)があれば、お使いのPCはBitLocker保護が使える機種です。また、メニューは存在しても、トグルスイッチがOFFになっている場合もあります。</t>
+    <t xml:space="preserve">win11ja-setting-bitlocker-able.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11ja-setting-bitlocker-unable.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-setting-bitlocker-incomplete.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>まず、「設定」アプリを開き、「プライバシーとセキュリティ」(①)に進みます。そこに「デバイスの暗号化」(②)があれば、お使いのPCはBitLocker保護が使える機種です。「デバイスの暗号化」メニューをクリックして進めます。</t>
     <rPh sb="4" eb="6">
       <t>セッテイ</t>
     </rPh>
@@ -7075,123 +7087,114 @@
     <rPh sb="81" eb="83">
       <t>キシュ</t>
     </rPh>
-    <rPh sb="94" eb="96">
-      <t>ソンザイ</t>
+    <rPh sb="92" eb="95">
+      <t>アンゴウカ</t>
+    </rPh>
+    <rPh sb="107" eb="108">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>古いWindows10 Homeをアップデートした場合は、「デバイスの暗号化」メニューがない場合もあります。その場合はそのPCではBitLockerが有効になることは通常は無い筈なので、次の章に進んでください。</t>
+    <rPh sb="35" eb="38">
+      <t>アンゴウカ</t>
+    </rPh>
+    <rPh sb="56" eb="58">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="75" eb="77">
+      <t>ユウコウ</t>
+    </rPh>
+    <rPh sb="83" eb="85">
+      <t>ツウジョウ</t>
+    </rPh>
+    <rPh sb="86" eb="87">
+      <t>ナ</t>
+    </rPh>
+    <rPh sb="88" eb="89">
+      <t>ハズ</t>
+    </rPh>
+    <rPh sb="93" eb="94">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="95" eb="96">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="97" eb="98">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-setting-bitlocker-enabled.png</t>
+  </si>
+  <si>
+    <t>サインインしていないので暗号化が完了していないと言われる場合があります。個人MSアカウントを作ったのにサインインしていないと言われた場合は、ネットワークに接続されていることを確認してボタンを押し、サインインしてみてください。どうしても解消しない場合はトグルスイッチをOFFにしてください。この警告が出ている状態のWindows11では、以降の手順での鍵の保存ができません。</t>
+    <rPh sb="12" eb="15">
+      <t>アンゴウカ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>カンリョウ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>イ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>コジン</t>
+    </rPh>
+    <rPh sb="46" eb="47">
+      <t>ツク</t>
+    </rPh>
+    <rPh sb="62" eb="63">
+      <t>イ</t>
+    </rPh>
+    <rPh sb="66" eb="68">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="77" eb="79">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="87" eb="89">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="95" eb="96">
+      <t>オ</t>
     </rPh>
     <rPh sb="117" eb="119">
+      <t>カイショウ</t>
+    </rPh>
+    <rPh sb="122" eb="124">
       <t>バアイ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>古いWindows10 Homeをアップデートした場合は、このメニューがない場合もあります。もしメニューがそもそもない場合はそのPCではBitLockerが有効になることは通常は無い筈なので、次の章に進んでください。</t>
-    <rPh sb="59" eb="61">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="78" eb="80">
-      <t>ユウコウ</t>
-    </rPh>
-    <rPh sb="86" eb="88">
-      <t>ツウジョウ</t>
-    </rPh>
-    <rPh sb="89" eb="90">
-      <t>ナ</t>
-    </rPh>
-    <rPh sb="91" eb="92">
-      <t>ハズ</t>
-    </rPh>
-    <rPh sb="96" eb="97">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="98" eb="99">
-      <t>ショウ</t>
-    </rPh>
-    <rPh sb="100" eb="101">
-      <t>スス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11ja-setting-bitlocker-able.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11ja-setting-bitlocker-unable.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11ja-setting-bitlocker-incomplete.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「デバイスの暗号化」のメニューを開くと、サインインしていないのでBitLockerが完了できないと言われる場合がありますが、個人MSアカウントを作ったのにサインインしていないと言われた場合は、ネットワークに接続されていることを確認してボタンを押し、サインインしてみてください。どうしても解消しない場合はBitLockerのトグルスイッチをOFFにしてください。この警告が出ている状態のWindows11では、以降の手順での鍵の保存ができません。</t>
-    <rPh sb="6" eb="9">
-      <t>アンゴウカ</t>
-    </rPh>
-    <rPh sb="16" eb="17">
-      <t>ヒラ</t>
-    </rPh>
-    <rPh sb="42" eb="44">
-      <t>カンリョウ</t>
-    </rPh>
-    <rPh sb="49" eb="50">
-      <t>イ</t>
-    </rPh>
-    <rPh sb="53" eb="55">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="62" eb="64">
-      <t>コジン</t>
-    </rPh>
-    <rPh sb="72" eb="73">
-      <t>ツク</t>
-    </rPh>
-    <rPh sb="88" eb="89">
-      <t>イ</t>
-    </rPh>
-    <rPh sb="92" eb="94">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="103" eb="105">
-      <t>セツゾク</t>
-    </rPh>
-    <rPh sb="113" eb="115">
-      <t>カクニン</t>
-    </rPh>
-    <rPh sb="121" eb="122">
-      <t>オ</t>
-    </rPh>
-    <rPh sb="143" eb="145">
-      <t>カイショウ</t>
-    </rPh>
-    <rPh sb="148" eb="150">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="182" eb="184">
+    <rPh sb="146" eb="148">
       <t>ケイコク</t>
     </rPh>
-    <rPh sb="185" eb="186">
+    <rPh sb="149" eb="150">
       <t>デ</t>
     </rPh>
-    <rPh sb="189" eb="191">
+    <rPh sb="153" eb="155">
       <t>ジョウタイ</t>
     </rPh>
-    <rPh sb="204" eb="206">
+    <rPh sb="168" eb="170">
       <t>イコウ</t>
     </rPh>
-    <rPh sb="207" eb="209">
+    <rPh sb="171" eb="173">
       <t>テジュン</t>
     </rPh>
-    <rPh sb="211" eb="212">
+    <rPh sb="175" eb="176">
       <t>カギ</t>
     </rPh>
-    <rPh sb="213" eb="215">
+    <rPh sb="177" eb="179">
       <t>ホゾン</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>メニューはあるがオフになっている場合、次の章に進んで構いませんが、「いつ勝手に有効にされるかわからない」ことには十分注意し、気づいたらすぐこの手順に従ってBitLocker鍵を保存するようにしてください。エクスプローラで「PC」をクリックした場合に出てくるシステムドライブのアイコンに南京錠マークがついていれば、BitLockerが有効になっています。南京錠マークが解錠されている状態が「アクセス権を得ている状態」で、施錠されている状態が「アクセス権が無くドライブの内容は見えない状態」です。</t>
+    <t>トグルスイッチがオフになっている場合、次の章に進んで構いませんが、「いつ勝手に有効にされるかわからない」ことには十分注意し、気づいたらすぐこの手順に従ってBitLocker鍵を保存するようにしてください。エクスプローラで「PC」をクリックした場合に出てくるシステムドライブのアイコンに南京錠マークがついていれば、BitLockerが有効になっています。南京錠マークが解錠されている状態が「アクセス権を得ている状態」で、施錠されている状態が「アクセス権が無くドライブの内容は見えない状態」です。</t>
     <rPh sb="16" eb="18">
       <t>バアイ</t>
     </rPh>
@@ -7257,6 +7260,34 @@
     </rPh>
     <rPh sb="240" eb="242">
       <t>ジョウタイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Windows11のプリインストールモデルでは「デバイスの暗号化」が最初から有効になっていることが多いです。以降の手続きに沿ってBitLocker鍵を保存しましょう。</t>
+    <rPh sb="34" eb="36">
+      <t>サイショ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>ユウコウ</t>
+    </rPh>
+    <rPh sb="49" eb="50">
+      <t>オオ</t>
+    </rPh>
+    <rPh sb="54" eb="56">
+      <t>イコウ</t>
+    </rPh>
+    <rPh sb="57" eb="59">
+      <t>テツヅ</t>
+    </rPh>
+    <rPh sb="61" eb="62">
+      <t>ソ</t>
+    </rPh>
+    <rPh sb="73" eb="74">
+      <t>カギ</t>
+    </rPh>
+    <rPh sb="75" eb="77">
+      <t>ホゾン</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -8963,10 +8994,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -9178,134 +9209,142 @@
     </row>
     <row r="27" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="D27" t="s">
         <v>391</v>
-      </c>
-      <c r="D27" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="D28" t="s">
         <v>392</v>
       </c>
-      <c r="D28" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="67.8" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="D29" t="s">
         <v>396</v>
       </c>
-      <c r="D29" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:4" ht="67.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
         <v>397</v>
       </c>
       <c r="D30" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="D31" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="6" t="s">
-        <v>305</v>
-      </c>
-      <c r="D32" t="s">
-        <v>302</v>
-      </c>
-    </row>
+    <row r="32" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="D33" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="D34" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D35" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="35" spans="2:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="6" t="s">
+    <row r="36" spans="2:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="36" spans="2:4" ht="50.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="6" t="s">
+    <row r="37" spans="2:4" ht="50.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="6" t="s">
         <v>309</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="D37" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="D38" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="39" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="6" t="s">
+    <row r="40" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="40" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="6" t="s">
+    <row r="41" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="41" spans="2:4" ht="46.8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="6" t="s">
+    <row r="42" spans="2:4" ht="46.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D42" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="42" spans="2:4" ht="131.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="6" t="s">
+    <row r="43" spans="2:4" ht="131.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="6" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="43" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B44" s="6" t="s">
+    <row r="44" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B45" s="6" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="46" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="6" t="s">
+    <row r="47" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D47" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="47" spans="2:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="2:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
win11ja: update web browser instr
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\fresta2024\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF82F5AB-E758-47FF-AFB4-F5C68679355F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE7CEE4-4B63-4D70-B5A2-3F73C7C9453A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="407">
   <si>
     <t>header1</t>
   </si>
@@ -5557,52 +5557,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Edgeは最初に何らかのMicrosoftアカウントとの連携をさせようとしますが、さらに他のWebブラウザの閲覧や検索履歴からもデータを取り出そうとします。少しでも個人情報保護につながるよう、ここではチェックボックスを外しておきましょう。</t>
-    <rPh sb="5" eb="7">
-      <t>サイショ</t>
-    </rPh>
-    <rPh sb="8" eb="9">
-      <t>ナン</t>
-    </rPh>
-    <rPh sb="28" eb="30">
-      <t>レンケイ</t>
-    </rPh>
-    <rPh sb="44" eb="45">
-      <t>タ</t>
-    </rPh>
-    <rPh sb="54" eb="56">
-      <t>エツラン</t>
-    </rPh>
-    <rPh sb="57" eb="59">
-      <t>ケンサク</t>
-    </rPh>
-    <rPh sb="59" eb="61">
-      <t>リレキ</t>
-    </rPh>
-    <rPh sb="68" eb="69">
-      <t>ト</t>
-    </rPh>
-    <rPh sb="70" eb="71">
-      <t>ダ</t>
-    </rPh>
-    <rPh sb="78" eb="79">
-      <t>スコ</t>
-    </rPh>
-    <rPh sb="82" eb="84">
-      <t>コジン</t>
-    </rPh>
-    <rPh sb="84" eb="86">
-      <t>ジョウホウ</t>
-    </rPh>
-    <rPh sb="86" eb="88">
-      <t>ホゴ</t>
-    </rPh>
-    <rPh sb="109" eb="110">
-      <t>ハズ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>次に、EdgeはあなたのGoogleアカウントも調べようとして、サインインを促します。少しでも個人情報保護につながるよう、「このデータを使用せずに続行する」で進めましょう。</t>
     <rPh sb="0" eb="1">
       <t>ツギ</t>
@@ -5625,104 +5579,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ここからいよいよWebブラウザを使う作業です。以降の作業では「デフォルトで設定されている選択肢をデフォルトでない方を選ぶ」作業が非常に多くなるので、脊髄反射で青やOKの文字があるボタンを押さないよう注意してください。まず、デフォルトで入っているEdge（Microsoft Edge）を起動します。</t>
-    <rPh sb="16" eb="17">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>サギョウ</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>イコウ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>サギョウ</t>
-    </rPh>
-    <rPh sb="37" eb="39">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="44" eb="47">
-      <t>センタクシ</t>
-    </rPh>
-    <rPh sb="56" eb="57">
-      <t>ホウ</t>
-    </rPh>
-    <rPh sb="58" eb="59">
-      <t>エラ</t>
-    </rPh>
-    <rPh sb="61" eb="63">
-      <t>サギョウ</t>
-    </rPh>
-    <rPh sb="64" eb="66">
-      <t>ヒジョウ</t>
-    </rPh>
-    <rPh sb="67" eb="68">
-      <t>オオ</t>
-    </rPh>
-    <rPh sb="74" eb="76">
-      <t>セキズイ</t>
-    </rPh>
-    <rPh sb="76" eb="78">
-      <t>ハンシャ</t>
-    </rPh>
-    <rPh sb="79" eb="80">
-      <t>アオ</t>
-    </rPh>
-    <rPh sb="84" eb="86">
-      <t>モジ</t>
-    </rPh>
-    <rPh sb="93" eb="94">
-      <t>オ</t>
-    </rPh>
-    <rPh sb="99" eb="101">
-      <t>チュウイ</t>
-    </rPh>
-    <rPh sb="117" eb="118">
-      <t>ハイ</t>
-    </rPh>
-    <rPh sb="143" eb="145">
-      <t>キドウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Webブラウザのタブが2枚になっていますが、デフォルトで表示されている「ようこそ」広告を見るだけ見ておきましょう。見ておかないとまた後で見せられるかもしれません。ここでは、レイアウトやカラーテーマを選べるというアピールです。「次へ」で進みます。</t>
-    <rPh sb="12" eb="13">
-      <t>マイ</t>
-    </rPh>
-    <rPh sb="28" eb="30">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="41" eb="43">
-      <t>コウコク</t>
-    </rPh>
-    <rPh sb="44" eb="45">
-      <t>ミ</t>
-    </rPh>
-    <rPh sb="48" eb="49">
-      <t>ミ</t>
-    </rPh>
-    <rPh sb="57" eb="58">
-      <t>ミ</t>
-    </rPh>
-    <rPh sb="66" eb="67">
-      <t>アト</t>
-    </rPh>
-    <rPh sb="68" eb="69">
-      <t>ミ</t>
-    </rPh>
-    <rPh sb="99" eb="100">
-      <t>エラ</t>
-    </rPh>
-    <rPh sb="113" eb="114">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="117" eb="118">
-      <t>スス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>特定のWebサイトにアクセスするのに、Webブラウザを起動してからサイトを検索したりブックマークを開くのではなく、タスクバーから直接アクセスできるというアピールです。「次へ」で進みます。</t>
     <rPh sb="0" eb="2">
       <t>トクテイ</t>
@@ -5744,113 +5600,6 @@
     </rPh>
     <rPh sb="88" eb="89">
       <t>スス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Edgeの最初の設定が終わりました。もう一つのタブも同様の広告ばかりなので、「X」ボタンで閉じてしまいましょう。</t>
-    <rPh sb="5" eb="7">
-      <t>サイショ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="11" eb="12">
-      <t>オ</t>
-    </rPh>
-    <rPh sb="20" eb="21">
-      <t>ヒト</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>ドウヨウ</t>
-    </rPh>
-    <rPh sb="29" eb="31">
-      <t>コウコク</t>
-    </rPh>
-    <rPh sb="45" eb="46">
-      <t>ト</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>現在のWindowsでは、PDFはEdgeによって閲覧するのが既定の状態です。前の章でデスクトップにBitLocker鍵を保存した場合、ダブルクリックして開くことができます。</t>
-    <rPh sb="0" eb="2">
-      <t>ゲンザイ</t>
-    </rPh>
-    <rPh sb="25" eb="27">
-      <t>エツラン</t>
-    </rPh>
-    <rPh sb="31" eb="33">
-      <t>キテイ</t>
-    </rPh>
-    <rPh sb="34" eb="36">
-      <t>ジョウタイ</t>
-    </rPh>
-    <rPh sb="39" eb="40">
-      <t>マエ</t>
-    </rPh>
-    <rPh sb="41" eb="42">
-      <t>ショウ</t>
-    </rPh>
-    <rPh sb="59" eb="60">
-      <t>カギ</t>
-    </rPh>
-    <rPh sb="61" eb="63">
-      <t>ホゾン</t>
-    </rPh>
-    <rPh sb="65" eb="67">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="77" eb="78">
-      <t>ヒラ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>BitLocker鍵の内容が表示されました。スマートフォンなどに写真を撮っておきましょう。</t>
-    <rPh sb="9" eb="10">
-      <t>カギ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>ナイヨウ</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="32" eb="34">
-      <t>シャシン</t>
-    </rPh>
-    <rPh sb="35" eb="36">
-      <t>ト</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>次に、Google Chromeをインストールします。Edgeの検索フォームに「Google Chrome download」などと入力して、google.comのChromeダウンロードサイトを探します。</t>
-    <rPh sb="0" eb="1">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="32" eb="34">
-      <t>ケンサク</t>
-    </rPh>
-    <rPh sb="66" eb="68">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="98" eb="99">
-      <t>サガ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>MicrosoftがGoogle Chromeは不必要というプロモーションをしてきますが、これは気にしなくて構いません。</t>
-    <rPh sb="24" eb="27">
-      <t>フヒツヨウ</t>
-    </rPh>
-    <rPh sb="48" eb="49">
-      <t>キ</t>
-    </rPh>
-    <rPh sb="54" eb="55">
-      <t>カマ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -7281,6 +7030,380 @@
     </rPh>
     <rPh sb="144" eb="146">
       <t>キロク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-edge-init01.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-edge-init02.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-edge-init03.png</t>
+  </si>
+  <si>
+    <t>win11ja-edge-init04.png</t>
+  </si>
+  <si>
+    <t>win11ja-edge-init00.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ここからいよいよWebブラウザを使う作業です。以降の作業では「デフォルトで設定されている選択肢をデフォルトでない方を選ぶ」作業が非常に多くなるので、脊髄反射で青やOKの文字があるボタンを押さないよう注意してください。まず、タスクバーにデフォルトでピン止めされているEdge（Microsoft Edge）を起動します。</t>
+    <rPh sb="16" eb="17">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>サギョウ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>イコウ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>サギョウ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="44" eb="47">
+      <t>センタクシ</t>
+    </rPh>
+    <rPh sb="56" eb="57">
+      <t>ホウ</t>
+    </rPh>
+    <rPh sb="58" eb="59">
+      <t>エラ</t>
+    </rPh>
+    <rPh sb="61" eb="63">
+      <t>サギョウ</t>
+    </rPh>
+    <rPh sb="64" eb="66">
+      <t>ヒジョウ</t>
+    </rPh>
+    <rPh sb="67" eb="68">
+      <t>オオ</t>
+    </rPh>
+    <rPh sb="74" eb="76">
+      <t>セキズイ</t>
+    </rPh>
+    <rPh sb="76" eb="78">
+      <t>ハンシャ</t>
+    </rPh>
+    <rPh sb="79" eb="80">
+      <t>アオ</t>
+    </rPh>
+    <rPh sb="84" eb="86">
+      <t>モジ</t>
+    </rPh>
+    <rPh sb="93" eb="94">
+      <t>オ</t>
+    </rPh>
+    <rPh sb="99" eb="101">
+      <t>チュウイ</t>
+    </rPh>
+    <rPh sb="125" eb="126">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="153" eb="155">
+      <t>キドウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ここからWebブラウザのタブが2枚になっていますが、まず最初から表示されている「ようこそ」広告を見るだけ見ておきましょう。見ておかないとまた後で見せられるかもしれません。ここでは、レイアウトやカラーテーマを選べるというアピールです。「次へ」で進みます。</t>
+    <rPh sb="16" eb="17">
+      <t>マイ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>サイショ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>コウコク</t>
+    </rPh>
+    <rPh sb="48" eb="49">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="52" eb="53">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="61" eb="62">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="70" eb="71">
+      <t>アト</t>
+    </rPh>
+    <rPh sb="72" eb="73">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="103" eb="104">
+      <t>エラ</t>
+    </rPh>
+    <rPh sb="117" eb="118">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="121" eb="122">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Edgeの最初の設定が終わりました。もう一つのタブも同様の広告なので、タブの「X」ボタンで閉じてしまいましょう。</t>
+    <rPh sb="5" eb="7">
+      <t>サイショ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>オ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>ヒト</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>ドウヨウ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>コウコク</t>
+    </rPh>
+    <rPh sb="45" eb="46">
+      <t>ト</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-edge-init05.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Edgeは最初に何らかのMicrosoftアカウントとの連携をさせようとします。最初に個人MSアカウントを作ったため、既定では全ての操作がこのアカウントに結び付けられます。さらに他のWebブラウザの閲覧や検索履歴からもデータを取り出そうとします。少しでも個人情報保護につながるよう、ここではチェックボックス(①)を外した上で、「次へ」(②)をクリックして進めましょう。</t>
+    <rPh sb="5" eb="7">
+      <t>サイショ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ナン</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>レンケイ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>サイショ</t>
+    </rPh>
+    <rPh sb="43" eb="45">
+      <t>コジン</t>
+    </rPh>
+    <rPh sb="53" eb="54">
+      <t>ツク</t>
+    </rPh>
+    <rPh sb="59" eb="61">
+      <t>キテイ</t>
+    </rPh>
+    <rPh sb="63" eb="64">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="66" eb="68">
+      <t>ソウサ</t>
+    </rPh>
+    <rPh sb="77" eb="78">
+      <t>ムス</t>
+    </rPh>
+    <rPh sb="79" eb="80">
+      <t>ツ</t>
+    </rPh>
+    <rPh sb="89" eb="90">
+      <t>タ</t>
+    </rPh>
+    <rPh sb="99" eb="101">
+      <t>エツラン</t>
+    </rPh>
+    <rPh sb="102" eb="104">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="104" eb="106">
+      <t>リレキ</t>
+    </rPh>
+    <rPh sb="113" eb="114">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="115" eb="116">
+      <t>ダ</t>
+    </rPh>
+    <rPh sb="123" eb="124">
+      <t>スコ</t>
+    </rPh>
+    <rPh sb="127" eb="129">
+      <t>コジン</t>
+    </rPh>
+    <rPh sb="129" eb="131">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="131" eb="133">
+      <t>ホゴ</t>
+    </rPh>
+    <rPh sb="157" eb="158">
+      <t>ハズ</t>
+    </rPh>
+    <rPh sb="160" eb="161">
+      <t>ウエ</t>
+    </rPh>
+    <rPh sb="164" eb="165">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="177" eb="178">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-bitlockerpdf-edge.png</t>
+  </si>
+  <si>
+    <t>現在のWindowsでは、PDFはEdgeによって閲覧するのが既定の状態です。前の章でデスクトップにBitLocker鍵を保存した場合、ダブルクリックして開くことができます。表示された内容をスマートフォンなどで写真に撮っておきましょう。</t>
+    <rPh sb="0" eb="2">
+      <t>ゲンザイ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>エツラン</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>キテイ</t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t>ジョウタイ</t>
+    </rPh>
+    <rPh sb="39" eb="40">
+      <t>マエ</t>
+    </rPh>
+    <rPh sb="41" eb="42">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="59" eb="60">
+      <t>カギ</t>
+    </rPh>
+    <rPh sb="61" eb="63">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="65" eb="67">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="77" eb="78">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="87" eb="89">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="92" eb="94">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="105" eb="107">
+      <t>シャシン</t>
+    </rPh>
+    <rPh sb="108" eb="109">
+      <t>ト</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-search-chrome-result.png</t>
+  </si>
+  <si>
+    <t>win11ja-search-chrome-dnld.png</t>
+  </si>
+  <si>
+    <t>次に、Google Chromeをインストールします。Edgeの検索フォームに「Google Chrome download」などと入力して、ダウンロードサイトを探します。</t>
+    <rPh sb="0" eb="1">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="66" eb="68">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="81" eb="82">
+      <t>サガ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MicrosoftがGoogle Chromeは不必要というプロモーションをしてきますが、これは気にしなくて構いません。また注意する必要があるのが、ここでの検索エンジンはMicrosoftのBingなので、ライバル企業の製品について本物をトップに持ってくるモチベーションは無いということです。ここで示す例では、一番上にあるのがMicrosoftのEdgeのプロモーション(①)、二番目にあるのは無料ソフトのレビューサイト（②、このようなサイトはしばしばウイルス入りソフトの配布の温床となっています）、三番目が本物のGoogle自身の配布サイト(③)です。②のようなサイトがいくつも連続する恐れもありますので注意してください。それでは&lt;a href="https://www.google.com/chrome/" target="_blank" rel="noreferrer"&gt;https://www.google.com/chrome/&lt;/a&gt;からGoogle Chromeをダウンロードしましょう。</t>
+    <rPh sb="24" eb="27">
+      <t>フヒツヨウ</t>
+    </rPh>
+    <rPh sb="48" eb="49">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="54" eb="55">
+      <t>カマ</t>
+    </rPh>
+    <rPh sb="107" eb="109">
+      <t>キギョウ</t>
+    </rPh>
+    <rPh sb="110" eb="112">
+      <t>セイヒン</t>
+    </rPh>
+    <rPh sb="116" eb="118">
+      <t>ホンモノ</t>
+    </rPh>
+    <rPh sb="123" eb="124">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="136" eb="137">
+      <t>ナ</t>
+    </rPh>
+    <rPh sb="149" eb="150">
+      <t>シメ</t>
+    </rPh>
+    <rPh sb="151" eb="152">
+      <t>レイ</t>
+    </rPh>
+    <rPh sb="155" eb="157">
+      <t>イチバン</t>
+    </rPh>
+    <rPh sb="157" eb="158">
+      <t>ウエ</t>
+    </rPh>
+    <rPh sb="189" eb="192">
+      <t>ニバンメ</t>
+    </rPh>
+    <rPh sb="197" eb="199">
+      <t>ムリョウ</t>
+    </rPh>
+    <rPh sb="230" eb="231">
+      <t>イ</t>
+    </rPh>
+    <rPh sb="236" eb="238">
+      <t>ハイフ</t>
+    </rPh>
+    <rPh sb="239" eb="241">
+      <t>オンショウ</t>
+    </rPh>
+    <rPh sb="250" eb="253">
+      <t>サンバンメ</t>
+    </rPh>
+    <rPh sb="254" eb="256">
+      <t>ホンモノ</t>
+    </rPh>
+    <rPh sb="263" eb="265">
+      <t>ジシン</t>
+    </rPh>
+    <rPh sb="266" eb="268">
+      <t>ハイフ</t>
+    </rPh>
+    <rPh sb="290" eb="292">
+      <t>レンゾク</t>
+    </rPh>
+    <rPh sb="294" eb="295">
+      <t>オソ</t>
+    </rPh>
+    <rPh sb="303" eb="305">
+      <t>チュウイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -8333,15 +8456,15 @@
     </row>
     <row r="16" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>337</v>
+        <v>329</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>7</v>
@@ -8366,7 +8489,7 @@
     </row>
     <row r="19" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>7</v>
@@ -8435,48 +8558,48 @@
         <v>289</v>
       </c>
       <c r="C25" t="s" ph="1">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>339</v>
+        <v>331</v>
       </c>
     </row>
     <row r="26" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="C26" t="s" ph="1">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="D26" t="s" ph="1">
-        <v>349</v>
+        <v>341</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="C27" t="s" ph="1">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="D27" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="C28" t="s" ph="1">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="D28" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="C29" t="s" ph="1">
         <v>7</v>
@@ -8487,13 +8610,13 @@
     </row>
     <row r="30" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="C30" t="s" ph="1">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="D30" t="s" ph="1">
-        <v>352</v>
+        <v>344</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
@@ -8534,23 +8657,23 @@
         <v>290</v>
       </c>
       <c r="D34" t="s" ph="1">
-        <v>340</v>
+        <v>332</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="C35" t="s" ph="1">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="D35" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="D36" t="s" ph="1">
         <v>293</v>
@@ -8558,7 +8681,7 @@
     </row>
     <row r="37" spans="2:5" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="C37" t="s" ph="1">
         <v>7</v>
@@ -8772,7 +8895,7 @@
     </row>
     <row r="10" spans="1:5" customFormat="1" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="D10" t="s" ph="1">
         <v>98</v>
@@ -8780,119 +8903,119 @@
     </row>
     <row r="11" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>369</v>
+        <v>361</v>
       </c>
     </row>
     <row r="12" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>370</v>
+        <v>362</v>
       </c>
     </row>
     <row r="13" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>346</v>
+        <v>338</v>
       </c>
     </row>
     <row r="14" spans="1:5" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="15" spans="1:5" customFormat="1" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>358</v>
+        <v>350</v>
       </c>
     </row>
     <row r="16" spans="1:5" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>332</v>
+        <v>324</v>
       </c>
     </row>
     <row r="17" spans="1:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="D17" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
     </row>
     <row r="18" spans="1:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B18" s="6" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>361</v>
+        <v>353</v>
       </c>
     </row>
     <row r="19" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>372</v>
+        <v>364</v>
       </c>
     </row>
     <row r="20" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>365</v>
+        <v>357</v>
       </c>
     </row>
     <row r="21" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>366</v>
+        <v>358</v>
       </c>
     </row>
     <row r="22" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>334</v>
+        <v>326</v>
       </c>
     </row>
     <row r="23" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>375</v>
+        <v>367</v>
       </c>
     </row>
     <row r="24" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>332</v>
+        <v>324</v>
       </c>
     </row>
     <row r="25" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
     </row>
     <row r="26" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -8905,7 +9028,7 @@
         <v>8</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -8989,7 +9112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+    <sheetView topLeftCell="A43" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
@@ -9057,29 +9180,29 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D11" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="D12" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -9087,13 +9210,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -9202,39 +9325,39 @@
     </row>
     <row r="27" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="D27" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="D28" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="D29" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="67.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="D30" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="D31" t="s">
         <v>257</v>
@@ -9331,10 +9454,10 @@
     </row>
     <row r="47" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="6" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="D47" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
     </row>
     <row r="48" spans="2:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9347,10 +9470,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4600B07F-730C-4FC5-BA07-70D58F12A670}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -9398,125 +9521,146 @@
     </row>
     <row r="6" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+        <v>396</v>
+      </c>
+      <c r="D6" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>318</v>
+        <v>400</v>
+      </c>
+      <c r="D7" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
+      </c>
+      <c r="D8" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>321</v>
+        <v>397</v>
+      </c>
+      <c r="D9" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>322</v>
+        <v>319</v>
+      </c>
+      <c r="D10" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>323</v>
+        <v>398</v>
+      </c>
+      <c r="D11" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B12" s="6"/>
       <c r="C12" ph="1"/>
     </row>
-    <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>324</v>
+        <v>402</v>
       </c>
       <c r="C13" ph="1"/>
-      <c r="D13" ph="1"/>
-    </row>
-    <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B14" s="6" t="s">
-        <v>325</v>
-      </c>
+      <c r="D13" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="B14" s="6"/>
       <c r="C14" ph="1"/>
       <c r="D14" ph="1"/>
     </row>
-    <row r="15" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="B15" s="6"/>
+    <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B15" s="6" t="s">
+        <v>405</v>
+      </c>
       <c r="C15" ph="1"/>
-      <c r="D15" ph="1"/>
-    </row>
-    <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="158.4" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>326</v>
+        <v>406</v>
       </c>
       <c r="C16" ph="1"/>
-    </row>
-    <row r="17" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B17" s="6" t="s">
-        <v>327</v>
-      </c>
-      <c r="C17" ph="1"/>
-      <c r="D17" ph="1"/>
-    </row>
-    <row r="18" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D17" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>207</v>
+        <v>133</v>
+      </c>
+      <c r="D18" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D19" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="66" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D20" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D21" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D22" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B23" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D23" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D24" t="s">
         <v>148</v>
       </c>
     </row>
+    <row r="23" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="B23" s="6"/>
+      <c r="C23" ph="1"/>
+      <c r="D23" ph="1"/>
+    </row>
+    <row r="24" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="C24" ph="1"/>
+      <c r="D24" ph="1"/>
+    </row>
     <row r="25" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="B25" s="6"/>
       <c r="C25" ph="1"/>
       <c r="D25" ph="1"/>
     </row>
@@ -9526,7 +9670,6 @@
     </row>
     <row r="27" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="C27" ph="1"/>
-      <c r="D27" ph="1"/>
     </row>
     <row r="28" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="C28" ph="1"/>
@@ -9534,26 +9677,19 @@
     </row>
     <row r="29" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="C29" ph="1"/>
+      <c r="D29" ph="1"/>
     </row>
     <row r="30" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="C30" ph="1"/>
-      <c r="D30" ph="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="C31" ph="1"/>
-      <c r="D31" ph="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="C32" ph="1"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B35" s="1"/>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B37" s="1"/>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B38" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -10372,7 +10508,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -10394,11 +10530,11 @@
         <v>4</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="C20" s="4" ph="1"/>
       <c r="D20" s="4" t="s" ph="1">
-        <v>333</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
win11ja: ch3: update abstract under chapter title
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\fresta2024\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991C1D4D-0B2D-4814-8F52-4DE4FA258A2F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C131B0-6A9B-4912-9EBE-660357DE2CD7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="408">
   <si>
     <t>header1</t>
   </si>
@@ -7052,67 +7052,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ここからいよいよWebブラウザを使う作業です。以降の作業では「デフォルトで設定されている選択肢をデフォルトでない方を選ぶ」作業が非常に多くなるので、脊髄反射で青やOKの文字があるボタンを押さないよう注意してください。まず、タスクバーにデフォルトでピン止めされているEdge（Microsoft Edge）を起動します。</t>
-    <rPh sb="16" eb="17">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>サギョウ</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>イコウ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>サギョウ</t>
-    </rPh>
-    <rPh sb="37" eb="39">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="44" eb="47">
-      <t>センタクシ</t>
-    </rPh>
-    <rPh sb="56" eb="57">
-      <t>ホウ</t>
-    </rPh>
-    <rPh sb="58" eb="59">
-      <t>エラ</t>
-    </rPh>
-    <rPh sb="61" eb="63">
-      <t>サギョウ</t>
-    </rPh>
-    <rPh sb="64" eb="66">
-      <t>ヒジョウ</t>
-    </rPh>
-    <rPh sb="67" eb="68">
-      <t>オオ</t>
-    </rPh>
-    <rPh sb="74" eb="76">
-      <t>セキズイ</t>
-    </rPh>
-    <rPh sb="76" eb="78">
-      <t>ハンシャ</t>
-    </rPh>
-    <rPh sb="79" eb="80">
-      <t>アオ</t>
-    </rPh>
-    <rPh sb="84" eb="86">
-      <t>モジ</t>
-    </rPh>
-    <rPh sb="93" eb="94">
-      <t>オ</t>
-    </rPh>
-    <rPh sb="99" eb="101">
-      <t>チュウイ</t>
-    </rPh>
-    <rPh sb="125" eb="126">
-      <t>ト</t>
-    </rPh>
-    <rPh sb="153" eb="155">
-      <t>キドウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>ここからWebブラウザのタブが2枚になっていますが、まず最初から表示されている「ようこそ」広告を見るだけ見ておきましょう。見ておかないとまた後で見せられるかもしれません。ここでは、レイアウトやカラーテーマを選べるというアピールです。「次へ」で進みます。</t>
     <rPh sb="16" eb="17">
       <t>マイ</t>
@@ -7332,80 +7271,129 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>MicrosoftがGoogle Chromeは不必要というプロモーションをしてきますが、これは気にしなくて構いません。また注意する必要があるのが、ここでの検索エンジンはMicrosoftのBingなので、ライバル企業の製品について本物をトップに持ってくるモチベーションは無いということです。ここで示す例では、一番上にあるのがMicrosoftのEdgeのプロモーション(①)、二番目にあるのは無料ソフトのレビューサイト（②、このようなサイトはしばしばウイルス入りソフトの配布の温床となっています）、三番目が本物のGoogle自身の配布サイト(③)です。②のようなサイトがいくつも連続する恐れもありますので注意してください。それでは&lt;a href="https://www.google.com/chrome/" target="_blank" rel="noreferrer"&gt;https://www.google.com/chrome/&lt;/a&gt;からGoogle Chromeをダウンロードしましょう。</t>
-    <rPh sb="24" eb="27">
-      <t>フヒツヨウ</t>
-    </rPh>
-    <rPh sb="48" eb="49">
-      <t>キ</t>
-    </rPh>
-    <rPh sb="54" eb="55">
-      <t>カマ</t>
-    </rPh>
-    <rPh sb="107" eb="109">
+    <t>注意する必要があるのが、ここでの検索エンジンはMicrosoftのBingなので、ライバル企業の製品について本物をトップに持ってくるモチベーションは無いということです。ここで示す例では、一番上にあるのがMicrosoftのEdgeのプロモーション(①)、二番目にあるのは無料ソフトのレビューサイト（②、このようなサイトはしばしばウイルス入りソフトの配布の温床となっています）、三番目が本物のGoogle自身の配布サイト(③)です。②のようなサイトがいくつも連続する恐れもありますので注意してください。それでは&lt;a href="https://www.google.com/chrome/" target="_blank" rel="noreferrer"&gt;https://www.google.com/chrome/&lt;/a&gt;からGoogle Chromeをダウンロードしましょう。</t>
+    <rPh sb="45" eb="47">
       <t>キギョウ</t>
     </rPh>
-    <rPh sb="110" eb="112">
+    <rPh sb="48" eb="50">
       <t>セイヒン</t>
     </rPh>
-    <rPh sb="116" eb="118">
+    <rPh sb="54" eb="56">
       <t>ホンモノ</t>
     </rPh>
-    <rPh sb="123" eb="124">
+    <rPh sb="61" eb="62">
       <t>モ</t>
     </rPh>
-    <rPh sb="136" eb="137">
+    <rPh sb="74" eb="75">
       <t>ナ</t>
     </rPh>
-    <rPh sb="149" eb="150">
+    <rPh sb="87" eb="88">
       <t>シメ</t>
     </rPh>
-    <rPh sb="151" eb="152">
+    <rPh sb="89" eb="90">
       <t>レイ</t>
     </rPh>
-    <rPh sb="155" eb="157">
+    <rPh sb="93" eb="95">
       <t>イチバン</t>
     </rPh>
-    <rPh sb="157" eb="158">
+    <rPh sb="95" eb="96">
       <t>ウエ</t>
     </rPh>
-    <rPh sb="189" eb="192">
+    <rPh sb="127" eb="130">
       <t>ニバンメ</t>
     </rPh>
-    <rPh sb="197" eb="199">
+    <rPh sb="135" eb="137">
       <t>ムリョウ</t>
     </rPh>
-    <rPh sb="230" eb="231">
+    <rPh sb="168" eb="169">
       <t>イ</t>
     </rPh>
-    <rPh sb="236" eb="238">
+    <rPh sb="174" eb="176">
       <t>ハイフ</t>
     </rPh>
-    <rPh sb="239" eb="241">
+    <rPh sb="177" eb="179">
       <t>オンショウ</t>
     </rPh>
-    <rPh sb="250" eb="253">
+    <rPh sb="188" eb="191">
       <t>サンバンメ</t>
     </rPh>
-    <rPh sb="254" eb="256">
+    <rPh sb="192" eb="194">
       <t>ホンモノ</t>
     </rPh>
-    <rPh sb="263" eb="265">
+    <rPh sb="201" eb="203">
       <t>ジシン</t>
     </rPh>
-    <rPh sb="266" eb="268">
+    <rPh sb="204" eb="206">
       <t>ハイフ</t>
     </rPh>
-    <rPh sb="290" eb="292">
+    <rPh sb="228" eb="230">
       <t>レンゾク</t>
     </rPh>
-    <rPh sb="294" eb="295">
+    <rPh sb="232" eb="233">
       <t>オソ</t>
     </rPh>
-    <rPh sb="303" eb="305">
+    <rPh sb="241" eb="243">
       <t>チュウイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ここからいよいよWebブラウザを使う作業です。以降の作業では「デフォルトで設定されている選択肢をデフォルトでない方を選ぶ」作業が非常に多くなるので、脊髄反射で青やOKの文字があるボタンを押さないよう注意してください。</t>
+    <rPh sb="16" eb="17">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>サギョウ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>イコウ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>サギョウ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="44" eb="47">
+      <t>センタクシ</t>
+    </rPh>
+    <rPh sb="56" eb="57">
+      <t>ホウ</t>
+    </rPh>
+    <rPh sb="58" eb="59">
+      <t>エラ</t>
+    </rPh>
+    <rPh sb="61" eb="63">
+      <t>サギョウ</t>
+    </rPh>
+    <rPh sb="64" eb="66">
+      <t>ヒジョウ</t>
+    </rPh>
+    <rPh sb="67" eb="68">
+      <t>オオ</t>
+    </rPh>
+    <rPh sb="74" eb="76">
+      <t>セキズイ</t>
+    </rPh>
+    <rPh sb="76" eb="78">
+      <t>ハンシャ</t>
+    </rPh>
+    <rPh sb="79" eb="80">
+      <t>アオ</t>
+    </rPh>
+    <rPh sb="84" eb="86">
+      <t>モジ</t>
+    </rPh>
+    <rPh sb="93" eb="94">
+      <t>オ</t>
+    </rPh>
+    <rPh sb="99" eb="101">
+      <t>チュウイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>まず、タスクバーにデフォルトでピン止めされているEdge（Microsoft Edge）を起動します。</t>
   </si>
 </sst>
 </file>
@@ -9470,10 +9458,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4600B07F-730C-4FC5-BA07-70D58F12A670}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -9519,144 +9507,145 @@
     <row r="5" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B5" s="6"/>
     </row>
-    <row r="6" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B7" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="D7" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+      <c r="B8" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="D8" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B9" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="D9" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B10" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="D6" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
-      <c r="B7" s="6" t="s">
+      <c r="D10" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B11" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="D11" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B12" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="D12" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="B13" s="6"/>
+      <c r="C13" ph="1"/>
+    </row>
+    <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B14" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="C14" ph="1"/>
+      <c r="D14" t="s">
         <v>400</v>
       </c>
-      <c r="D7" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B8" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="D8" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="B9" s="6" t="s">
-        <v>397</v>
-      </c>
-      <c r="D9" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B10" s="6" t="s">
-        <v>319</v>
-      </c>
-      <c r="D10" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B11" s="6" t="s">
-        <v>398</v>
-      </c>
-      <c r="D11" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="B12" s="6"/>
-      <c r="C12" ph="1"/>
-    </row>
-    <row r="13" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="B13" s="6" t="s">
-        <v>402</v>
-      </c>
-      <c r="C13" ph="1"/>
-      <c r="D13" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="B14" s="6"/>
-      <c r="C14" ph="1"/>
-      <c r="D14" ph="1"/>
-    </row>
-    <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B15" s="6" t="s">
-        <v>405</v>
-      </c>
+    </row>
+    <row r="15" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="B15" s="6"/>
       <c r="C15" ph="1"/>
-      <c r="D15" t="s">
+      <c r="D15" ph="1"/>
+    </row>
+    <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B16" s="6" t="s">
         <v>404</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="158.4" x14ac:dyDescent="0.2">
-      <c r="B16" s="6" t="s">
-        <v>406</v>
       </c>
       <c r="C16" ph="1"/>
       <c r="D16" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B17" s="1" t="s">
+    <row r="17" spans="2:4" ht="132" x14ac:dyDescent="0.2">
+      <c r="B17" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="C17" ph="1"/>
+      <c r="D17" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="66" x14ac:dyDescent="0.2">
-      <c r="B18" s="1" t="s">
+    <row r="19" spans="2:4" ht="66" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D19" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D21" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="1" t="s">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="B23" s="6"/>
-      <c r="C23" ph="1"/>
-      <c r="D23" ph="1"/>
-    </row>
     <row r="24" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="B24" s="6"/>
       <c r="C24" ph="1"/>
       <c r="D24" ph="1"/>
     </row>
@@ -9670,10 +9659,10 @@
     </row>
     <row r="27" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="C27" ph="1"/>
+      <c r="D27" ph="1"/>
     </row>
     <row r="28" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="C28" ph="1"/>
-      <c r="D28" ph="1"/>
     </row>
     <row r="29" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="C29" ph="1"/>
@@ -9681,15 +9670,19 @@
     </row>
     <row r="30" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="C30" ph="1"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B34" s="1"/>
+      <c r="D30" ph="1"/>
+    </row>
+    <row r="31" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="C31" ph="1"/>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B37" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
win11ja: update pdf browsing
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\fresta2024\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF3A60B2-6193-44FA-B1D0-E3497787AAC7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA025093-6EC9-4028-9DB2-F780E18317A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,18 +18,17 @@
     <sheet name="ch1" sheetId="3" r:id="rId3"/>
     <sheet name="ch2" sheetId="6" r:id="rId4"/>
     <sheet name="ch3" sheetId="16" r:id="rId5"/>
-    <sheet name="ch4" sheetId="12" r:id="rId6"/>
-    <sheet name="ch5" sheetId="15" r:id="rId7"/>
-    <sheet name="ch6" sheetId="4" r:id="rId8"/>
-    <sheet name="ch7" sheetId="5" r:id="rId9"/>
-    <sheet name="ch8" sheetId="9" r:id="rId10"/>
+    <sheet name="ch4" sheetId="15" r:id="rId6"/>
+    <sheet name="ch5" sheetId="4" r:id="rId7"/>
+    <sheet name="ch6" sheetId="5" r:id="rId8"/>
+    <sheet name="ch7" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="396">
   <si>
     <t>header1</t>
   </si>
@@ -170,39 +169,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">自分のパソコンの基本的なスペックを確認しておきましょう。CPUの型式、OSのビット数、記憶容量など。
-なお、この章は広島大学の学生番号がわかる前に実施することができます。 </t>
-    <rPh sb="56" eb="57">
-      <t>ショウ</t>
-    </rPh>
-    <rPh sb="58" eb="60">
-      <t>ヒロシマ</t>
-    </rPh>
-    <rPh sb="60" eb="62">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="63" eb="65">
-      <t>ガクセイ</t>
-    </rPh>
-    <rPh sb="65" eb="67">
-      <t>バンゴウ</t>
-    </rPh>
-    <rPh sb="71" eb="72">
-      <t>マエ</t>
-    </rPh>
-    <rPh sb="73" eb="75">
-      <t>ジッシ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Google Chrome を使えるようにしましょう。</t>
-    <rPh sb="15" eb="16">
-      <t>ツカ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Microsoft Office を使えるようにしましょう。</t>
     <rPh sb="18" eb="19">
       <t>ツカ</t>
@@ -301,34 +267,6 @@
     </rPh>
     <rPh sb="61" eb="64">
       <t>カイギチュウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>この章はネットワーク環境があれば、学生番号がわからなくても実施できます。自宅のネットワークでも、大学のネットワークでも構いません。</t>
-    <rPh sb="2" eb="3">
-      <t>ショウ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>カンキョウ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>ガクセイ</t>
-    </rPh>
-    <rPh sb="19" eb="21">
-      <t>バンゴウ</t>
-    </rPh>
-    <rPh sb="29" eb="31">
-      <t>ジッシ</t>
-    </rPh>
-    <rPh sb="36" eb="38">
-      <t>ジタク</t>
-    </rPh>
-    <rPh sb="48" eb="50">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="59" eb="60">
-      <t>カマ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -2257,121 +2195,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>パソコンのスペック確認 (学生番号が無くても可能です)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>初期設定 (学生番号が無くても可能です)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Google Chromeのインストール (学生番号が無くても可能です)</t>
-    <rPh sb="22" eb="24">
-      <t>ガクセイ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>バンゴウ</t>
-    </rPh>
-    <rPh sb="27" eb="28">
-      <t>ナ</t>
-    </rPh>
-    <rPh sb="31" eb="33">
-      <t>カノウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>まず画面の最下部のタスクバーに「e」を模した青緑のアイコンがありますので、これをクリックしてMicrosoft Edgeを起動します。</t>
-    <rPh sb="2" eb="4">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="5" eb="8">
-      <t>サイカブ</t>
-    </rPh>
-    <rPh sb="19" eb="20">
-      <t>モ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>アオミドリ</t>
-    </rPh>
-    <rPh sb="61" eb="63">
-      <t>キドウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>起動すると他のブラウザの情報を取り込もうとしますが、まだ無いので、チェックを外し、ユーザデータを使用せずに開始をクリックします。</t>
-    <rPh sb="0" eb="2">
-      <t>キドウ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>ホカ</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>ジョウホウ</t>
-    </rPh>
-    <rPh sb="15" eb="16">
-      <t>ト</t>
-    </rPh>
-    <rPh sb="17" eb="18">
-      <t>コ</t>
-    </rPh>
-    <rPh sb="28" eb="29">
-      <t>ナ</t>
-    </rPh>
-    <rPh sb="38" eb="39">
-      <t>ハズ</t>
-    </rPh>
-    <rPh sb="48" eb="50">
-      <t>シヨウ</t>
-    </rPh>
-    <rPh sb="53" eb="55">
-      <t>カイシ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ターゲット広告を行う「Webエクスペリエンスのカスタマイズ」のチェックも外した上で開始します。</t>
-    <rPh sb="5" eb="7">
-      <t>コウコク</t>
-    </rPh>
-    <rPh sb="8" eb="9">
-      <t>オコナ</t>
-    </rPh>
-    <rPh sb="36" eb="37">
-      <t>ハズ</t>
-    </rPh>
-    <rPh sb="39" eb="40">
-      <t>ウエ</t>
-    </rPh>
-    <rPh sb="41" eb="43">
-      <t>カイシ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ブラウザの配色設定をしようとしますが、かまっている時間がないので、上段の「+」ボタンを押して新規のタブを開きます。</t>
-    <rPh sb="5" eb="7">
-      <t>ハイショク</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="25" eb="27">
-      <t>ジカン</t>
-    </rPh>
-    <rPh sb="33" eb="35">
-      <t>ジョウダン</t>
-    </rPh>
-    <rPh sb="43" eb="44">
-      <t>オ</t>
-    </rPh>
-    <rPh sb="46" eb="48">
-      <t>シンキ</t>
-    </rPh>
-    <rPh sb="52" eb="53">
-      <t>ヒラ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -2513,26 +2337,6 @@
     <rPh sb="23" eb="25">
       <t>キドウ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11ja-start-edge-taskbar.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11ja-edge-prep1.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11ja-edge-prep2.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11ja-edge-prep3.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11ja-edge-layout.png</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -3184,34 +2988,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>大学で授業を受ける際に使う、アカウント名が英数字のアカウントを作りましょう</t>
-    <rPh sb="0" eb="2">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ジュギョウ</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>ウ</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>サイ</t>
-    </rPh>
-    <rPh sb="11" eb="12">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="19" eb="20">
-      <t>メイ</t>
-    </rPh>
-    <rPh sb="21" eb="24">
-      <t>エイスウジ</t>
-    </rPh>
-    <rPh sb="31" eb="32">
-      <t>ツク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">Windows11の使用許諾契約が表示されます。
 ここには、みなさんがどういう条件でWindows を利用できるかということが細かく書かれています。内容を確認して「同意」をクリックしてください。
 ※ この内容は、「設定」→「システム」→「バージョン情報」の画面で「マイクロソフトライセンス条項を読む」をクリックすると、いつでも読めます。
@@ -3257,143 +3033,6 @@
     </rPh>
     <rPh sb="28" eb="29">
       <t>カタ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Edgeの規定の新規タブには大量の広告が入ってくるので、オンライン授業などで画面共有の際に憚られるような画面になる場合があります。右上の歯車アイコンを押して、画面レイアウトを「シンプル」にしましょう。これでEdgeの基本的な設定は終わります。
-このwebテキストをスマートフォンなどで見ている方は、これ以降では、様々なwebページにアクセスするため、この初期設定テキストを設定対象のPCの上のEdgeで見ながら作業すると簡単です。</t>
-    <rPh sb="5" eb="7">
-      <t>キテイ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>シンキ</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>タイリョウ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>コウコク</t>
-    </rPh>
-    <rPh sb="20" eb="21">
-      <t>ハイ</t>
-    </rPh>
-    <rPh sb="33" eb="35">
-      <t>ジュギョウ</t>
-    </rPh>
-    <rPh sb="38" eb="40">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="40" eb="42">
-      <t>キョウユウ</t>
-    </rPh>
-    <rPh sb="43" eb="44">
-      <t>サイ</t>
-    </rPh>
-    <rPh sb="45" eb="46">
-      <t>ハバカ</t>
-    </rPh>
-    <rPh sb="52" eb="54">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="57" eb="59">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="65" eb="66">
-      <t>ミギ</t>
-    </rPh>
-    <rPh sb="66" eb="67">
-      <t>ウエ</t>
-    </rPh>
-    <rPh sb="68" eb="70">
-      <t>ハグルマ</t>
-    </rPh>
-    <rPh sb="75" eb="76">
-      <t>オ</t>
-    </rPh>
-    <rPh sb="79" eb="81">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="108" eb="111">
-      <t>キホンテキ</t>
-    </rPh>
-    <rPh sb="112" eb="114">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="115" eb="116">
-      <t>オ</t>
-    </rPh>
-    <rPh sb="142" eb="143">
-      <t>ミ</t>
-    </rPh>
-    <rPh sb="146" eb="147">
-      <t>カタ</t>
-    </rPh>
-    <rPh sb="151" eb="153">
-      <t>イコウ</t>
-    </rPh>
-    <rPh sb="156" eb="158">
-      <t>サマザマ</t>
-    </rPh>
-    <rPh sb="177" eb="179">
-      <t>ショキ</t>
-    </rPh>
-    <rPh sb="179" eb="181">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="186" eb="188">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="188" eb="190">
-      <t>タイショウ</t>
-    </rPh>
-    <rPh sb="194" eb="195">
-      <t>ウエ</t>
-    </rPh>
-    <rPh sb="201" eb="202">
-      <t>ミ</t>
-    </rPh>
-    <rPh sb="205" eb="207">
-      <t>サギョウ</t>
-    </rPh>
-    <rPh sb="210" eb="212">
-      <t>カンタン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>それでは&lt;a href="https://www.google.com/chrome/" target="_blank" rel="noreferrer"&gt;https://www.google.com/chrome/&lt;/a&gt;からGoogle Chromeをダウンロードしましょう。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">ここでは、Microsoft Edgeの初期設定とGoogle Chrome のインストールを行います。Microsoft Edgeの初期設定が終わったら、このwebテキストをMicrosoft Edgeで表示させて作業を進めるのが簡単です。
- </t>
-    <rPh sb="20" eb="22">
-      <t>ショキ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="67" eb="69">
-      <t>ショキ</t>
-    </rPh>
-    <rPh sb="69" eb="71">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="72" eb="73">
-      <t>オ</t>
-    </rPh>
-    <rPh sb="103" eb="105">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="108" eb="110">
-      <t>サギョウ</t>
-    </rPh>
-    <rPh sb="111" eb="112">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="116" eb="118">
-      <t>カンタン</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -4476,21 +4115,6 @@
   </si>
   <si>
     <t>FRESTA-TEXT-2023 Win11 chap.0</t>
-  </si>
-  <si>
-    <t>FRESTA-TEXT-2023 Win11 chap.4</t>
-  </si>
-  <si>
-    <t>FRESTA-TEXT-2023 Windows11 chap.5</t>
-  </si>
-  <si>
-    <t>FRESTA-TEXT-2023 Win11 chap.6</t>
-  </si>
-  <si>
-    <t>FRESTA-TEXT-2023 Win11 chap.7</t>
-  </si>
-  <si>
-    <t>FRESTA-TEXT-2023 Win11 chap.8</t>
   </si>
   <si>
     <t xml:space="preserve">広島大学では、図書館、講義室、福利施設など学内の多くの共用スペースで、「HiNET Wi-Fi」が利用できます。ここでは、HiNET Wi-Fiを通して、あなたのPCで学内ネットワークとインターネットを利用できるようにする方法を説明します。一度設定すると、次回からは（同じ基地局に対しては）設定不要です。 </t>
@@ -5265,22 +4889,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Edgeの初期設定、BitLockerキーの保存、Google Chromeのインストール、無料OneDriveの解除（学生番号が無くても可能です）</t>
-    <rPh sb="60" eb="62">
-      <t>ガクセイ</t>
-    </rPh>
-    <rPh sb="62" eb="64">
-      <t>バンゴウ</t>
-    </rPh>
-    <rPh sb="65" eb="66">
-      <t>ナ</t>
-    </rPh>
-    <rPh sb="69" eb="71">
-      <t>カノウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>FRESTA-TEXT-2023 Win11 chap.1</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -7200,55 +6808,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-bitlockerpdf-edge.png</t>
-  </si>
-  <si>
-    <t>現在のWindowsでは、PDFはEdgeによって閲覧するのが既定の状態です。前の章でデスクトップにBitLocker鍵を保存した場合、ダブルクリックして開くことができます。表示された内容をスマートフォンなどで写真に撮っておきましょう。</t>
-    <rPh sb="0" eb="2">
-      <t>ゲンザイ</t>
-    </rPh>
-    <rPh sb="25" eb="27">
-      <t>エツラン</t>
-    </rPh>
-    <rPh sb="31" eb="33">
-      <t>キテイ</t>
-    </rPh>
-    <rPh sb="34" eb="36">
-      <t>ジョウタイ</t>
-    </rPh>
-    <rPh sb="39" eb="40">
-      <t>マエ</t>
-    </rPh>
-    <rPh sb="41" eb="42">
-      <t>ショウ</t>
-    </rPh>
-    <rPh sb="59" eb="60">
-      <t>カギ</t>
-    </rPh>
-    <rPh sb="61" eb="63">
-      <t>ホゾン</t>
-    </rPh>
-    <rPh sb="65" eb="67">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="77" eb="78">
-      <t>ヒラ</t>
-    </rPh>
-    <rPh sb="87" eb="89">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="92" eb="94">
-      <t>ナイヨウ</t>
-    </rPh>
-    <rPh sb="105" eb="107">
-      <t>シャシン</t>
-    </rPh>
-    <rPh sb="108" eb="109">
-      <t>ト</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>win11ja-search-chrome-result.png</t>
   </si>
   <si>
@@ -7271,61 +6830,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ここからいよいよWebブラウザを使う作業です。以降の作業では「デフォルトで設定されている選択肢をデフォルトでない方を選ぶ」作業が非常に多くなるので、脊髄反射で青やOKの文字があるボタンを押さないよう注意してください。</t>
-    <rPh sb="16" eb="17">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>サギョウ</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>イコウ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>サギョウ</t>
-    </rPh>
-    <rPh sb="37" eb="39">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="44" eb="47">
-      <t>センタクシ</t>
-    </rPh>
-    <rPh sb="56" eb="57">
-      <t>ホウ</t>
-    </rPh>
-    <rPh sb="58" eb="59">
-      <t>エラ</t>
-    </rPh>
-    <rPh sb="61" eb="63">
-      <t>サギョウ</t>
-    </rPh>
-    <rPh sb="64" eb="66">
-      <t>ヒジョウ</t>
-    </rPh>
-    <rPh sb="67" eb="68">
-      <t>オオ</t>
-    </rPh>
-    <rPh sb="74" eb="76">
-      <t>セキズイ</t>
-    </rPh>
-    <rPh sb="76" eb="78">
-      <t>ハンシャ</t>
-    </rPh>
-    <rPh sb="79" eb="80">
-      <t>アオ</t>
-    </rPh>
-    <rPh sb="84" eb="86">
-      <t>モジ</t>
-    </rPh>
-    <rPh sb="93" eb="94">
-      <t>オ</t>
-    </rPh>
-    <rPh sb="99" eb="101">
-      <t>チュウイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>まず、タスクバーにデフォルトでピン止めされているEdge（Microsoft Edge）を起動します。</t>
   </si>
   <si>
@@ -7399,6 +6903,189 @@
     <rPh sb="354" eb="356">
       <t>イカ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Webブラウザを起動してGoogle Chromeをインストールし、印刷したBitLocker鍵の内容を確認しましょう</t>
+    <rPh sb="8" eb="10">
+      <t>キドウ</t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t>インサツ</t>
+    </rPh>
+    <rPh sb="47" eb="48">
+      <t>カギ</t>
+    </rPh>
+    <rPh sb="49" eb="51">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="52" eb="54">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2023 Win11 chap.7</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2023 Win11 chap.6</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2023 Win11 chap.5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2023 Windows11 chap.4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ここからいよいよWebブラウザを使う作業です。以降の作業では「デフォルトで設定されている選択肢をデフォルトでない方を選ぶ」作業が非常に多くなるので、目立つよう着色されたボタンや、「OK」の文字があるボタンを反射的に押さないよう注意してください。</t>
+    <rPh sb="16" eb="17">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>サギョウ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>イコウ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>サギョウ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="44" eb="47">
+      <t>センタクシ</t>
+    </rPh>
+    <rPh sb="56" eb="57">
+      <t>ホウ</t>
+    </rPh>
+    <rPh sb="58" eb="59">
+      <t>エラ</t>
+    </rPh>
+    <rPh sb="61" eb="63">
+      <t>サギョウ</t>
+    </rPh>
+    <rPh sb="64" eb="66">
+      <t>ヒジョウ</t>
+    </rPh>
+    <rPh sb="67" eb="68">
+      <t>オオ</t>
+    </rPh>
+    <rPh sb="74" eb="76">
+      <t>メダ</t>
+    </rPh>
+    <rPh sb="79" eb="81">
+      <t>チャクショク</t>
+    </rPh>
+    <rPh sb="94" eb="96">
+      <t>モジ</t>
+    </rPh>
+    <rPh sb="103" eb="105">
+      <t>ハンシャ</t>
+    </rPh>
+    <rPh sb="105" eb="106">
+      <t>テキ</t>
+    </rPh>
+    <rPh sb="107" eb="108">
+      <t>オ</t>
+    </rPh>
+    <rPh sb="113" eb="115">
+      <t>チュウイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Edgeの初期設定、Google Chromeのインストール、BitLockerキーの保存</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>パソコンのスペック確認、個人MSアカウントのOneDriveリンクの解除 (学生番号が無くても可能です)</t>
+    <rPh sb="12" eb="14">
+      <t>コジン</t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t>カイジョ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">自分のパソコンの基本的なスペックを確認しておきましょう。CPUの型式、OSのビット数、記憶容量など。また、容量が小さい個人MSアカウントのOneDriveリンクも解除しておきます。
+なお、この章は広島大学の学生番号がわかる前に実施することができます。 </t>
+    <rPh sb="53" eb="55">
+      <t>ヨウリョウ</t>
+    </rPh>
+    <rPh sb="56" eb="57">
+      <t>チイ</t>
+    </rPh>
+    <rPh sb="59" eb="61">
+      <t>コジン</t>
+    </rPh>
+    <rPh sb="81" eb="83">
+      <t>カイジョ</t>
+    </rPh>
+    <rPh sb="96" eb="97">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="98" eb="100">
+      <t>ヒロシマ</t>
+    </rPh>
+    <rPh sb="100" eb="102">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="103" eb="105">
+      <t>ガクセイ</t>
+    </rPh>
+    <rPh sb="105" eb="107">
+      <t>バンゴウ</t>
+    </rPh>
+    <rPh sb="111" eb="112">
+      <t>マエ</t>
+    </rPh>
+    <rPh sb="113" eb="115">
+      <t>ジッシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>前の章でデスクトップにBitLocker鍵を保存した場合、ダブルクリックして開くことができます。現在のWindowsでは、PDFはEdgeによって閲覧するのが既定の状態ですが、Google Chromeでも表示できます。</t>
+    <rPh sb="48" eb="50">
+      <t>ゲンザイ</t>
+    </rPh>
+    <rPh sb="73" eb="75">
+      <t>エツラン</t>
+    </rPh>
+    <rPh sb="79" eb="81">
+      <t>キテイ</t>
+    </rPh>
+    <rPh sb="82" eb="84">
+      <t>ジョウタイ</t>
+    </rPh>
+    <rPh sb="103" eb="105">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>表示された内容をスマートフォンなどで写真に撮っておきましょう。</t>
+  </si>
+  <si>
+    <t>「メモ帳」などのアプリも候補に出ていますが、実際に正しく表示できるわけではありません。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-bitlockerpdf-dblclick.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-bitlockerpdf-content.pdf</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-pdf-wrong-app.png</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -7840,7 +7527,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>272</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7856,7 +7543,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>273</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7864,7 +7551,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>274</v>
+        <v>256</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -7878,387 +7565,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392D1BFF-FF5C-4A7E-8C9C-E750AF0FFFAF}">
-  <dimension ref="A1:D46"/>
-  <sheetViews>
-    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="34.21875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
-      <c r="B14" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D16" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D17" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D19" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="96" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D23" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="D24" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B26" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
-      <c r="B28" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B30" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D30" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D31" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D32" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B33" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C33" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C34" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B35" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C35" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B36" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C36" t="s">
-        <v>7</v>
-      </c>
-      <c r="D36" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B37" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C37" t="s">
-        <v>7</v>
-      </c>
-      <c r="D37" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="B38" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C38" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B39" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C39" t="s">
-        <v>7</v>
-      </c>
-      <c r="D39" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" ht="105.6" x14ac:dyDescent="0.2">
-      <c r="B40" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C40" t="s">
-        <v>51</v>
-      </c>
-      <c r="D40" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" ht="79.2" x14ac:dyDescent="0.2">
-      <c r="B41" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C41" t="s">
-        <v>7</v>
-      </c>
-      <c r="D41" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B42" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C42" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B43" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C43" t="s">
-        <v>7</v>
-      </c>
-      <c r="D43" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" ht="66" x14ac:dyDescent="0.2">
-      <c r="B44" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C44" t="s">
-        <v>7</v>
-      </c>
-      <c r="D44" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B45" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C45" t="s">
-        <v>7</v>
-      </c>
-      <c r="D45" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" ht="66" x14ac:dyDescent="0.2">
-      <c r="B46" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C46" t="s">
-        <v>7</v>
-      </c>
-      <c r="D46" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -8290,7 +7603,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -8298,7 +7611,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -8314,7 +7627,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>275</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="304.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -8322,7 +7635,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>314</v>
+        <v>290</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -8336,13 +7649,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C7" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -8350,21 +7663,21 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
@@ -8378,7 +7691,7 @@
         <v>7</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="105.6" ph="1" x14ac:dyDescent="0.2">
@@ -8386,24 +7699,24 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>310</v>
+        <v>287</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
@@ -8411,13 +7724,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
@@ -8425,13 +7738,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -8439,32 +7752,32 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C15" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>330</v>
+        <v>306</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>329</v>
+        <v>305</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>369</v>
+        <v>345</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -8472,238 +7785,238 @@
         <v>4</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>370</v>
+        <v>346</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
-        <v>296</v>
+        <v>273</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>289</v>
+        <v>266</v>
       </c>
       <c r="C25" t="s" ph="1">
-        <v>334</v>
+        <v>310</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>331</v>
+        <v>307</v>
       </c>
     </row>
     <row r="26" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>345</v>
+        <v>321</v>
       </c>
       <c r="C26" t="s" ph="1">
-        <v>334</v>
+        <v>310</v>
       </c>
       <c r="D26" t="s" ph="1">
-        <v>341</v>
+        <v>317</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="C27" t="s" ph="1">
-        <v>334</v>
+        <v>310</v>
       </c>
       <c r="D27" t="s">
-        <v>346</v>
+        <v>322</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>348</v>
+        <v>324</v>
       </c>
       <c r="C28" t="s" ph="1">
-        <v>334</v>
+        <v>310</v>
       </c>
       <c r="D28" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>342</v>
+        <v>318</v>
       </c>
       <c r="C29" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D29" t="s" ph="1">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
       <c r="C30" t="s" ph="1">
-        <v>334</v>
+        <v>310</v>
       </c>
       <c r="D30" t="s" ph="1">
-        <v>344</v>
+        <v>320</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C31" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D31" t="s" ph="1">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C32" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D32" t="s" ph="1">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C33" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D33" t="s" ph="1">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>290</v>
+        <v>267</v>
       </c>
       <c r="D34" t="s" ph="1">
-        <v>332</v>
+        <v>308</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="C35" t="s" ph="1">
-        <v>334</v>
+        <v>310</v>
       </c>
       <c r="D35" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>336</v>
+        <v>312</v>
       </c>
       <c r="D36" t="s" ph="1">
-        <v>293</v>
+        <v>270</v>
       </c>
     </row>
     <row r="37" spans="2:5" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>335</v>
+        <v>311</v>
       </c>
       <c r="C37" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D37" t="s" ph="1">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C38" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D38" t="s" ph="1">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="2:5" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C39" t="s" ph="1">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D39" t="s" ph="1">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="2:5" ph="1" x14ac:dyDescent="0.2">
@@ -8809,8 +8122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8821,20 +8134,20 @@
     <col min="4" max="4" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="52.8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="66" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>125</v>
+        <v>388</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -8850,166 +8163,166 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>312</v>
+        <v>288</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C7" t="s" ph="1">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E7" ph="1"/>
     </row>
     <row r="8" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C8" t="s" ph="1">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:5" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C9" t="s" ph="1">
+        <v>91</v>
+      </c>
+      <c r="D9" t="s" ph="1">
         <v>94</v>
-      </c>
-      <c r="D9" t="s" ph="1">
-        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:5" customFormat="1" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>359</v>
+        <v>335</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>360</v>
+        <v>336</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>361</v>
+        <v>337</v>
       </c>
     </row>
     <row r="12" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>363</v>
+        <v>339</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>362</v>
+        <v>338</v>
       </c>
     </row>
     <row r="13" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>337</v>
+        <v>313</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>338</v>
+        <v>314</v>
       </c>
     </row>
     <row r="14" spans="1:5" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>340</v>
+        <v>316</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>339</v>
+        <v>315</v>
       </c>
     </row>
     <row r="15" spans="1:5" customFormat="1" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>351</v>
+        <v>327</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>350</v>
+        <v>326</v>
       </c>
     </row>
     <row r="16" spans="1:5" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>321</v>
+        <v>297</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>324</v>
+        <v>300</v>
       </c>
     </row>
     <row r="17" spans="1:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="D17" t="s">
         <v>328</v>
-      </c>
-      <c r="D17" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="18" spans="1:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B18" s="6" t="s">
-        <v>354</v>
+        <v>330</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>353</v>
+        <v>329</v>
       </c>
     </row>
     <row r="19" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>355</v>
+        <v>331</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>364</v>
+        <v>340</v>
       </c>
     </row>
     <row r="20" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>356</v>
+        <v>332</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>357</v>
+        <v>333</v>
       </c>
     </row>
     <row r="21" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>327</v>
+        <v>303</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>358</v>
+        <v>334</v>
       </c>
     </row>
     <row r="22" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>322</v>
+        <v>298</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>326</v>
+        <v>302</v>
       </c>
     </row>
     <row r="23" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>367</v>
+        <v>343</v>
       </c>
     </row>
     <row r="24" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>365</v>
+        <v>341</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>324</v>
+        <v>300</v>
       </c>
     </row>
     <row r="25" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>372</v>
+        <v>348</v>
       </c>
     </row>
     <row r="26" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -9022,7 +8335,7 @@
         <v>8</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>323</v>
+        <v>299</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -9036,37 +8349,37 @@
         <v>4</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D29" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D30" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D31" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9074,13 +8387,13 @@
         <v>4</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="2:2" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -9106,7 +8419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+    <sheetView zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
@@ -9123,7 +8436,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -9131,7 +8444,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>266</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9147,7 +8460,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>313</v>
+        <v>289</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -9155,7 +8468,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>265</v>
+        <v>247</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -9174,29 +8487,29 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>373</v>
+        <v>349</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>374</v>
+        <v>350</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>379</v>
+        <v>355</v>
       </c>
       <c r="D11" t="s">
-        <v>375</v>
+        <v>351</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>376</v>
+        <v>352</v>
       </c>
       <c r="D12" t="s">
-        <v>377</v>
+        <v>353</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -9204,13 +8517,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>380</v>
+        <v>356</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>378</v>
+        <v>354</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -9218,7 +8531,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -9229,7 +8542,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -9240,21 +8553,21 @@
         <v>4</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D19" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -9262,13 +8575,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9276,13 +8589,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>282</v>
+        <v>259</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9290,13 +8603,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>294</v>
+        <v>271</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -9309,149 +8622,149 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="82.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>269</v>
+        <v>251</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>384</v>
+        <v>360</v>
       </c>
       <c r="D27" t="s">
-        <v>381</v>
+        <v>357</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>385</v>
+        <v>361</v>
       </c>
       <c r="D28" t="s">
-        <v>382</v>
+        <v>358</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>388</v>
+        <v>364</v>
       </c>
       <c r="D29" t="s">
-        <v>386</v>
+        <v>362</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="67.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>387</v>
+        <v>363</v>
       </c>
       <c r="D30" t="s">
-        <v>383</v>
+        <v>359</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>389</v>
+        <v>365</v>
       </c>
       <c r="D31" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>304</v>
+        <v>281</v>
       </c>
       <c r="D33" t="s">
-        <v>301</v>
+        <v>278</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>302</v>
+        <v>279</v>
       </c>
       <c r="D34" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>305</v>
+        <v>282</v>
       </c>
       <c r="D35" t="s">
-        <v>306</v>
+        <v>283</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>309</v>
+        <v>286</v>
       </c>
       <c r="D36" t="s">
-        <v>307</v>
+        <v>284</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="50.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>308</v>
+        <v>285</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
       <c r="D38" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
-        <v>291</v>
+        <v>268</v>
       </c>
       <c r="D39" t="s">
-        <v>292</v>
+        <v>269</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="6" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
       <c r="D40" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="6" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
       <c r="D41" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="46.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="6" t="s">
-        <v>315</v>
+        <v>291</v>
       </c>
       <c r="D42" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="131.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="6" t="s">
-        <v>316</v>
+        <v>292</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" s="6" t="s">
-        <v>264</v>
+        <v>246</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="6" t="s">
-        <v>390</v>
+        <v>366</v>
       </c>
       <c r="D47" t="s">
-        <v>386</v>
+        <v>362</v>
       </c>
     </row>
     <row r="48" spans="2:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9464,10 +8777,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4600B07F-730C-4FC5-BA07-70D58F12A670}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -9483,15 +8796,15 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s" ph="1">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>311</v>
+        <v>387</v>
       </c>
     </row>
     <row r="3" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -9507,7 +8820,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>317</v>
+        <v>293</v>
       </c>
     </row>
     <row r="5" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -9515,153 +8828,161 @@
     </row>
     <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>405</v>
+        <v>386</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>406</v>
+        <v>379</v>
       </c>
       <c r="D7" t="s">
-        <v>395</v>
+        <v>371</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>399</v>
+        <v>375</v>
       </c>
       <c r="D8" t="s">
-        <v>391</v>
+        <v>367</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>318</v>
+        <v>294</v>
       </c>
       <c r="D9" t="s">
-        <v>392</v>
+        <v>368</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>396</v>
+        <v>372</v>
       </c>
       <c r="D10" t="s">
-        <v>393</v>
+        <v>369</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>319</v>
+        <v>295</v>
       </c>
       <c r="D11" t="s">
-        <v>394</v>
+        <v>370</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>397</v>
+        <v>373</v>
       </c>
       <c r="D12" t="s">
-        <v>398</v>
+        <v>374</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B13" s="6"/>
       <c r="C13" ph="1"/>
     </row>
-    <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>401</v>
+        <v>378</v>
       </c>
       <c r="C14" ph="1"/>
       <c r="D14" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="B15" s="6"/>
+        <v>377</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="132" x14ac:dyDescent="0.2">
+      <c r="B15" s="6" t="s">
+        <v>380</v>
+      </c>
       <c r="C15" ph="1"/>
-      <c r="D15" ph="1"/>
+      <c r="D15" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B16" s="6" t="s">
-        <v>404</v>
-      </c>
-      <c r="C16" ph="1"/>
+      <c r="B16" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="D16" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="132" x14ac:dyDescent="0.2">
-      <c r="B17" s="6" t="s">
-        <v>407</v>
-      </c>
-      <c r="C17" ph="1"/>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="66" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>124</v>
+      </c>
       <c r="D17" t="s">
-        <v>402</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D19" t="s">
         <v>132</v>
-      </c>
-      <c r="D18" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="66" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D19" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D20" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D21" t="s">
         <v>134</v>
       </c>
-      <c r="D20" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D21" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B22" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D22" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="1" t="s">
-        <v>137</v>
-      </c>
+    </row>
+    <row r="22" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="B22" s="6"/>
+      <c r="C22" ph="1"/>
+      <c r="D22" ph="1"/>
+    </row>
+    <row r="23" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B23" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="C23" ph="1"/>
       <c r="D23" t="s">
-        <v>148</v>
+        <v>393</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="B24" s="6"/>
+      <c r="B24" t="s">
+        <v>391</v>
+      </c>
       <c r="C24" ph="1"/>
-      <c r="D24" ph="1"/>
+      <c r="D24" t="s" ph="1">
+        <v>394</v>
+      </c>
     </row>
     <row r="25" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>392</v>
+      </c>
       <c r="C25" ph="1"/>
-      <c r="D25" ph="1"/>
+      <c r="D25" t="s" ph="1">
+        <v>395</v>
+      </c>
     </row>
     <row r="26" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="C26" ph="1"/>
-      <c r="D26" ph="1"/>
     </row>
     <row r="27" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="C27" ph="1"/>
@@ -9669,26 +8990,19 @@
     </row>
     <row r="28" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="C28" ph="1"/>
+      <c r="D28" ph="1"/>
     </row>
     <row r="29" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="C29" ph="1"/>
-      <c r="D29" ph="1"/>
-    </row>
-    <row r="30" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="C30" ph="1"/>
-      <c r="D30" ph="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="C31" ph="1"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B34" s="1"/>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B36" s="1"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B37" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -9698,189 +9012,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C43F54BA-B356-43A4-B76F-707ED0C70724}">
-  <dimension ref="A1:D21"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="82.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="30.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D10" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D11" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D12" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D13" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="66" x14ac:dyDescent="0.2">
-      <c r="B14" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D14" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D16" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="B17" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D17" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B18" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D19" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D20" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D21" t="s">
-        <v>148</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D6E33FB-2290-439B-854D-9A45A4600EF5}">
   <dimension ref="A1:D87"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:XFD44"/>
+    <sheetView zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -9896,7 +9032,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -9904,7 +9040,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9920,7 +9056,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>277</v>
+        <v>385</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -9931,7 +9067,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>268</v>
+        <v>250</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -9950,7 +9086,7 @@
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -9963,7 +9099,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -9974,18 +9110,18 @@
     </row>
     <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9993,7 +9129,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -10001,18 +9137,18 @@
     </row>
     <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="D15" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="D16" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -10020,13 +9156,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="198" x14ac:dyDescent="0.2">
@@ -10034,18 +9170,18 @@
         <v>4</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>283</v>
+        <v>260</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -10053,21 +9189,21 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>236</v>
+        <v>218</v>
       </c>
       <c r="D21" t="s">
-        <v>237</v>
+        <v>219</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -10075,21 +9211,21 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>284</v>
+        <v>261</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>238</v>
+        <v>220</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
       <c r="D23" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -10097,13 +9233,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>285</v>
+        <v>262</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -10111,7 +9247,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>249</v>
+        <v>231</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -10127,40 +9263,40 @@
     </row>
     <row r="28" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="D29" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="D30" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>286</v>
+        <v>263</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -10168,7 +9304,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -10187,80 +9323,80 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="D36" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="D37" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="D39" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="D40" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>287</v>
+        <v>264</v>
       </c>
       <c r="D41" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="C42" t="s">
         <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>299</v>
+        <v>276</v>
       </c>
       <c r="C43" t="s">
         <v>4</v>
       </c>
       <c r="D43" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -10268,7 +9404,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -10276,7 +9412,7 @@
     </row>
     <row r="47" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="C47" t="s">
         <v>4</v>
@@ -10287,7 +9423,7 @@
     </row>
     <row r="48" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
-        <v>300</v>
+        <v>277</v>
       </c>
       <c r="C48" t="s">
         <v>7</v>
@@ -10315,7 +9451,7 @@
     </row>
     <row r="51" spans="2:4" ht="132" x14ac:dyDescent="0.2">
       <c r="B51" s="1" t="s">
-        <v>271</v>
+        <v>253</v>
       </c>
       <c r="C51" t="s">
         <v>7</v>
@@ -10361,12 +9497,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -10382,7 +9518,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -10390,7 +9526,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -10406,7 +9542,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>278</v>
+        <v>384</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -10414,7 +9550,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>297</v>
+        <v>274</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -10430,7 +9566,7 @@
     </row>
     <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -10438,18 +9574,18 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>298</v>
+        <v>275</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -10457,21 +9593,21 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="D15" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -10479,13 +9615,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -10493,13 +9629,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -10507,13 +9643,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>368</v>
+        <v>344</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -10529,11 +9665,11 @@
         <v>4</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="C20" s="4" ph="1"/>
       <c r="D20" s="4" t="s" ph="1">
-        <v>325</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -10543,12 +9679,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -10564,7 +9700,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -10572,7 +9708,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -10588,22 +9724,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>279</v>
+        <v>383</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -10611,7 +9747,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>281</v>
+        <v>258</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -10636,13 +9772,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>288</v>
+        <v>265</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -10650,21 +9786,21 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>295</v>
+        <v>272</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D13" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -10672,12 +9808,12 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -10685,33 +9821,407 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="D18" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="D19" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>215</v>
+        <v>197</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392D1BFF-FF5C-4A7E-8C9C-E750AF0FFFAF}">
+  <dimension ref="A1:D46"/>
+  <sheetViews>
+    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="34.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D16" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D17" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D19" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D23" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D24" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D30" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D31" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D32" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B38" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B39" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" ht="105.6" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" ht="79.2" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B43" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" ht="66" x14ac:dyDescent="0.2">
+      <c r="B44" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B45" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" ht="66" x14ac:dyDescent="0.2">
+      <c r="B46" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
win11ja: fix incorrect suffix
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\fresta2024\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA025093-6EC9-4028-9DB2-F780E18317A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A122C8-311A-4075-9960-B9E9E342450C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7081,11 +7081,11 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-bitlockerpdf-content.pdf</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>win11ja-pdf-wrong-app.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-bitlockerpdf-content.png</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -8780,7 +8780,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8969,7 +8969,7 @@
       </c>
       <c r="C24" ph="1"/>
       <c r="D24" t="s" ph="1">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -8978,7 +8978,7 @@
       </c>
       <c r="C25" ph="1"/>
       <c r="D25" t="s" ph="1">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
win11ja: introduce sections in ch3
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\fresta2024\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A122C8-311A-4075-9960-B9E9E342450C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41778B20-AA42-46D7-9514-3B9A935DC4D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="399">
   <si>
     <t>header1</t>
   </si>
@@ -6941,64 +6941,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ここからいよいよWebブラウザを使う作業です。以降の作業では「デフォルトで設定されている選択肢をデフォルトでない方を選ぶ」作業が非常に多くなるので、目立つよう着色されたボタンや、「OK」の文字があるボタンを反射的に押さないよう注意してください。</t>
-    <rPh sb="16" eb="17">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>サギョウ</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>イコウ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>サギョウ</t>
-    </rPh>
-    <rPh sb="37" eb="39">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="44" eb="47">
-      <t>センタクシ</t>
-    </rPh>
-    <rPh sb="56" eb="57">
-      <t>ホウ</t>
-    </rPh>
-    <rPh sb="58" eb="59">
-      <t>エラ</t>
-    </rPh>
-    <rPh sb="61" eb="63">
-      <t>サギョウ</t>
-    </rPh>
-    <rPh sb="64" eb="66">
-      <t>ヒジョウ</t>
-    </rPh>
-    <rPh sb="67" eb="68">
-      <t>オオ</t>
-    </rPh>
-    <rPh sb="74" eb="76">
-      <t>メダ</t>
-    </rPh>
-    <rPh sb="79" eb="81">
-      <t>チャクショク</t>
-    </rPh>
-    <rPh sb="94" eb="96">
-      <t>モジ</t>
-    </rPh>
-    <rPh sb="103" eb="105">
-      <t>ハンシャ</t>
-    </rPh>
-    <rPh sb="105" eb="106">
-      <t>テキ</t>
-    </rPh>
-    <rPh sb="107" eb="108">
-      <t>オ</t>
-    </rPh>
-    <rPh sb="113" eb="115">
-      <t>チュウイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Edgeの初期設定、Google Chromeのインストール、BitLockerキーの保存</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -7086,6 +7028,99 @@
   </si>
   <si>
     <t>win11ja-bitlockerpdf-content.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ここからいよいよWebブラウザを使う作業です。以降の作業では「デフォルトで設定されている選択肢をデフォルトでない方を選ぶ」作業が非常に多くなるので、目立つよう着色されたボタンや、「OK」の文字があるボタンを反射的に押さないよう注意してください。
+&lt;ul&gt;
+&lt;li&gt;&lt;a href="#edge_first_run"&gt;Microsoft Edgeの起動&lt;/a&gt;&lt;/li&gt;
+&lt;li&gt;&lt;a href="#install_chrome"&gt;Google Chromeのインストール&lt;/a&gt;&lt;/li&gt;
+&lt;li&gt;&lt;a href="#display_pdf"&gt;BitLocker鍵の表示&lt;/a&gt;&lt;/li&gt;
+&lt;/ul&gt;</t>
+    <rPh sb="16" eb="17">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>サギョウ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>イコウ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>サギョウ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="44" eb="47">
+      <t>センタクシ</t>
+    </rPh>
+    <rPh sb="56" eb="57">
+      <t>ホウ</t>
+    </rPh>
+    <rPh sb="58" eb="59">
+      <t>エラ</t>
+    </rPh>
+    <rPh sb="61" eb="63">
+      <t>サギョウ</t>
+    </rPh>
+    <rPh sb="64" eb="66">
+      <t>ヒジョウ</t>
+    </rPh>
+    <rPh sb="67" eb="68">
+      <t>オオ</t>
+    </rPh>
+    <rPh sb="74" eb="76">
+      <t>メダ</t>
+    </rPh>
+    <rPh sb="79" eb="81">
+      <t>チャクショク</t>
+    </rPh>
+    <rPh sb="94" eb="96">
+      <t>モジ</t>
+    </rPh>
+    <rPh sb="103" eb="105">
+      <t>ハンシャ</t>
+    </rPh>
+    <rPh sb="105" eb="106">
+      <t>テキ</t>
+    </rPh>
+    <rPh sb="107" eb="108">
+      <t>オ</t>
+    </rPh>
+    <rPh sb="113" eb="115">
+      <t>チュウイ</t>
+    </rPh>
+    <rPh sb="173" eb="175">
+      <t>キドウ</t>
+    </rPh>
+    <rPh sb="283" eb="285">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2 name="edge_first_run"&gt;Microsoft Edgeの起動&lt;/h2&gt;</t>
+    <rPh sb="37" eb="39">
+      <t>キドウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2 name="install_chrome"&gt;Google Chromeのインストール&lt;/h2&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2 name="display_pdf"&gt;保存したBitLocker鍵PDFの表示&lt;/h2&gt;</t>
+    <rPh sb="23" eb="25">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>カギ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>ヒョウジ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -8139,7 +8174,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
@@ -8147,7 +8182,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -8420,7 +8455,7 @@
   <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8777,10 +8812,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4600B07F-730C-4FC5-BA07-70D58F12A670}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8804,7 +8839,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="3" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -8826,183 +8861,213 @@
     <row r="5" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B5" s="6"/>
     </row>
-    <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B7" s="6" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="6" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="6"/>
+    </row>
+    <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B10" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D10" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
-      <c r="B8" s="6" t="s">
+    <row r="11" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+      <c r="B11" s="6" t="s">
         <v>375</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D11" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B9" s="6" t="s">
+    <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B12" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D12" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="B10" s="6" t="s">
+    <row r="13" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B13" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D13" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B11" s="6" t="s">
-        <v>295</v>
-      </c>
-      <c r="D11" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B12" s="6" t="s">
-        <v>373</v>
-      </c>
-      <c r="D12" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="B13" s="6"/>
-      <c r="C13" ph="1"/>
     </row>
     <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="D14" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B15" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="D15" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="6"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="6" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="B18" s="6"/>
+      <c r="C18" ph="1"/>
+    </row>
+    <row r="19" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B19" s="6" t="s">
         <v>378</v>
       </c>
-      <c r="C14" ph="1"/>
-      <c r="D14" t="s">
+      <c r="C19" ph="1"/>
+      <c r="D19" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="132" x14ac:dyDescent="0.2">
-      <c r="B15" s="6" t="s">
+    <row r="20" spans="2:4" ht="132" x14ac:dyDescent="0.2">
+      <c r="B20" s="6" t="s">
         <v>380</v>
       </c>
-      <c r="C15" ph="1"/>
-      <c r="D15" t="s">
+      <c r="C20" ph="1"/>
+      <c r="D20" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B16" s="1" t="s">
+    <row r="21" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D21" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="66" x14ac:dyDescent="0.2">
-      <c r="B17" s="1" t="s">
+    <row r="22" spans="2:4" ht="66" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D22" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B18" s="1" t="s">
+    <row r="23" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D23" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
+    <row r="24" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D24" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s">
+    <row r="25" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D25" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D26" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="B22" s="6"/>
-      <c r="C22" ph="1"/>
-      <c r="D22" ph="1"/>
-    </row>
-    <row r="23" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B23" s="6" t="s">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="6"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B28" s="6" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="B29" s="6"/>
+      <c r="C29" ph="1"/>
+    </row>
+    <row r="30" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B30" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="C30" ph="1"/>
+      <c r="D30" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
         <v>390</v>
       </c>
-      <c r="C23" ph="1"/>
-      <c r="D23" t="s">
+      <c r="C31" ph="1"/>
+      <c r="D31" t="s" ph="1">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>391</v>
+      </c>
+      <c r="C32" ph="1"/>
+      <c r="D32" t="s" ph="1">
         <v>393</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>391</v>
-      </c>
-      <c r="C24" ph="1"/>
-      <c r="D24" t="s" ph="1">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
-        <v>392</v>
-      </c>
-      <c r="C25" ph="1"/>
-      <c r="D25" t="s" ph="1">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="C26" ph="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="C27" ph="1"/>
-      <c r="D27" ph="1"/>
-    </row>
-    <row r="28" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="C28" ph="1"/>
-      <c r="D28" ph="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="C29" ph="1"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B33" s="1"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B34" s="1"/>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B35" s="1"/>
+    <row r="33" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="C33" ph="1"/>
+    </row>
+    <row r="34" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="C34" ph="1"/>
+      <c r="D34" ph="1"/>
+    </row>
+    <row r="35" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="C35" ph="1"/>
+      <c r="D35" ph="1"/>
+    </row>
+    <row r="36" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="C36" ph="1"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B40" s="1"/>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="C43" ph="1"/>
+      <c r="D43" ph="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
win11ja: remove OneDrive mention from ch4
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\fresta2024\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41778B20-AA42-46D7-9514-3B9A935DC4D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26EBE25A-4EC5-4CE3-8E5B-7905B7A438C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="397">
   <si>
     <t>header1</t>
   </si>
@@ -72,18 +72,7 @@
     <t>win10-6-01.svg</t>
   </si>
   <si>
-    <t>win10-6-25.svg</t>
-  </si>
-  <si>
     <t>win10-6-26.svg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">次に、OneDriveについて。一般に広く使われているGoogleDriveやDropBoxと同様に、PC用のアプリがあります。これを入れておくと、PC上の特定のフォルダとOneDriveの内容が自動的に同期されるようになります。スマホのアプリにもOneDriveがありますが、これは自動的に同期はしません。全部を同期するとスマホの容量を圧迫するからでしょう。
-OneDriveのアプリは、Web版のOneDrive サイトから入手できます。
-詳細はメディアセンターWebサイトの&lt;a href="https://www.media.hiroshima-u.ac.jp/services/onedriveforbusiness/"&gt;「クラウドファイル保管サービス(OneDrive for Business)」&lt;/a&gt;
-で。
-  </t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t xml:space="preserve">キーボードレイアウトの追加についての質問に答えます。追加のレイアウトはないので、「スキップ」としましょう。
@@ -7562,7 +7551,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7578,7 +7567,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7586,7 +7575,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -7600,7 +7589,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7638,7 +7627,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -7646,7 +7635,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -7662,7 +7651,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="304.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -7670,7 +7659,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -7684,13 +7673,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C7" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -7698,21 +7687,21 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
@@ -7720,13 +7709,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="105.6" ph="1" x14ac:dyDescent="0.2">
@@ -7734,24 +7723,24 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
@@ -7759,13 +7748,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
@@ -7773,13 +7762,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C14" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -7787,32 +7776,32 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -7820,238 +7809,238 @@
         <v>4</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C25" t="s" ph="1">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="26" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C26" t="s" ph="1">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D26" t="s" ph="1">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C27" t="s" ph="1">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D27" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C28" t="s" ph="1">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D28" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C29" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D29" t="s" ph="1">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C30" t="s" ph="1">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D30" t="s" ph="1">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C31" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D31" t="s" ph="1">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C32" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D32" t="s" ph="1">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C33" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D33" t="s" ph="1">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D34" t="s" ph="1">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C35" t="s" ph="1">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D35" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D36" t="s" ph="1">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="37" spans="2:5" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C37" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D37" t="s" ph="1">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C38" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D38" t="s" ph="1">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="2:5" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C39" t="s" ph="1">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D39" t="s" ph="1">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="2:5" ph="1" x14ac:dyDescent="0.2">
@@ -8174,7 +8163,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
@@ -8182,7 +8171,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -8198,166 +8187,166 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C7" t="s" ph="1">
+        <v>89</v>
+      </c>
+      <c r="D7" t="s" ph="1">
         <v>91</v>
-      </c>
-      <c r="D7" t="s" ph="1">
-        <v>93</v>
       </c>
       <c r="E7" ph="1"/>
     </row>
     <row r="8" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C8" t="s" ph="1">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:5" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C9" t="s" ph="1">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:5" customFormat="1" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="12" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="13" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="14" spans="1:5" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="15" spans="1:5" customFormat="1" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="16" spans="1:5" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="17" spans="1:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D17" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="18" spans="1:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B18" s="6" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="19" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="20" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="21" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="22" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="23" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="24" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="25" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="26" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -8370,7 +8359,7 @@
         <v>8</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -8384,37 +8373,37 @@
         <v>4</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D29" t="s">
         <v>108</v>
-      </c>
-      <c r="D29" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D30" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D31" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8422,13 +8411,13 @@
         <v>4</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="2:2" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -8471,7 +8460,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8479,7 +8468,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8495,7 +8484,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -8503,7 +8492,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8522,29 +8511,29 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D11" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D12" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -8552,13 +8541,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -8566,7 +8555,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -8577,7 +8566,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -8588,21 +8577,21 @@
         <v>4</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -8610,13 +8599,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8624,13 +8613,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8638,13 +8627,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -8657,149 +8646,149 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="82.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D27" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D28" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D29" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="67.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D30" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D31" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D33" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D34" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D35" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D36" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="50.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D38" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D39" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D40" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D41" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="46.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="6" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D42" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="131.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="6" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" s="6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D47" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="48" spans="2:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8814,7 +8803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4600B07F-730C-4FC5-BA07-70D58F12A670}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
@@ -8831,7 +8820,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="2" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -8839,7 +8828,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="3" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -8855,7 +8844,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="5" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -8863,7 +8852,7 @@
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -8871,7 +8860,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -8879,50 +8868,50 @@
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D10" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D11" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D12" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D13" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D14" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D15" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -8930,7 +8919,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -8939,68 +8928,68 @@
     </row>
     <row r="19" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C19" ph="1"/>
       <c r="D19" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="132" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C20" ph="1"/>
       <c r="D20" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D21" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D22" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D23" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D24" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D25" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
@@ -9008,7 +8997,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -9017,29 +9006,29 @@
     </row>
     <row r="30" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C30" ph="1"/>
       <c r="D30" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C31" ph="1"/>
       <c r="D31" t="s" ph="1">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C32" ph="1"/>
       <c r="D32" t="s" ph="1">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -9080,8 +9069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D6E33FB-2290-439B-854D-9A45A4600EF5}">
   <dimension ref="A1:D87"/>
   <sheetViews>
-    <sheetView zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:XFD49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -9097,7 +9086,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -9105,7 +9094,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9121,7 +9110,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -9132,7 +9121,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -9151,7 +9140,7 @@
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -9164,7 +9153,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -9175,18 +9164,18 @@
     </row>
     <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9194,7 +9183,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -9202,18 +9191,18 @@
     </row>
     <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D16" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -9221,13 +9210,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="198" x14ac:dyDescent="0.2">
@@ -9235,18 +9224,18 @@
         <v>4</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9254,21 +9243,21 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D21" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9276,21 +9265,21 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D23" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9298,13 +9287,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -9312,7 +9301,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -9328,40 +9317,40 @@
     </row>
     <row r="28" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D29" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D30" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -9369,7 +9358,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -9388,80 +9377,80 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D36" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D39" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D40" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D41" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C42" t="s">
         <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C43" t="s">
         <v>4</v>
       </c>
       <c r="D43" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -9469,7 +9458,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -9477,7 +9466,7 @@
     </row>
     <row r="47" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C47" t="s">
         <v>4</v>
@@ -9488,71 +9477,63 @@
     </row>
     <row r="48" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C48" t="s">
         <v>7</v>
       </c>
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="2:4" ht="105.6" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B49" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D49" t="s" ph="1">
         <v>16</v>
       </c>
-      <c r="C49" t="s">
+    </row>
+    <row r="50" spans="2:4" ht="132" x14ac:dyDescent="0.2">
+      <c r="B50" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C50" t="s">
         <v>7</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D50" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="2:4" ht="92.4" x14ac:dyDescent="0.2">
-      <c r="B50" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D50" t="s" ph="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" ht="132" x14ac:dyDescent="0.2">
-      <c r="B51" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="C51" t="s">
-        <v>7</v>
-      </c>
-      <c r="D51" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="D52" ph="1"/>
-    </row>
-    <row r="63" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="D63" ph="1"/>
-    </row>
-    <row r="65" spans="4:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="D65" ph="1"/>
-    </row>
-    <row r="69" spans="4:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="D69" ph="1"/>
-    </row>
-    <row r="73" spans="4:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="D73" ph="1"/>
-    </row>
-    <row r="77" spans="4:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="D77" ph="1"/>
-    </row>
-    <row r="79" spans="4:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="D79" ph="1"/>
-    </row>
-    <row r="81" spans="4:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="D81" ph="1"/>
-    </row>
-    <row r="85" spans="4:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="D85" ph="1"/>
-    </row>
-    <row r="87" spans="4:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="D51" ph="1"/>
+    </row>
+    <row r="62" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="D62" ph="1"/>
+    </row>
+    <row r="64" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="D64" ph="1"/>
+    </row>
+    <row r="68" spans="4:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="D68" ph="1"/>
+    </row>
+    <row r="72" spans="4:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="D72" ph="1"/>
+    </row>
+    <row r="76" spans="4:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="D76" ph="1"/>
+    </row>
+    <row r="78" spans="4:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="D78" ph="1"/>
+    </row>
+    <row r="80" spans="4:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="D80" ph="1"/>
+    </row>
+    <row r="84" spans="4:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="D84" ph="1"/>
+    </row>
+    <row r="86" spans="4:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="D86" ph="1"/>
+    </row>
+    <row r="87" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D87" ph="1"/>
     </row>
   </sheetData>
@@ -9583,7 +9564,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -9591,7 +9572,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9607,7 +9588,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -9615,7 +9596,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -9631,7 +9612,7 @@
     </row>
     <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -9639,18 +9620,18 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -9658,21 +9639,21 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D15" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -9680,13 +9661,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9694,13 +9675,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -9708,13 +9689,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -9730,11 +9711,11 @@
         <v>4</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C20" s="4" ph="1"/>
       <c r="D20" s="4" t="s" ph="1">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -9765,7 +9746,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -9773,7 +9754,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9789,22 +9770,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9812,7 +9793,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -9823,7 +9804,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -9837,13 +9818,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9851,21 +9832,21 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -9873,12 +9854,12 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9886,33 +9867,33 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D18" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D19" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -9943,7 +9924,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -9951,7 +9932,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9967,22 +9948,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9990,7 +9971,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -10006,15 +9987,15 @@
     </row>
     <row r="14" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.2">
@@ -10022,10 +10003,10 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D16" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -10033,39 +10014,39 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D19" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -10073,36 +10054,36 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D23" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D24" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -10113,180 +10094,180 @@
     </row>
     <row r="30" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D30" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D31" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D32" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C34" t="s">
         <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C35" t="s">
         <v>7</v>
       </c>
       <c r="D35" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C36" t="s">
         <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C37" t="s">
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C38" t="s">
         <v>7</v>
       </c>
       <c r="D38" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C39" t="s">
         <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C40" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D40" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C41" t="s">
         <v>7</v>
       </c>
       <c r="D41" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C42" t="s">
         <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C43" t="s">
         <v>7</v>
       </c>
       <c r="D43" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C44" t="s">
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C45" t="s">
         <v>7</v>
       </c>
       <c r="D45" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="2:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C46" t="s">
         <v>7</v>
       </c>
       <c r="D46" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
win11ja: limit OneDrive instr to version 2023
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\fresta2024\fresta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26EBE25A-4EC5-4CE3-8E5B-7905B7A438C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C89965F9-F24E-4EBE-AB90-BBDC2053341E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="423">
   <si>
     <t>header1</t>
   </si>
@@ -279,16 +279,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>&lt;h2&gt;&lt;a name="office"&gt;&lt;/a&gt;Microsoft Officeを入れる&lt;/h2&gt;</t>
-    <rPh sb="42" eb="43">
-      <t>ナ</t>
-    </rPh>
-    <rPh sb="46" eb="48">
-      <t>バアイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">広島大学では、マイクロソフト社との包括ライセンス契約（Microsoft Enrollment for Education Solutions）を結んでいます。これによって広島大学の学生は広島大学が定める利用要領に基づいて、いくつかのマイクロソフト社製ソフトウェア製品（Microsoft Office等）を無償で利用することができます。
 Microsoft Office については、広島大学の学生は個人所有のPCで５台まで無償で利用することができます。
 &lt;strong&gt;ただし卒業後は利用できなくなりますので、ご注意ください。&lt;/strong&gt;
@@ -2443,19 +2433,6 @@
     </rPh>
     <rPh sb="80" eb="82">
       <t>カクニン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Microsoft Officeのサインイン (学生番号が必要です)</t>
-    <rPh sb="24" eb="26">
-      <t>ガクセイ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>バンゴウ</t>
-    </rPh>
-    <rPh sb="29" eb="31">
-      <t>ヒツヨウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -4603,14 +4580,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">Microsoft Officeにサインインします。
-&lt;ul&gt;
-&lt;li&gt;&lt;a href="#office"&gt;Microsoft Officeのサインイン&lt;/a&gt;&lt;/li&gt;
-&lt;/ul&gt;
- </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>win10-4-01.png</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -5201,25 +5170,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>「設定」から「アカウント」に進むと、右ペインにアカウント名、リワードと並んで「OneDrive」というアイコンがあります。</t>
-    <rPh sb="1" eb="3">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="14" eb="15">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="18" eb="19">
-      <t>ミギ</t>
-    </rPh>
-    <rPh sb="28" eb="29">
-      <t>メイ</t>
-    </rPh>
-    <rPh sb="35" eb="36">
-      <t>ナラ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>次に、お使いのアカウントが5GBまでしか保存できない無料のOneDriveサービスにリンクされていないことを確認しましょう。もしリンクされている場合は解除します。なぜなら無料のOneDriveは5GBしか格納できないので、一瞬で使い切るからです。</t>
     <rPh sb="0" eb="1">
       <t>ツギ</t>
@@ -5693,116 +5643,6 @@
   </si>
   <si>
     <t>win11ja-onedrive-app.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>雲アイコンを右クリックしてOneDriveアプリのウィンドウを開き、歯車アイコン(①)をクリックして「設定」メニュー(②)に進みましょう。「お使いのPCのアップデート状況により、アプリの画面が微妙に異なります。</t>
-    <rPh sb="0" eb="1">
-      <t>クモ</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>ミギ</t>
-    </rPh>
-    <rPh sb="31" eb="32">
-      <t>ヒラ</t>
-    </rPh>
-    <rPh sb="34" eb="36">
-      <t>ハグルマ</t>
-    </rPh>
-    <rPh sb="51" eb="53">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="62" eb="63">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="71" eb="72">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="83" eb="85">
-      <t>ジョウキョウ</t>
-    </rPh>
-    <rPh sb="93" eb="95">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="96" eb="98">
-      <t>ビミョウ</t>
-    </rPh>
-    <rPh sb="99" eb="100">
-      <t>コト</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「設定」ウィンドウの状況に応じて、「アカウント」タブ(A)を開くか、左サイドメニューの「アカウント」(B)を選択してください。リンクされたアカウントがある場合はそのアカウント名が表示されています。もしアカウント名が無い場合は、次の章に進んでください。</t>
-    <rPh sb="1" eb="3">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>ジョウキョウ</t>
-    </rPh>
-    <rPh sb="13" eb="14">
-      <t>オウ</t>
-    </rPh>
-    <rPh sb="30" eb="31">
-      <t>ヒラ</t>
-    </rPh>
-    <rPh sb="34" eb="35">
-      <t>ヒダリ</t>
-    </rPh>
-    <rPh sb="54" eb="56">
-      <t>センタク</t>
-    </rPh>
-    <rPh sb="77" eb="79">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="87" eb="88">
-      <t>メイ</t>
-    </rPh>
-    <rPh sb="89" eb="91">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="105" eb="106">
-      <t>メイ</t>
-    </rPh>
-    <rPh sb="107" eb="108">
-      <t>ナ</t>
-    </rPh>
-    <rPh sb="109" eb="111">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="113" eb="114">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="115" eb="116">
-      <t>ショウ</t>
-    </rPh>
-    <rPh sb="117" eb="118">
-      <t>スス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>アカウント名が表示されている場合は、「このPCのリンクを解除」をクリックします。</t>
-    <rPh sb="5" eb="6">
-      <t>メイ</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="28" eb="30">
-      <t>カイジョ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11ja-onedrive-unlink-pc.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11ja-onedrive-unlink-warning.png</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -5899,10 +5739,6 @@
     <rPh sb="38" eb="39">
       <t>シメ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11ja-onedrive-withaccount.png</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -7110,6 +6946,705 @@
     <rPh sb="41" eb="43">
       <t>ヒョウジ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Microsoft Officeのサインイン、OneDriveの設定 (学生番号が必要です)</t>
+    <rPh sb="32" eb="34">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>ガクセイ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>バンゴウ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Microsoft Officeにサインインします。
+&lt;ul&gt;
+&lt;li&gt;&lt;a href="#office"&gt;Microsoft Officeのサインイン&lt;/a&gt;&lt;/li&gt;
+&lt;li&gt;&lt;a href="#onedrive"&gt;OneDriveの設定&lt;/a&gt;&lt;/li&gt;
+&lt;/ul&gt;
+ </t>
+    <rPh sb="119" eb="121">
+      <t>セッテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2 name="office"&gt;Microsoft Officeを入れる&lt;/h2&gt;</t>
+    <rPh sb="35" eb="36">
+      <t>ナ</t>
+    </rPh>
+    <rPh sb="39" eb="41">
+      <t>バアイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2 name="onedrive"&gt;IMCアカウントのOneDrive連携の設定&lt;/h2&gt;</t>
+    <rPh sb="37" eb="39">
+      <t>レンケイ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="43" eb="45">
+      <t>バアイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>最初に、OneDriveは無料MSアカウントの場合容量が5GBと小さいので、リンクを解除しました。IMCアカウントのOneDriveは大学が有償契約をしてますので、3TBまで保存できます。
+現在のOffice365はMSアカウントとリンクしたサブスクリプション制のため、デフォルトの保存先がOneDriveになっています。ブラウザからアクセスしたり、あるいはデフォルトでない保存先として手元のPCを選ぶこともできますが、OneDriveの設定をすることでIMCアカウントのOneDriveを手元のPCと同期させることもできます。あるいは、デフォルトの保存先を手元のPC(ローカルPC)に変更することもできます。OneDriveを手元のPCと同期させるには以下の手順を実施し、デフォルトの保存先をローカルPCにする場合には次に示す&lt;a href="#office_default_local"&gt;「Officeのデフォルト保存先をローカルPCにする」&lt;/a&gt;の手順を実施してください。</t>
+    <rPh sb="0" eb="2">
+      <t>サイショ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ムリョウ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>ヨウリョウ</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>チイ</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>カイジョ</t>
+    </rPh>
+    <rPh sb="67" eb="69">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="70" eb="72">
+      <t>ユウショウ</t>
+    </rPh>
+    <rPh sb="72" eb="74">
+      <t>ケイヤク</t>
+    </rPh>
+    <rPh sb="87" eb="89">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="95" eb="97">
+      <t>ゲンザイ</t>
+    </rPh>
+    <rPh sb="130" eb="131">
+      <t>セイ</t>
+    </rPh>
+    <rPh sb="141" eb="143">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="143" eb="144">
+      <t>サキ</t>
+    </rPh>
+    <rPh sb="187" eb="189">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="189" eb="190">
+      <t>サキ</t>
+    </rPh>
+    <rPh sb="193" eb="195">
+      <t>テモト</t>
+    </rPh>
+    <rPh sb="199" eb="200">
+      <t>エラ</t>
+    </rPh>
+    <rPh sb="219" eb="221">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="245" eb="247">
+      <t>テモト</t>
+    </rPh>
+    <rPh sb="251" eb="253">
+      <t>ドウキ</t>
+    </rPh>
+    <rPh sb="275" eb="277">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="277" eb="278">
+      <t>サキ</t>
+    </rPh>
+    <rPh sb="279" eb="281">
+      <t>テモト</t>
+    </rPh>
+    <rPh sb="293" eb="295">
+      <t>ヘンコウ</t>
+    </rPh>
+    <rPh sb="314" eb="316">
+      <t>テモト</t>
+    </rPh>
+    <rPh sb="320" eb="322">
+      <t>ドウキ</t>
+    </rPh>
+    <rPh sb="327" eb="329">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="330" eb="332">
+      <t>テジュン</t>
+    </rPh>
+    <rPh sb="333" eb="335">
+      <t>ジッシ</t>
+    </rPh>
+    <rPh sb="343" eb="345">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="345" eb="346">
+      <t>サキ</t>
+    </rPh>
+    <rPh sb="356" eb="358">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="360" eb="361">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="362" eb="363">
+      <t>シメ</t>
+    </rPh>
+    <rPh sb="409" eb="411">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="411" eb="412">
+      <t>サキ</t>
+    </rPh>
+    <rPh sb="428" eb="430">
+      <t>テジュン</t>
+    </rPh>
+    <rPh sb="431" eb="433">
+      <t>ジッシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「設定」から「アカウント」に進むと、右ペインにアカウント名、リワードと並んで「OneDrive」というアイコンがあります。これをクリックすると使用するOneDriveアカウントを入力させる画面が開きます。</t>
+    <rPh sb="1" eb="3">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>スス</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>ミギ</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>メイ</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>ナラ</t>
+    </rPh>
+    <rPh sb="71" eb="73">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="89" eb="91">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="94" eb="96">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="97" eb="98">
+      <t>ヒラ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IMCアカウントとパスワードを入力します。</t>
+    <rPh sb="15" eb="17">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IMCアカウントと同期するOneDriveフォルダはOneDrive - Hiroshima Universityになります。</t>
+    <rPh sb="9" eb="11">
+      <t>ドウキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-imc-onedrive-dirname.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-onedrive-exclude-desktop.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-onedrive-dir-selector.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>進めていくと、OneDriveを使ってバックアップするフォルダを選ぶ画面になります。バージョンによってレイアウトが異なります。</t>
+    <rPh sb="0" eb="1">
+      <t>スス</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>エラ</t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="57" eb="58">
+      <t>コト</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ここで、「デスクトップ」だけは&lt;strong&gt;必ず&lt;/strong&gt;除外してください。教員が授業で使うソフトの中にはOneDriveバックアップ対象のフォルダだと正しく動作しないものがあり、そのようなソフトをインストールできるフォルダを自分で作成できる基点を残す必要があるからです。後からでもデスクトップもバックアップ対象に追加することはできます。</t>
+    <rPh sb="23" eb="24">
+      <t>カナラ</t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t>ジョガイ</t>
+    </rPh>
+    <rPh sb="43" eb="45">
+      <t>キョウイン</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>ジュギョウ</t>
+    </rPh>
+    <rPh sb="49" eb="50">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="55" eb="56">
+      <t>ナカ</t>
+    </rPh>
+    <rPh sb="72" eb="74">
+      <t>タイショウ</t>
+    </rPh>
+    <rPh sb="81" eb="82">
+      <t>タダ</t>
+    </rPh>
+    <rPh sb="84" eb="86">
+      <t>ドウサ</t>
+    </rPh>
+    <rPh sb="118" eb="120">
+      <t>ジブン</t>
+    </rPh>
+    <rPh sb="121" eb="123">
+      <t>サクセイ</t>
+    </rPh>
+    <rPh sb="126" eb="128">
+      <t>キテン</t>
+    </rPh>
+    <rPh sb="129" eb="130">
+      <t>ノコ</t>
+    </rPh>
+    <rPh sb="131" eb="133">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="141" eb="142">
+      <t>アト</t>
+    </rPh>
+    <rPh sb="159" eb="161">
+      <t>タイショウ</t>
+    </rPh>
+    <rPh sb="162" eb="164">
+      <t>ツイカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-onedrive-start-backup.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>バックアップ対象フォルダを選んだらバックアップを開始します。</t>
+    <rPh sb="6" eb="8">
+      <t>タイショウ</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>エラ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>カイシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>エクスプローラの左サイドバーから「ホーム」を選び、バックアップ対象としたフォルダに雲マークが出ていることを確認しましょう。</t>
+    <rPh sb="8" eb="9">
+      <t>ヒダリ</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>エラ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>タイショウ</t>
+    </rPh>
+    <rPh sb="41" eb="42">
+      <t>クモ</t>
+    </rPh>
+    <rPh sb="46" eb="47">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="53" eb="55">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OneDrive同期は、同じファイルやディレクトリを複数のOneDriveアカウントで同期させることはできません。個人MSアカウントへの同期が知らないうちに入っている可能性がありますので、念のため通知エリアを確認し、第1章の手順に従ってリンクを解除してください。</t>
+    <rPh sb="8" eb="10">
+      <t>ドウキ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>フクスウ</t>
+    </rPh>
+    <rPh sb="43" eb="45">
+      <t>ドウキ</t>
+    </rPh>
+    <rPh sb="57" eb="59">
+      <t>コジン</t>
+    </rPh>
+    <rPh sb="68" eb="70">
+      <t>ドウキ</t>
+    </rPh>
+    <rPh sb="71" eb="72">
+      <t>シ</t>
+    </rPh>
+    <rPh sb="78" eb="79">
+      <t>ハイ</t>
+    </rPh>
+    <rPh sb="83" eb="86">
+      <t>カノウセイ</t>
+    </rPh>
+    <rPh sb="94" eb="95">
+      <t>ネン</t>
+    </rPh>
+    <rPh sb="98" eb="100">
+      <t>ツウチ</t>
+    </rPh>
+    <rPh sb="104" eb="106">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="108" eb="109">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="110" eb="111">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="112" eb="114">
+      <t>テジュン</t>
+    </rPh>
+    <rPh sb="115" eb="116">
+      <t>シタガ</t>
+    </rPh>
+    <rPh sb="122" eb="124">
+      <t>カイジョ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>無料OneDriveへのリンク解除</t>
+    <rPh sb="0" eb="2">
+      <t>ムリョウ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>カイジョ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>再び「アカウント」タブまたは「アカウント」メニューに戻り、「このPCのリンクを解除」をクリックします。</t>
+    <rPh sb="0" eb="1">
+      <t>フタタ</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>モド</t>
+    </rPh>
+    <rPh sb="39" eb="41">
+      <t>カイジョ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>対象のフォルダを選ぶウィンドウになります。「バックアップの停止」を1つずつクリックしましょう。「バックアップの停止」が無いフォルダもあるかもしれませんが、それはまだそのままにしておきます。</t>
+    <rPh sb="55" eb="57">
+      <t>テイシ</t>
+    </rPh>
+    <rPh sb="59" eb="60">
+      <t>ナ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>このような通知が出ますが、「バックアップを停止」で進めます。</t>
+    <rPh sb="5" eb="7">
+      <t>ツウチ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>テイシ</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>全てのフォルダのバックアップを解除すると、「バックアップの開始」のボタンがグレーアウトするので、ウィンドウを「X」ボタンで閉じます。</t>
+    <rPh sb="0" eb="1">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>カイジョ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>カイシ</t>
+    </rPh>
+    <rPh sb="61" eb="62">
+      <t>ト</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>雲アイコンを右クリックしてOneDriveアプリのウィンドウを開き、歯車アイコン(①)をクリックして「設定」メニュー(②)に進みましょう。「お使いのPCのアップデート状況により、アプリの画面が微妙に異なります。
+以降では現状最も多いと思われる2023年版での手順を示します。2024年版の手順は附録で示します。</t>
+    <rPh sb="0" eb="1">
+      <t>クモ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ミギ</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t>ハグルマ</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="62" eb="63">
+      <t>スス</t>
+    </rPh>
+    <rPh sb="71" eb="72">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="83" eb="85">
+      <t>ジョウキョウ</t>
+    </rPh>
+    <rPh sb="93" eb="95">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="96" eb="98">
+      <t>ビミョウ</t>
+    </rPh>
+    <rPh sb="99" eb="100">
+      <t>コト</t>
+    </rPh>
+    <rPh sb="106" eb="108">
+      <t>イコウ</t>
+    </rPh>
+    <rPh sb="110" eb="112">
+      <t>ゲンジョウ</t>
+    </rPh>
+    <rPh sb="112" eb="113">
+      <t>モット</t>
+    </rPh>
+    <rPh sb="114" eb="115">
+      <t>オオ</t>
+    </rPh>
+    <rPh sb="117" eb="118">
+      <t>オモ</t>
+    </rPh>
+    <rPh sb="125" eb="127">
+      <t>ネンバン</t>
+    </rPh>
+    <rPh sb="129" eb="131">
+      <t>テジュン</t>
+    </rPh>
+    <rPh sb="132" eb="133">
+      <t>シメ</t>
+    </rPh>
+    <rPh sb="141" eb="143">
+      <t>ネンバン</t>
+    </rPh>
+    <rPh sb="144" eb="146">
+      <t>テジュン</t>
+    </rPh>
+    <rPh sb="147" eb="149">
+      <t>フロク</t>
+    </rPh>
+    <rPh sb="150" eb="151">
+      <t>シメ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アカウント名が表示されている場合は、「バックアップ」タブ(①)を表示させ、「バックアップを管理」(②)のボタンを押します。</t>
+    <rPh sb="5" eb="6">
+      <t>メイ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>カンリ</t>
+    </rPh>
+    <rPh sb="56" eb="57">
+      <t>オ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「このフォルダーはバックアップされなくなりました」という通知が出るので、閉じます。この操作を「バックアップを停止」が表示されているフォルダ全てに対して繰り返します。</t>
+    <rPh sb="28" eb="30">
+      <t>ツウチ</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="43" eb="45">
+      <t>ソウサ</t>
+    </rPh>
+    <rPh sb="54" eb="56">
+      <t>テイシ</t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="69" eb="70">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="72" eb="73">
+      <t>タイ</t>
+    </rPh>
+    <rPh sb="75" eb="76">
+      <t>ク</t>
+    </rPh>
+    <rPh sb="77" eb="78">
+      <t>カエ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>全てバックアップ対象から外すと、これから改めてバックアップを開始する段階のウィンドウになっており、すべてのフォルダの右上にチェック記号が入っています(バックアップ予定を示しています)。こののチェックを全て外します。</t>
+    <rPh sb="0" eb="1">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>タイショウ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>ハズ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>アラタ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>カイシ</t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t>ダンカイ</t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t>ミギウエ</t>
+    </rPh>
+    <rPh sb="65" eb="67">
+      <t>キゴウ</t>
+    </rPh>
+    <rPh sb="68" eb="69">
+      <t>ハイ</t>
+    </rPh>
+    <rPh sb="81" eb="83">
+      <t>ヨテイ</t>
+    </rPh>
+    <rPh sb="84" eb="85">
+      <t>シメ</t>
+    </rPh>
+    <rPh sb="100" eb="101">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="102" eb="103">
+      <t>ハズ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>まず「アカウント」タブを開いてください。リンクされたアカウントがある場合はそのアカウント名が表示されています。もしアカウント名が無い場合は、OneDriveがリンクされていないので、次の章に進んでください。</t>
+    <rPh sb="12" eb="13">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="44" eb="45">
+      <t>メイ</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="62" eb="63">
+      <t>メイ</t>
+    </rPh>
+    <rPh sb="64" eb="65">
+      <t>ナ</t>
+    </rPh>
+    <rPh sb="66" eb="68">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="91" eb="92">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="93" eb="94">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="95" eb="96">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-odrv23-withaccount.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-odrv23-backup.png</t>
+  </si>
+  <si>
+    <t>win11ja-odrv23-backup-mgr.png</t>
+  </si>
+  <si>
+    <t>win11ja-odrv23-backup-stopwarn1.png</t>
+  </si>
+  <si>
+    <t>win11ja-odrv23-backup-stopwarn2.png</t>
+  </si>
+  <si>
+    <t>win11ja-odrv23-backup-select.png</t>
+  </si>
+  <si>
+    <t>win11ja-odrv23-backup-unselect.png</t>
+  </si>
+  <si>
+    <t>win11ja-odrv23-unlink-pc.png</t>
+  </si>
+  <si>
+    <t>win11ja-odrv23-unlink-warning.png</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -7551,7 +8086,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7567,7 +8102,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7575,7 +8110,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -7589,7 +8124,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7627,7 +8162,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -7635,7 +8170,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -7651,7 +8186,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="304.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -7659,7 +8194,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -7673,13 +8208,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C7" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -7687,21 +8222,21 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
@@ -7715,7 +8250,7 @@
         <v>7</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="105.6" ph="1" x14ac:dyDescent="0.2">
@@ -7723,24 +8258,24 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
@@ -7748,13 +8283,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
@@ -7762,13 +8297,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -7776,32 +8311,32 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -7809,238 +8344,238 @@
         <v>4</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C25" t="s" ph="1">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="26" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C26" t="s" ph="1">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D26" t="s" ph="1">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C27" t="s" ph="1">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D27" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C28" t="s" ph="1">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D28" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C29" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D29" t="s" ph="1">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C30" t="s" ph="1">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D30" t="s" ph="1">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C31" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D31" t="s" ph="1">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C32" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D32" t="s" ph="1">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C33" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D33" t="s" ph="1">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D34" t="s" ph="1">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="C35" t="s" ph="1">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D35" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D36" t="s" ph="1">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="37" spans="2:5" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C37" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D37" t="s" ph="1">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C38" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D38" t="s" ph="1">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="2:5" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C39" t="s" ph="1">
+        <v>88</v>
+      </c>
+      <c r="D39" t="s" ph="1">
         <v>89</v>
-      </c>
-      <c r="D39" t="s" ph="1">
-        <v>90</v>
       </c>
     </row>
     <row r="40" spans="2:5" ph="1" x14ac:dyDescent="0.2">
@@ -8144,10 +8679,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8163,7 +8698,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
@@ -8171,7 +8706,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -8187,250 +8722,315 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C7" t="s" ph="1">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E7" ph="1"/>
     </row>
     <row r="8" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C8" t="s" ph="1">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:5" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C9" t="s" ph="1">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:5" customFormat="1" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>335</v>
+        <v>326</v>
       </c>
     </row>
     <row r="12" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>336</v>
+        <v>327</v>
       </c>
     </row>
     <row r="13" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="14" spans="1:5" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="15" spans="1:5" customFormat="1" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="6" t="s">
-        <v>295</v>
-      </c>
-      <c r="D16" t="s" ph="1">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="6"/>
+    </row>
+    <row r="17" spans="2:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="6"/>
+    </row>
+    <row r="19" spans="2:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="D19" t="s" ph="1">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="6" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="6" t="s">
-        <v>302</v>
-      </c>
-      <c r="D17" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="6" t="s">
-        <v>328</v>
-      </c>
-      <c r="D18" t="s" ph="1">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="6" t="s">
+      <c r="D20" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" customFormat="1" ht="64.8" customHeight="1" ph="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="D21" t="s" ph="1">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="D22" t="s" ph="1">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="D23" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" customFormat="1" ht="45.6" customHeight="1" ph="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="D24" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="D25" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="D26" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="D27" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="D28" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="D29" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D30" t="s" ph="1">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D31" t="s" ph="1">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="D32" t="s" ph="1">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="D19" t="s" ph="1">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="D20" t="s" ph="1">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="D21" t="s" ph="1">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="D22" t="s" ph="1">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="D23" t="s" ph="1">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="D24" t="s" ph="1">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="6"/>
-      <c r="C26"/>
-      <c r="D26"/>
-    </row>
-    <row r="27" spans="1:4" ht="132" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="D33" t="s" ph="1">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="6"/>
+      <c r="C35"/>
+      <c r="D35"/>
+    </row>
+    <row r="36" spans="1:4" ht="132" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>297</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="B36" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="C36" t="s">
         <v>4</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D36" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="37" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>4</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B37" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" t="s">
         <v>101</v>
       </c>
-      <c r="C28" t="s">
+    </row>
+    <row r="38" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B38" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D38" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B39" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D39" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B40" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D40" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>4</v>
       </c>
-      <c r="D28" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B29" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D29" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B30" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D30" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B31" s="6" t="s">
+      <c r="B41" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="D31" t="s">
+      <c r="C41" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="C32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="6"/>
-    </row>
-    <row r="34" spans="2:2" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="6"/>
-    </row>
-    <row r="37" spans="2:2" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="6"/>
-    </row>
-    <row r="38" spans="2:2" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="6"/>
+    <row r="42" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="6"/>
+    </row>
+    <row r="43" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="6"/>
+    </row>
+    <row r="46" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="6"/>
+    </row>
+    <row r="47" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="6"/>
+    </row>
+    <row r="48" spans="1:4" customFormat="1" ph="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="6"/>
+    </row>
+    <row r="49" spans="2:2" customFormat="1" ph="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -8460,7 +9060,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8468,7 +9068,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8484,7 +9084,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -8492,7 +9092,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8511,29 +9111,29 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="D11" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="D12" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -8541,13 +9141,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -8555,7 +9155,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -8566,7 +9166,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -8577,21 +9177,21 @@
         <v>4</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -8599,13 +9199,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8613,13 +9213,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8627,13 +9227,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -8646,149 +9246,149 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="82.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="D27" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="D28" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="D29" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="67.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="D30" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="D31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D33" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D34" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D35" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D36" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="50.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D38" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D39" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="6" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D40" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D41" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="46.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="6" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D42" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="131.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="6" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" s="6" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="6" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="D47" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
     </row>
     <row r="48" spans="2:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8820,7 +9420,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
     </row>
     <row r="2" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -8828,7 +9428,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
     </row>
     <row r="3" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -8844,7 +9444,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="5" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -8852,7 +9452,7 @@
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -8860,7 +9460,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -8868,50 +9468,50 @@
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="D10" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="D11" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D12" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="D13" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D14" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="D15" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -8919,7 +9519,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -8928,68 +9528,68 @@
     </row>
     <row r="19" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="C19" ph="1"/>
       <c r="D19" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="132" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="C20" ph="1"/>
       <c r="D20" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
@@ -8997,7 +9597,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -9006,29 +9606,29 @@
     </row>
     <row r="30" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="C30" ph="1"/>
       <c r="D30" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="C31" ph="1"/>
       <c r="D31" t="s" ph="1">
-        <v>392</v>
+        <v>382</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="C32" ph="1"/>
       <c r="D32" t="s" ph="1">
-        <v>391</v>
+        <v>381</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -9069,7 +9669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D6E33FB-2290-439B-854D-9A45A4600EF5}">
   <dimension ref="A1:D87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+    <sheetView zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
       <selection activeCell="A49" sqref="A49:XFD49"/>
     </sheetView>
   </sheetViews>
@@ -9086,7 +9686,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -9094,7 +9694,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9110,7 +9710,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -9121,7 +9721,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -9140,7 +9740,7 @@
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -9153,7 +9753,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -9164,18 +9764,18 @@
     </row>
     <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9183,7 +9783,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -9191,18 +9791,18 @@
     </row>
     <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D16" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -9210,13 +9810,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="198" x14ac:dyDescent="0.2">
@@ -9224,18 +9824,18 @@
         <v>4</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9243,21 +9843,21 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D21" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9265,21 +9865,21 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D23" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9287,13 +9887,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -9301,7 +9901,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -9317,40 +9917,40 @@
     </row>
     <row r="28" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D29" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D30" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -9358,7 +9958,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -9377,80 +9977,80 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D36" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D37" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D39" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D40" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D41" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C42" t="s">
         <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C43" t="s">
         <v>4</v>
       </c>
       <c r="D43" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -9458,7 +10058,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -9466,7 +10066,7 @@
     </row>
     <row r="47" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C47" t="s">
         <v>4</v>
@@ -9477,7 +10077,7 @@
     </row>
     <row r="48" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C48" t="s">
         <v>7</v>
@@ -9494,7 +10094,7 @@
     </row>
     <row r="50" spans="2:4" ht="132" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C50" t="s">
         <v>7</v>
@@ -9545,10 +10145,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A23" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -9572,7 +10172,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>137</v>
+        <v>387</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9588,15 +10188,15 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>272</v>
+        <v>388</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -9620,18 +10220,18 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>389</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -9639,21 +10239,21 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -9661,13 +10261,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9675,13 +10275,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -9689,33 +10289,93 @@
         <v>4</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="B19" s="5"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>4</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="4" customFormat="1" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+    <row r="22" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="4" customFormat="1" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>294</v>
-      </c>
-      <c r="C20" s="4" ph="1"/>
-      <c r="D20" s="4" t="s" ph="1">
-        <v>299</v>
+      <c r="B25" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="C25" s="4" ph="1"/>
+      <c r="D25" s="4" t="s" ph="1">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="D27" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D28" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="D29" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="D30" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
+        <v>402</v>
       </c>
     </row>
   </sheetData>
@@ -9746,7 +10406,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -9754,7 +10414,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9770,17 +10430,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -9793,7 +10453,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -9818,13 +10478,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9832,21 +10492,21 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -9854,12 +10514,12 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9867,33 +10527,33 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D19" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -9924,7 +10584,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -9932,7 +10592,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9948,22 +10608,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9987,7 +10647,7 @@
     </row>
     <row r="14" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
         <v>18</v>
@@ -9995,7 +10655,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.2">
@@ -10003,10 +10663,10 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D16" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -10014,39 +10674,39 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D19" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -10054,36 +10714,36 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D23" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D24" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -10094,59 +10754,59 @@
     </row>
     <row r="30" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D30" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D31" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D32" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C34" t="s">
         <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C35" t="s">
         <v>7</v>
       </c>
       <c r="D35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -10157,117 +10817,117 @@
         <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C37" t="s">
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C38" t="s">
         <v>7</v>
       </c>
       <c r="D38" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C39" t="s">
         <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C41" t="s">
         <v>7</v>
       </c>
       <c r="D41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C42" t="s">
         <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C43" t="s">
         <v>7</v>
       </c>
       <c r="D43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C44" t="s">
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C45" t="s">
         <v>7</v>
       </c>
       <c r="D45" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="2:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C46" t="s">
         <v>7</v>
       </c>
       <c r="D46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
win11ja: instr OneDrive23 update
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{530DAC4E-3AD6-4409-8FF7-56A5E3DB05EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C62AE31-9A69-4D3D-9818-0E838C92BE50}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5240,10 +5240,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-onedrive-add-account.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>「オンラインのみのファイルは削除されます」という警告が出ますが、これは手元のエクスプローラでアクセスできなくなるという意味です。Webブラウザ経由でOneDriveにアクセスする形では残っていますので、解除しましょう。</t>
     <rPh sb="14" eb="16">
       <t>サクジョ</t>
@@ -7646,6 +7642,9 @@
       <t>カイジョ</t>
     </rPh>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-odrv-add-account-close.png</t>
   </si>
 </sst>
 </file>
@@ -8322,15 +8321,15 @@
     </row>
     <row r="16" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>7</v>
@@ -8355,7 +8354,7 @@
     </row>
     <row r="19" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>7</v>
@@ -8424,48 +8423,48 @@
         <v>262</v>
       </c>
       <c r="C25" t="s" ph="1">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="26" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C26" t="s" ph="1">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D26" t="s" ph="1">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C27" t="s" ph="1">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D27" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="C28" t="s" ph="1">
+        <v>303</v>
+      </c>
+      <c r="D28" t="s">
         <v>318</v>
-      </c>
-      <c r="C28" t="s" ph="1">
-        <v>304</v>
-      </c>
-      <c r="D28" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C29" t="s" ph="1">
         <v>7</v>
@@ -8476,13 +8475,13 @@
     </row>
     <row r="30" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="C30" t="s" ph="1">
+        <v>303</v>
+      </c>
+      <c r="D30" t="s" ph="1">
         <v>313</v>
-      </c>
-      <c r="C30" t="s" ph="1">
-        <v>304</v>
-      </c>
-      <c r="D30" t="s" ph="1">
-        <v>314</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
@@ -8523,23 +8522,23 @@
         <v>263</v>
       </c>
       <c r="D34" t="s" ph="1">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C35" t="s" ph="1">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D35" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D36" t="s" ph="1">
         <v>266</v>
@@ -8547,7 +8546,7 @@
     </row>
     <row r="37" spans="2:5" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C37" t="s" ph="1">
         <v>7</v>
@@ -8682,7 +8681,7 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8698,7 +8697,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
@@ -8706,7 +8705,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -8761,7 +8760,7 @@
     </row>
     <row r="10" spans="1:5" customFormat="1" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D10" t="s" ph="1">
         <v>92</v>
@@ -8769,42 +8768,42 @@
     </row>
     <row r="11" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="D11" t="s" ph="1">
         <v>325</v>
-      </c>
-      <c r="D11" t="s" ph="1">
-        <v>326</v>
       </c>
     </row>
     <row r="12" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="13" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="D13" t="s" ph="1">
         <v>307</v>
-      </c>
-      <c r="D13" t="s" ph="1">
-        <v>308</v>
       </c>
     </row>
     <row r="14" spans="1:5" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="15" spans="1:5" customFormat="1" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="16" spans="1:5" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -8812,7 +8811,7 @@
     </row>
     <row r="17" spans="2:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="18" spans="2:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -8828,111 +8827,111 @@
     </row>
     <row r="20" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D20" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="21" spans="2:4" customFormat="1" ht="64.8" customHeight="1" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="22" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="D22" t="s" ph="1">
         <v>412</v>
-      </c>
-      <c r="D22" t="s" ph="1">
-        <v>413</v>
       </c>
     </row>
     <row r="23" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D23" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="24" spans="2:4" customFormat="1" ht="45.6" customHeight="1" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D24" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="25" spans="2:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D25" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="26" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D26" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="27" spans="2:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D27" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="28" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D28" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="29" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D29" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="30" spans="2:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D30" t="s" ph="1">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="31" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="D31" t="s" ph="1">
-        <v>296</v>
+      <c r="D31" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="32" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D32" t="s" ph="1">
         <v>330</v>
-      </c>
-      <c r="D32" t="s" ph="1">
-        <v>331</v>
       </c>
     </row>
     <row r="33" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D33" t="s" ph="1">
         <v>294</v>
@@ -8940,7 +8939,7 @@
     </row>
     <row r="34" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="35" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -9111,29 +9110,29 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="D12" t="s">
         <v>340</v>
-      </c>
-      <c r="D12" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -9141,13 +9140,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -9256,39 +9255,39 @@
     </row>
     <row r="27" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D27" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D28" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D29" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="67.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D30" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D31" t="s">
         <v>235</v>
@@ -9385,10 +9384,10 @@
     </row>
     <row r="47" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D47" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="48" spans="2:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9420,7 +9419,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="2" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -9428,7 +9427,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="3" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -9452,7 +9451,7 @@
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -9460,7 +9459,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -9468,18 +9467,18 @@
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D10" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D11" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9487,15 +9486,15 @@
         <v>289</v>
       </c>
       <c r="D12" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D13" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9503,15 +9502,15 @@
         <v>290</v>
       </c>
       <c r="D14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="D15" t="s">
         <v>361</v>
-      </c>
-      <c r="D15" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -9519,7 +9518,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -9528,20 +9527,20 @@
     </row>
     <row r="19" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C19" ph="1"/>
       <c r="D19" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="132" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C20" ph="1"/>
       <c r="D20" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9597,7 +9596,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -9606,29 +9605,29 @@
     </row>
     <row r="30" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C30" ph="1"/>
       <c r="D30" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C31" ph="1"/>
       <c r="D31" t="s" ph="1">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C32" ph="1"/>
       <c r="D32" t="s" ph="1">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -9710,7 +9709,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -10172,7 +10171,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -10188,7 +10187,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -10196,7 +10195,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -10231,7 +10230,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -10289,7 +10288,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -10303,7 +10302,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -10316,12 +10315,12 @@
     </row>
     <row r="22" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="4" customFormat="1" ht="39.6" x14ac:dyDescent="0.2">
@@ -10329,7 +10328,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C25" s="4" ph="1"/>
       <c r="D25" s="4" t="s" ph="1">
@@ -10338,44 +10337,44 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="D27" t="s">
         <v>394</v>
-      </c>
-      <c r="D27" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D28" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D29" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D30" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>
@@ -10430,7 +10429,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -10608,7 +10607,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
win11ja: update image for noaccount check
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C62AE31-9A69-4D3D-9818-0E838C92BE50}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287B921E-46F8-4703-8EDA-C7DD4F6A1B70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5800,10 +5800,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-onedrive-noaccount.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>「ライセンス契約に同意します」で「同意する」をクリックします。
 &lt;p class="spl"&gt;※本来は「利用許諾契約書を読む」で契約事項を読んでから同意するものです。「ファイル」→「アカウント」→「Excelのバージョン情報」と辿ればいつでも読めるので、時間のある時に読んでおいてください。&lt;/p&gt;
 これでOfficeを使用するための準備が完了しました。&lt;span class="check"&gt;check 13&lt;span&gt;&lt;/span&gt;
@@ -7645,6 +7641,10 @@
   </si>
   <si>
     <t>win11ja-odrv-add-account-close.png</t>
+  </si>
+  <si>
+    <t>win11ja-odrv23-noaccount.png</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -8329,7 +8329,7 @@
     </row>
     <row r="17" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>7</v>
@@ -8354,7 +8354,7 @@
     </row>
     <row r="19" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>7</v>
@@ -8527,7 +8527,7 @@
     </row>
     <row r="35" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C35" t="s" ph="1">
         <v>303</v>
@@ -8681,7 +8681,7 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8697,7 +8697,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
@@ -8705,7 +8705,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -8811,7 +8811,7 @@
     </row>
     <row r="17" spans="2:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="18" spans="2:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -8835,7 +8835,7 @@
     </row>
     <row r="21" spans="2:4" customFormat="1" ht="64.8" customHeight="1" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D21" t="s" ph="1">
         <v>322</v>
@@ -8843,66 +8843,66 @@
     </row>
     <row r="22" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="D22" t="s" ph="1">
         <v>411</v>
-      </c>
-      <c r="D22" t="s" ph="1">
-        <v>412</v>
       </c>
     </row>
     <row r="23" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D23" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="24" spans="2:4" customFormat="1" ht="45.6" customHeight="1" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D24" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="25" spans="2:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D25" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="26" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D26" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="27" spans="2:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D27" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="28" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D28" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="29" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D29" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="30" spans="2:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -8910,7 +8910,7 @@
         <v>296</v>
       </c>
       <c r="D30" t="s" ph="1">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="31" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
@@ -8918,7 +8918,7 @@
         <v>292</v>
       </c>
       <c r="D31" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="32" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
@@ -8926,7 +8926,7 @@
         <v>329</v>
       </c>
       <c r="D32" t="s" ph="1">
-        <v>330</v>
+        <v>422</v>
       </c>
     </row>
     <row r="33" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -8939,7 +8939,7 @@
     </row>
     <row r="34" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="35" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -9110,29 +9110,29 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D11" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="D12" t="s">
         <v>339</v>
-      </c>
-      <c r="D12" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -9140,13 +9140,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -9255,39 +9255,39 @@
     </row>
     <row r="27" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D27" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D28" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D29" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="67.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D30" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D31" t="s">
         <v>235</v>
@@ -9384,10 +9384,10 @@
     </row>
     <row r="47" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D47" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="48" spans="2:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9419,7 +9419,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="2" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -9427,7 +9427,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="3" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -9451,7 +9451,7 @@
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -9459,7 +9459,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -9467,18 +9467,18 @@
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D10" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D11" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9486,15 +9486,15 @@
         <v>289</v>
       </c>
       <c r="D12" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D13" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9502,15 +9502,15 @@
         <v>290</v>
       </c>
       <c r="D14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="D15" t="s">
         <v>360</v>
-      </c>
-      <c r="D15" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -9518,7 +9518,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -9527,20 +9527,20 @@
     </row>
     <row r="19" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C19" ph="1"/>
       <c r="D19" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="132" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C20" ph="1"/>
       <c r="D20" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9596,7 +9596,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -9605,29 +9605,29 @@
     </row>
     <row r="30" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C30" ph="1"/>
       <c r="D30" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C31" ph="1"/>
       <c r="D31" t="s" ph="1">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C32" ph="1"/>
       <c r="D32" t="s" ph="1">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -9709,7 +9709,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -10171,7 +10171,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -10187,7 +10187,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -10195,7 +10195,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -10230,7 +10230,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -10288,7 +10288,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -10302,7 +10302,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -10315,12 +10315,12 @@
     </row>
     <row r="22" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="4" customFormat="1" ht="39.6" x14ac:dyDescent="0.2">
@@ -10328,7 +10328,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C25" s="4" ph="1"/>
       <c r="D25" s="4" t="s" ph="1">
@@ -10337,44 +10337,44 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D27" t="s">
         <v>393</v>
-      </c>
-      <c r="D27" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D28" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D29" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D30" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
   </sheetData>
@@ -10429,7 +10429,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -10607,7 +10607,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
win11ja: add ch1 section titles
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287B921E-46F8-4703-8EDA-C7DD4F6A1B70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB74853-1626-4FC5-BF0F-E4AF0E38704A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="426">
   <si>
     <t>header1</t>
   </si>
@@ -6772,44 +6772,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">自分のパソコンの基本的なスペックを確認しておきましょう。CPUの型式、OSのビット数、記憶容量など。また、容量が小さい個人MSアカウントのOneDriveリンクも解除しておきます。
-なお、この章は広島大学の学生番号がわかる前に実施することができます。 </t>
-    <rPh sb="53" eb="55">
-      <t>ヨウリョウ</t>
-    </rPh>
-    <rPh sb="56" eb="57">
-      <t>チイ</t>
-    </rPh>
-    <rPh sb="59" eb="61">
-      <t>コジン</t>
-    </rPh>
-    <rPh sb="81" eb="83">
-      <t>カイジョ</t>
-    </rPh>
-    <rPh sb="96" eb="97">
-      <t>ショウ</t>
-    </rPh>
-    <rPh sb="98" eb="100">
-      <t>ヒロシマ</t>
-    </rPh>
-    <rPh sb="100" eb="102">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="103" eb="105">
-      <t>ガクセイ</t>
-    </rPh>
-    <rPh sb="105" eb="107">
-      <t>バンゴウ</t>
-    </rPh>
-    <rPh sb="111" eb="112">
-      <t>マエ</t>
-    </rPh>
-    <rPh sb="113" eb="115">
-      <t>ジッシ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>前の章でデスクトップにBitLocker鍵を保存した場合、ダブルクリックして開くことができます。現在のWindowsでは、PDFはEdgeによって閲覧するのが既定の状態ですが、Google Chromeでも表示できます。</t>
     <rPh sb="48" eb="50">
       <t>ゲンザイ</t>
@@ -7339,16 +7301,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>無料OneDriveへのリンク解除</t>
-    <rPh sb="0" eb="2">
-      <t>ムリョウ</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>カイジョ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>対象のフォルダを選ぶウィンドウになります。「バックアップの停止」を1つずつクリックしましょう。「バックアップの停止」が無いフォルダもあるかもしれませんが、それはまだそのままにしておきます。</t>
     <rPh sb="55" eb="57">
       <t>テイシ</t>
@@ -7644,6 +7596,124 @@
   </si>
   <si>
     <t>win11ja-odrv23-noaccount.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">自分のパソコンの基本的なスペックを確認しておきましょう。CPUの型式、記憶容量など。また、容量が少ない無償MSアカウントのOneDriveリンクも解除しておきます。
+なお、この章は広島大学の学生番号がわかる前に実施することができます。 </t>
+    <rPh sb="45" eb="47">
+      <t>ヨウリョウ</t>
+    </rPh>
+    <rPh sb="48" eb="49">
+      <t>スク</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>ムショウ</t>
+    </rPh>
+    <rPh sb="73" eb="75">
+      <t>カイジョ</t>
+    </rPh>
+    <rPh sb="88" eb="89">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="90" eb="92">
+      <t>ヒロシマ</t>
+    </rPh>
+    <rPh sb="92" eb="94">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="95" eb="97">
+      <t>ガクセイ</t>
+    </rPh>
+    <rPh sb="97" eb="99">
+      <t>バンゴウ</t>
+    </rPh>
+    <rPh sb="103" eb="104">
+      <t>マエ</t>
+    </rPh>
+    <rPh sb="105" eb="107">
+      <t>ジッシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>この章ではパソコンの基本的なスペックを確認します。
+また、容量が少ない無償MSアカウントにOneDriveリンクが設定されている場合があるので、これを解除します。
+Surfaceで日本語キーボードが正しく動作するかも確認しておきましょう。
+&lt;ul&gt;
+&lt;li&gt;&lt;a href="#spec"&gt;PCのスペック確認&lt;/a&gt;&lt;/li&gt;
+&lt;li&gt;&lt;a href="#onedrive_unlink"&gt;OneDriveのリンク解除&lt;/a&gt;&lt;/li&gt;
+&lt;li&gt;&lt;a href="#keyboard_layout"&gt;キーボード動作確認&lt;/a&gt;&lt;/li&gt;
+&lt;/ul&gt;</t>
+    <rPh sb="2" eb="3">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="10" eb="13">
+      <t>キホンテキ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>ヨウリョウ</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>スク</t>
+    </rPh>
+    <rPh sb="57" eb="59">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="64" eb="66">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="75" eb="77">
+      <t>カイジョ</t>
+    </rPh>
+    <rPh sb="90" eb="93">
+      <t>ニホンゴ</t>
+    </rPh>
+    <rPh sb="99" eb="100">
+      <t>タダ</t>
+    </rPh>
+    <rPh sb="102" eb="104">
+      <t>ドウサ</t>
+    </rPh>
+    <rPh sb="108" eb="110">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="152" eb="154">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="207" eb="209">
+      <t>カイジョ</t>
+    </rPh>
+    <rPh sb="255" eb="257">
+      <t>ドウサ</t>
+    </rPh>
+    <rPh sb="257" eb="259">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2 name="spec"&gt;PCのスペック確認&lt;/h2&gt;</t>
+    <rPh sb="23" eb="25">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2 name="spec"&gt;OneDriveのリンク解除&lt;/h2&gt;</t>
+    <rPh sb="28" eb="30">
+      <t>カイジョ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2 name="keyboard_layout"&gt;キーボードのレイアウト確認&lt;/h2&gt;</t>
+    <rPh sb="38" eb="40">
+      <t>カクニン</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -8143,8 +8213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="A17" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.2"/>
@@ -8678,10 +8748,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8697,7 +8767,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>374</v>
+        <v>421</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
@@ -8724,312 +8794,319 @@
         <v>283</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B7" s="6" t="s">
+    <row r="6" spans="1:5" ht="132" x14ac:dyDescent="0.2">
+      <c r="B6" s="6" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="6" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B10" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C7" t="s" ph="1">
+      <c r="C10" t="s" ph="1">
         <v>88</v>
       </c>
-      <c r="D7" t="s" ph="1">
+      <c r="D10" t="s" ph="1">
         <v>90</v>
       </c>
-      <c r="E7" ph="1"/>
-    </row>
-    <row r="8" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C8" t="s" ph="1">
-        <v>88</v>
-      </c>
-      <c r="D8" t="s" ph="1">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C9" t="s" ph="1">
-        <v>88</v>
-      </c>
-      <c r="D9" t="s" ph="1">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" customFormat="1" ht="92.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="6" t="s">
-        <v>323</v>
-      </c>
-      <c r="D10" t="s" ph="1">
-        <v>92</v>
-      </c>
+      <c r="E10" ph="1"/>
     </row>
     <row r="11" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" t="s" ph="1">
+        <v>88</v>
+      </c>
+      <c r="D11" t="s" ph="1">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" t="s" ph="1">
+        <v>88</v>
+      </c>
+      <c r="D12" t="s" ph="1">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" customFormat="1" ht="92.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="D13" t="s" ph="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="D11" t="s" ph="1">
+      <c r="D14" t="s" ph="1">
         <v>325</v>
       </c>
     </row>
-    <row r="12" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="6" t="s">
+    <row r="15" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="D12" t="s" ph="1">
+      <c r="D15" t="s" ph="1">
         <v>326</v>
       </c>
     </row>
-    <row r="13" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="6" t="s">
+    <row r="16" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="D13" t="s" ph="1">
+      <c r="D16" t="s" ph="1">
         <v>307</v>
       </c>
     </row>
-    <row r="14" spans="1:5" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="6" t="s">
+    <row r="17" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="D14" t="s" ph="1">
+      <c r="D17" t="s" ph="1">
         <v>308</v>
       </c>
     </row>
-    <row r="15" spans="1:5" customFormat="1" ht="66" ph="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="6" t="s">
+    <row r="18" spans="2:4" customFormat="1" ht="66" ph="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="D15" t="s" ph="1">
+      <c r="D18" t="s" ph="1">
         <v>319</v>
       </c>
     </row>
-    <row r="16" spans="1:5" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="6"/>
-    </row>
-    <row r="17" spans="2:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="6" t="s">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="D22" t="s" ph="1">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="D23" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" customFormat="1" ht="64.8" customHeight="1" ph="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="D24" t="s" ph="1">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="D25" t="s" ph="1">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="D26" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" customFormat="1" ht="45.6" customHeight="1" ph="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="D27" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="6" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="6"/>
-    </row>
-    <row r="19" spans="2:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="D19" t="s" ph="1">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="6" t="s">
-        <v>297</v>
-      </c>
-      <c r="D20" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" customFormat="1" ht="64.8" customHeight="1" ph="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="6" t="s">
+      <c r="D28" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="6" t="s">
         <v>406</v>
       </c>
-      <c r="D21" t="s" ph="1">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="6" t="s">
-        <v>410</v>
-      </c>
-      <c r="D22" t="s" ph="1">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="6" t="s">
+      <c r="D29" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="6" t="s">
         <v>407</v>
       </c>
-      <c r="D23" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" customFormat="1" ht="45.6" customHeight="1" ph="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="6" t="s">
+      <c r="D30" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="6" t="s">
         <v>403</v>
       </c>
-      <c r="D24" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="6" t="s">
-        <v>404</v>
-      </c>
-      <c r="D25" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="6" t="s">
-        <v>408</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="D31" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="27" spans="2:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="6" t="s">
-        <v>409</v>
-      </c>
-      <c r="D27" t="s">
+    <row r="32" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="D32" t="s">
         <v>416</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="6" t="s">
-        <v>405</v>
-      </c>
-      <c r="D28" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="6" t="s">
-        <v>420</v>
-      </c>
-      <c r="D29" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="D30" t="s" ph="1">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="D31" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="D32" t="s" ph="1">
-        <v>422</v>
       </c>
     </row>
     <row r="33" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>328</v>
+        <v>296</v>
       </c>
       <c r="D33" t="s" ph="1">
-        <v>294</v>
+        <v>417</v>
       </c>
     </row>
     <row r="34" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D34" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D35" t="s" ph="1">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D36" t="s" ph="1">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="35" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="6"/>
-      <c r="C35"/>
-      <c r="D35"/>
-    </row>
-    <row r="36" spans="1:4" ht="132" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B39" s="6" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="132" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>8</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B41" s="6" t="s">
         <v>293</v>
-      </c>
-      <c r="C36" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>4</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="C37" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B38" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D38" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B39" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D39" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B40" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D40" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>99</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
       </c>
       <c r="D41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B43" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D43" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B44" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D44" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B45" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D45" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C46" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="6"/>
-    </row>
-    <row r="43" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="6"/>
-    </row>
-    <row r="46" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="6"/>
     </row>
     <row r="47" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B47" s="6"/>
     </row>
-    <row r="48" spans="1:4" customFormat="1" ph="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B48" s="6"/>
     </row>
-    <row r="49" spans="2:2" customFormat="1" ph="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="6"/>
+    <row r="51" spans="2:2" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="6"/>
+    </row>
+    <row r="52" spans="2:2" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B52" s="6"/>
+    </row>
+    <row r="53" spans="2:2" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="6"/>
+    </row>
+    <row r="54" spans="2:2" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B54" s="6"/>
+    </row>
+    <row r="55" spans="2:2" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B55" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -9451,7 +9528,7 @@
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -9459,7 +9536,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -9518,7 +9595,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -9596,7 +9673,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -9605,29 +9682,29 @@
     </row>
     <row r="30" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C30" ph="1"/>
       <c r="D30" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C31" ph="1"/>
       <c r="D31" t="s" ph="1">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C32" ph="1"/>
       <c r="D32" t="s" ph="1">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -10132,7 +10209,7 @@
     <row r="86" spans="4:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="D86" ph="1"/>
     </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="4:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="D87" ph="1"/>
     </row>
   </sheetData>
@@ -10171,7 +10248,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -10195,7 +10272,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -10230,7 +10307,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -10302,7 +10379,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -10315,12 +10392,12 @@
     </row>
     <row r="22" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="4" customFormat="1" ht="39.6" x14ac:dyDescent="0.2">
@@ -10328,7 +10405,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C25" s="4" ph="1"/>
       <c r="D25" s="4" t="s" ph="1">
@@ -10337,44 +10414,44 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="D27" t="s">
         <v>392</v>
-      </c>
-      <c r="D27" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D28" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D29" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D30" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
win11ja: test internal link
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB74853-1626-4FC5-BF0F-E4AF0E38704A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F614B9E-1C66-4EF3-AA1D-A7168FA5E304}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7710,8 +7710,8 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>&lt;h2 name="keyboard_layout"&gt;キーボードのレイアウト確認&lt;/h2&gt;</t>
-    <rPh sb="38" eb="40">
+    <t>&lt;h2&gt;&lt;a name="keyboard_layout"&gt;キーボードのレイアウト確認&lt;/a&gt;&lt;/h2&gt;</t>
+    <rPh sb="41" eb="43">
       <t>カクニン</t>
     </rPh>
     <phoneticPr fontId="1"/>
@@ -8751,13 +8751,13 @@
   <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="60.21875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="63.33203125" style="6" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
     <col min="4" max="4" width="30.6640625" customWidth="1"/>
   </cols>
@@ -9016,7 +9016,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
         <v>425</v>
       </c>

</xml_diff>

<commit_message>
win11ja: not name but id
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F614B9E-1C66-4EF3-AA1D-A7168FA5E304}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A4B756-B40D-4B23-9FBE-EB88BA2A5198}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7696,22 +7696,22 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>&lt;h2 name="spec"&gt;PCのスペック確認&lt;/h2&gt;</t>
-    <rPh sb="23" eb="25">
+    <t>&lt;h2 id="spec"&gt;OneDriveのリンク解除&lt;/h2&gt;</t>
+    <rPh sb="26" eb="28">
+      <t>カイジョ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2 id="keyboard_layout"&gt;キーボードのレイアウト確認&lt;/h2&gt;</t>
+    <rPh sb="36" eb="38">
       <t>カクニン</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>&lt;h2 name="spec"&gt;OneDriveのリンク解除&lt;/h2&gt;</t>
-    <rPh sb="28" eb="30">
-      <t>カイジョ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&lt;h2&gt;&lt;a name="keyboard_layout"&gt;キーボードのレイアウト確認&lt;/a&gt;&lt;/h2&gt;</t>
-    <rPh sb="41" eb="43">
+    <t>&lt;h2 id="spec"&gt;PCのスペック確認&lt;/h2&gt;</t>
+    <rPh sb="21" eb="23">
       <t>カクニン</t>
     </rPh>
     <phoneticPr fontId="1"/>
@@ -8750,8 +8750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8801,7 +8801,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
@@ -8888,7 +8888,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="22" spans="2:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -9016,9 +9016,9 @@
         <v>334</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="132" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
win11ja: fix wrong id
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A4B756-B40D-4B23-9FBE-EB88BA2A5198}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E3020A-119A-4991-AAFD-0A17BDC82AD6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7696,13 +7696,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>&lt;h2 id="spec"&gt;OneDriveのリンク解除&lt;/h2&gt;</t>
-    <rPh sb="26" eb="28">
-      <t>カイジョ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>&lt;h2 id="keyboard_layout"&gt;キーボードのレイアウト確認&lt;/h2&gt;</t>
     <rPh sb="36" eb="38">
       <t>カクニン</t>
@@ -7713,6 +7706,13 @@
     <t>&lt;h2 id="spec"&gt;PCのスペック確認&lt;/h2&gt;</t>
     <rPh sb="21" eb="23">
       <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2 id="onedrive_unlink"&gt;OneDriveのリンク解除&lt;/h2&gt;</t>
+    <rPh sb="37" eb="39">
+      <t>カイジョ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -8750,8 +8750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8801,7 +8801,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
@@ -8888,7 +8888,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
     </row>
     <row r="22" spans="2:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -9018,7 +9018,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="132" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
win11ja: update the image how to open control panel
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E3020A-119A-4991-AAFD-0A17BDC82AD6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77C9048-9EDA-4A6A-82A7-52529A06C487}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -63,9 +63,6 @@
     <t>win10-4-01.svg</t>
   </si>
   <si>
-    <t>&lt;h2&gt;&lt;a name="windows_update"&gt;&lt;/a&gt;Windows Updateの設定&lt;/h2&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;h2&gt;&lt;a name="momiji"&gt;&lt;/a&gt;もみじ (広大学生用ポータルサイト)&lt;/h2&gt; </t>
   </si>
   <si>
@@ -2100,10 +2097,6 @@
     <rPh sb="268" eb="270">
       <t>サクジョ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&lt;h2&gt;ウイルススキャン&lt;/h2&gt;</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -3831,39 +3824,6 @@
     </rPh>
     <rPh sb="41" eb="43">
       <t>ユウコウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Windows Update を使って、WindowsとOfficeがつねに最新版で使えるように設定します。
-さらに、Defenderでのフルスキャン（全てのファイルに対するウィルスチェック）のやり方を確認しておきます。
-&lt;ul&gt;&lt;li&gt;&lt;a href="#windows_update"&gt;Windows Updateの設定&lt;/a&gt;&lt;/li&gt;
-&lt;li&gt;&lt;a href="#defender"&gt;Defenderでのフルスキャン&lt;/a&gt;&lt;/li&gt;
-&lt;li&gt;&lt;a href="#save_bitlocker_key"&gt;BitLocker鍵の保存&lt;/a&gt;&lt;/li&gt;
-&lt;li&gt;&lt;a href="#enable_bitlocker"&gt;(付録)BitLockerの有効化&lt;/a&gt;&lt;/li&gt;
-&lt;/ul&gt;
-この章は、インターネットに接続していれば、広島大学の学生証をもらう前に実施することができます。 
- </t>
-    <rPh sb="265" eb="266">
-      <t>カギ</t>
-    </rPh>
-    <rPh sb="267" eb="269">
-      <t>ホゾン</t>
-    </rPh>
-    <rPh sb="312" eb="314">
-      <t>フロク</t>
-    </rPh>
-    <rPh sb="325" eb="327">
-      <t>ユウコウ</t>
-    </rPh>
-    <rPh sb="327" eb="328">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="349" eb="351">
-      <t>ジタク</t>
-    </rPh>
-    <rPh sb="360" eb="362">
-      <t>セツゾク</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -4597,9 +4557,6 @@
   </t>
   </si>
   <si>
-    <t>win11ja-lope-ctrl.png</t>
-  </si>
-  <si>
     <t>コントロールパネルの表示方法を「カテゴリ」にします。デフォルトではカテゴリになっている筈です。</t>
     <rPh sb="10" eb="12">
       <t>ヒョウジ</t>
@@ -4614,25 +4571,6 @@
   </si>
   <si>
     <t>win11ja-ctrl-disp-mode.png</t>
-  </si>
-  <si>
-    <t>タスクバーのルーペボタン(①)を押して検索フォーム(②)を出し、そこに「control」と入力して、コントロールパネル(③)アプリを起動します。</t>
-    <rPh sb="16" eb="17">
-      <t>オ</t>
-    </rPh>
-    <rPh sb="19" eb="21">
-      <t>ケンサク</t>
-    </rPh>
-    <rPh sb="28" eb="29">
-      <t>ダ</t>
-    </rPh>
-    <rPh sb="44" eb="46">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="65" eb="67">
-      <t>キドウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>コントロールパネルのカテゴリ「システムとセキュリティ」に進みます。</t>
@@ -6249,70 +6187,6 @@
   </si>
   <si>
     <t>win11ja-setting-bitlocker-enabled.png</t>
-  </si>
-  <si>
-    <t>サインインしていないので暗号化が完了していないと言われる場合があります。個人MSアカウントを作ったのにサインインしていないと言われた場合は、ネットワークに接続されていることを確認してボタンを押し、サインインしてみてください。どうしても解消しない場合はトグルスイッチをOFFにしてください。この警告が出ている状態のWindows11では、以降の手順での鍵の保存ができません。</t>
-    <rPh sb="12" eb="15">
-      <t>アンゴウカ</t>
-    </rPh>
-    <rPh sb="16" eb="18">
-      <t>カンリョウ</t>
-    </rPh>
-    <rPh sb="24" eb="25">
-      <t>イ</t>
-    </rPh>
-    <rPh sb="28" eb="30">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="36" eb="38">
-      <t>コジン</t>
-    </rPh>
-    <rPh sb="46" eb="47">
-      <t>ツク</t>
-    </rPh>
-    <rPh sb="62" eb="63">
-      <t>イ</t>
-    </rPh>
-    <rPh sb="66" eb="68">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="77" eb="79">
-      <t>セツゾク</t>
-    </rPh>
-    <rPh sb="87" eb="89">
-      <t>カクニン</t>
-    </rPh>
-    <rPh sb="95" eb="96">
-      <t>オ</t>
-    </rPh>
-    <rPh sb="117" eb="119">
-      <t>カイショウ</t>
-    </rPh>
-    <rPh sb="122" eb="124">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="146" eb="148">
-      <t>ケイコク</t>
-    </rPh>
-    <rPh sb="149" eb="150">
-      <t>デ</t>
-    </rPh>
-    <rPh sb="153" eb="155">
-      <t>ジョウタイ</t>
-    </rPh>
-    <rPh sb="168" eb="170">
-      <t>イコウ</t>
-    </rPh>
-    <rPh sb="171" eb="173">
-      <t>テジュン</t>
-    </rPh>
-    <rPh sb="175" eb="176">
-      <t>カギ</t>
-    </rPh>
-    <rPh sb="177" eb="179">
-      <t>ホゾン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>Windows11のプリインストールモデルでは「デバイスの暗号化」が最初から有効になっていることが多いです。以降の手続きに沿ってBitLocker鍵を保存しましょう。</t>
@@ -7713,6 +7587,143 @@
     <t>&lt;h2 id="onedrive_unlink"&gt;OneDriveのリンク解除&lt;/h2&gt;</t>
     <rPh sb="37" eb="39">
       <t>カイジョ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Windows Update を使って、WindowsとOfficeがつねに最新版で使えるように設定します。
+さらに、Defenderでのフルスキャン（全てのファイルに対するウィルスチェック）のやり方を確認しておきます。
+&lt;ul&gt;
+&lt;li&gt;&lt;a href="#windows_update"&gt;Windows Updateの設定&lt;/a&gt;&lt;/li&gt;
+&lt;li&gt;&lt;a href="#defender"&gt;Defenderでのフルスキャン&lt;/a&gt;&lt;/li&gt;
+&lt;li&gt;&lt;a href="#save_bitlocker_key"&gt;BitLocker鍵の保存&lt;/a&gt;&lt;/li&gt;
+&lt;li&gt;&lt;a href="#enable_bitlocker"&gt;(付録)BitLockerの有効化&lt;/a&gt;&lt;/li&gt;
+&lt;/ul&gt;
+この章は、インターネットに接続していれば、広島大学の学生証をもらう前に実施することができます。 
+ </t>
+    <rPh sb="266" eb="267">
+      <t>カギ</t>
+    </rPh>
+    <rPh sb="268" eb="270">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="313" eb="315">
+      <t>フロク</t>
+    </rPh>
+    <rPh sb="326" eb="328">
+      <t>ユウコウ</t>
+    </rPh>
+    <rPh sb="328" eb="329">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="350" eb="352">
+      <t>ジタク</t>
+    </rPh>
+    <rPh sb="361" eb="363">
+      <t>セツゾク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2 id="windows_update"&gt;Windows Updateの設定&lt;/h2&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2 id="defender"&gt;ウイルススキャン&lt;/h2&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>サインインしていないので暗号化が完了していないと言われる場合があります。個人MSアカウントを作ったのにサインインしていないと言われた場合は、ネットワークに接続されていることを確認してボタンを押し、サインインしてみてください。どうしても解消しない場合は「デバイスの暗号化」のトグルスイッチをオフにしてください。この警告が出ている状態のWindows11では、以降の手順での鍵の保存ができません。</t>
+    <rPh sb="12" eb="15">
+      <t>アンゴウカ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>カンリョウ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>イ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>コジン</t>
+    </rPh>
+    <rPh sb="46" eb="47">
+      <t>ツク</t>
+    </rPh>
+    <rPh sb="62" eb="63">
+      <t>イ</t>
+    </rPh>
+    <rPh sb="66" eb="68">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="77" eb="79">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="87" eb="89">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="95" eb="96">
+      <t>オ</t>
+    </rPh>
+    <rPh sb="117" eb="119">
+      <t>カイショウ</t>
+    </rPh>
+    <rPh sb="122" eb="124">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="131" eb="134">
+      <t>アンゴウカ</t>
+    </rPh>
+    <rPh sb="156" eb="158">
+      <t>ケイコク</t>
+    </rPh>
+    <rPh sb="159" eb="160">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="163" eb="165">
+      <t>ジョウタイ</t>
+    </rPh>
+    <rPh sb="178" eb="180">
+      <t>イコウ</t>
+    </rPh>
+    <rPh sb="181" eb="183">
+      <t>テジュン</t>
+    </rPh>
+    <rPh sb="185" eb="186">
+      <t>カギ</t>
+    </rPh>
+    <rPh sb="187" eb="189">
+      <t>ホゾン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-open-ctrlpanel.png</t>
+  </si>
+  <si>
+    <t>スタートボタン(①)を押して検索フォーム(②)に「control panel」と入力していると、コントロールパネルが候補として出てくるので「開く」(③)をクリックしてコントロールパネルを起動します。</t>
+    <rPh sb="11" eb="12">
+      <t>オ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="39" eb="41">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t>コウホ</t>
+    </rPh>
+    <rPh sb="63" eb="64">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="70" eb="71">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="92" eb="94">
+      <t>キドウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -8155,7 +8166,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8171,7 +8182,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -8179,7 +8190,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -8193,7 +8204,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8231,7 +8242,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -8239,7 +8250,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -8255,7 +8266,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="304.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -8263,7 +8274,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -8277,13 +8288,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C7" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -8291,21 +8302,21 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
@@ -8313,13 +8324,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="105.6" ph="1" x14ac:dyDescent="0.2">
@@ -8327,24 +8338,24 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
@@ -8352,13 +8363,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
@@ -8366,13 +8377,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C14" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -8380,32 +8391,32 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C15" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>298</v>
+        <v>293</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -8413,238 +8424,238 @@
         <v>4</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C25" t="s" ph="1">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="26" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="C26" t="s" ph="1">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D26" t="s" ph="1">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="C27" t="s" ph="1">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D27" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="C28" t="s" ph="1">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D28" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="C29" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D29" t="s" ph="1">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="C30" t="s" ph="1">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D30" t="s" ph="1">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C31" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D31" t="s" ph="1">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C32" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D32" t="s" ph="1">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C33" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D33" t="s" ph="1">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D34" t="s" ph="1">
-        <v>301</v>
+        <v>296</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="C35" t="s" ph="1">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D35" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="D36" t="s" ph="1">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="37" spans="2:5" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="C37" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D37" t="s" ph="1">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C38" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D38" t="s" ph="1">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="2:5" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C39" t="s" ph="1">
+        <v>87</v>
+      </c>
+      <c r="D39" t="s" ph="1">
         <v>88</v>
-      </c>
-      <c r="D39" t="s" ph="1">
-        <v>89</v>
       </c>
     </row>
     <row r="40" spans="2:5" ph="1" x14ac:dyDescent="0.2">
@@ -8750,7 +8761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -8767,7 +8778,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
@@ -8775,7 +8786,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -8791,234 +8802,234 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="132" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C10" t="s" ph="1">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E10" ph="1"/>
     </row>
     <row r="11" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C11" t="s" ph="1">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:5" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C12" t="s" ph="1">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:5" customFormat="1" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="15" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>326</v>
+        <v>321</v>
       </c>
     </row>
     <row r="16" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>307</v>
+        <v>302</v>
       </c>
     </row>
     <row r="17" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>308</v>
+        <v>303</v>
       </c>
     </row>
     <row r="18" spans="2:4" customFormat="1" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B18" s="6" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>319</v>
+        <v>314</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
     </row>
     <row r="22" spans="2:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>294</v>
+        <v>289</v>
       </c>
     </row>
     <row r="23" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="D23" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
     </row>
     <row r="24" spans="2:4" customFormat="1" ht="64.8" customHeight="1" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>322</v>
+        <v>317</v>
       </c>
     </row>
     <row r="25" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>409</v>
+        <v>403</v>
       </c>
     </row>
     <row r="26" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="D26" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
     </row>
     <row r="27" spans="2:4" customFormat="1" ht="45.6" customHeight="1" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="D27" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
     </row>
     <row r="28" spans="2:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="D28" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
     </row>
     <row r="29" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="D29" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
     </row>
     <row r="30" spans="2:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="D30" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
     </row>
     <row r="31" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="D31" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
     </row>
     <row r="32" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="D32" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
     </row>
     <row r="33" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="D33" t="s" ph="1">
-        <v>417</v>
+        <v>411</v>
       </c>
     </row>
     <row r="34" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="D34" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
     </row>
     <row r="35" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="D35" t="s" ph="1">
-        <v>420</v>
+        <v>414</v>
       </c>
     </row>
     <row r="36" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D36" t="s" ph="1">
-        <v>294</v>
+        <v>289</v>
       </c>
     </row>
     <row r="37" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -9026,7 +9037,7 @@
         <v>8</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
@@ -9040,37 +9051,37 @@
         <v>4</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C42" t="s">
         <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B43" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D43" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B44" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B45" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D45" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9078,13 +9089,13 @@
         <v>4</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C46" t="s">
         <v>4</v>
       </c>
       <c r="D46" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -9119,8 +9130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -9136,7 +9147,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -9144,7 +9155,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9160,15 +9171,15 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="132" x14ac:dyDescent="0.2">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="145.19999999999999" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>243</v>
+        <v>420</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -9179,7 +9190,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>11</v>
+        <v>421</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9187,29 +9198,29 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="D11" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D12" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -9217,13 +9228,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -9231,7 +9242,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>114</v>
+        <v>422</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -9242,7 +9253,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -9253,21 +9264,21 @@
         <v>4</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D19" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -9275,13 +9286,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9289,13 +9300,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9303,13 +9314,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -9322,149 +9333,149 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="82.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="D27" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="D28" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D29" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="67.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>349</v>
+        <v>423</v>
       </c>
       <c r="D30" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="D31" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>276</v>
+        <v>425</v>
       </c>
       <c r="D33" t="s">
-        <v>273</v>
+        <v>424</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D34" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D35" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D36" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="50.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D38" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D39" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="6" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D40" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D41" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="46.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="6" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="D42" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="131.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="6" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" s="6" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="6" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="D47" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
     </row>
     <row r="48" spans="2:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9479,7 +9490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4600B07F-730C-4FC5-BA07-70D58F12A670}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
@@ -9496,7 +9507,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
     </row>
     <row r="2" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -9504,7 +9515,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
     </row>
     <row r="3" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -9520,7 +9531,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
     </row>
     <row r="5" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -9528,7 +9539,7 @@
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -9536,7 +9547,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -9544,50 +9555,50 @@
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="D10" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="D11" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="D12" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="D13" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="D14" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="D15" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -9595,7 +9606,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -9604,68 +9615,68 @@
     </row>
     <row r="19" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="C19" ph="1"/>
       <c r="D19" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="132" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="C20" ph="1"/>
       <c r="D20" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D21" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D22" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D23" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D24" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D25" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D26" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
@@ -9673,7 +9684,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -9682,29 +9693,29 @@
     </row>
     <row r="30" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="C30" ph="1"/>
       <c r="D30" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="C31" ph="1"/>
       <c r="D31" t="s" ph="1">
-        <v>379</v>
+        <v>373</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="C32" ph="1"/>
       <c r="D32" t="s" ph="1">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -9762,7 +9773,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -9770,7 +9781,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9786,7 +9797,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -9797,7 +9808,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -9816,12 +9827,12 @@
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -9829,29 +9840,29 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9859,7 +9870,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -9867,18 +9878,18 @@
     </row>
     <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D15" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D16" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -9886,13 +9897,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="198" x14ac:dyDescent="0.2">
@@ -9900,18 +9911,18 @@
         <v>4</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9919,21 +9930,21 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D21" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9941,21 +9952,21 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D23" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9963,13 +9974,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -9977,7 +9988,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -9993,40 +10004,40 @@
     </row>
     <row r="28" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D29" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D30" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -10034,7 +10045,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -10053,80 +10064,80 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D36" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D37" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D39" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D40" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D41" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C42" t="s">
         <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C43" t="s">
         <v>4</v>
       </c>
       <c r="D43" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -10134,7 +10145,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -10142,7 +10153,7 @@
     </row>
     <row r="47" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C47" t="s">
         <v>4</v>
@@ -10153,7 +10164,7 @@
     </row>
     <row r="48" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C48" t="s">
         <v>7</v>
@@ -10162,21 +10173,21 @@
     </row>
     <row r="49" spans="2:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B49" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D49" t="s" ph="1">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="50" spans="2:4" ht="132" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C50" t="s">
         <v>7</v>
       </c>
       <c r="D50" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="51" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -10240,7 +10251,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -10248,7 +10259,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -10264,7 +10275,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -10272,7 +10283,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -10288,7 +10299,7 @@
     </row>
     <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -10296,18 +10307,18 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -10315,21 +10326,21 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -10337,13 +10348,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -10351,13 +10362,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -10365,13 +10376,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -10379,7 +10390,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -10392,12 +10403,12 @@
     </row>
     <row r="22" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="4" customFormat="1" ht="39.6" x14ac:dyDescent="0.2">
@@ -10405,53 +10416,53 @@
         <v>4</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="C25" s="4" ph="1"/>
       <c r="D25" s="4" t="s" ph="1">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="D27" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="D28" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="D29" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="D30" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
     </row>
   </sheetData>
@@ -10482,7 +10493,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -10490,7 +10501,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -10506,22 +10517,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -10529,7 +10540,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -10540,7 +10551,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -10554,13 +10565,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -10568,21 +10579,21 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -10590,12 +10601,12 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -10603,33 +10614,33 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D18" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D19" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -10660,7 +10671,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -10668,7 +10679,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -10684,22 +10695,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -10707,7 +10718,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -10723,15 +10734,15 @@
     </row>
     <row r="14" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.2">
@@ -10739,10 +10750,10 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D16" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -10750,39 +10761,39 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D17" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D19" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -10790,36 +10801,36 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D23" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -10830,180 +10841,180 @@
     </row>
     <row r="30" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D30" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D31" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D32" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C34" t="s">
         <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C35" t="s">
         <v>7</v>
       </c>
       <c r="D35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C36" t="s">
         <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C37" t="s">
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C38" t="s">
         <v>7</v>
       </c>
       <c r="D38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C39" t="s">
         <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C41" t="s">
         <v>7</v>
       </c>
       <c r="D41" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C42" t="s">
         <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C43" t="s">
         <v>7</v>
       </c>
       <c r="D43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C44" t="s">
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C45" t="s">
         <v>7</v>
       </c>
       <c r="D45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="2:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C46" t="s">
         <v>7</v>
       </c>
       <c r="D46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
win11ja: drop Teams instr.
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CE3857-5AF7-48C7-AB78-BC3B0B74E9B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802382C7-3203-4249-99B6-6BF25D2AF08C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="391">
   <si>
     <t>header1</t>
   </si>
@@ -184,37 +184,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>サインインしたアカウントには、そのアカウントのネット接続状態が表示されます。「会議」に出席している場合は、この接続状態が「会議中」になります。</t>
-    <rPh sb="26" eb="28">
-      <t>セツゾク</t>
-    </rPh>
-    <rPh sb="28" eb="30">
-      <t>ジョウタイ</t>
-    </rPh>
-    <rPh sb="31" eb="33">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="39" eb="41">
-      <t>カイギ</t>
-    </rPh>
-    <rPh sb="43" eb="45">
-      <t>シュッセキ</t>
-    </rPh>
-    <rPh sb="49" eb="51">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="55" eb="57">
-      <t>セツゾク</t>
-    </rPh>
-    <rPh sb="57" eb="59">
-      <t>ジョウタイ</t>
-    </rPh>
-    <rPh sb="61" eb="64">
-      <t>カイギチュウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>&lt;p class="spl"&gt;※学生番号と、学生番号と一緒にもらえる「広大パスワード」が必要です。&lt;/p&gt;</t>
     <rPh sb="16" eb="18">
       <t>ガクセイ</t>
@@ -304,903 +273,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ch7-teams-signined0.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ch7-teams-my-status.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ch7-teams-list-teams.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>チームとは、特定の教職員や学生をまとめたグループのことを指します。多くの授業では、「もみじ」の履修手続きが締め切られた後、それを反映したチームが作られ、オンライン授業を実施するものについては皆さんが授業別のチームに所属した状態になる筈です。必修科目であっても履修手続きの前に自動的に登録されるわけではないので、「自分が履修すべき科目だから、自動的にTeamsに先に登録してくれる」というわけではないことに注意してください。</t>
-    <rPh sb="6" eb="8">
-      <t>トクテイ</t>
-    </rPh>
-    <rPh sb="9" eb="12">
-      <t>キョウショクイン</t>
-    </rPh>
-    <rPh sb="13" eb="15">
-      <t>ガクセイ</t>
-    </rPh>
-    <rPh sb="28" eb="29">
-      <t>サ</t>
-    </rPh>
-    <rPh sb="33" eb="34">
-      <t>オオ</t>
-    </rPh>
-    <rPh sb="36" eb="38">
-      <t>ジュギョウ</t>
-    </rPh>
-    <rPh sb="47" eb="49">
-      <t>リシュウ</t>
-    </rPh>
-    <rPh sb="49" eb="51">
-      <t>テツヅ</t>
-    </rPh>
-    <rPh sb="53" eb="54">
-      <t>シ</t>
-    </rPh>
-    <rPh sb="55" eb="56">
-      <t>キ</t>
-    </rPh>
-    <rPh sb="59" eb="60">
-      <t>アト</t>
-    </rPh>
-    <rPh sb="64" eb="66">
-      <t>ハンエイ</t>
-    </rPh>
-    <rPh sb="72" eb="73">
-      <t>ツク</t>
-    </rPh>
-    <rPh sb="81" eb="83">
-      <t>ジュギョウ</t>
-    </rPh>
-    <rPh sb="84" eb="86">
-      <t>ジッシ</t>
-    </rPh>
-    <rPh sb="95" eb="96">
-      <t>ミナ</t>
-    </rPh>
-    <rPh sb="99" eb="101">
-      <t>ジュギョウ</t>
-    </rPh>
-    <rPh sb="101" eb="102">
-      <t>ベツ</t>
-    </rPh>
-    <rPh sb="107" eb="109">
-      <t>ショゾク</t>
-    </rPh>
-    <rPh sb="111" eb="113">
-      <t>ジョウタイ</t>
-    </rPh>
-    <rPh sb="116" eb="117">
-      <t>ハズ</t>
-    </rPh>
-    <rPh sb="120" eb="122">
-      <t>ヒッシュウ</t>
-    </rPh>
-    <rPh sb="122" eb="124">
-      <t>カモク</t>
-    </rPh>
-    <rPh sb="129" eb="131">
-      <t>リシュウ</t>
-    </rPh>
-    <rPh sb="131" eb="133">
-      <t>テツヅ</t>
-    </rPh>
-    <rPh sb="135" eb="136">
-      <t>マエ</t>
-    </rPh>
-    <rPh sb="137" eb="140">
-      <t>ジドウテキ</t>
-    </rPh>
-    <rPh sb="141" eb="143">
-      <t>トウロク</t>
-    </rPh>
-    <rPh sb="156" eb="158">
-      <t>ジブン</t>
-    </rPh>
-    <rPh sb="159" eb="161">
-      <t>リシュウ</t>
-    </rPh>
-    <rPh sb="164" eb="166">
-      <t>カモク</t>
-    </rPh>
-    <rPh sb="170" eb="173">
-      <t>ジドウテキ</t>
-    </rPh>
-    <rPh sb="180" eb="181">
-      <t>サキ</t>
-    </rPh>
-    <rPh sb="182" eb="184">
-      <t>トウロク</t>
-    </rPh>
-    <rPh sb="202" eb="204">
-      <t>チュウイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ch7-teams-selected-team.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Teamsの機能のうち、オンライン授業で特に使われる機能は「チャット」と「チーム」、チームの中の「チャネル」、チャネルの中の「会議」です。「カレンダー」機能がありますが、大学側から履修状況に応じた更新などをかけることはないので、必要であれば自分で設定するようにしてください。</t>
-    <rPh sb="6" eb="8">
-      <t>キノウ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>ジュギョウ</t>
-    </rPh>
-    <rPh sb="20" eb="21">
-      <t>トク</t>
-    </rPh>
-    <rPh sb="22" eb="23">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>キノウ</t>
-    </rPh>
-    <rPh sb="46" eb="47">
-      <t>ナカ</t>
-    </rPh>
-    <rPh sb="60" eb="61">
-      <t>ナカ</t>
-    </rPh>
-    <rPh sb="63" eb="65">
-      <t>カイギ</t>
-    </rPh>
-    <rPh sb="76" eb="78">
-      <t>キノウ</t>
-    </rPh>
-    <rPh sb="85" eb="87">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="87" eb="88">
-      <t>ガワ</t>
-    </rPh>
-    <rPh sb="90" eb="92">
-      <t>リシュウ</t>
-    </rPh>
-    <rPh sb="92" eb="94">
-      <t>ジョウキョウ</t>
-    </rPh>
-    <rPh sb="95" eb="96">
-      <t>オウ</t>
-    </rPh>
-    <rPh sb="98" eb="100">
-      <t>コウシン</t>
-    </rPh>
-    <rPh sb="114" eb="116">
-      <t>ヒツヨウ</t>
-    </rPh>
-    <rPh sb="120" eb="122">
-      <t>ジブン</t>
-    </rPh>
-    <rPh sb="123" eb="125">
-      <t>セッテイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ch7-teams-features.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>自分が所属するチームから一つチームを選ぶと、そのチームのチャネル一覧を見ることができます。その一つのチャネルを選んでチャットしたり、「会議」を行ったりします。たとえばこの授業は週1回実施されるたびに新たにチャネルを作っています。</t>
-    <rPh sb="0" eb="2">
-      <t>ジブン</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ショゾク</t>
-    </rPh>
-    <rPh sb="12" eb="13">
-      <t>ヒト</t>
-    </rPh>
-    <rPh sb="18" eb="19">
-      <t>エラ</t>
-    </rPh>
-    <rPh sb="32" eb="34">
-      <t>イチラン</t>
-    </rPh>
-    <rPh sb="35" eb="36">
-      <t>ミ</t>
-    </rPh>
-    <rPh sb="85" eb="87">
-      <t>ジュギョウ</t>
-    </rPh>
-    <rPh sb="88" eb="89">
-      <t>シュウ</t>
-    </rPh>
-    <rPh sb="90" eb="91">
-      <t>カイ</t>
-    </rPh>
-    <rPh sb="91" eb="93">
-      <t>ジッシ</t>
-    </rPh>
-    <rPh sb="99" eb="100">
-      <t>アラ</t>
-    </rPh>
-    <rPh sb="107" eb="108">
-      <t>ツク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ch7-teams-tvmeeting-scheduled.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>オンライン授業のうち、双方向(所定の授業時間に、教員も受講生もネットワークに接続して同時に進めるもの)のものがこの「会議」機能で行われます。授業時間を反映して最初から「会議」がスケジュールされている場合もありますが、先に授業をTeamsにスケジュールせず、授業時間になって教員が手動で開始する場合も多いです。スケジュールにないことが休講であると勘違いしないようにしてください。教員のアカウントの状態も確認することが望ましいです。これはスケジュールされている例ですが、スケジュールなしで開始されている場合は同様の表示がチャットのタイムラインに「会議中」と出ます。</t>
-    <rPh sb="5" eb="7">
-      <t>ジュギョウ</t>
-    </rPh>
-    <rPh sb="11" eb="14">
-      <t>ソウホウコウ</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>ショテイ</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>ジュギョウ</t>
-    </rPh>
-    <rPh sb="20" eb="22">
-      <t>ジカン</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>キョウイン</t>
-    </rPh>
-    <rPh sb="27" eb="30">
-      <t>ジュコウセイ</t>
-    </rPh>
-    <rPh sb="38" eb="40">
-      <t>セツゾク</t>
-    </rPh>
-    <rPh sb="42" eb="44">
-      <t>ドウジ</t>
-    </rPh>
-    <rPh sb="45" eb="46">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="58" eb="60">
-      <t>カイギ</t>
-    </rPh>
-    <rPh sb="61" eb="63">
-      <t>キノウ</t>
-    </rPh>
-    <rPh sb="64" eb="65">
-      <t>オコナ</t>
-    </rPh>
-    <rPh sb="70" eb="72">
-      <t>ジュギョウ</t>
-    </rPh>
-    <rPh sb="72" eb="74">
-      <t>ジカン</t>
-    </rPh>
-    <rPh sb="75" eb="77">
-      <t>ハンエイ</t>
-    </rPh>
-    <rPh sb="79" eb="81">
-      <t>サイショ</t>
-    </rPh>
-    <rPh sb="84" eb="86">
-      <t>カイギ</t>
-    </rPh>
-    <rPh sb="99" eb="101">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="108" eb="109">
-      <t>サキ</t>
-    </rPh>
-    <rPh sb="110" eb="112">
-      <t>ジュギョウ</t>
-    </rPh>
-    <rPh sb="128" eb="130">
-      <t>ジュギョウ</t>
-    </rPh>
-    <rPh sb="130" eb="132">
-      <t>ジカン</t>
-    </rPh>
-    <rPh sb="136" eb="138">
-      <t>キョウイン</t>
-    </rPh>
-    <rPh sb="139" eb="141">
-      <t>シュドウ</t>
-    </rPh>
-    <rPh sb="142" eb="144">
-      <t>カイシ</t>
-    </rPh>
-    <rPh sb="146" eb="148">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="149" eb="150">
-      <t>オオ</t>
-    </rPh>
-    <rPh sb="166" eb="168">
-      <t>キュウコウ</t>
-    </rPh>
-    <rPh sb="172" eb="174">
-      <t>カンチガ</t>
-    </rPh>
-    <rPh sb="188" eb="190">
-      <t>キョウイン</t>
-    </rPh>
-    <rPh sb="197" eb="199">
-      <t>ジョウタイ</t>
-    </rPh>
-    <rPh sb="200" eb="202">
-      <t>カクニン</t>
-    </rPh>
-    <rPh sb="207" eb="208">
-      <t>ノゾ</t>
-    </rPh>
-    <rPh sb="228" eb="229">
-      <t>レイ</t>
-    </rPh>
-    <rPh sb="242" eb="244">
-      <t>カイシ</t>
-    </rPh>
-    <rPh sb="249" eb="251">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="252" eb="254">
-      <t>ドウヨウ</t>
-    </rPh>
-    <rPh sb="255" eb="257">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="271" eb="274">
-      <t>カイギチュウ</t>
-    </rPh>
-    <rPh sb="276" eb="277">
-      <t>デ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ch7-teams-tvmeeting-before-enter.png</t>
-  </si>
-  <si>
-    <t>ch7-teams-tvmeeting-before-enter-config.png</t>
-  </si>
-  <si>
-    <t>ch7-teams-tvmeeting-config-after-enter.png</t>
-  </si>
-  <si>
-    <t>ch7-teams-tvmeeting-sharing.png</t>
-  </si>
-  <si>
-    <t>実習系の授業などでは自分のPCの状態をTV会議で相手方に見せるべき状況もあります。この時は、共有ボタンからデスクトップ(複数のモニタを接続している場合に複数出ます)、ウィンドウ(アプリケーションごと)を選ぶことができます。</t>
-    <rPh sb="0" eb="2">
-      <t>ジッシュウ</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>ケイ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>ジュギョウ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>ジブン</t>
-    </rPh>
-    <rPh sb="16" eb="18">
-      <t>ジョウタイ</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>カイギ</t>
-    </rPh>
-    <rPh sb="24" eb="27">
-      <t>アイテガタ</t>
-    </rPh>
-    <rPh sb="28" eb="29">
-      <t>ミ</t>
-    </rPh>
-    <rPh sb="33" eb="35">
-      <t>ジョウキョウ</t>
-    </rPh>
-    <rPh sb="43" eb="44">
-      <t>トキ</t>
-    </rPh>
-    <rPh sb="46" eb="48">
-      <t>キョウユウ</t>
-    </rPh>
-    <rPh sb="60" eb="62">
-      <t>フクスウ</t>
-    </rPh>
-    <rPh sb="67" eb="69">
-      <t>セツゾク</t>
-    </rPh>
-    <rPh sb="73" eb="75">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="76" eb="78">
-      <t>フクスウ</t>
-    </rPh>
-    <rPh sb="78" eb="79">
-      <t>デ</t>
-    </rPh>
-    <rPh sb="101" eb="102">
-      <t>エラ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ch7-teams-indicator.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>サインイン済みだとこのような状態になります。</t>
-    <rPh sb="5" eb="6">
-      <t>ズ</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>ジョウタイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ch7-teams-signout-from-mainmenu.png</t>
-  </si>
-  <si>
-    <t>ch7-teams-selected-channel-chat.png</t>
-  </si>
-  <si>
-    <t>chartn</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>主催者が開始していない「会議」でも、出席することができます。「会議」に出席しようとすると、すぐ会議出席で画像や音声が流れるわけではなく、まずPCの設定画面になります。実際に接続する前に、手元のPCのカメラのON/OFF、マイクのON/OFF、スピーカのON/OFFを設定することができます。</t>
-    <rPh sb="0" eb="3">
-      <t>シュサイシャ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>カイシ</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>カイギ</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>シュッセキ</t>
-    </rPh>
-    <rPh sb="31" eb="33">
-      <t>カイギ</t>
-    </rPh>
-    <rPh sb="35" eb="37">
-      <t>シュッセキ</t>
-    </rPh>
-    <rPh sb="47" eb="49">
-      <t>カイギ</t>
-    </rPh>
-    <rPh sb="49" eb="51">
-      <t>シュッセキ</t>
-    </rPh>
-    <rPh sb="52" eb="54">
-      <t>ガゾウ</t>
-    </rPh>
-    <rPh sb="55" eb="57">
-      <t>オンセイ</t>
-    </rPh>
-    <rPh sb="58" eb="59">
-      <t>ナガ</t>
-    </rPh>
-    <rPh sb="73" eb="75">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="75" eb="77">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="83" eb="85">
-      <t>ジッサイ</t>
-    </rPh>
-    <rPh sb="86" eb="88">
-      <t>セツゾク</t>
-    </rPh>
-    <rPh sb="90" eb="91">
-      <t>マエ</t>
-    </rPh>
-    <rPh sb="93" eb="95">
-      <t>テモト</t>
-    </rPh>
-    <rPh sb="133" eb="135">
-      <t>セッテイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Surfaceをドックにつないでいたり、あるいはBluetoothで外部のヘッドセットを使っている場合などには、複数のマイクやスピーカがあるので、カスタムセットアップを開いて自分が使いたいものが選ばれているように確認する習慣をつけましょう。</t>
-    <rPh sb="34" eb="36">
-      <t>ガイブ</t>
-    </rPh>
-    <rPh sb="44" eb="45">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="49" eb="51">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="56" eb="58">
-      <t>フクスウ</t>
-    </rPh>
-    <rPh sb="84" eb="85">
-      <t>ヒラ</t>
-    </rPh>
-    <rPh sb="87" eb="89">
-      <t>ジブン</t>
-    </rPh>
-    <rPh sb="90" eb="91">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="97" eb="98">
-      <t>エラ</t>
-    </rPh>
-    <rPh sb="106" eb="108">
-      <t>カクニン</t>
-    </rPh>
-    <rPh sb="110" eb="112">
-      <t>シュウカン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>会議に入ると出席者のアイコンが並ぶ画面に変わります。会議中も、カメラのON/OFF, マイクのON/OFFを切り替えることができます。吹き出しのアイコンをクリックすると、このTV会議のウィンドウの中にテキストチャットのタイムラインが表示されるようになります。その隣の「…」を展開して「デバイスの設定」を開くと、会議に入った後でもカメラ機器やマイク機器を取り換えることができます。接続してみたらどうもスピーカで聞いていると会議がおかしなことになる、などの問題がある時は変更しましょう。</t>
-    <rPh sb="0" eb="2">
-      <t>カイギ</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>ハイ</t>
-    </rPh>
-    <rPh sb="6" eb="9">
-      <t>シュッセキシャ</t>
-    </rPh>
-    <rPh sb="15" eb="16">
-      <t>ナラ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="20" eb="21">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="26" eb="29">
-      <t>カイギチュウ</t>
-    </rPh>
-    <rPh sb="54" eb="55">
-      <t>キ</t>
-    </rPh>
-    <rPh sb="56" eb="57">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="67" eb="68">
-      <t>フ</t>
-    </rPh>
-    <rPh sb="69" eb="70">
-      <t>ダ</t>
-    </rPh>
-    <rPh sb="89" eb="91">
-      <t>カイギ</t>
-    </rPh>
-    <rPh sb="98" eb="99">
-      <t>ナカ</t>
-    </rPh>
-    <rPh sb="116" eb="118">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="131" eb="132">
-      <t>トナリ</t>
-    </rPh>
-    <rPh sb="137" eb="139">
-      <t>テンカイ</t>
-    </rPh>
-    <rPh sb="147" eb="149">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="151" eb="152">
-      <t>ヒラ</t>
-    </rPh>
-    <rPh sb="155" eb="157">
-      <t>カイギ</t>
-    </rPh>
-    <rPh sb="158" eb="159">
-      <t>ハイ</t>
-    </rPh>
-    <rPh sb="161" eb="162">
-      <t>アト</t>
-    </rPh>
-    <rPh sb="167" eb="169">
-      <t>キキ</t>
-    </rPh>
-    <rPh sb="173" eb="175">
-      <t>キキ</t>
-    </rPh>
-    <rPh sb="176" eb="177">
-      <t>ト</t>
-    </rPh>
-    <rPh sb="178" eb="179">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="189" eb="191">
-      <t>セツゾク</t>
-    </rPh>
-    <rPh sb="204" eb="205">
-      <t>キ</t>
-    </rPh>
-    <rPh sb="210" eb="212">
-      <t>カイギ</t>
-    </rPh>
-    <rPh sb="226" eb="228">
-      <t>モンダイ</t>
-    </rPh>
-    <rPh sb="231" eb="232">
-      <t>トキ</t>
-    </rPh>
-    <rPh sb="233" eb="235">
-      <t>ヘンコウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>このウィンドウを閉じても、裏でTeamsは動いており、chatなどのメッセージを受信しています。通知領域にTeamsのアイコンが出ています。このアイコンをクリックすればもう一度Teamsの画面が開かれます。</t>
-    <rPh sb="86" eb="88">
-      <t>イチド</t>
-    </rPh>
-    <rPh sb="94" eb="96">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="97" eb="98">
-      <t>ヒラ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>会議に出ていなくても、チャットをしていなくても、Teamsの画面を閉じていても、サインインしている状態では、ネットワークに接続していれば、他の人には「連絡可能」な状態として見えています。Teamsの自分のアイコンをクリックして出るメニューからサインアウトすることができます。サインアウトすると通知アイコンも無くなり、チャットで話しかけられても何も通知されなくなります。ただし、Microsoftのサーバ側ではこの間に貴方に話しかけられたチャットが記録されており、再度サインインすると過去の未読のメッセージを読むことができます。</t>
-    <rPh sb="0" eb="2">
-      <t>カイギ</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>デ</t>
-    </rPh>
-    <rPh sb="30" eb="32">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="33" eb="34">
-      <t>ト</t>
-    </rPh>
-    <rPh sb="61" eb="63">
-      <t>セツゾク</t>
-    </rPh>
-    <rPh sb="69" eb="70">
-      <t>ホカ</t>
-    </rPh>
-    <rPh sb="71" eb="72">
-      <t>ヒト</t>
-    </rPh>
-    <rPh sb="75" eb="77">
-      <t>レンラク</t>
-    </rPh>
-    <rPh sb="77" eb="79">
-      <t>カノウ</t>
-    </rPh>
-    <rPh sb="81" eb="83">
-      <t>ジョウタイ</t>
-    </rPh>
-    <rPh sb="86" eb="87">
-      <t>ミ</t>
-    </rPh>
-    <rPh sb="99" eb="101">
-      <t>ジブン</t>
-    </rPh>
-    <rPh sb="113" eb="114">
-      <t>デ</t>
-    </rPh>
-    <rPh sb="148" eb="150">
-      <t>ツウチ</t>
-    </rPh>
-    <rPh sb="155" eb="156">
-      <t>ナ</t>
-    </rPh>
-    <rPh sb="165" eb="166">
-      <t>ハナシ</t>
-    </rPh>
-    <rPh sb="173" eb="174">
-      <t>ナニ</t>
-    </rPh>
-    <rPh sb="175" eb="177">
-      <t>ツウチ</t>
-    </rPh>
-    <rPh sb="203" eb="204">
-      <t>ガワ</t>
-    </rPh>
-    <rPh sb="208" eb="209">
-      <t>アイダ</t>
-    </rPh>
-    <rPh sb="210" eb="212">
-      <t>アナタ</t>
-    </rPh>
-    <rPh sb="213" eb="214">
-      <t>ハナ</t>
-    </rPh>
-    <rPh sb="225" eb="227">
-      <t>キロク</t>
-    </rPh>
-    <rPh sb="233" eb="235">
-      <t>サイド</t>
-    </rPh>
-    <rPh sb="243" eb="245">
-      <t>カコ</t>
-    </rPh>
-    <rPh sb="246" eb="248">
-      <t>ミドク</t>
-    </rPh>
-    <rPh sb="255" eb="256">
-      <t>ヨ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>広島大学でのオンライン授業(同時双方向のもの、また、チャットによる質問相談など)は、主にMicrosoft Teamsを使って行っています。この動作を確認しましょう。履修登録以前に実際に作業できることは限られていますので、必要に応じて参照してください。
-オンライン授業のソフトウェアとしては、Teamsの他にZoomや、YouTube Liveなどもあり、たとえばZoomで行われている授業をTeamsで受講する、といったことはできません。Teams以外を用いる授業の場合は、教員が先に説明する筈ですので、環境設定などは教員の指示を参考にしてください。</t>
-    <rPh sb="0" eb="2">
-      <t>ヒロシマ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>ジュギョウ</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>ドウジ</t>
-    </rPh>
-    <rPh sb="16" eb="19">
-      <t>ソウホウコウ</t>
-    </rPh>
-    <rPh sb="33" eb="35">
-      <t>シツモン</t>
-    </rPh>
-    <rPh sb="35" eb="37">
-      <t>ソウダン</t>
-    </rPh>
-    <rPh sb="42" eb="43">
-      <t>オモ</t>
-    </rPh>
-    <rPh sb="60" eb="61">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="63" eb="64">
-      <t>オコナ</t>
-    </rPh>
-    <rPh sb="72" eb="74">
-      <t>ドウサ</t>
-    </rPh>
-    <rPh sb="75" eb="77">
-      <t>カクニン</t>
-    </rPh>
-    <rPh sb="83" eb="85">
-      <t>リシュウ</t>
-    </rPh>
-    <rPh sb="85" eb="87">
-      <t>トウロク</t>
-    </rPh>
-    <rPh sb="87" eb="89">
-      <t>イゼン</t>
-    </rPh>
-    <rPh sb="90" eb="92">
-      <t>ジッサイ</t>
-    </rPh>
-    <rPh sb="93" eb="95">
-      <t>サギョウ</t>
-    </rPh>
-    <rPh sb="101" eb="102">
-      <t>カギ</t>
-    </rPh>
-    <rPh sb="111" eb="113">
-      <t>ヒツヨウ</t>
-    </rPh>
-    <rPh sb="114" eb="115">
-      <t>オウ</t>
-    </rPh>
-    <rPh sb="117" eb="119">
-      <t>サンショウ</t>
-    </rPh>
-    <rPh sb="132" eb="134">
-      <t>ジュギョウ</t>
-    </rPh>
-    <rPh sb="152" eb="153">
-      <t>ホカ</t>
-    </rPh>
-    <rPh sb="187" eb="188">
-      <t>オコナ</t>
-    </rPh>
-    <rPh sb="193" eb="195">
-      <t>ジュギョウ</t>
-    </rPh>
-    <rPh sb="202" eb="204">
-      <t>ジュコウ</t>
-    </rPh>
-    <rPh sb="225" eb="227">
-      <t>イガイ</t>
-    </rPh>
-    <rPh sb="228" eb="229">
-      <t>モチ</t>
-    </rPh>
-    <rPh sb="231" eb="233">
-      <t>ジュギョウ</t>
-    </rPh>
-    <rPh sb="234" eb="236">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="238" eb="240">
-      <t>キョウイン</t>
-    </rPh>
-    <rPh sb="241" eb="242">
-      <t>サキ</t>
-    </rPh>
-    <rPh sb="243" eb="245">
-      <t>セツメイ</t>
-    </rPh>
-    <rPh sb="247" eb="248">
-      <t>ハズ</t>
-    </rPh>
-    <rPh sb="253" eb="255">
-      <t>カンキョウ</t>
-    </rPh>
-    <rPh sb="255" eb="257">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="260" eb="262">
-      <t>キョウイン</t>
-    </rPh>
-    <rPh sb="263" eb="265">
-      <t>シジ</t>
-    </rPh>
-    <rPh sb="266" eb="268">
-      <t>サンコウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>チャネルの中では、基本的なコミュニケーション方法としてチャットが使われるようになっています。チームの中でチャットした場合には、同じチームに所属する皆さんに見えます。左側のメニューにある「チャット」は、貴方がチャットで入力したことがあるチャネルの一覧が出てくるので、「あるチャネルで会話している最中に、他のチャネルで自分の発言に返事があった」ということに気づくこともできます。
-基本的に授業関係のテキストチャットは自分の都合のよい時間に発言してよいのですが、返事もまた相手の都合のよい時間に返ってくるものなので、即答を求めないようにしましょう。
-このチャット機能は、同じチームに所属してない人とも使うことができます。ただし、アカウント名を持っている人が対象です。相手のアカウントを教えてもらったら、「新しいチャット」で質問することができます。</t>
-    <rPh sb="5" eb="6">
-      <t>ナカ</t>
-    </rPh>
-    <rPh sb="9" eb="12">
-      <t>キホンテキ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>ホウホウ</t>
-    </rPh>
-    <rPh sb="32" eb="33">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="50" eb="51">
-      <t>ナカ</t>
-    </rPh>
-    <rPh sb="58" eb="60">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="63" eb="64">
-      <t>オナ</t>
-    </rPh>
-    <rPh sb="69" eb="71">
-      <t>ショゾク</t>
-    </rPh>
-    <rPh sb="73" eb="74">
-      <t>ミナ</t>
-    </rPh>
-    <rPh sb="77" eb="78">
-      <t>ミ</t>
-    </rPh>
-    <rPh sb="163" eb="165">
-      <t>ヘンジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>win11ja-select-lang.png</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -2572,133 +1644,6 @@
       <t>ゾッコウ</t>
     </rPh>
     <rPh sb="344" eb="345">
-      <t>スス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Microsoft Teamsには「職場または学校用」のものと、「小企業用」のものの2つがあります。自分のPCのタスクバーの検索フォームから「Teams」を検索すると、「学校用Teamsだけが有る」「学校用と小企業用Teamsがある」「小企業用Teamsだけがある」の3つの可能性があります。アイコンが少し違います。</t>
-    <rPh sb="50" eb="52">
-      <t>ジブン</t>
-    </rPh>
-    <rPh sb="62" eb="64">
-      <t>ケンサク</t>
-    </rPh>
-    <rPh sb="78" eb="80">
-      <t>ケンサク</t>
-    </rPh>
-    <rPh sb="85" eb="87">
-      <t>ガッコウ</t>
-    </rPh>
-    <rPh sb="87" eb="88">
-      <t>ヨウ</t>
-    </rPh>
-    <rPh sb="96" eb="97">
-      <t>ア</t>
-    </rPh>
-    <rPh sb="100" eb="102">
-      <t>ガッコウ</t>
-    </rPh>
-    <rPh sb="102" eb="103">
-      <t>ヨウ</t>
-    </rPh>
-    <rPh sb="104" eb="107">
-      <t>ショウキギョウ</t>
-    </rPh>
-    <rPh sb="107" eb="108">
-      <t>ヨウ</t>
-    </rPh>
-    <rPh sb="118" eb="121">
-      <t>ショウキギョウ</t>
-    </rPh>
-    <rPh sb="121" eb="122">
-      <t>ヨウ</t>
-    </rPh>
-    <rPh sb="137" eb="140">
-      <t>カノウセイ</t>
-    </rPh>
-    <rPh sb="151" eb="152">
-      <t>スコ</t>
-    </rPh>
-    <rPh sb="153" eb="154">
-      <t>チガ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>IMCアカウント(@hiroshima-u.ac.jpを含む)を入力し、さらにパスワードも入力してサインインします。</t>
-    <rPh sb="28" eb="29">
-      <t>フク</t>
-    </rPh>
-    <rPh sb="32" eb="34">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="45" eb="47">
-      <t>ニュウリョク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&lt;strong&gt;学校用Teams&lt;/strong&gt;を起動します。学校用Teamsの場合には「職場または…」とメッセージが出ますが、小企業用Teamsはサインインのメニューがあり、「職場学校用Teamsのダウンロード」リンクがあります。お使いのPCに学校用Teamsが無い場合には、このリンクからダウンロードしてインストールし、学校用Teamsを起動しなおしてください。
-学校用Teamsの「開始する」で進めます。</t>
-    <rPh sb="8" eb="11">
-      <t>ガッコウヨウ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>キドウ</t>
-    </rPh>
-    <rPh sb="32" eb="35">
-      <t>ガッコウヨウ</t>
-    </rPh>
-    <rPh sb="41" eb="43">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="46" eb="48">
-      <t>ショクバ</t>
-    </rPh>
-    <rPh sb="60" eb="61">
-      <t>デ</t>
-    </rPh>
-    <rPh sb="65" eb="68">
-      <t>ショウキギョウ</t>
-    </rPh>
-    <rPh sb="68" eb="69">
-      <t>ヨウ</t>
-    </rPh>
-    <rPh sb="90" eb="92">
-      <t>ショクバ</t>
-    </rPh>
-    <rPh sb="92" eb="94">
-      <t>ガッコウ</t>
-    </rPh>
-    <rPh sb="94" eb="95">
-      <t>ヨウ</t>
-    </rPh>
-    <rPh sb="118" eb="119">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="124" eb="127">
-      <t>ガッコウヨウ</t>
-    </rPh>
-    <rPh sb="133" eb="134">
-      <t>ナ</t>
-    </rPh>
-    <rPh sb="135" eb="137">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="163" eb="166">
-      <t>ガッコウヨウ</t>
-    </rPh>
-    <rPh sb="172" eb="174">
-      <t>キドウ</t>
-    </rPh>
-    <rPh sb="185" eb="188">
-      <t>ガッコウヨウ</t>
-    </rPh>
-    <rPh sb="195" eb="197">
-      <t>カイシ</t>
-    </rPh>
-    <rPh sb="201" eb="202">
       <t>スス</t>
     </rPh>
     <phoneticPr fontId="1"/>
@@ -2873,15 +1818,6 @@
   </si>
   <si>
     <t>win11ja-lookup-msoffice-app.png</t>
-  </si>
-  <si>
-    <t>win11ja-teams-variants.png</t>
-  </si>
-  <si>
-    <t>win11ja-teams-first-dialog.png</t>
-  </si>
-  <si>
-    <t>win11ja-teams-signin.png</t>
   </si>
   <si>
     <t xml:space="preserve">広島大学で情報サービスを使うときに必要な２種類のIDをもういちど確認しましょう。二種類とも学生番号をもとにしています。
@@ -7716,13 +6652,6 @@
   </si>
   <si>
     <t>&lt;h2 id="office365"&gt;Office365のインストール&lt;/h2&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&lt;h2 id="teams"&gt;Teamsの使い方&lt;/h2&gt;</t>
-    <rPh sb="21" eb="22">
-      <t>ツカ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -8164,7 +7093,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>238</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8180,7 +7109,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>239</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -8188,7 +7117,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>240</v>
+        <v>206</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -8202,7 +7131,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>184</v>
+        <v>150</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8240,7 +7169,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>105</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -8248,7 +7177,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -8264,7 +7193,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>241</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="304.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -8272,7 +7201,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>271</v>
+        <v>237</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -8286,13 +7215,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="C7" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>50</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -8300,21 +7229,21 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>106</v>
+        <v>78</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>51</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>52</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
@@ -8328,7 +7257,7 @@
         <v>7</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>53</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="105.6" ph="1" x14ac:dyDescent="0.2">
@@ -8336,24 +7265,24 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>268</v>
+        <v>234</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>54</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>55</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
@@ -8361,13 +7290,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>57</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
@@ -8375,13 +7304,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>58</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -8389,32 +7318,32 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>59</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>285</v>
+        <v>251</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>284</v>
+        <v>250</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>317</v>
+        <v>283</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>62</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -8422,238 +7351,238 @@
         <v>4</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>63</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>318</v>
+        <v>284</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>65</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>66</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
-        <v>257</v>
+        <v>223</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>68</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
-        <v>70</v>
+        <v>42</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>69</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>72</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>73</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>250</v>
+        <v>216</v>
       </c>
       <c r="C25" t="s" ph="1">
-        <v>289</v>
+        <v>255</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>286</v>
+        <v>252</v>
       </c>
     </row>
     <row r="26" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>300</v>
+        <v>266</v>
       </c>
       <c r="C26" t="s" ph="1">
-        <v>289</v>
+        <v>255</v>
       </c>
       <c r="D26" t="s" ph="1">
-        <v>296</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>302</v>
+        <v>268</v>
       </c>
       <c r="C27" t="s" ph="1">
-        <v>289</v>
+        <v>255</v>
       </c>
       <c r="D27" t="s">
-        <v>301</v>
+        <v>267</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>303</v>
+        <v>269</v>
       </c>
       <c r="C28" t="s" ph="1">
-        <v>289</v>
+        <v>255</v>
       </c>
       <c r="D28" t="s">
-        <v>304</v>
+        <v>270</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>297</v>
+        <v>263</v>
       </c>
       <c r="C29" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D29" t="s" ph="1">
-        <v>84</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>298</v>
+        <v>264</v>
       </c>
       <c r="C30" t="s" ph="1">
-        <v>289</v>
+        <v>255</v>
       </c>
       <c r="D30" t="s" ph="1">
-        <v>299</v>
+        <v>265</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="C31" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D31" t="s" ph="1">
-        <v>76</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="C32" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D32" t="s" ph="1">
-        <v>77</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="C33" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D33" t="s" ph="1">
-        <v>80</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>251</v>
+        <v>217</v>
       </c>
       <c r="D34" t="s" ph="1">
-        <v>287</v>
+        <v>253</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>319</v>
+        <v>285</v>
       </c>
       <c r="C35" t="s" ph="1">
-        <v>289</v>
+        <v>255</v>
       </c>
       <c r="D35" t="s">
-        <v>288</v>
+        <v>254</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>291</v>
+        <v>257</v>
       </c>
       <c r="D36" t="s" ph="1">
-        <v>254</v>
+        <v>220</v>
       </c>
     </row>
     <row r="37" spans="2:5" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>290</v>
+        <v>256</v>
       </c>
       <c r="C37" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D37" t="s" ph="1">
-        <v>81</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="C38" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D38" t="s" ph="1">
-        <v>82</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="2:5" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="C39" t="s" ph="1">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="D39" t="s" ph="1">
-        <v>86</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="2:5" ph="1" x14ac:dyDescent="0.2">
@@ -8776,7 +7705,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>401</v>
+        <v>367</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
@@ -8784,7 +7713,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>358</v>
+        <v>324</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -8800,234 +7729,234 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>269</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="132" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>402</v>
+        <v>368</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>404</v>
+        <v>370</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s" ph="1">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="E10" ph="1"/>
     </row>
     <row r="11" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="C11" t="s" ph="1">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>103</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:5" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="C12" t="s" ph="1">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>88</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:5" customFormat="1" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>309</v>
+        <v>275</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>89</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>310</v>
+        <v>276</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>311</v>
+        <v>277</v>
       </c>
     </row>
     <row r="15" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>313</v>
+        <v>279</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>312</v>
+        <v>278</v>
       </c>
     </row>
     <row r="16" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>292</v>
+        <v>258</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>295</v>
+        <v>261</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>294</v>
+        <v>260</v>
       </c>
     </row>
     <row r="18" spans="2:4" customFormat="1" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B18" s="6" t="s">
-        <v>306</v>
+        <v>272</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>305</v>
+        <v>271</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>405</v>
+        <v>371</v>
       </c>
     </row>
     <row r="22" spans="2:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
-        <v>277</v>
+        <v>243</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>280</v>
+        <v>246</v>
       </c>
     </row>
     <row r="23" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
-        <v>283</v>
+        <v>249</v>
       </c>
       <c r="D23" t="s">
-        <v>307</v>
+        <v>273</v>
       </c>
     </row>
     <row r="24" spans="2:4" customFormat="1" ht="64.8" customHeight="1" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>384</v>
+        <v>350</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>308</v>
+        <v>274</v>
       </c>
     </row>
     <row r="25" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>388</v>
+        <v>354</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>389</v>
+        <v>355</v>
       </c>
     </row>
     <row r="26" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>385</v>
+        <v>351</v>
       </c>
       <c r="D26" t="s">
-        <v>390</v>
+        <v>356</v>
       </c>
     </row>
     <row r="27" spans="2:4" customFormat="1" ht="45.6" customHeight="1" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>381</v>
+        <v>347</v>
       </c>
       <c r="D27" t="s">
-        <v>391</v>
+        <v>357</v>
       </c>
     </row>
     <row r="28" spans="2:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>382</v>
+        <v>348</v>
       </c>
       <c r="D28" t="s">
-        <v>392</v>
+        <v>358</v>
       </c>
     </row>
     <row r="29" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>386</v>
+        <v>352</v>
       </c>
       <c r="D29" t="s">
-        <v>393</v>
+        <v>359</v>
       </c>
     </row>
     <row r="30" spans="2:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>387</v>
+        <v>353</v>
       </c>
       <c r="D30" t="s">
-        <v>394</v>
+        <v>360</v>
       </c>
     </row>
     <row r="31" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>383</v>
+        <v>349</v>
       </c>
       <c r="D31" t="s">
-        <v>395</v>
+        <v>361</v>
       </c>
     </row>
     <row r="32" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
-        <v>398</v>
+        <v>364</v>
       </c>
       <c r="D32" t="s">
-        <v>396</v>
+        <v>362</v>
       </c>
     </row>
     <row r="33" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>282</v>
+        <v>248</v>
       </c>
       <c r="D33" t="s" ph="1">
-        <v>397</v>
+        <v>363</v>
       </c>
     </row>
     <row r="34" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>278</v>
+        <v>244</v>
       </c>
       <c r="D34" t="s">
-        <v>399</v>
+        <v>365</v>
       </c>
     </row>
     <row r="35" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
-        <v>315</v>
+        <v>281</v>
       </c>
       <c r="D35" t="s" ph="1">
-        <v>400</v>
+        <v>366</v>
       </c>
     </row>
     <row r="36" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>314</v>
+        <v>280</v>
       </c>
       <c r="D36" t="s" ph="1">
-        <v>280</v>
+        <v>246</v>
       </c>
     </row>
     <row r="37" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>320</v>
+        <v>286</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
-        <v>403</v>
+        <v>369</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -9035,7 +7964,7 @@
         <v>8</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>279</v>
+        <v>245</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
@@ -9049,37 +7978,37 @@
         <v>4</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="C42" t="s">
         <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B43" s="6" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D43" t="s">
-        <v>104</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B44" s="6" t="s">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="D44" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B45" s="6" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="D45" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9087,13 +8016,13 @@
         <v>4</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="C46" t="s">
         <v>4</v>
       </c>
       <c r="D46" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -9145,7 +8074,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>233</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -9153,7 +8082,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>232</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9169,7 +8098,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>270</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="145.19999999999999" x14ac:dyDescent="0.2">
@@ -9177,7 +8106,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>406</v>
+        <v>372</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -9188,7 +8117,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>407</v>
+        <v>373</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9196,29 +8125,29 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>321</v>
+        <v>287</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>322</v>
+        <v>288</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>327</v>
+        <v>293</v>
       </c>
       <c r="D11" t="s">
-        <v>323</v>
+        <v>289</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>324</v>
+        <v>290</v>
       </c>
       <c r="D12" t="s">
-        <v>325</v>
+        <v>291</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -9226,13 +8155,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>328</v>
+        <v>294</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>326</v>
+        <v>292</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -9240,7 +8169,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>408</v>
+        <v>374</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -9251,7 +8180,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -9262,21 +8191,21 @@
         <v>4</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>149</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="D19" t="s">
-        <v>150</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -9284,13 +8213,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>151</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9298,13 +8227,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>243</v>
+        <v>209</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>152</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9312,13 +8241,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>255</v>
+        <v>221</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>153</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -9331,149 +8260,149 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>229</v>
+        <v>195</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="82.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>235</v>
+        <v>201</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>332</v>
+        <v>298</v>
       </c>
       <c r="D27" t="s">
-        <v>329</v>
+        <v>295</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>333</v>
+        <v>299</v>
       </c>
       <c r="D28" t="s">
-        <v>330</v>
+        <v>296</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>335</v>
+        <v>301</v>
       </c>
       <c r="D29" t="s">
-        <v>334</v>
+        <v>300</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="67.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>409</v>
+        <v>375</v>
       </c>
       <c r="D30" t="s">
-        <v>331</v>
+        <v>297</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>336</v>
+        <v>302</v>
       </c>
       <c r="D31" t="s">
-        <v>224</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>411</v>
+        <v>377</v>
       </c>
       <c r="D33" t="s">
-        <v>410</v>
+        <v>376</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>261</v>
+        <v>227</v>
       </c>
       <c r="D34" t="s">
-        <v>262</v>
+        <v>228</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>263</v>
+        <v>229</v>
       </c>
       <c r="D35" t="s">
-        <v>264</v>
+        <v>230</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>267</v>
+        <v>233</v>
       </c>
       <c r="D36" t="s">
-        <v>265</v>
+        <v>231</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="50.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>266</v>
+        <v>232</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
-        <v>222</v>
+        <v>188</v>
       </c>
       <c r="D38" t="s">
-        <v>226</v>
+        <v>192</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
-        <v>252</v>
+        <v>218</v>
       </c>
       <c r="D39" t="s">
-        <v>253</v>
+        <v>219</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="6" t="s">
-        <v>230</v>
+        <v>196</v>
       </c>
       <c r="D40" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="6" t="s">
-        <v>223</v>
+        <v>189</v>
       </c>
       <c r="D41" t="s">
-        <v>227</v>
+        <v>193</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="46.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="6" t="s">
-        <v>272</v>
+        <v>238</v>
       </c>
       <c r="D42" t="s">
-        <v>228</v>
+        <v>194</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="131.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="6" t="s">
-        <v>273</v>
+        <v>239</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" s="6" t="s">
-        <v>231</v>
+        <v>197</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="6" t="s">
-        <v>337</v>
+        <v>303</v>
       </c>
       <c r="D47" t="s">
-        <v>334</v>
+        <v>300</v>
       </c>
     </row>
     <row r="48" spans="2:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9505,7 +8434,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>352</v>
+        <v>318</v>
       </c>
     </row>
     <row r="2" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -9513,7 +8442,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>357</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -9529,7 +8458,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>274</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -9537,7 +8466,7 @@
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>365</v>
+        <v>331</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -9545,7 +8474,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>412</v>
+        <v>378</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -9553,50 +8482,50 @@
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>350</v>
+        <v>316</v>
       </c>
       <c r="D10" t="s">
-        <v>342</v>
+        <v>308</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>346</v>
+        <v>312</v>
       </c>
       <c r="D11" t="s">
-        <v>338</v>
+        <v>304</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>275</v>
+        <v>241</v>
       </c>
       <c r="D12" t="s">
-        <v>339</v>
+        <v>305</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>343</v>
+        <v>309</v>
       </c>
       <c r="D13" t="s">
-        <v>340</v>
+        <v>306</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>276</v>
+        <v>242</v>
       </c>
       <c r="D14" t="s">
-        <v>341</v>
+        <v>307</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>344</v>
+        <v>310</v>
       </c>
       <c r="D15" t="s">
-        <v>345</v>
+        <v>311</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -9604,7 +8533,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>413</v>
+        <v>379</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -9613,68 +8542,68 @@
     </row>
     <row r="19" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>349</v>
+        <v>315</v>
       </c>
       <c r="C19" ph="1"/>
       <c r="D19" t="s">
-        <v>348</v>
+        <v>314</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="132" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>351</v>
+        <v>317</v>
       </c>
       <c r="C20" ph="1"/>
       <c r="D20" t="s">
-        <v>347</v>
+        <v>313</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>116</v>
+        <v>88</v>
       </c>
       <c r="D21" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="D22" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="D23" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="D24" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="D25" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="D26" t="s">
-        <v>127</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
@@ -9682,7 +8611,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>414</v>
+        <v>380</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -9691,29 +8620,29 @@
     </row>
     <row r="30" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>359</v>
+        <v>325</v>
       </c>
       <c r="C30" ph="1"/>
       <c r="D30" t="s">
-        <v>362</v>
+        <v>328</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>360</v>
+        <v>326</v>
       </c>
       <c r="C31" ph="1"/>
       <c r="D31" t="s" ph="1">
-        <v>364</v>
+        <v>330</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>361</v>
+        <v>327</v>
       </c>
       <c r="C32" ph="1"/>
       <c r="D32" t="s" ph="1">
-        <v>363</v>
+        <v>329</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -9771,7 +8700,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>195</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -9779,7 +8708,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>216</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9795,7 +8724,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>356</v>
+        <v>322</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -9806,7 +8735,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>234</v>
+        <v>200</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -9825,12 +8754,12 @@
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>196</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>415</v>
+        <v>381</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -9838,7 +8767,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -9849,18 +8778,18 @@
     </row>
     <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>198</v>
+        <v>164</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>159</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>416</v>
+        <v>382</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9868,7 +8797,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>194</v>
+        <v>160</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -9876,18 +8805,18 @@
     </row>
     <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>199</v>
+        <v>165</v>
       </c>
       <c r="D15" t="s">
-        <v>200</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>201</v>
+        <v>167</v>
       </c>
       <c r="D16" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -9895,13 +8824,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>140</v>
+        <v>109</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>141</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="198" x14ac:dyDescent="0.2">
@@ -9909,18 +8838,18 @@
         <v>4</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>244</v>
+        <v>210</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>202</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>417</v>
+        <v>383</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9928,21 +8857,21 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>203</v>
+        <v>169</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>204</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>205</v>
+        <v>171</v>
       </c>
       <c r="D21" t="s">
-        <v>206</v>
+        <v>172</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9950,21 +8879,21 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>245</v>
+        <v>211</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>208</v>
+        <v>174</v>
       </c>
       <c r="D23" t="s">
-        <v>209</v>
+        <v>175</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9972,13 +8901,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>246</v>
+        <v>212</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>210</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -9986,7 +8915,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>418</v>
+        <v>384</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -10002,40 +8931,40 @@
     </row>
     <row r="28" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>211</v>
+        <v>177</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>166</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>212</v>
+        <v>178</v>
       </c>
       <c r="D29" t="s">
-        <v>141</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="D30" t="s">
-        <v>182</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>247</v>
+        <v>213</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>213</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -10043,7 +8972,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>419</v>
+        <v>385</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -10062,80 +8991,80 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>214</v>
+        <v>180</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>215</v>
+        <v>181</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="D36" t="s">
-        <v>179</v>
+        <v>145</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="D37" t="s">
-        <v>160</v>
+        <v>129</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>183</v>
+        <v>149</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>129</v>
+        <v>101</v>
       </c>
       <c r="D39" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>142</v>
+        <v>111</v>
       </c>
       <c r="D40" t="s">
-        <v>162</v>
+        <v>131</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>248</v>
+        <v>214</v>
       </c>
       <c r="D41" t="s">
-        <v>163</v>
+        <v>132</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
-        <v>143</v>
+        <v>112</v>
       </c>
       <c r="C42" t="s">
         <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>164</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>259</v>
+        <v>225</v>
       </c>
       <c r="C43" t="s">
         <v>4</v>
       </c>
       <c r="D43" t="s">
-        <v>165</v>
+        <v>134</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -10143,7 +9072,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>420</v>
+        <v>386</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -10151,7 +9080,7 @@
     </row>
     <row r="47" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="C47" t="s">
         <v>4</v>
@@ -10162,7 +9091,7 @@
     </row>
     <row r="48" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
-        <v>260</v>
+        <v>226</v>
       </c>
       <c r="C48" t="s">
         <v>7</v>
@@ -10171,7 +9100,7 @@
     </row>
     <row r="49" spans="2:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B49" s="1" t="s">
-        <v>421</v>
+        <v>387</v>
       </c>
       <c r="D49" t="s" ph="1">
         <v>14</v>
@@ -10179,7 +9108,7 @@
     </row>
     <row r="50" spans="2:4" ht="132" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
-        <v>237</v>
+        <v>203</v>
       </c>
       <c r="C50" t="s">
         <v>7</v>
@@ -10257,7 +9186,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>366</v>
+        <v>332</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -10273,7 +9202,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>355</v>
+        <v>321</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -10281,7 +9210,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>367</v>
+        <v>333</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -10305,18 +9234,18 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>422</v>
+        <v>388</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -10324,21 +9253,21 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>132</v>
+        <v>104</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>154</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>135</v>
+        <v>107</v>
       </c>
       <c r="D15" t="s">
-        <v>155</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -10346,13 +9275,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>133</v>
+        <v>105</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -10360,13 +9289,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>134</v>
+        <v>106</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>157</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -10374,13 +9303,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>316</v>
+        <v>282</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -10388,7 +9317,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>423</v>
+        <v>389</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -10401,12 +9330,12 @@
     </row>
     <row r="22" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>368</v>
+        <v>334</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>380</v>
+        <v>346</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="4" customFormat="1" ht="39.6" x14ac:dyDescent="0.2">
@@ -10414,53 +9343,53 @@
         <v>4</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>369</v>
+        <v>335</v>
       </c>
       <c r="C25" s="4" ph="1"/>
       <c r="D25" s="4" t="s" ph="1">
-        <v>281</v>
+        <v>247</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>370</v>
+        <v>336</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>371</v>
+        <v>337</v>
       </c>
       <c r="D27" t="s">
-        <v>372</v>
+        <v>338</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>375</v>
+        <v>341</v>
       </c>
       <c r="D28" t="s">
-        <v>374</v>
+        <v>340</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>376</v>
+        <v>342</v>
       </c>
       <c r="D29" t="s">
-        <v>373</v>
+        <v>339</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>378</v>
+        <v>344</v>
       </c>
       <c r="D30" t="s">
-        <v>377</v>
+        <v>343</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>379</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -10491,7 +9420,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>191</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -10499,7 +9428,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>190</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -10515,22 +9444,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>354</v>
+        <v>320</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>236</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>186</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -10538,7 +9467,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>242</v>
+        <v>208</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -10563,13 +9492,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>249</v>
+        <v>215</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>146</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -10577,21 +9506,21 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>256</v>
+        <v>222</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>147</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="D13" t="s">
-        <v>148</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -10599,12 +9528,12 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>192</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -10612,33 +9541,33 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>187</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>188</v>
+        <v>154</v>
       </c>
       <c r="D18" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
-        <v>189</v>
+        <v>155</v>
       </c>
       <c r="D19" t="s">
-        <v>217</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>193</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>185</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -10650,10 +9579,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392D1BFF-FF5C-4A7E-8C9C-E750AF0FFFAF}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="D46" sqref="B26:D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -10669,7 +9598,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>145</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -10677,7 +9606,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>144</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -10693,22 +9622,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>353</v>
+        <v>319</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>145</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>424</v>
+        <v>390</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -10732,7 +9661,7 @@
     </row>
     <row r="14" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
@@ -10740,7 +9669,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>219</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.2">
@@ -10748,10 +9677,10 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="D16" t="s">
-        <v>179</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -10759,39 +9688,39 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="D17" t="s">
-        <v>160</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>183</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>129</v>
+        <v>101</v>
       </c>
       <c r="D19" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>218</v>
+        <v>184</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>167</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>220</v>
+        <v>186</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>168</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -10799,222 +9728,29 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>131</v>
+        <v>103</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>169</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="D23" t="s">
-        <v>170</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>221</v>
+        <v>187</v>
       </c>
       <c r="D24" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B26" s="1" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
-      <c r="B28" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B30" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D30" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D31" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D32" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B33" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C33" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C34" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B35" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C35" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B36" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C36" t="s">
-        <v>7</v>
-      </c>
-      <c r="D36" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B37" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C37" t="s">
-        <v>7</v>
-      </c>
-      <c r="D37" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="B38" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C38" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B39" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C39" t="s">
-        <v>7</v>
-      </c>
-      <c r="D39" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" ht="105.6" x14ac:dyDescent="0.2">
-      <c r="B40" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C40" t="s">
-        <v>42</v>
-      </c>
-      <c r="D40" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" ht="79.2" x14ac:dyDescent="0.2">
-      <c r="B41" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C41" t="s">
-        <v>7</v>
-      </c>
-      <c r="D41" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B42" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C42" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B43" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C43" t="s">
-        <v>7</v>
-      </c>
-      <c r="D43" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" ht="66" x14ac:dyDescent="0.2">
-      <c r="B44" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C44" t="s">
-        <v>7</v>
-      </c>
-      <c r="D44" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B45" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C45" t="s">
-        <v>7</v>
-      </c>
-      <c r="D45" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" ht="66" x14ac:dyDescent="0.2">
-      <c r="B46" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C46" t="s">
-        <v>7</v>
-      </c>
-      <c r="D46" t="s">
-        <v>40</v>
-      </c>
-    </row>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
win11ja: update o365 init
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F38DBD-87CE-4293-921B-13FD74600E7E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA634C81-A067-4316-8AA9-F8E66A9334C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="395">
   <si>
     <t>header1</t>
   </si>
@@ -1541,110 +1541,6 @@
     </rPh>
     <rPh sb="26" eb="27">
       <t>ハズ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>現在のMicrosoft OfficeにはMicrosoftアカウントと関係なく使える(買い切り版と言われます)Microsoft Office 2021と、Microsoftアカウントに対して一定期間の使用許諾が与えられる(または購入)できるMicrosoft Office 365の2つがあります。PCショップでOffice2021プリインストールモデルを買った場合はすぐ使える筈ですが、Office365プリインストールの場合にはMicrosoftアカウントとの関連付けが求められます。広島大学のOffice365アカウントを使うために「別のアカウントを使用する」をクリックして進めます。さらに「サインイン」で進めます。
-手動でOffice365をインストールした場合は、「続行」で進めることができます。</t>
-    <rPh sb="0" eb="2">
-      <t>ゲンザイ</t>
-    </rPh>
-    <rPh sb="36" eb="38">
-      <t>カンケイ</t>
-    </rPh>
-    <rPh sb="40" eb="41">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="44" eb="45">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="46" eb="47">
-      <t>キ</t>
-    </rPh>
-    <rPh sb="48" eb="49">
-      <t>バン</t>
-    </rPh>
-    <rPh sb="50" eb="51">
-      <t>イ</t>
-    </rPh>
-    <rPh sb="94" eb="95">
-      <t>タイ</t>
-    </rPh>
-    <rPh sb="97" eb="99">
-      <t>イッテイ</t>
-    </rPh>
-    <rPh sb="99" eb="101">
-      <t>キカン</t>
-    </rPh>
-    <rPh sb="102" eb="104">
-      <t>シヨウ</t>
-    </rPh>
-    <rPh sb="104" eb="106">
-      <t>キョダク</t>
-    </rPh>
-    <rPh sb="107" eb="108">
-      <t>アタ</t>
-    </rPh>
-    <rPh sb="116" eb="118">
-      <t>コウニュウ</t>
-    </rPh>
-    <rPh sb="180" eb="181">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="183" eb="185">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="188" eb="189">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="191" eb="192">
-      <t>ハズ</t>
-    </rPh>
-    <rPh sb="214" eb="216">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="234" eb="236">
-      <t>カンレン</t>
-    </rPh>
-    <rPh sb="236" eb="237">
-      <t>ヅ</t>
-    </rPh>
-    <rPh sb="239" eb="240">
-      <t>モト</t>
-    </rPh>
-    <rPh sb="246" eb="248">
-      <t>ヒロシマ</t>
-    </rPh>
-    <rPh sb="248" eb="250">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="266" eb="267">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="272" eb="273">
-      <t>ベツ</t>
-    </rPh>
-    <rPh sb="280" eb="282">
-      <t>シヨウ</t>
-    </rPh>
-    <rPh sb="292" eb="293">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="308" eb="309">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="314" eb="316">
-      <t>シュドウ</t>
-    </rPh>
-    <rPh sb="335" eb="337">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="340" eb="342">
-      <t>ゾッコウ</t>
-    </rPh>
-    <rPh sb="344" eb="345">
-      <t>スス</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -4705,120 +4601,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>既に持っているメールアドレスでMSアカウントを作るように案内されますが、混乱を避けるため、「新しいメールアドレスを取得」を選びます。以降では、ここで新規に作るものを「個人MSアカウント」あるいは「無料MSアカウント」と呼びます。
-これとは別に大学在籍期間中に大学が有償契約したMSアカウントもありますが、卒業、あるいは大学院進学で学籍番号が無効になると使えなくなります。</t>
-    <rPh sb="0" eb="1">
-      <t>スデ</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>モ</t>
-    </rPh>
-    <rPh sb="23" eb="24">
-      <t>ツク</t>
-    </rPh>
-    <rPh sb="28" eb="30">
-      <t>アンナイ</t>
-    </rPh>
-    <rPh sb="36" eb="38">
-      <t>コンラン</t>
-    </rPh>
-    <rPh sb="39" eb="40">
-      <t>サ</t>
-    </rPh>
-    <rPh sb="46" eb="47">
-      <t>アタラ</t>
-    </rPh>
-    <rPh sb="57" eb="59">
-      <t>シュトク</t>
-    </rPh>
-    <rPh sb="61" eb="62">
-      <t>エラ</t>
-    </rPh>
-    <rPh sb="66" eb="68">
-      <t>イコウ</t>
-    </rPh>
-    <rPh sb="74" eb="76">
-      <t>シンキ</t>
-    </rPh>
-    <rPh sb="77" eb="78">
-      <t>ツク</t>
-    </rPh>
-    <rPh sb="83" eb="85">
-      <t>コジン</t>
-    </rPh>
-    <rPh sb="98" eb="100">
-      <t>ムリョウ</t>
-    </rPh>
-    <rPh sb="109" eb="110">
-      <t>ヨ</t>
-    </rPh>
-    <rPh sb="119" eb="120">
-      <t>ベツ</t>
-    </rPh>
-    <rPh sb="121" eb="123">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="123" eb="125">
-      <t>ザイセキ</t>
-    </rPh>
-    <rPh sb="125" eb="128">
-      <t>キカンチュウ</t>
-    </rPh>
-    <rPh sb="129" eb="131">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="132" eb="134">
-      <t>ユウショウ</t>
-    </rPh>
-    <rPh sb="134" eb="136">
-      <t>ケイヤク</t>
-    </rPh>
-    <rPh sb="152" eb="154">
-      <t>ソツギョウ</t>
-    </rPh>
-    <rPh sb="159" eb="162">
-      <t>ダイガクイン</t>
-    </rPh>
-    <rPh sb="162" eb="164">
-      <t>シンガク</t>
-    </rPh>
-    <rPh sb="165" eb="167">
-      <t>ガクセキ</t>
-    </rPh>
-    <rPh sb="167" eb="169">
-      <t>バンゴウ</t>
-    </rPh>
-    <rPh sb="170" eb="172">
-      <t>ムコウ</t>
-    </rPh>
-    <rPh sb="176" eb="177">
-      <t>ツカ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Webブラウザの履歴を個人MSアカウントに保存するかどうか尋ねられることがありますが、「今はしない」で進めましょう。</t>
-    <rPh sb="8" eb="10">
-      <t>リレキ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>コジン</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>ホゾン</t>
-    </rPh>
-    <rPh sb="29" eb="30">
-      <t>タズ</t>
-    </rPh>
-    <rPh sb="44" eb="45">
-      <t>イマ</t>
-    </rPh>
-    <rPh sb="51" eb="52">
-      <t>スス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>OneDriveと無料MSアカウントが連携していないことを確認できたら、次の章に進みましょう。</t>
     <rPh sb="9" eb="11">
       <t>ムリョウ</t>
@@ -5265,85 +5047,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Edgeは最初に何らかのMicrosoftアカウントとの連携をさせようとします。最初に個人MSアカウントを作ったため、既定では全ての操作がこのアカウントに結び付けられます。さらに他のWebブラウザの閲覧や検索履歴からもデータを取り出そうとします。少しでも個人情報保護につながるよう、ここではチェックボックス(①)を外した上で、「次へ」(②)をクリックして進めましょう。</t>
-    <rPh sb="5" eb="7">
-      <t>サイショ</t>
-    </rPh>
-    <rPh sb="8" eb="9">
-      <t>ナン</t>
-    </rPh>
-    <rPh sb="28" eb="30">
-      <t>レンケイ</t>
-    </rPh>
-    <rPh sb="40" eb="42">
-      <t>サイショ</t>
-    </rPh>
-    <rPh sb="43" eb="45">
-      <t>コジン</t>
-    </rPh>
-    <rPh sb="53" eb="54">
-      <t>ツク</t>
-    </rPh>
-    <rPh sb="59" eb="61">
-      <t>キテイ</t>
-    </rPh>
-    <rPh sb="63" eb="64">
-      <t>スベ</t>
-    </rPh>
-    <rPh sb="66" eb="68">
-      <t>ソウサ</t>
-    </rPh>
-    <rPh sb="77" eb="78">
-      <t>ムス</t>
-    </rPh>
-    <rPh sb="79" eb="80">
-      <t>ツ</t>
-    </rPh>
-    <rPh sb="89" eb="90">
-      <t>タ</t>
-    </rPh>
-    <rPh sb="99" eb="101">
-      <t>エツラン</t>
-    </rPh>
-    <rPh sb="102" eb="104">
-      <t>ケンサク</t>
-    </rPh>
-    <rPh sb="104" eb="106">
-      <t>リレキ</t>
-    </rPh>
-    <rPh sb="113" eb="114">
-      <t>ト</t>
-    </rPh>
-    <rPh sb="115" eb="116">
-      <t>ダ</t>
-    </rPh>
-    <rPh sb="123" eb="124">
-      <t>スコ</t>
-    </rPh>
-    <rPh sb="127" eb="129">
-      <t>コジン</t>
-    </rPh>
-    <rPh sb="129" eb="131">
-      <t>ジョウホウ</t>
-    </rPh>
-    <rPh sb="131" eb="133">
-      <t>ホゴ</t>
-    </rPh>
-    <rPh sb="157" eb="158">
-      <t>ハズ</t>
-    </rPh>
-    <rPh sb="160" eb="161">
-      <t>ウエ</t>
-    </rPh>
-    <rPh sb="164" eb="165">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="177" eb="178">
-      <t>スス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>win11ja-search-chrome-result.png</t>
   </si>
   <si>
@@ -5478,16 +5181,6 @@
   </si>
   <si>
     <t>Edgeの初期設定、Google Chromeのインストール、BitLockerキーの保存</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>パソコンのスペック確認、個人MSアカウントのOneDriveリンクの解除 (学生番号が無くても可能です)</t>
-    <rPh sb="12" eb="14">
-      <t>コジン</t>
-    </rPh>
-    <rPh sb="34" eb="36">
-      <t>カイジョ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -5914,61 +5607,6 @@
     </rPh>
     <rPh sb="53" eb="55">
       <t>カクニン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>OneDrive同期は、同じファイルやディレクトリを複数のOneDriveアカウントで同期させることはできません。個人MSアカウントへの同期が知らないうちに入っている可能性がありますので、念のため通知エリアを確認し、第1章の手順に従ってリンクを解除してください。</t>
-    <rPh sb="8" eb="10">
-      <t>ドウキ</t>
-    </rPh>
-    <rPh sb="12" eb="13">
-      <t>オナ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>フクスウ</t>
-    </rPh>
-    <rPh sb="43" eb="45">
-      <t>ドウキ</t>
-    </rPh>
-    <rPh sb="57" eb="59">
-      <t>コジン</t>
-    </rPh>
-    <rPh sb="68" eb="70">
-      <t>ドウキ</t>
-    </rPh>
-    <rPh sb="71" eb="72">
-      <t>シ</t>
-    </rPh>
-    <rPh sb="78" eb="79">
-      <t>ハイ</t>
-    </rPh>
-    <rPh sb="83" eb="86">
-      <t>カノウセイ</t>
-    </rPh>
-    <rPh sb="94" eb="95">
-      <t>ネン</t>
-    </rPh>
-    <rPh sb="98" eb="100">
-      <t>ツウチ</t>
-    </rPh>
-    <rPh sb="104" eb="106">
-      <t>カクニン</t>
-    </rPh>
-    <rPh sb="108" eb="109">
-      <t>ダイ</t>
-    </rPh>
-    <rPh sb="110" eb="111">
-      <t>ショウ</t>
-    </rPh>
-    <rPh sb="112" eb="114">
-      <t>テジュン</t>
-    </rPh>
-    <rPh sb="115" eb="116">
-      <t>シタガ</t>
-    </rPh>
-    <rPh sb="122" eb="124">
-      <t>カイジョ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -6431,73 +6069,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>サインインしていないので暗号化が完了していないと言われる場合があります。個人MSアカウントを作ったのにサインインしていないと言われた場合は、ネットワークに接続されていることを確認してボタンを押し、サインインしてみてください。どうしても解消しない場合は「デバイスの暗号化」のトグルスイッチをオフにしてください。この警告が出ている状態のWindows11では、以降の手順での鍵の保存ができません。</t>
-    <rPh sb="12" eb="15">
-      <t>アンゴウカ</t>
-    </rPh>
-    <rPh sb="16" eb="18">
-      <t>カンリョウ</t>
-    </rPh>
-    <rPh sb="24" eb="25">
-      <t>イ</t>
-    </rPh>
-    <rPh sb="28" eb="30">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="36" eb="38">
-      <t>コジン</t>
-    </rPh>
-    <rPh sb="46" eb="47">
-      <t>ツク</t>
-    </rPh>
-    <rPh sb="62" eb="63">
-      <t>イ</t>
-    </rPh>
-    <rPh sb="66" eb="68">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="77" eb="79">
-      <t>セツゾク</t>
-    </rPh>
-    <rPh sb="87" eb="89">
-      <t>カクニン</t>
-    </rPh>
-    <rPh sb="95" eb="96">
-      <t>オ</t>
-    </rPh>
-    <rPh sb="117" eb="119">
-      <t>カイショウ</t>
-    </rPh>
-    <rPh sb="122" eb="124">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="131" eb="134">
-      <t>アンゴウカ</t>
-    </rPh>
-    <rPh sb="156" eb="158">
-      <t>ケイコク</t>
-    </rPh>
-    <rPh sb="159" eb="160">
-      <t>デ</t>
-    </rPh>
-    <rPh sb="163" eb="165">
-      <t>ジョウタイ</t>
-    </rPh>
-    <rPh sb="178" eb="180">
-      <t>イコウ</t>
-    </rPh>
-    <rPh sb="181" eb="183">
-      <t>テジュン</t>
-    </rPh>
-    <rPh sb="185" eb="186">
-      <t>カギ</t>
-    </rPh>
-    <rPh sb="187" eb="189">
-      <t>ホゾン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>win11ja-open-ctrlpanel.png</t>
   </si>
   <si>
@@ -6655,6 +6226,475 @@
     <rPh sb="310" eb="311">
       <t>スス</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>現在のMicrosoft OfficeにはMicrosoftアカウントと関係なく使える(買い切り版と言われます)Microsoft Office 2021と、Microsoftアカウントに対して一定期間の使用許諾が与えられる(または購入)できるMicrosoft Office 365の2つがあります。PCショップでOffice2021プリインストールモデルを買った場合は、使えるようにする方法を販売店に確認してください（必ずしも電源投入直後に使えるとは限りません）。
+もしOffice365プリインストールで、MSアカウントなしで使っている場合、「このアカウントにはまだOfficeがありません」のようなメッセージが出ますので、「別のアカウントを使用する」からIMCアカウントでサインインしてください。</t>
+    <rPh sb="0" eb="2">
+      <t>ゲンザイ</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>カンケイ</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="44" eb="45">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="46" eb="47">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="48" eb="49">
+      <t>バン</t>
+    </rPh>
+    <rPh sb="50" eb="51">
+      <t>イ</t>
+    </rPh>
+    <rPh sb="94" eb="95">
+      <t>タイ</t>
+    </rPh>
+    <rPh sb="97" eb="99">
+      <t>イッテイ</t>
+    </rPh>
+    <rPh sb="99" eb="101">
+      <t>キカン</t>
+    </rPh>
+    <rPh sb="102" eb="104">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="104" eb="106">
+      <t>キョダク</t>
+    </rPh>
+    <rPh sb="107" eb="108">
+      <t>アタ</t>
+    </rPh>
+    <rPh sb="116" eb="118">
+      <t>コウニュウ</t>
+    </rPh>
+    <rPh sb="180" eb="181">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="183" eb="185">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="187" eb="188">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="195" eb="197">
+      <t>ホウホウ</t>
+    </rPh>
+    <rPh sb="198" eb="200">
+      <t>ハンバイ</t>
+    </rPh>
+    <rPh sb="200" eb="201">
+      <t>テン</t>
+    </rPh>
+    <rPh sb="202" eb="204">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="211" eb="212">
+      <t>カナラ</t>
+    </rPh>
+    <rPh sb="215" eb="217">
+      <t>デンゲン</t>
+    </rPh>
+    <rPh sb="217" eb="219">
+      <t>トウニュウ</t>
+    </rPh>
+    <rPh sb="219" eb="221">
+      <t>チョクゴ</t>
+    </rPh>
+    <rPh sb="222" eb="223">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="227" eb="228">
+      <t>カギ</t>
+    </rPh>
+    <rPh sb="266" eb="267">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="271" eb="273">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="309" eb="310">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="316" eb="317">
+      <t>ベツ</t>
+    </rPh>
+    <rPh sb="324" eb="326">
+      <t>シヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OneDrive同期は、同じファイルやディレクトリを複数のOneDriveアカウントで同期させることはできません。私物MSアカウントへの同期が知らないうちに入っている可能性がありますので、念のため通知エリアを確認し、第1章の手順に従ってリンクを解除してください。</t>
+    <rPh sb="8" eb="10">
+      <t>ドウキ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>フクスウ</t>
+    </rPh>
+    <rPh sb="43" eb="45">
+      <t>ドウキ</t>
+    </rPh>
+    <rPh sb="68" eb="70">
+      <t>ドウキ</t>
+    </rPh>
+    <rPh sb="71" eb="72">
+      <t>シ</t>
+    </rPh>
+    <rPh sb="78" eb="79">
+      <t>ハイ</t>
+    </rPh>
+    <rPh sb="83" eb="86">
+      <t>カノウセイ</t>
+    </rPh>
+    <rPh sb="94" eb="95">
+      <t>ネン</t>
+    </rPh>
+    <rPh sb="98" eb="100">
+      <t>ツウチ</t>
+    </rPh>
+    <rPh sb="104" eb="106">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="108" eb="109">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="110" eb="111">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="112" eb="114">
+      <t>テジュン</t>
+    </rPh>
+    <rPh sb="115" eb="116">
+      <t>シタガ</t>
+    </rPh>
+    <rPh sb="122" eb="124">
+      <t>カイジョ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>既に持っているメールアドレスでMSアカウントを作るように案内されますが、混乱を避けるため、「新しいメールアドレスを取得」を選びます。以降では、ここで新規に作るものを「私物MSアカウント」あるいは「無料MSアカウント」と呼びます。
+これとは別に大学在籍期間中に大学が有償契約したMSアカウントもありますが、卒業、あるいは大学院進学で学籍番号が無効になると使えなくなります。</t>
+    <rPh sb="0" eb="1">
+      <t>スデ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>ツク</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>アンナイ</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>コンラン</t>
+    </rPh>
+    <rPh sb="39" eb="40">
+      <t>サ</t>
+    </rPh>
+    <rPh sb="46" eb="47">
+      <t>アタラ</t>
+    </rPh>
+    <rPh sb="57" eb="59">
+      <t>シュトク</t>
+    </rPh>
+    <rPh sb="61" eb="62">
+      <t>エラ</t>
+    </rPh>
+    <rPh sb="66" eb="68">
+      <t>イコウ</t>
+    </rPh>
+    <rPh sb="74" eb="76">
+      <t>シンキ</t>
+    </rPh>
+    <rPh sb="77" eb="78">
+      <t>ツク</t>
+    </rPh>
+    <rPh sb="98" eb="100">
+      <t>ムリョウ</t>
+    </rPh>
+    <rPh sb="109" eb="110">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="119" eb="120">
+      <t>ベツ</t>
+    </rPh>
+    <rPh sb="121" eb="123">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="123" eb="125">
+      <t>ザイセキ</t>
+    </rPh>
+    <rPh sb="125" eb="128">
+      <t>キカンチュウ</t>
+    </rPh>
+    <rPh sb="129" eb="131">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="132" eb="134">
+      <t>ユウショウ</t>
+    </rPh>
+    <rPh sb="134" eb="136">
+      <t>ケイヤク</t>
+    </rPh>
+    <rPh sb="152" eb="154">
+      <t>ソツギョウ</t>
+    </rPh>
+    <rPh sb="159" eb="162">
+      <t>ダイガクイン</t>
+    </rPh>
+    <rPh sb="162" eb="164">
+      <t>シンガク</t>
+    </rPh>
+    <rPh sb="165" eb="167">
+      <t>ガクセキ</t>
+    </rPh>
+    <rPh sb="167" eb="169">
+      <t>バンゴウ</t>
+    </rPh>
+    <rPh sb="170" eb="172">
+      <t>ムコウ</t>
+    </rPh>
+    <rPh sb="176" eb="177">
+      <t>ツカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Webブラウザの履歴を私物MSアカウントに保存するかどうか尋ねられることがありますが、「今はしない」で進めましょう。</t>
+    <rPh sb="8" eb="10">
+      <t>リレキ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>タズ</t>
+    </rPh>
+    <rPh sb="44" eb="45">
+      <t>イマ</t>
+    </rPh>
+    <rPh sb="51" eb="52">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>パソコンのスペック確認、私物MSアカウントのOneDriveリンクの解除 (学生番号が無くても可能です)</t>
+    <rPh sb="34" eb="36">
+      <t>カイジョ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>サインインしていないので暗号化が完了していないと言われる場合があります。私物MSアカウントを作ったのにサインインしていないと言われた場合は、ネットワークに接続されていることを確認してボタンを押し、サインインしてみてください。どうしても解消しない場合は「デバイスの暗号化」のトグルスイッチをオフにしてください。この警告が出ている状態のWindows11では、以降の手順での鍵の保存ができません。</t>
+    <rPh sb="12" eb="15">
+      <t>アンゴウカ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>カンリョウ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>イ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="46" eb="47">
+      <t>ツク</t>
+    </rPh>
+    <rPh sb="62" eb="63">
+      <t>イ</t>
+    </rPh>
+    <rPh sb="66" eb="68">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="77" eb="79">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="87" eb="89">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="95" eb="96">
+      <t>オ</t>
+    </rPh>
+    <rPh sb="117" eb="119">
+      <t>カイショウ</t>
+    </rPh>
+    <rPh sb="122" eb="124">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="131" eb="134">
+      <t>アンゴウカ</t>
+    </rPh>
+    <rPh sb="156" eb="158">
+      <t>ケイコク</t>
+    </rPh>
+    <rPh sb="159" eb="160">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="163" eb="165">
+      <t>ジョウタイ</t>
+    </rPh>
+    <rPh sb="178" eb="180">
+      <t>イコウ</t>
+    </rPh>
+    <rPh sb="181" eb="183">
+      <t>テジュン</t>
+    </rPh>
+    <rPh sb="185" eb="186">
+      <t>カギ</t>
+    </rPh>
+    <rPh sb="187" eb="189">
+      <t>ホゾン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Edgeは最初に何らかのMicrosoftアカウントとの連携をさせようとします。最初に私物MSアカウントを作ったため、既定では全ての操作がこのアカウントに結び付けられます。さらに他のWebブラウザの閲覧や検索履歴からもデータを取り出そうとします。少しでも個人情報保護につながるよう、ここではチェックボックス(①)を外した上で、「次へ」(②)をクリックして進めましょう。</t>
+    <rPh sb="5" eb="7">
+      <t>サイショ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ナン</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>レンケイ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>サイショ</t>
+    </rPh>
+    <rPh sb="53" eb="54">
+      <t>ツク</t>
+    </rPh>
+    <rPh sb="59" eb="61">
+      <t>キテイ</t>
+    </rPh>
+    <rPh sb="63" eb="64">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="66" eb="68">
+      <t>ソウサ</t>
+    </rPh>
+    <rPh sb="77" eb="78">
+      <t>ムス</t>
+    </rPh>
+    <rPh sb="79" eb="80">
+      <t>ツ</t>
+    </rPh>
+    <rPh sb="89" eb="90">
+      <t>タ</t>
+    </rPh>
+    <rPh sb="99" eb="101">
+      <t>エツラン</t>
+    </rPh>
+    <rPh sb="102" eb="104">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="104" eb="106">
+      <t>リレキ</t>
+    </rPh>
+    <rPh sb="113" eb="114">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="115" eb="116">
+      <t>ダ</t>
+    </rPh>
+    <rPh sb="123" eb="124">
+      <t>スコ</t>
+    </rPh>
+    <rPh sb="127" eb="129">
+      <t>コジン</t>
+    </rPh>
+    <rPh sb="129" eb="131">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="131" eb="133">
+      <t>ホゴ</t>
+    </rPh>
+    <rPh sb="157" eb="158">
+      <t>ハズ</t>
+    </rPh>
+    <rPh sb="160" eb="161">
+      <t>ウエ</t>
+    </rPh>
+    <rPh sb="164" eb="165">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="177" eb="178">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>このような警告が出なかった場合、「空白のブック」などをクリックして新たなExcelデータを作ってみましょう。</t>
+    <rPh sb="5" eb="7">
+      <t>ケイコク</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>クウハク</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>アラ</t>
+    </rPh>
+    <rPh sb="45" eb="46">
+      <t>ツク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>無料の私物MSアカウントではOffice365のライセンスが無いため、契約を促すウィンドウが表示されます。「変更」のリンクからIMCアカウントでのサインインに切り替えます。</t>
+    <rPh sb="0" eb="2">
+      <t>ムリョウ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>シブツ</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>ナ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>ケイヤク</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>ウナガ</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="54" eb="56">
+      <t>ヘンコウ</t>
+    </rPh>
+    <rPh sb="79" eb="80">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="81" eb="82">
+      <t>カ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-excel-newbook.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-o365-no-subs.png</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -7096,7 +7136,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7112,7 +7152,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7120,7 +7160,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -7134,7 +7174,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7154,8 +7194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A31" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B35" sqref="A6:D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.2"/>
@@ -7196,7 +7236,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="304.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -7204,7 +7244,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -7268,7 +7308,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>7</v>
@@ -7293,7 +7333,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>7</v>
@@ -7332,15 +7372,15 @@
     </row>
     <row r="16" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>7</v>
@@ -7365,7 +7405,7 @@
     </row>
     <row r="19" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>284</v>
+        <v>386</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>7</v>
@@ -7387,7 +7427,7 @@
     </row>
     <row r="21" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>7</v>
@@ -7431,51 +7471,51 @@
     </row>
     <row r="25" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C25" t="s" ph="1">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="26" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C26" t="s" ph="1">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D26" t="s" ph="1">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C27" t="s" ph="1">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D27" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="C28" t="s" ph="1">
+        <v>254</v>
+      </c>
+      <c r="D28" t="s">
         <v>269</v>
-      </c>
-      <c r="C28" t="s" ph="1">
-        <v>255</v>
-      </c>
-      <c r="D28" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C29" t="s" ph="1">
         <v>7</v>
@@ -7486,13 +7526,13 @@
     </row>
     <row r="30" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="C30" t="s" ph="1">
+        <v>254</v>
+      </c>
+      <c r="D30" t="s" ph="1">
         <v>264</v>
-      </c>
-      <c r="C30" t="s" ph="1">
-        <v>255</v>
-      </c>
-      <c r="D30" t="s" ph="1">
-        <v>265</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
@@ -7530,34 +7570,34 @@
     </row>
     <row r="34" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D34" t="s" ph="1">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>285</v>
+        <v>387</v>
       </c>
       <c r="C35" t="s" ph="1">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D35" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D36" t="s" ph="1">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="37" spans="2:5" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C37" t="s" ph="1">
         <v>7</v>
@@ -7708,7 +7748,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
@@ -7716,7 +7756,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>324</v>
+        <v>388</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -7732,17 +7772,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="132" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
@@ -7781,7 +7821,7 @@
     </row>
     <row r="13" spans="1:5" customFormat="1" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D13" t="s" ph="1">
         <v>61</v>
@@ -7789,177 +7829,177 @@
     </row>
     <row r="14" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="D14" t="s" ph="1">
         <v>276</v>
-      </c>
-      <c r="D14" t="s" ph="1">
-        <v>277</v>
       </c>
     </row>
     <row r="15" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="16" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="D16" t="s" ph="1">
         <v>258</v>
-      </c>
-      <c r="D16" t="s" ph="1">
-        <v>259</v>
       </c>
     </row>
     <row r="17" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="18" spans="2:4" customFormat="1" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B18" s="6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
     </row>
     <row r="22" spans="2:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="23" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D23" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="24" spans="2:4" customFormat="1" ht="64.8" customHeight="1" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="25" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>355</v>
+        <v>349</v>
       </c>
     </row>
     <row r="26" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="D26" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
     </row>
     <row r="27" spans="2:4" customFormat="1" ht="45.6" customHeight="1" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="D27" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
     </row>
     <row r="28" spans="2:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="D28" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="29" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="D29" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
     </row>
     <row r="30" spans="2:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D30" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
     </row>
     <row r="31" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="D31" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
     </row>
     <row r="32" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="D32" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
     </row>
     <row r="33" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D33" t="s" ph="1">
-        <v>363</v>
+        <v>357</v>
       </c>
     </row>
     <row r="34" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D34" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
     </row>
     <row r="35" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D35" t="s" ph="1">
-        <v>366</v>
+        <v>360</v>
       </c>
     </row>
     <row r="36" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D36" t="s" ph="1">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="37" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -7967,7 +8007,7 @@
         <v>8</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
@@ -8077,7 +8117,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8085,7 +8125,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8101,7 +8141,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="145.19999999999999" x14ac:dyDescent="0.2">
@@ -8109,7 +8149,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8120,7 +8160,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8128,29 +8168,29 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D11" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D12" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -8158,13 +8198,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -8172,7 +8212,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -8200,7 +8240,7 @@
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -8208,7 +8248,7 @@
         <v>85</v>
       </c>
       <c r="D19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -8222,7 +8262,7 @@
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8230,13 +8270,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8244,13 +8284,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -8263,149 +8303,149 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="82.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D27" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D28" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D29" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="67.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>375</v>
+        <v>389</v>
       </c>
       <c r="D30" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D31" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="D33" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D34" t="s">
         <v>227</v>
-      </c>
-      <c r="D34" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="D35" t="s">
         <v>229</v>
-      </c>
-      <c r="D35" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D36" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="50.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D38" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="D39" t="s">
         <v>218</v>
-      </c>
-      <c r="D39" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D40" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D41" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="46.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D42" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="131.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="6" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D47" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="48" spans="2:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8437,7 +8477,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="2" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -8445,7 +8485,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -8461,7 +8501,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -8469,7 +8509,7 @@
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -8477,7 +8517,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -8485,50 +8525,50 @@
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D10" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>312</v>
+        <v>390</v>
       </c>
       <c r="D11" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D12" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D13" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D14" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D15" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -8536,7 +8576,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -8545,20 +8585,20 @@
     </row>
     <row r="19" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C19" ph="1"/>
       <c r="D19" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="132" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C20" ph="1"/>
       <c r="D20" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8614,7 +8654,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -8623,29 +8663,29 @@
     </row>
     <row r="30" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="C30" ph="1"/>
       <c r="D30" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="C31" ph="1"/>
       <c r="D31" t="s" ph="1">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="C32" ph="1"/>
       <c r="D32" t="s" ph="1">
-        <v>329</v>
+        <v>324</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -8686,7 +8726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D6E33FB-2290-439B-854D-9A45A4600EF5}">
   <dimension ref="A1:D87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+    <sheetView topLeftCell="A46" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
       <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
@@ -8703,7 +8743,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8711,7 +8751,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8727,7 +8767,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -8738,7 +8778,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8757,12 +8797,12 @@
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -8770,7 +8810,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -8781,18 +8821,18 @@
     </row>
     <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8800,7 +8840,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -8808,18 +8848,18 @@
     </row>
     <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D15" t="s">
         <v>165</v>
-      </c>
-      <c r="D15" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -8827,13 +8867,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
         <v>109</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="198" x14ac:dyDescent="0.2">
@@ -8841,18 +8881,18 @@
         <v>4</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8860,21 +8900,21 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
         <v>169</v>
-      </c>
-      <c r="C20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D21" t="s">
         <v>171</v>
-      </c>
-      <c r="D21" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8882,21 +8922,21 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D23" t="s">
         <v>174</v>
-      </c>
-      <c r="D23" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8904,13 +8944,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -8918,7 +8958,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -8934,40 +8974,40 @@
     </row>
     <row r="28" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D30" t="s">
         <v>147</v>
-      </c>
-      <c r="D30" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -8975,7 +9015,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -8994,21 +9034,21 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
         <v>180</v>
-      </c>
-      <c r="C35" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D36" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9016,12 +9056,12 @@
         <v>100</v>
       </c>
       <c r="D37" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9029,45 +9069,45 @@
         <v>101</v>
       </c>
       <c r="D39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D40" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D41" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C42" t="s">
         <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C43" t="s">
         <v>4</v>
       </c>
       <c r="D43" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -9075,7 +9115,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -9083,7 +9123,7 @@
     </row>
     <row r="47" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C47" t="s">
         <v>4</v>
@@ -9094,7 +9134,7 @@
     </row>
     <row r="48" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C48" t="s">
         <v>7</v>
@@ -9103,7 +9143,7 @@
     </row>
     <row r="49" spans="2:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B49" s="6" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="D49" t="s" ph="1">
         <v>14</v>
@@ -9111,7 +9151,7 @@
     </row>
     <row r="50" spans="2:4" ht="132" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C50" t="s">
         <v>7</v>
@@ -9162,10 +9202,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -9189,7 +9229,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9205,7 +9245,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -9213,7 +9253,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -9237,18 +9277,18 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -9262,137 +9302,153 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="D15" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D15" t="s">
+    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="D16" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D17" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" t="s">
+    <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
+    <row r="20" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="5"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s">
-        <v>388</v>
-      </c>
-    </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
+      <c r="B21" s="5"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="4" customFormat="1" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="C27" s="4" ph="1"/>
+      <c r="D27" s="4" t="s" ph="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="D29" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D30" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D31" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="4" customFormat="1" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>335</v>
-      </c>
-      <c r="C25" s="4" ph="1"/>
-      <c r="D25" s="4" t="s" ph="1">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B26" s="1" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="D27" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="D32" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B28" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="D28" t="s">
+    <row r="33" spans="2:2" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
         <v>340</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="D29" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="D30" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B31" s="1" t="s">
-        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -9423,7 +9479,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -9431,7 +9487,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9447,17 +9503,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -9470,7 +9526,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -9495,13 +9551,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9509,13 +9565,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -9523,7 +9579,7 @@
         <v>81</v>
       </c>
       <c r="D13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -9536,7 +9592,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9544,33 +9600,33 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D19" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -9585,7 +9641,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="D46" sqref="B26:D46"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -9601,7 +9657,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -9609,7 +9665,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9625,22 +9681,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9672,7 +9728,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.2">
@@ -9680,10 +9736,10 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9694,12 +9750,12 @@
         <v>100</v>
       </c>
       <c r="D17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9707,23 +9763,23 @@
         <v>101</v>
       </c>
       <c r="D19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9734,7 +9790,7 @@
         <v>103</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -9742,15 +9798,15 @@
         <v>102</v>
       </c>
       <c r="D23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
win11ja: do not make empty excel book
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA634C81-A067-4316-8AA9-F8E66A9334C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3834474D-AD9C-4E18-A397-95D065D102B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="400">
   <si>
     <t>header1</t>
   </si>
@@ -5180,10 +5180,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Edgeの初期設定、Google Chromeのインストール、BitLockerキーの保存</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>前の章でデスクトップにBitLocker鍵を保存した場合、ダブルクリックして開くことができます。現在のWindowsでは、PDFはEdgeによって閲覧するのが既定の状態ですが、Google Chromeでも表示できます。</t>
     <rPh sb="48" eb="50">
       <t>ゲンザイ</t>
@@ -6160,16 +6156,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>&lt;h2 id="office"&gt;Microsoft Officeを入れる&lt;/h2&gt;</t>
-    <rPh sb="33" eb="34">
-      <t>ナ</t>
-    </rPh>
-    <rPh sb="37" eb="39">
-      <t>バアイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>&lt;h2 id="onedrive"&gt;IMCアカウントのOneDrive連携の設定&lt;/h2&gt;</t>
     <rPh sb="35" eb="37">
       <t>レンケイ</t>
@@ -6637,29 +6623,53 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>このような警告が出なかった場合、「空白のブック」などをクリックして新たなExcelデータを作ってみましょう。</t>
-    <rPh sb="5" eb="7">
-      <t>ケイコク</t>
-    </rPh>
-    <rPh sb="8" eb="9">
-      <t>デ</t>
-    </rPh>
-    <rPh sb="13" eb="15">
+    <t>win11ja-o365-no-subs.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2 id="office"&gt;Microsoft Officeのサインイン&lt;/h2&gt;</t>
+    <rPh sb="39" eb="41">
       <t>バアイ</t>
     </rPh>
-    <rPh sb="17" eb="19">
-      <t>クウハク</t>
-    </rPh>
-    <rPh sb="33" eb="34">
-      <t>アラ</t>
-    </rPh>
-    <rPh sb="45" eb="46">
-      <t>ツク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>無料の私物MSアカウントではOffice365のライセンスが無いため、契約を促すウィンドウが表示されます。「変更」のリンクからIMCアカウントでのサインインに切り替えます。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2 id="fix_default_save"&gt;Microsoft Officeのデフォルトの保存先の変更&lt;/h2&gt;</t>
+    <rPh sb="49" eb="51">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="51" eb="52">
+      <t>サキ</t>
+    </rPh>
+    <rPh sb="53" eb="55">
+      <t>ヘンコウ</t>
+    </rPh>
+    <rPh sb="56" eb="58">
+      <t>バアイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Edgeの初期設定、Google Chromeのインストール、BitLockerキーの確認(学生番号が無くても可能です)</t>
+    <rPh sb="43" eb="45">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>ガクセイ</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>バンゴウ</t>
+    </rPh>
+    <rPh sb="51" eb="52">
+      <t>ナ</t>
+    </rPh>
+    <rPh sb="55" eb="57">
+      <t>カノウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>無料の私物MSアカウントではOffice365のライセンスが無いため、契約を促すウィンドウが表示されます。ネットワーク経由で確認するので、Excelを起動してからしばらくして出ることがあります。「変更」のリンクからIMCアカウントでのサインインに切り替えます。</t>
     <rPh sb="0" eb="2">
       <t>ムリョウ</t>
     </rPh>
@@ -6678,23 +6688,137 @@
     <rPh sb="46" eb="48">
       <t>ヒョウジ</t>
     </rPh>
-    <rPh sb="54" eb="56">
+    <rPh sb="59" eb="61">
+      <t>ケイユ</t>
+    </rPh>
+    <rPh sb="62" eb="64">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="75" eb="77">
+      <t>キドウ</t>
+    </rPh>
+    <rPh sb="87" eb="88">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="98" eb="100">
       <t>ヘンコウ</t>
     </rPh>
-    <rPh sb="79" eb="80">
+    <rPh sb="123" eb="124">
       <t>キ</t>
     </rPh>
-    <rPh sb="81" eb="82">
+    <rPh sb="125" eb="126">
       <t>カ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-excel-newbook.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11ja-o365-no-subs.png</t>
+    <t>スタートメニューからExcelを起動し、左サイドバーのメニューから「オプション」(①)に進みます。「オプション」設定画面の左サイドメニューから「保存」(②)を選び、「既定でコンピューターに保存する」にチェックを入れます。</t>
+    <rPh sb="16" eb="18">
+      <t>キドウ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>ヒダリ</t>
+    </rPh>
+    <rPh sb="44" eb="45">
+      <t>スス</t>
+    </rPh>
+    <rPh sb="83" eb="85">
+      <t>キテイ</t>
+    </rPh>
+    <rPh sb="94" eb="96">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="105" eb="106">
+      <t>イ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-excel-option-save.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-excel-default-is-odrv.png</t>
+  </si>
+  <si>
+    <t>Office365はデフォルトの保存先がOneDriveになっています。たとえば新たにExcelファイルを作成して「名前を付けて保存」しようとするとその最初の候補はOneDriveに送信される設定になっています。OneDrive連携が不調になったりすると見えなくなってしまうので、デフォルトの保存先を手元のPCに変更しましょう。</t>
+    <rPh sb="16" eb="18">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>サキ</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>アラ</t>
+    </rPh>
+    <rPh sb="53" eb="55">
+      <t>サクセイ</t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t>ナマエ</t>
+    </rPh>
+    <rPh sb="61" eb="62">
+      <t>ツ</t>
+    </rPh>
+    <rPh sb="64" eb="66">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="76" eb="78">
+      <t>サイショ</t>
+    </rPh>
+    <rPh sb="79" eb="81">
+      <t>コウホ</t>
+    </rPh>
+    <rPh sb="91" eb="93">
+      <t>ソウシン</t>
+    </rPh>
+    <rPh sb="96" eb="98">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="114" eb="116">
+      <t>レンケイ</t>
+    </rPh>
+    <rPh sb="117" eb="119">
+      <t>フチョウ</t>
+    </rPh>
+    <rPh sb="127" eb="128">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="146" eb="148">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="148" eb="149">
+      <t>サキ</t>
+    </rPh>
+    <rPh sb="150" eb="152">
+      <t>テモト</t>
+    </rPh>
+    <rPh sb="156" eb="158">
+      <t>ヘンコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-excel-default-is-local.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>改めて「名前を付けて保存」を選ぶとデフォルトは「このPC」になっています。</t>
+    <rPh sb="0" eb="1">
+      <t>アラタ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ナマエ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ツ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>エラ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -7405,7 +7529,7 @@
     </row>
     <row r="19" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>7</v>
@@ -7578,7 +7702,7 @@
     </row>
     <row r="35" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C35" t="s" ph="1">
         <v>254</v>
@@ -7748,7 +7872,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
@@ -7756,7 +7880,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -7777,12 +7901,12 @@
     </row>
     <row r="6" spans="1:5" ht="132" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
@@ -7869,7 +7993,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="22" spans="2:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -7890,7 +8014,7 @@
     </row>
     <row r="24" spans="2:4" customFormat="1" ht="64.8" customHeight="1" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D24" t="s" ph="1">
         <v>273</v>
@@ -7898,66 +8022,66 @@
     </row>
     <row r="25" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="D25" t="s" ph="1">
         <v>348</v>
-      </c>
-      <c r="D25" t="s" ph="1">
-        <v>349</v>
       </c>
     </row>
     <row r="26" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D26" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="27" spans="2:4" customFormat="1" ht="45.6" customHeight="1" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D27" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="28" spans="2:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D28" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="29" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D29" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="30" spans="2:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D30" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="31" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D31" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="32" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D32" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="33" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -7965,7 +8089,7 @@
         <v>247</v>
       </c>
       <c r="D33" t="s" ph="1">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="34" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
@@ -7973,7 +8097,7 @@
         <v>243</v>
       </c>
       <c r="D34" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="35" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
@@ -7981,7 +8105,7 @@
         <v>280</v>
       </c>
       <c r="D35" t="s" ph="1">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="36" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -7999,7 +8123,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -8100,7 +8224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -8149,7 +8273,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8160,7 +8284,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8212,7 +8336,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -8337,7 +8461,7 @@
     </row>
     <row r="30" spans="1:4" ht="67.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D30" t="s">
         <v>294</v>
@@ -8354,10 +8478,10 @@
     <row r="32" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D33" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
@@ -8461,7 +8585,7 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8480,12 +8604,12 @@
         <v>314</v>
       </c>
     </row>
-    <row r="2" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s" ph="1">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>319</v>
+        <v>392</v>
       </c>
     </row>
     <row r="3" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -8509,7 +8633,7 @@
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -8517,7 +8641,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -8533,7 +8657,7 @@
     </row>
     <row r="11" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D11" t="s">
         <v>301</v>
@@ -8576,7 +8700,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -8654,7 +8778,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -8663,29 +8787,29 @@
     </row>
     <row r="30" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C30" ph="1"/>
       <c r="D30" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C31" ph="1"/>
       <c r="D31" t="s" ph="1">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C32" ph="1"/>
       <c r="D32" t="s" ph="1">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -8802,7 +8926,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -8832,7 +8956,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8892,7 +9016,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8958,7 +9082,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -9015,7 +9139,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -9115,7 +9239,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -9143,7 +9267,7 @@
     </row>
     <row r="49" spans="2:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B49" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D49" t="s" ph="1">
         <v>14</v>
@@ -9202,10 +9326,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -9229,7 +9353,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9253,7 +9377,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -9288,7 +9412,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>380</v>
+        <v>390</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -9307,148 +9431,178 @@
     </row>
     <row r="15" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D15" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="D16" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="5"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="D16" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B17" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="D17" t="s">
+    </row>
+    <row r="23" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="C20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="5"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="1" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
+      <c r="D24" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="D25" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B26" s="5"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="4" customFormat="1" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="8" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B26" s="1" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="4" customFormat="1" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="8" t="s">
+      <c r="C32" s="4" ph="1"/>
+      <c r="D32" s="4" t="s" ph="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="C27" s="4" ph="1"/>
-      <c r="D27" s="4" t="s" ph="1">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B28" s="1" t="s">
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
+      <c r="D34" t="s">
         <v>332</v>
       </c>
-      <c r="D29" t="s">
+    </row>
+    <row r="35" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D35" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D36" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B30" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="D30" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="B31" s="1" t="s">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="D37" t="s">
         <v>337</v>
       </c>
-      <c r="D31" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="1" t="s">
+    </row>
+    <row r="38" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B38" s="1" t="s">
         <v>339</v>
-      </c>
-      <c r="D32" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B33" s="1" t="s">
-        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -9696,7 +9850,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
win11ja: update onedrive enabling instr.
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3834474D-AD9C-4E18-A397-95D065D102B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130419F5-05D3-4ACE-9F7D-57F61B17F449}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="406">
   <si>
     <t>header1</t>
   </si>
@@ -5315,128 +5315,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>最初に、OneDriveは無料MSアカウントの場合容量が5GBと小さいので、リンクを解除しました。IMCアカウントのOneDriveは大学が有償契約をしてますので、3TBまで保存できます。
-現在のOffice365はMSアカウントとリンクしたサブスクリプション制のため、デフォルトの保存先がOneDriveになっています。ブラウザからアクセスしたり、あるいはデフォルトでない保存先として手元のPCを選ぶこともできますが、OneDriveの設定をすることでIMCアカウントのOneDriveを手元のPCと同期させることもできます。あるいは、デフォルトの保存先を手元のPC(ローカルPC)に変更することもできます。OneDriveを手元のPCと同期させるには以下の手順を実施し、デフォルトの保存先をローカルPCにする場合には次に示す&lt;a href="#office_default_local"&gt;「Officeのデフォルト保存先をローカルPCにする」&lt;/a&gt;の手順を実施してください。</t>
-    <rPh sb="0" eb="2">
-      <t>サイショ</t>
-    </rPh>
-    <rPh sb="13" eb="15">
-      <t>ムリョウ</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="25" eb="27">
-      <t>ヨウリョウ</t>
-    </rPh>
-    <rPh sb="32" eb="33">
-      <t>チイ</t>
-    </rPh>
-    <rPh sb="42" eb="44">
-      <t>カイジョ</t>
-    </rPh>
-    <rPh sb="67" eb="69">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="70" eb="72">
-      <t>ユウショウ</t>
-    </rPh>
-    <rPh sb="72" eb="74">
-      <t>ケイヤク</t>
-    </rPh>
-    <rPh sb="87" eb="89">
-      <t>ホゾン</t>
-    </rPh>
-    <rPh sb="95" eb="97">
-      <t>ゲンザイ</t>
-    </rPh>
-    <rPh sb="130" eb="131">
-      <t>セイ</t>
-    </rPh>
-    <rPh sb="141" eb="143">
-      <t>ホゾン</t>
-    </rPh>
-    <rPh sb="143" eb="144">
-      <t>サキ</t>
-    </rPh>
-    <rPh sb="187" eb="189">
-      <t>ホゾン</t>
-    </rPh>
-    <rPh sb="189" eb="190">
-      <t>サキ</t>
-    </rPh>
-    <rPh sb="193" eb="195">
-      <t>テモト</t>
-    </rPh>
-    <rPh sb="199" eb="200">
-      <t>エラ</t>
-    </rPh>
-    <rPh sb="219" eb="221">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="245" eb="247">
-      <t>テモト</t>
-    </rPh>
-    <rPh sb="251" eb="253">
-      <t>ドウキ</t>
-    </rPh>
-    <rPh sb="275" eb="277">
-      <t>ホゾン</t>
-    </rPh>
-    <rPh sb="277" eb="278">
-      <t>サキ</t>
-    </rPh>
-    <rPh sb="279" eb="281">
-      <t>テモト</t>
-    </rPh>
-    <rPh sb="293" eb="295">
-      <t>ヘンコウ</t>
-    </rPh>
-    <rPh sb="314" eb="316">
-      <t>テモト</t>
-    </rPh>
-    <rPh sb="320" eb="322">
-      <t>ドウキ</t>
-    </rPh>
-    <rPh sb="327" eb="329">
-      <t>イカ</t>
-    </rPh>
-    <rPh sb="330" eb="332">
-      <t>テジュン</t>
-    </rPh>
-    <rPh sb="333" eb="335">
-      <t>ジッシ</t>
-    </rPh>
-    <rPh sb="343" eb="345">
-      <t>ホゾン</t>
-    </rPh>
-    <rPh sb="345" eb="346">
-      <t>サキ</t>
-    </rPh>
-    <rPh sb="356" eb="358">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="360" eb="361">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="362" eb="363">
-      <t>シメ</t>
-    </rPh>
-    <rPh sb="409" eb="411">
-      <t>ホゾン</t>
-    </rPh>
-    <rPh sb="411" eb="412">
-      <t>サキ</t>
-    </rPh>
-    <rPh sb="428" eb="430">
-      <t>テジュン</t>
-    </rPh>
-    <rPh sb="431" eb="433">
-      <t>ジッシ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>「設定」から「アカウント」に進むと、右ペインにアカウント名、リワードと並んで「OneDrive」というアイコンがあります。これをクリックすると使用するOneDriveアカウントを入力させる画面が開きます。</t>
     <rPh sb="1" eb="3">
       <t>セッテイ</t>
@@ -5468,13 +5346,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>IMCアカウントとパスワードを入力します。</t>
-    <rPh sb="15" eb="17">
-      <t>ニュウリョク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>IMCアカウントと同期するOneDriveフォルダはOneDrive - Hiroshima Universityになります。</t>
     <rPh sb="9" eb="11">
       <t>ドウキ</t>
@@ -5482,15 +5353,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-imc-onedrive-dirname.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>win11ja-onedrive-exclude-desktop.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11ja-onedrive-dir-selector.png</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -5569,19 +5432,6 @@
   </si>
   <si>
     <t>win11ja-onedrive-start-backup.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>バックアップ対象フォルダを選んだらバックアップを開始します。</t>
-    <rPh sb="6" eb="8">
-      <t>タイショウ</t>
-    </rPh>
-    <rPh sb="13" eb="14">
-      <t>エラ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>カイシ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -6156,19 +6006,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>&lt;h2 id="onedrive"&gt;IMCアカウントのOneDrive連携の設定&lt;/h2&gt;</t>
-    <rPh sb="35" eb="37">
-      <t>レンケイ</t>
-    </rPh>
-    <rPh sb="38" eb="40">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="41" eb="43">
-      <t>バアイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>&lt;h2 id="office365"&gt;Office365のインストール&lt;/h2&gt;</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -6316,58 +6153,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>OneDrive同期は、同じファイルやディレクトリを複数のOneDriveアカウントで同期させることはできません。私物MSアカウントへの同期が知らないうちに入っている可能性がありますので、念のため通知エリアを確認し、第1章の手順に従ってリンクを解除してください。</t>
-    <rPh sb="8" eb="10">
-      <t>ドウキ</t>
-    </rPh>
-    <rPh sb="12" eb="13">
-      <t>オナ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>フクスウ</t>
-    </rPh>
-    <rPh sb="43" eb="45">
-      <t>ドウキ</t>
-    </rPh>
-    <rPh sb="68" eb="70">
-      <t>ドウキ</t>
-    </rPh>
-    <rPh sb="71" eb="72">
-      <t>シ</t>
-    </rPh>
-    <rPh sb="78" eb="79">
-      <t>ハイ</t>
-    </rPh>
-    <rPh sb="83" eb="86">
-      <t>カノウセイ</t>
-    </rPh>
-    <rPh sb="94" eb="95">
-      <t>ネン</t>
-    </rPh>
-    <rPh sb="98" eb="100">
-      <t>ツウチ</t>
-    </rPh>
-    <rPh sb="104" eb="106">
-      <t>カクニン</t>
-    </rPh>
-    <rPh sb="108" eb="109">
-      <t>ダイ</t>
-    </rPh>
-    <rPh sb="110" eb="111">
-      <t>ショウ</t>
-    </rPh>
-    <rPh sb="112" eb="114">
-      <t>テジュン</t>
-    </rPh>
-    <rPh sb="115" eb="116">
-      <t>シタガ</t>
-    </rPh>
-    <rPh sb="122" eb="124">
-      <t>カイジョ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>既に持っているメールアドレスでMSアカウントを作るように案内されますが、混乱を避けるため、「新しいメールアドレスを取得」を選びます。以降では、ここで新規に作るものを「私物MSアカウント」あるいは「無料MSアカウント」と呼びます。
 これとは別に大学在籍期間中に大学が有償契約したMSアカウントもありますが、卒業、あるいは大学院進学で学籍番号が無効になると使えなくなります。</t>
     <rPh sb="0" eb="1">
@@ -6818,6 +6603,280 @@
     </rPh>
     <rPh sb="14" eb="15">
       <t>エラ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>最初に、OneDriveは無料MSアカウントの場合容量が5GBと小さいので、リンクを解除しました。IMCアカウントのOneDriveは大学が有償契約をしていますので、3TBまで保存できます。
+OneDriveを以下の手順で手元のPCと同期させることもできます。ただし、この設定をしても手元のPCのストレージが3TBあるように見えるわけではなく、手元のPCのストレージ容量以上のものは同期できません。卒業・進学時に混乱を招きやすいので、必要がある方のみ、十分注意してこの設定を使ってください。</t>
+    <rPh sb="0" eb="2">
+      <t>サイショ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ムリョウ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>ヨウリョウ</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>チイ</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>カイジョ</t>
+    </rPh>
+    <rPh sb="67" eb="69">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="70" eb="72">
+      <t>ユウショウ</t>
+    </rPh>
+    <rPh sb="72" eb="74">
+      <t>ケイヤク</t>
+    </rPh>
+    <rPh sb="88" eb="90">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="105" eb="107">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="108" eb="110">
+      <t>テジュン</t>
+    </rPh>
+    <rPh sb="111" eb="113">
+      <t>テモト</t>
+    </rPh>
+    <rPh sb="117" eb="119">
+      <t>ドウキ</t>
+    </rPh>
+    <rPh sb="136" eb="138">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="142" eb="144">
+      <t>テモト</t>
+    </rPh>
+    <rPh sb="162" eb="163">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="172" eb="174">
+      <t>テモト</t>
+    </rPh>
+    <rPh sb="183" eb="185">
+      <t>ヨウリョウ</t>
+    </rPh>
+    <rPh sb="185" eb="187">
+      <t>イジョウ</t>
+    </rPh>
+    <rPh sb="191" eb="193">
+      <t>ドウキ</t>
+    </rPh>
+    <rPh sb="199" eb="201">
+      <t>ソツギョウ</t>
+    </rPh>
+    <rPh sb="202" eb="204">
+      <t>シンガク</t>
+    </rPh>
+    <rPh sb="204" eb="205">
+      <t>ジ</t>
+    </rPh>
+    <rPh sb="206" eb="208">
+      <t>コンラン</t>
+    </rPh>
+    <rPh sb="209" eb="210">
+      <t>マネ</t>
+    </rPh>
+    <rPh sb="217" eb="219">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="222" eb="223">
+      <t>カタ</t>
+    </rPh>
+    <rPh sb="226" eb="228">
+      <t>ジュウブン</t>
+    </rPh>
+    <rPh sb="228" eb="230">
+      <t>チュウイ</t>
+    </rPh>
+    <rPh sb="234" eb="236">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="237" eb="238">
+      <t>ツカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2 id="onedrive"&gt;IMCアカウントのOneDrive連携の設定(必須ではありません)&lt;/h2&gt;</t>
+    <rPh sb="35" eb="37">
+      <t>レンケイ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>ヒッス</t>
+    </rPh>
+    <rPh sb="52" eb="54">
+      <t>バアイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OneDrive同期は、同じファイルやディレクトリを複数のOneDriveアカウントで同期させることはできません。私物MSアカウントへの同期が知らないうちに入っている可能性がありますので、以下の設定を行う場合は念のため&lt;a href="../ch1.html#onedrive_unlink"&gt;第1章の手順&lt;/a&gt;に従ってリンクを確認し、解除しておいてください。</t>
+    <rPh sb="8" eb="10">
+      <t>ドウキ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>フクスウ</t>
+    </rPh>
+    <rPh sb="43" eb="45">
+      <t>ドウキ</t>
+    </rPh>
+    <rPh sb="68" eb="70">
+      <t>ドウキ</t>
+    </rPh>
+    <rPh sb="71" eb="72">
+      <t>シ</t>
+    </rPh>
+    <rPh sb="78" eb="79">
+      <t>ハイ</t>
+    </rPh>
+    <rPh sb="83" eb="86">
+      <t>カノウセイ</t>
+    </rPh>
+    <rPh sb="94" eb="96">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="97" eb="99">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="100" eb="101">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="102" eb="104">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="105" eb="106">
+      <t>ネン</t>
+    </rPh>
+    <rPh sb="158" eb="159">
+      <t>シタガ</t>
+    </rPh>
+    <rPh sb="165" eb="167">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="169" eb="171">
+      <t>カイジョ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IMCアカウントとパスワードを入力します。「すべてのアプリにサインインしたままにする」が出た場合には、これまでと同様「組織がデバイスを管理できるようにする」のチェックを外し「いいえ、このアプリのみにサインインします」で進めてください。</t>
+    <rPh sb="15" eb="17">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="44" eb="45">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="56" eb="58">
+      <t>ドウヨウ</t>
+    </rPh>
+    <rPh sb="59" eb="61">
+      <t>ソシキ</t>
+    </rPh>
+    <rPh sb="67" eb="69">
+      <t>カンリ</t>
+    </rPh>
+    <rPh sb="84" eb="85">
+      <t>ハズ</t>
+    </rPh>
+    <rPh sb="109" eb="110">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-odrv23-add-acct.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-imc-odrv-dirname.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-odrv23-dir-selector.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-explorer-with-desktop.png</t>
+  </si>
+  <si>
+    <t>win11ja-onedrive-explorer-home.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>バックアップ対象フォルダを修正したらバックアップを開始します。</t>
+    <rPh sb="6" eb="8">
+      <t>タイショウ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>シュウセイ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>カイシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>指示に沿って進めていくと、準備が完了してOneDriveフォルダを開くことになります。</t>
+    <rPh sb="0" eb="2">
+      <t>シジ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ソ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>スス</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ジュンビ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>カンリョウ</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>ヒラ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-onedrive-backup-ready.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>表示されたOneDriveフォルダには除外した「デスクトップ」も存在します。PCのデスクトップとして表示されないデスクトップなので、注意してください。</t>
+    <rPh sb="0" eb="2">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>ジョガイ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>ソンザイ</t>
+    </rPh>
+    <rPh sb="50" eb="52">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="66" eb="68">
+      <t>チュウイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -7529,7 +7588,7 @@
     </row>
     <row r="19" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>7</v>
@@ -7702,7 +7761,7 @@
     </row>
     <row r="35" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="C35" t="s" ph="1">
         <v>254</v>
@@ -7872,7 +7931,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
@@ -7880,7 +7939,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -7901,12 +7960,12 @@
     </row>
     <row r="6" spans="1:5" ht="132" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
@@ -7993,7 +8052,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
     </row>
     <row r="22" spans="2:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -8014,7 +8073,7 @@
     </row>
     <row r="24" spans="2:4" customFormat="1" ht="64.8" customHeight="1" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D24" t="s" ph="1">
         <v>273</v>
@@ -8022,66 +8081,66 @@
     </row>
     <row r="25" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>348</v>
+        <v>343</v>
       </c>
     </row>
     <row r="26" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="D26" t="s">
         <v>344</v>
-      </c>
-      <c r="D26" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="27" spans="2:4" customFormat="1" ht="45.6" customHeight="1" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="D27" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
     </row>
     <row r="28" spans="2:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="D28" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="29" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="D29" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
     </row>
     <row r="30" spans="2:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="D30" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
     </row>
     <row r="31" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="D31" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
     </row>
     <row r="32" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="D32" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
     </row>
     <row r="33" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -8089,7 +8148,7 @@
         <v>247</v>
       </c>
       <c r="D33" t="s" ph="1">
-        <v>356</v>
+        <v>351</v>
       </c>
     </row>
     <row r="34" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
@@ -8097,7 +8156,7 @@
         <v>243</v>
       </c>
       <c r="D34" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="35" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
@@ -8105,7 +8164,7 @@
         <v>280</v>
       </c>
       <c r="D35" t="s" ph="1">
-        <v>359</v>
+        <v>354</v>
       </c>
     </row>
     <row r="36" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
@@ -8123,7 +8182,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -8273,7 +8332,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8284,7 +8343,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8336,7 +8395,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -8461,7 +8520,7 @@
     </row>
     <row r="30" spans="1:4" ht="67.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="D30" t="s">
         <v>294</v>
@@ -8478,10 +8537,10 @@
     <row r="32" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="D33" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
@@ -8609,7 +8668,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
     </row>
     <row r="3" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -8641,7 +8700,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -8657,7 +8716,7 @@
     </row>
     <row r="11" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="D11" t="s">
         <v>301</v>
@@ -8700,7 +8759,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -8778,7 +8837,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -8926,7 +8985,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -8956,7 +9015,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9016,7 +9075,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9082,7 +9141,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -9139,7 +9198,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -9239,7 +9298,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -9267,7 +9326,7 @@
     </row>
     <row r="49" spans="2:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B49" s="6" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="D49" t="s" ph="1">
         <v>14</v>
@@ -9326,10 +9385,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -9412,7 +9471,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -9431,7 +9490,7 @@
     </row>
     <row r="15" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="D15" t="s">
         <v>123</v>
@@ -9439,10 +9498,10 @@
     </row>
     <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="D16" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -9492,7 +9551,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9500,29 +9559,29 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="D24" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="D25" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -9530,7 +9589,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>379</v>
+        <v>394</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -9541,52 +9600,63 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="4" customFormat="1" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B31" s="1" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" s="4" customFormat="1" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>329</v>
-      </c>
-      <c r="C32" s="4" ph="1"/>
-      <c r="D32" s="4" t="s" ph="1">
+      <c r="C31" s="4" ph="1"/>
+      <c r="D31" s="4" t="s" ph="1">
         <v>246</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="D32" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+        <v>329</v>
+      </c>
+      <c r="D33" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>331</v>
       </c>
       <c r="D34" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="35" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B35" s="1" t="s">
-        <v>335</v>
-      </c>
       <c r="D35" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>336</v>
+        <v>402</v>
       </c>
       <c r="D36" t="s">
         <v>333</v>
@@ -9594,15 +9664,26 @@
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>338</v>
+        <v>403</v>
       </c>
       <c r="D37" t="s">
-        <v>337</v>
+        <v>404</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>339</v>
+        <v>405</v>
+      </c>
+      <c r="D38" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B39" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="D39" t="s">
+        <v>401</v>
       </c>
     </row>
   </sheetData>
@@ -9850,7 +9931,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
win11ja: fix incorrect image file name
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197FB789-5807-442E-AF32-3A9BCA0B4CBE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDB837B-52F5-4CDA-93E1-446CF75B0B85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6647,10 +6647,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-odrv23-add-acct.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>win11ja-imc-odrv-dirname.png</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -6881,6 +6877,9 @@
   </si>
   <si>
     <t>win11ja-setting-acct-odrv.png</t>
+  </si>
+  <si>
+    <t>win11ja-odrv-add-acct.png</t>
   </si>
 </sst>
 </file>
@@ -9390,7 +9389,7 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -9604,12 +9603,12 @@
     </row>
     <row r="29" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="4" customFormat="1" ht="39.6" x14ac:dyDescent="0.2">
@@ -9621,7 +9620,7 @@
       </c>
       <c r="C31" s="4" ph="1"/>
       <c r="D31" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9629,7 +9628,7 @@
         <v>393</v>
       </c>
       <c r="D32" t="s">
-        <v>394</v>
+        <v>405</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
@@ -9637,7 +9636,7 @@
         <v>328</v>
       </c>
       <c r="D33" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9645,7 +9644,7 @@
         <v>330</v>
       </c>
       <c r="D34" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9658,7 +9657,7 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D36" t="s">
         <v>332</v>
@@ -9666,18 +9665,18 @@
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="D37" t="s">
         <v>400</v>
-      </c>
-      <c r="D37" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D38" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9685,7 +9684,7 @@
         <v>333</v>
       </c>
       <c r="D39" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
win11ja: separate OneDrive setting to ch8
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9591B24-D3E8-492D-BD98-5D4C73195AB2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC3C4E2-4CF3-4D92-83CE-2BDC9D221883}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -22,13 +22,14 @@
     <sheet name="ch5" sheetId="4" r:id="rId7"/>
     <sheet name="ch6" sheetId="5" r:id="rId8"/>
     <sheet name="ch7" sheetId="9" r:id="rId9"/>
+    <sheet name="ch8" sheetId="18" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="442">
   <si>
     <t>header1</t>
   </si>
@@ -760,25 +761,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>画面が黒くなり、デスクトップ環境の設定がはじまります。しばらく待ちましょう。</t>
-    <rPh sb="0" eb="2">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>クロ</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>カンキョウ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="31" eb="32">
-      <t>マ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>win11ja-msaccount-faceid.png</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1622,19 +1604,6 @@
   </si>
   <si>
     <t>（付録)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Office365のインストール手順、Microsoft Teamsの使い方</t>
-    <rPh sb="16" eb="18">
-      <t>テジュン</t>
-    </rPh>
-    <rPh sb="35" eb="36">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="37" eb="38">
-      <t>カタ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -3440,92 +3409,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Windows11は、ネット環境が無いとここから進めることができません。一度ネット環境に接続してください。このスクリーンショットは大学のネット環境のHU-CUPに接続していますが、自宅のネット環境でも問題ありません。ネット環境に接続されると、「次へ」のボタンが押せるようになるので、押しましょう。
-どうしても自宅にネット環境が無いという人は大学に来て&lt;a href="ch7.html"&gt;HU-CUPへの接続手順&lt;/a&gt;を参考にして接続しましょう(基地局リストを出すところまでの手順が済んでいる状態です)。</t>
-    <rPh sb="14" eb="16">
-      <t>カンキョウ</t>
-    </rPh>
-    <rPh sb="17" eb="18">
-      <t>ナ</t>
-    </rPh>
-    <rPh sb="24" eb="25">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="36" eb="38">
-      <t>イチド</t>
-    </rPh>
-    <rPh sb="41" eb="43">
-      <t>カンキョウ</t>
-    </rPh>
-    <rPh sb="44" eb="46">
-      <t>セツゾク</t>
-    </rPh>
-    <rPh sb="65" eb="67">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="71" eb="73">
-      <t>カンキョウ</t>
-    </rPh>
-    <rPh sb="81" eb="83">
-      <t>セツゾク</t>
-    </rPh>
-    <rPh sb="90" eb="92">
-      <t>ジタク</t>
-    </rPh>
-    <rPh sb="96" eb="98">
-      <t>カンキョウ</t>
-    </rPh>
-    <rPh sb="100" eb="102">
-      <t>モンダイ</t>
-    </rPh>
-    <rPh sb="154" eb="156">
-      <t>ジタク</t>
-    </rPh>
-    <rPh sb="160" eb="162">
-      <t>カンキョウ</t>
-    </rPh>
-    <rPh sb="163" eb="164">
-      <t>ナ</t>
-    </rPh>
-    <rPh sb="168" eb="169">
-      <t>ヒト</t>
-    </rPh>
-    <rPh sb="170" eb="172">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="173" eb="174">
-      <t>キ</t>
-    </rPh>
-    <rPh sb="202" eb="204">
-      <t>セツゾク</t>
-    </rPh>
-    <rPh sb="204" eb="206">
-      <t>テジュン</t>
-    </rPh>
-    <rPh sb="211" eb="213">
-      <t>サンコウ</t>
-    </rPh>
-    <rPh sb="216" eb="218">
-      <t>セツゾク</t>
-    </rPh>
-    <rPh sb="224" eb="227">
-      <t>キチキョク</t>
-    </rPh>
-    <rPh sb="231" eb="232">
-      <t>ダ</t>
-    </rPh>
-    <rPh sb="239" eb="241">
-      <t>テジュン</t>
-    </rPh>
-    <rPh sb="242" eb="243">
-      <t>ス</t>
-    </rPh>
-    <rPh sb="247" eb="249">
-      <t>ジョウタイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>FRESTA-TEXT-2023 Win11 chap.1</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -6819,6 +6702,742 @@
       <t>バアイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>画面が黒くなり、デスクトップ環境の設定がはじまります。しばらく待ちましょう。もし有線LANで接続している場合は、ここでLANケーブルを外すなどして接続を切ってください。</t>
+    <rPh sb="0" eb="2">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>クロ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>カンキョウ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>マ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>ユウセン</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="52" eb="54">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="67" eb="68">
+      <t>ハズ</t>
+    </rPh>
+    <rPh sb="73" eb="75">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="76" eb="77">
+      <t>キ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Windows11は、ネット環境が無いとここから進めることができません。一度ネット環境に接続してください。このスクリーンショットは大学のネット環境のHU-CUPに接続していますが、自宅のネット環境でも問題ありません。ネット環境に接続されると、「次へ」のボタンが押せるようになるので、押しましょう。ここで、無線LANで接続する場合は「自動的に接続する」のチェックを外しておいてください。
+どうしても自宅にネット環境が無いという人は大学に来て&lt;a href="ch7.html"&gt;HU-CUPへの接続手順&lt;/a&gt;を参考にして接続しましょう(基地局リストを出すところまでの手順が済んでいる状態です)。
+</t>
+    <rPh sb="14" eb="16">
+      <t>カンキョウ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>ナ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>スス</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>イチド</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>カンキョウ</t>
+    </rPh>
+    <rPh sb="44" eb="46">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="65" eb="67">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="71" eb="73">
+      <t>カンキョウ</t>
+    </rPh>
+    <rPh sb="81" eb="83">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="90" eb="92">
+      <t>ジタク</t>
+    </rPh>
+    <rPh sb="96" eb="98">
+      <t>カンキョウ</t>
+    </rPh>
+    <rPh sb="100" eb="102">
+      <t>モンダイ</t>
+    </rPh>
+    <rPh sb="158" eb="160">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="162" eb="164">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="181" eb="182">
+      <t>ハズ</t>
+    </rPh>
+    <rPh sb="198" eb="200">
+      <t>ジタク</t>
+    </rPh>
+    <rPh sb="204" eb="206">
+      <t>カンキョウ</t>
+    </rPh>
+    <rPh sb="207" eb="208">
+      <t>ナ</t>
+    </rPh>
+    <rPh sb="212" eb="213">
+      <t>ヒト</t>
+    </rPh>
+    <rPh sb="214" eb="216">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="217" eb="218">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="246" eb="248">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="248" eb="250">
+      <t>テジュン</t>
+    </rPh>
+    <rPh sb="255" eb="257">
+      <t>サンコウ</t>
+    </rPh>
+    <rPh sb="260" eb="262">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="268" eb="271">
+      <t>キチキョク</t>
+    </rPh>
+    <rPh sb="275" eb="276">
+      <t>ダ</t>
+    </rPh>
+    <rPh sb="283" eb="285">
+      <t>テジュン</t>
+    </rPh>
+    <rPh sb="286" eb="287">
+      <t>ス</t>
+    </rPh>
+    <rPh sb="291" eb="293">
+      <t>ジョウタイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Office365のインストール手順</t>
+    <rPh sb="16" eb="18">
+      <t>テジュン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2023 Win11 chap.8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OneDriveの状況確認、リンク解除、リンク設定</t>
+    <rPh sb="9" eb="11">
+      <t>ジョウキョウ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>カイジョ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>セッテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;ul&gt;
+&lt;li&gt;&lt;a href="#check_status"&gt;OneDriveの状況確認&lt;/a&gt;
+  &lt;ul&gt;
+     &lt;li&gt;&lt;a href="#check_status_2023"&gt;バージョン2023&lt;/a&gt;&lt;/li&gt;
+     &lt;li&gt;&lt;a href="#check_status_2024"&gt;バージョン2024&lt;/a&gt;&lt;/li&gt;
+  &lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;&lt;a href="#unlink"&gt;OneDriveのリンク解除&lt;/a&gt;
+  &lt;ul&gt;
+     &lt;li&gt;&lt;a href="#unlink_2023"&gt;バージョン2023&lt;/a&gt;&lt;/li&gt;
+     &lt;li&gt;&lt;a href="#unlink_2024"&gt;バージョン2024&lt;/a&gt;&lt;/li&gt;
+  &lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;&lt;a href="#unlink"&gt;OneDriveのリンク設定&lt;/a&gt;
+  &lt;ul&gt;
+     &lt;li&gt;&lt;a href="#link_2023"&gt;バージョン2023&lt;/a&gt;&lt;/li&gt;
+     &lt;li&gt;&lt;a href="#link_2024"&gt;バージョン2024&lt;/a&gt;&lt;/li&gt;
+  &lt;/ul&gt;
+&lt;/li&gt;
+&lt;/ul&gt;</t>
+    <rPh sb="42" eb="44">
+      <t>ジョウキョウ</t>
+    </rPh>
+    <rPh sb="44" eb="46">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="220" eb="222">
+      <t>カイジョ</t>
+    </rPh>
+    <rPh sb="384" eb="386">
+      <t>セッテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2 id="check_status"&gt;OneDriveの状況確認&lt;/h2&gt;</t>
+    <rPh sb="31" eb="33">
+      <t>ジョウキョウ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2 id="unlink"&gt;OneDriveのリンク解除&lt;/h2&gt;</t>
+    <rPh sb="28" eb="30">
+      <t>カイジョ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2 id="link"&gt;OneDriveのリンク設定&lt;/h2&gt;</t>
+    <rPh sb="26" eb="28">
+      <t>セッテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h3 id="unlink_2022"&gt;OneDriveのリンク解除（バージョン2022）&lt;/h3&gt;</t>
+    <rPh sb="33" eb="35">
+      <t>カイジョ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h3 id="unlink_2024"&gt;OneDriveのリンク解除（バージョン2024）&lt;/h3&gt;</t>
+    <rPh sb="33" eb="35">
+      <t>カイジョ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h3 id="link_2024"&gt;OneDriveの状況確認（バージョン2024）&lt;/h3&gt;</t>
+    <rPh sb="28" eb="30">
+      <t>ジョウキョウ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h3 id="link_2022"&gt;OneDriveの状況確認（バージョン2022）&lt;/h3&gt;</t>
+    <rPh sb="28" eb="30">
+      <t>ジョウキョウ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h3 id="check_status_2022"&gt;OneDriveの状況確認（バージョン2022）&lt;/h3&gt;</t>
+    <rPh sb="36" eb="38">
+      <t>ジョウキョウ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h3 id="check_status_2024"&gt;OneDriveの状況確認（バージョン2024）&lt;/h3&gt;</t>
+    <rPh sb="36" eb="38">
+      <t>ジョウキョウ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OneDriveサービスを使うためのOneDriveアプリは2023年中に変更があり、2022年からの古いものと、2024年に切り替わる予定の新しいもので画面構成が異なります。概念的には同じですが、それぞれのスクリーンショットを示しながら解説します。</t>
+    <rPh sb="13" eb="14">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="34" eb="35">
+      <t>ネン</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>チュウ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>ヘンコウ</t>
+    </rPh>
+    <rPh sb="47" eb="48">
+      <t>ネン</t>
+    </rPh>
+    <rPh sb="51" eb="52">
+      <t>フル</t>
+    </rPh>
+    <rPh sb="61" eb="62">
+      <t>ネン</t>
+    </rPh>
+    <rPh sb="63" eb="64">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="65" eb="66">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="68" eb="70">
+      <t>ヨテイ</t>
+    </rPh>
+    <rPh sb="71" eb="72">
+      <t>アタラ</t>
+    </rPh>
+    <rPh sb="77" eb="79">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="79" eb="81">
+      <t>コウセイ</t>
+    </rPh>
+    <rPh sb="82" eb="83">
+      <t>コト</t>
+    </rPh>
+    <rPh sb="88" eb="91">
+      <t>ガイネンテキ</t>
+    </rPh>
+    <rPh sb="93" eb="94">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="114" eb="115">
+      <t>シメ</t>
+    </rPh>
+    <rPh sb="119" eb="121">
+      <t>カイセツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>雲アイコンを右クリックしてOneDriveアプリのウィンドウを開き、歯車アイコン(①)をクリックして「設定」メニュー(②)に進みましょう。「お使いのPCのアップデート状況により、アプリの画面が微妙に異なります。
+以降では状況確認、リンク解除、リンク設定の3つの手順について、現状最も多いと思われる2022年版での手順を先に示し、2024年版での手順をその後に示します。</t>
+    <rPh sb="0" eb="1">
+      <t>クモ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ミギ</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t>ハグルマ</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="62" eb="63">
+      <t>スス</t>
+    </rPh>
+    <rPh sb="71" eb="72">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="83" eb="85">
+      <t>ジョウキョウ</t>
+    </rPh>
+    <rPh sb="93" eb="95">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="96" eb="98">
+      <t>ビミョウ</t>
+    </rPh>
+    <rPh sb="99" eb="100">
+      <t>コト</t>
+    </rPh>
+    <rPh sb="106" eb="108">
+      <t>イコウ</t>
+    </rPh>
+    <rPh sb="110" eb="112">
+      <t>ジョウキョウ</t>
+    </rPh>
+    <rPh sb="112" eb="114">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="118" eb="120">
+      <t>カイジョ</t>
+    </rPh>
+    <rPh sb="124" eb="126">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="130" eb="132">
+      <t>テジュン</t>
+    </rPh>
+    <rPh sb="137" eb="139">
+      <t>ゲンジョウ</t>
+    </rPh>
+    <rPh sb="139" eb="140">
+      <t>モット</t>
+    </rPh>
+    <rPh sb="141" eb="142">
+      <t>オオ</t>
+    </rPh>
+    <rPh sb="144" eb="145">
+      <t>オモ</t>
+    </rPh>
+    <rPh sb="152" eb="154">
+      <t>ネンバン</t>
+    </rPh>
+    <rPh sb="156" eb="158">
+      <t>テジュン</t>
+    </rPh>
+    <rPh sb="159" eb="160">
+      <t>サキ</t>
+    </rPh>
+    <rPh sb="161" eb="162">
+      <t>シメ</t>
+    </rPh>
+    <rPh sb="168" eb="170">
+      <t>ネンバン</t>
+    </rPh>
+    <rPh sb="172" eb="174">
+      <t>テジュン</t>
+    </rPh>
+    <rPh sb="177" eb="178">
+      <t>アト</t>
+    </rPh>
+    <rPh sb="179" eb="180">
+      <t>シメ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>まずOneDriveアプリのウィンドウを開き、「ヘルプと設定」(①)をクリックして、コンテキストメニューの「設定」(②)に進みます。</t>
+    <rPh sb="20" eb="21">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="54" eb="56">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="61" eb="62">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-odrv22-open-setting.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-odrv22-withaccount.png</t>
+  </si>
+  <si>
+    <t>win11ja-odrv22-noaccount.png</t>
+  </si>
+  <si>
+    <t>OneDrive設定のウィンドウが開きます。「アカウント」(①)タブを確認します。メールアドレスが表示されていれば連携済みです。</t>
+    <rPh sb="8" eb="10">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="49" eb="51">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="57" eb="59">
+      <t>レンケイ</t>
+    </rPh>
+    <rPh sb="59" eb="60">
+      <t>ズ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「連携されているアカウントがありません」と表示された場合は、&lt;a href="block_autostart"&gt;OneDriveアプリの自動起動の抑止&lt;/a&gt;に進んでください。</t>
+    <rPh sb="1" eb="3">
+      <t>レンケイ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="68" eb="70">
+      <t>ジドウ</t>
+    </rPh>
+    <rPh sb="70" eb="72">
+      <t>キドウ</t>
+    </rPh>
+    <rPh sb="73" eb="75">
+      <t>ヨクシ</t>
+    </rPh>
+    <rPh sb="80" eb="81">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>連携されている場合は「バックアップ」(②)タブを表示し、「バックアップを管理」(②)ボタンを押します。</t>
+    <rPh sb="0" eb="2">
+      <t>レンケイ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>カンリ</t>
+    </rPh>
+    <rPh sb="46" eb="47">
+      <t>オ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-odrv22-backup.png</t>
+  </si>
+  <si>
+    <t>win11ja-odrv22-backup-mgr.png</t>
+  </si>
+  <si>
+    <t>バックアップ対象のフォルダを選ぶウィンドウが表示されます。全ての「バックアップを停止」を実行します。</t>
+    <rPh sb="6" eb="8">
+      <t>タイショウ</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>エラ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>テイシ</t>
+    </rPh>
+    <rPh sb="44" eb="46">
+      <t>ジッコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1つのフォルダの「バックアップを停止」をクリックするとこのような警告が出ますが、「バックアップを停止」で進めます。</t>
+    <rPh sb="16" eb="18">
+      <t>テイシ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>ケイコク</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>テイシ</t>
+    </rPh>
+    <rPh sb="52" eb="53">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-odrv22-backup-stopwarn1.png</t>
+  </si>
+  <si>
+    <t>win11ja-odrv22-backup-stopwarn2.png</t>
+  </si>
+  <si>
+    <t>さらにこのようなメッセージが出ます。「閉じる」で進めます。</t>
+    <rPh sb="14" eb="15">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>全てのフォルダのバックアップを停止すると、改めてバックアップを開始する状態になっています。各フォルダアイコンの右上のチェックを外し、全てバックアップ対象から除外します。</t>
+    <rPh sb="0" eb="1">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>テイシ</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>アラタ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>カイシ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>ジョウタイ</t>
+    </rPh>
+    <rPh sb="45" eb="46">
+      <t>カク</t>
+    </rPh>
+    <rPh sb="55" eb="57">
+      <t>ミギウエ</t>
+    </rPh>
+    <rPh sb="63" eb="64">
+      <t>ハズ</t>
+    </rPh>
+    <rPh sb="66" eb="67">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="74" eb="76">
+      <t>タイショウ</t>
+    </rPh>
+    <rPh sb="78" eb="80">
+      <t>ジョガイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-odrv22-backup-select.png</t>
+  </si>
+  <si>
+    <t>全てのフォルダのバックアップの予定を解除すると「バックアップの開始」はグレーアウトします。右上の「X」ボタンでこのウィンドウを閉じます。</t>
+    <rPh sb="0" eb="1">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ヨテイ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>カイジョ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>カイシ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>ミギウエ</t>
+    </rPh>
+    <rPh sb="63" eb="64">
+      <t>ト</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-odrv22-backup-unselect.png</t>
+  </si>
+  <si>
+    <t>再び「アカウント」(①)タブを表示し、「このPCのリンクを解除」(②)をクリックします。</t>
+    <rPh sb="0" eb="1">
+      <t>フタタ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>カイジョ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-odrv22-unlink-pc.png</t>
+  </si>
+  <si>
+    <t>win11ja-odrv-close-signin.png</t>
+  </si>
+  <si>
+    <t>設定ウィンドウが閉じ、サインインを促すウィンドウが開くので、右上の「X」ボタンで閉じます。</t>
+    <rPh sb="0" eb="2">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>ウナガ</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>ミギウエ</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>ト</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>あらためてOneDrive設定ウィンドウを開き、「設定」(①)タブを開いて「WindowsにサインインしたときにOneDriveを自動的に開始する」(②)のチェックを外し、OKで閉じます。ここでアカウントにサインインし直し、通知領域に雲マークが無いことを確認しましょう。</t>
+    <rPh sb="13" eb="15">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="34" eb="35">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="65" eb="68">
+      <t>ジドウテキ</t>
+    </rPh>
+    <rPh sb="69" eb="71">
+      <t>カイシ</t>
+    </rPh>
+    <rPh sb="83" eb="84">
+      <t>ハズ</t>
+    </rPh>
+    <rPh sb="89" eb="90">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="109" eb="110">
+      <t>ナオ</t>
+    </rPh>
+    <rPh sb="112" eb="114">
+      <t>ツウチ</t>
+    </rPh>
+    <rPh sb="114" eb="116">
+      <t>リョウイキ</t>
+    </rPh>
+    <rPh sb="117" eb="118">
+      <t>クモ</t>
+    </rPh>
+    <rPh sb="122" eb="123">
+      <t>ナ</t>
+    </rPh>
+    <rPh sb="127" eb="129">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-odrv22-uncheck-autostart.png</t>
   </si>
 </sst>
 </file>
@@ -7259,7 +7878,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7275,7 +7894,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7283,7 +7902,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -7297,13 +7916,255 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3BA29DB-AD8A-49B1-A518-6FE0E420BFD4}">
+  <dimension ref="A1:D49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="72.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="34.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="264" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B12" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="C12" ph="1"/>
+      <c r="D12" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+      <c r="B13" s="6" t="s">
+        <v>417</v>
+      </c>
+      <c r="C13" ph="1"/>
+      <c r="D13" t="s" ph="1">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="D16" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D17" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="D18" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="D19" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="D20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="D21" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="D22" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="D23" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="D24" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D25" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="D26" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="D27" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B39" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B43" s="1" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B46" s="1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B49" s="1" t="s">
+        <v>412</v>
       </c>
     </row>
   </sheetData>
@@ -7317,8 +8178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B35" sqref="A6:D39"/>
+    <sheetView topLeftCell="A35" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.2"/>
@@ -7335,7 +8196,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -7343,7 +8204,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -7359,7 +8220,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="304.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -7367,7 +8228,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -7381,7 +8242,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7" t="s" ph="1">
         <v>7</v>
@@ -7395,7 +8256,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>7</v>
@@ -7406,7 +8267,7 @@
     </row>
     <row r="9" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D9" t="s" ph="1">
         <v>24</v>
@@ -7426,12 +8287,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="105.6" ph="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="132" ph="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>233</v>
+        <v>402</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>7</v>
@@ -7456,7 +8317,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>7</v>
@@ -7495,15 +8356,15 @@
     </row>
     <row r="16" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>7</v>
@@ -7528,7 +8389,7 @@
     </row>
     <row r="19" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>7</v>
@@ -7550,7 +8411,7 @@
     </row>
     <row r="21" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>7</v>
@@ -7594,68 +8455,68 @@
     </row>
     <row r="25" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C25" t="s" ph="1">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="26" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C26" t="s" ph="1">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D26" t="s" ph="1">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C27" t="s" ph="1">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D27" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C28" t="s" ph="1">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D28" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C29" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D29" t="s" ph="1">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C30" t="s" ph="1">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D30" t="s" ph="1">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
@@ -7693,34 +8554,34 @@
     </row>
     <row r="34" spans="2:5" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D34" t="s" ph="1">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C35" t="s" ph="1">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D35" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D36" t="s" ph="1">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="37" spans="2:5" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C37" t="s" ph="1">
         <v>7</v>
@@ -7729,9 +8590,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="2:5" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:5" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
-        <v>55</v>
+        <v>401</v>
       </c>
       <c r="C38" t="s" ph="1">
         <v>7</v>
@@ -7742,13 +8603,13 @@
     </row>
     <row r="39" spans="2:5" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C39" t="s" ph="1">
+        <v>56</v>
+      </c>
+      <c r="D39" t="s" ph="1">
         <v>57</v>
-      </c>
-      <c r="D39" t="s" ph="1">
-        <v>58</v>
       </c>
     </row>
     <row r="40" spans="2:5" ph="1" x14ac:dyDescent="0.2">
@@ -7855,7 +8716,7 @@
   <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B23" sqref="B23:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -7871,7 +8732,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
@@ -7879,7 +8740,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -7895,234 +8756,234 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="132" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s" ph="1">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E10" ph="1"/>
     </row>
     <row r="11" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s" ph="1">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:5" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C12" t="s" ph="1">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:5" customFormat="1" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="15" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="16" spans="1:5" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="17" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="18" spans="2:4" customFormat="1" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="B18" s="6" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="22" spans="2:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="D22" t="s" ph="1">
         <v>242</v>
-      </c>
-      <c r="D22" t="s" ph="1">
-        <v>245</v>
       </c>
     </row>
     <row r="23" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D23" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="24" spans="2:4" customFormat="1" ht="64.8" customHeight="1" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="25" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="26" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D26" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="27" spans="2:4" customFormat="1" ht="45.6" customHeight="1" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D27" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="28" spans="2:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D28" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="29" spans="2:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D29" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="30" spans="2:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D30" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="31" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D31" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="32" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D32" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="33" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D33" t="s" ph="1">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="34" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D34" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="35" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D35" t="s" ph="1">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="36" spans="1:4" customFormat="1" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D36" t="s" ph="1">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="37" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -8130,7 +8991,7 @@
         <v>8</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
@@ -8144,37 +9005,37 @@
         <v>4</v>
       </c>
       <c r="B42" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" t="s">
         <v>69</v>
-      </c>
-      <c r="C42" t="s">
-        <v>4</v>
-      </c>
-      <c r="D42" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B43" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D43" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B44" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D44" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B45" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8182,13 +9043,13 @@
         <v>4</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C46" t="s">
         <v>4</v>
       </c>
       <c r="D46" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -8240,7 +9101,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8248,7 +9109,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8264,7 +9125,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="145.19999999999999" x14ac:dyDescent="0.2">
@@ -8272,7 +9133,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8283,7 +9144,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8291,29 +9152,29 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D11" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D12" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -8321,13 +9182,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -8335,7 +9196,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -8346,7 +9207,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -8357,21 +9218,21 @@
         <v>4</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D19" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -8379,13 +9240,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8393,13 +9254,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8407,13 +9268,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -8426,149 +9287,149 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="82.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D27" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D28" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D29" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="67.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D30" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D31" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D33" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D34" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D35" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D36" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="50.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D38" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D39" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D40" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D41" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="46.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="6" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D42" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="131.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="6" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="6" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D47" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="48" spans="2:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8600,7 +9461,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="2" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
@@ -8608,7 +9469,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="3" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -8624,7 +9485,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -8632,7 +9493,7 @@
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -8640,7 +9501,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -8648,50 +9509,50 @@
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D10" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="D11" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D12" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D13" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D14" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D15" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -8699,7 +9560,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -8708,68 +9569,68 @@
     </row>
     <row r="19" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C19" ph="1"/>
       <c r="D19" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="132" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C20" ph="1"/>
       <c r="D20" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
@@ -8777,7 +9638,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -8786,29 +9647,29 @@
     </row>
     <row r="30" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C30" ph="1"/>
       <c r="D30" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C31" ph="1"/>
       <c r="D31" t="s" ph="1">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C32" ph="1"/>
       <c r="D32" t="s" ph="1">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -8866,7 +9727,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8874,7 +9735,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8890,7 +9751,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -8901,7 +9762,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8920,12 +9781,12 @@
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -8933,7 +9794,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -8944,18 +9805,18 @@
     </row>
     <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8963,7 +9824,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -8971,18 +9832,18 @@
     </row>
     <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -8990,13 +9851,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
         <v>108</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="198" x14ac:dyDescent="0.2">
@@ -9004,18 +9865,18 @@
         <v>4</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9023,21 +9884,21 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D21" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9045,21 +9906,21 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D23" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9067,13 +9928,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -9081,7 +9942,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -9097,40 +9958,40 @@
     </row>
     <row r="28" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D30" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -9138,7 +9999,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -9157,80 +10018,80 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D36" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D37" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D39" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D40" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D41" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C42" t="s">
         <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C43" t="s">
         <v>4</v>
       </c>
       <c r="D43" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -9238,7 +10099,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -9246,7 +10107,7 @@
     </row>
     <row r="47" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C47" t="s">
         <v>4</v>
@@ -9257,7 +10118,7 @@
     </row>
     <row r="48" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C48" t="s">
         <v>7</v>
@@ -9266,7 +10127,7 @@
     </row>
     <row r="49" spans="2:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B49" s="6" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="D49" t="s" ph="1">
         <v>14</v>
@@ -9274,7 +10135,7 @@
     </row>
     <row r="50" spans="2:4" ht="132" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C50" t="s">
         <v>7</v>
@@ -9327,7 +10188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -9352,7 +10213,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9368,7 +10229,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -9376,7 +10237,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -9400,18 +10261,18 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -9419,29 +10280,29 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D16" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -9449,13 +10310,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9463,13 +10324,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -9477,13 +10338,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -9491,7 +10352,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9499,29 +10360,29 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="D24" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D25" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -9529,7 +10390,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -9542,12 +10403,12 @@
     </row>
     <row r="29" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="4" customFormat="1" ht="39.6" x14ac:dyDescent="0.2">
@@ -9555,67 +10416,67 @@
         <v>4</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C31" s="4" ph="1"/>
       <c r="D31" s="4" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D32" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D33" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="D34" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D35" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="D36" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="D37" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D38" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
   </sheetData>
@@ -9646,7 +10507,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -9654,7 +10515,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9670,17 +10531,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -9693,7 +10554,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -9718,13 +10579,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9732,21 +10593,21 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -9754,12 +10615,12 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9767,33 +10628,33 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D19" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -9808,7 +10669,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -9824,7 +10685,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>113</v>
+        <v>403</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -9832,7 +10693,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9848,22 +10709,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>113</v>
+        <v>403</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9895,7 +10756,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.2">
@@ -9903,10 +10764,10 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D16" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9914,39 +10775,39 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D17" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D19" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9954,26 +10815,26 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D23" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D24" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
win11ja: update chapter order
</commit_message>
<xml_diff>
--- a/win11.xlsx
+++ b/win11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC3C4E2-4CF3-4D92-83CE-2BDC9D221883}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6E7276-0792-48EA-B619-4C6448E01FCD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="856" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="459">
   <si>
     <t>header1</t>
   </si>
@@ -6425,6 +6425,9 @@
   </si>
   <si>
     <t>win11ja-imc-odrv-dirname.png</t>
+  </si>
+  <si>
+    <t>win11ja-imc-odrv-dirname.png</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -6864,22 +6867,321 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>&lt;h2 id="check_status"&gt;OneDriveの状況確認&lt;/h2&gt;</t>
+    <rPh sb="31" eb="33">
+      <t>ジョウキョウ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h3 id="unlink_2024"&gt;OneDriveのリンク解除（バージョン2024）&lt;/h3&gt;</t>
+    <rPh sb="33" eb="35">
+      <t>カイジョ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h3 id="link_2024"&gt;OneDriveの状況確認（バージョン2024）&lt;/h3&gt;</t>
+    <rPh sb="28" eb="30">
+      <t>ジョウキョウ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h3 id="link_2022"&gt;OneDriveの状況確認（バージョン2022）&lt;/h3&gt;</t>
+    <rPh sb="28" eb="30">
+      <t>ジョウキョウ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OneDriveサービスを使うためのOneDriveアプリは2023年中に変更があり、2022年からの古いものと、2024年に切り替わる予定の新しいもので画面構成が異なります。概念的には同じですが、それぞれのスクリーンショットを示しながら解説します。</t>
+    <rPh sb="13" eb="14">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="34" eb="35">
+      <t>ネン</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>チュウ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>ヘンコウ</t>
+    </rPh>
+    <rPh sb="47" eb="48">
+      <t>ネン</t>
+    </rPh>
+    <rPh sb="51" eb="52">
+      <t>フル</t>
+    </rPh>
+    <rPh sb="61" eb="62">
+      <t>ネン</t>
+    </rPh>
+    <rPh sb="63" eb="64">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="65" eb="66">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="68" eb="70">
+      <t>ヨテイ</t>
+    </rPh>
+    <rPh sb="71" eb="72">
+      <t>アタラ</t>
+    </rPh>
+    <rPh sb="77" eb="79">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="79" eb="81">
+      <t>コウセイ</t>
+    </rPh>
+    <rPh sb="82" eb="83">
+      <t>コト</t>
+    </rPh>
+    <rPh sb="88" eb="91">
+      <t>ガイネンテキ</t>
+    </rPh>
+    <rPh sb="93" eb="94">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="114" eb="115">
+      <t>シメ</t>
+    </rPh>
+    <rPh sb="119" eb="121">
+      <t>カイセツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>まずOneDriveアプリのウィンドウを開き、「ヘルプと設定」(①)をクリックして、コンテキストメニューの「設定」(②)に進みます。</t>
+    <rPh sb="20" eb="21">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="54" eb="56">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="61" eb="62">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-odrv22-open-setting.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-odrv22-withaccount.png</t>
+  </si>
+  <si>
+    <t>win11ja-odrv22-noaccount.png</t>
+  </si>
+  <si>
+    <t>win11ja-odrv22-backup.png</t>
+  </si>
+  <si>
+    <t>win11ja-odrv22-backup-mgr.png</t>
+  </si>
+  <si>
+    <t>バックアップ対象のフォルダを選ぶウィンドウが表示されます。全ての「バックアップを停止」を実行します。</t>
+    <rPh sb="6" eb="8">
+      <t>タイショウ</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>エラ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>テイシ</t>
+    </rPh>
+    <rPh sb="44" eb="46">
+      <t>ジッコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1つのフォルダの「バックアップを停止」をクリックするとこのような警告が出ますが、「バックアップを停止」で進めます。</t>
+    <rPh sb="16" eb="18">
+      <t>テイシ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>ケイコク</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>テイシ</t>
+    </rPh>
+    <rPh sb="52" eb="53">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-odrv22-backup-stopwarn1.png</t>
+  </si>
+  <si>
+    <t>win11ja-odrv22-backup-stopwarn2.png</t>
+  </si>
+  <si>
+    <t>さらにこのようなメッセージが出ます。「閉じる」で進めます。</t>
+    <rPh sb="14" eb="15">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>全てのフォルダのバックアップを停止すると、改めてバックアップを開始する状態になっています。各フォルダアイコンの右上のチェックを外し、全てバックアップ対象から除外します。</t>
+    <rPh sb="0" eb="1">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>テイシ</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>アラタ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>カイシ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>ジョウタイ</t>
+    </rPh>
+    <rPh sb="45" eb="46">
+      <t>カク</t>
+    </rPh>
+    <rPh sb="55" eb="57">
+      <t>ミギウエ</t>
+    </rPh>
+    <rPh sb="63" eb="64">
+      <t>ハズ</t>
+    </rPh>
+    <rPh sb="66" eb="67">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="74" eb="76">
+      <t>タイショウ</t>
+    </rPh>
+    <rPh sb="78" eb="80">
+      <t>ジョガイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-odrv22-backup-select.png</t>
+  </si>
+  <si>
+    <t>全てのフォルダのバックアップの予定を解除すると「バックアップの開始」はグレーアウトします。右上の「X」ボタンでこのウィンドウを閉じます。</t>
+    <rPh sb="0" eb="1">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ヨテイ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>カイジョ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>カイシ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>ミギウエ</t>
+    </rPh>
+    <rPh sb="63" eb="64">
+      <t>ト</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-odrv22-backup-unselect.png</t>
+  </si>
+  <si>
+    <t>再び「アカウント」(①)タブを表示し、「このPCのリンクを解除」(②)をクリックします。</t>
+    <rPh sb="0" eb="1">
+      <t>フタタ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>カイジョ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-odrv22-unlink-pc.png</t>
+  </si>
+  <si>
+    <t>win11ja-odrv-close-signin.png</t>
+  </si>
+  <si>
+    <t>設定ウィンドウが閉じ、サインインを促すウィンドウが開くので、右上の「X」ボタンで閉じます。</t>
+    <rPh sb="0" eb="2">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>ウナガ</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>ミギウエ</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>ト</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-odrv22-uncheck-autostart.png</t>
+  </si>
+  <si>
+    <t>win11ja-odrv-app.png</t>
+  </si>
+  <si>
     <t>&lt;ul&gt;
 &lt;li&gt;&lt;a href="#check_status"&gt;OneDriveの状況確認&lt;/a&gt;
   &lt;ul&gt;
-     &lt;li&gt;&lt;a href="#check_status_2023"&gt;バージョン2023&lt;/a&gt;&lt;/li&gt;
+     &lt;li&gt;&lt;a href="#check_status_2022"&gt;バージョン2022&lt;/a&gt;&lt;/li&gt;
      &lt;li&gt;&lt;a href="#check_status_2024"&gt;バージョン2024&lt;/a&gt;&lt;/li&gt;
   &lt;/ul&gt;
 &lt;/li&gt;
 &lt;li&gt;&lt;a href="#unlink"&gt;OneDriveのリンク解除&lt;/a&gt;
   &lt;ul&gt;
-     &lt;li&gt;&lt;a href="#unlink_2023"&gt;バージョン2023&lt;/a&gt;&lt;/li&gt;
+     &lt;li&gt;&lt;a href="#unlink_2022"&gt;バージョン2022&lt;/a&gt;&lt;/li&gt;
      &lt;li&gt;&lt;a href="#unlink_2024"&gt;バージョン2024&lt;/a&gt;&lt;/li&gt;
   &lt;/ul&gt;
 &lt;/li&gt;
 &lt;li&gt;&lt;a href="#unlink"&gt;OneDriveのリンク設定&lt;/a&gt;
   &lt;ul&gt;
-     &lt;li&gt;&lt;a href="#link_2023"&gt;バージョン2023&lt;/a&gt;&lt;/li&gt;
+     &lt;li&gt;&lt;a href="#link_2022"&gt;バージョン2022&lt;/a&gt;&lt;/li&gt;
      &lt;li&gt;&lt;a href="#link_2024"&gt;バージョン2024&lt;/a&gt;&lt;/li&gt;
   &lt;/ul&gt;
 &lt;/li&gt;
@@ -6899,144 +7201,154 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>&lt;h2 id="check_status"&gt;OneDriveの状況確認&lt;/h2&gt;</t>
-    <rPh sb="31" eb="33">
-      <t>ジョウキョウ</t>
-    </rPh>
-    <rPh sb="33" eb="35">
+    <t>OneDrive設定のウィンドウが開きます。「アカウント」(①)タブを確認します。メールアドレスが表示されていればリンク済みです。</t>
+    <rPh sb="8" eb="10">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
       <t>カクニン</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&lt;h2 id="unlink"&gt;OneDriveのリンク解除&lt;/h2&gt;</t>
-    <rPh sb="28" eb="30">
+    <rPh sb="49" eb="51">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="60" eb="61">
+      <t>ズ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「連携されているアカウントがありません」と表示された場合はリンクされていませんが、ユーザの指示なしに自動的にリンクをはじめる場合があります。&lt;a href="unlink_2022"&gt;解除手順&lt;/a&gt;の準備として確認した場合は、&lt;a href="block_autostart_2022"&gt;自動起動の停止&lt;/a&gt;も実施してください。</t>
+    <rPh sb="1" eb="3">
+      <t>レンケイ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>シジ</t>
+    </rPh>
+    <rPh sb="50" eb="53">
+      <t>ジドウテキ</t>
+    </rPh>
+    <rPh sb="62" eb="64">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="92" eb="94">
       <t>カイジョ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&lt;h2 id="link"&gt;OneDriveのリンク設定&lt;/h2&gt;</t>
-    <rPh sb="26" eb="28">
+    <rPh sb="94" eb="96">
+      <t>テジュン</t>
+    </rPh>
+    <rPh sb="101" eb="103">
+      <t>ジュンビ</t>
+    </rPh>
+    <rPh sb="106" eb="108">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="110" eb="112">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="145" eb="147">
+      <t>ジドウ</t>
+    </rPh>
+    <rPh sb="147" eb="149">
+      <t>キドウ</t>
+    </rPh>
+    <rPh sb="150" eb="152">
+      <t>テイシ</t>
+    </rPh>
+    <rPh sb="157" eb="159">
+      <t>ジッシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OneDriveの設定ウィンドウを開いて、「バックアップ」(②)タブを表示し、「バックアップを管理」(②)ボタンを押します。</t>
+    <rPh sb="9" eb="11">
       <t>セッテイ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&lt;h3 id="unlink_2022"&gt;OneDriveのリンク解除（バージョン2022）&lt;/h3&gt;</t>
-    <rPh sb="33" eb="35">
-      <t>カイジョ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&lt;h3 id="unlink_2024"&gt;OneDriveのリンク解除（バージョン2024）&lt;/h3&gt;</t>
-    <rPh sb="33" eb="35">
-      <t>カイジョ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&lt;h3 id="link_2024"&gt;OneDriveの状況確認（バージョン2024）&lt;/h3&gt;</t>
-    <rPh sb="28" eb="30">
-      <t>ジョウキョウ</t>
-    </rPh>
+    <rPh sb="17" eb="18">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="47" eb="49">
+      <t>カンリ</t>
+    </rPh>
+    <rPh sb="57" eb="58">
+      <t>オ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OneDrive設定ウィンドウを開き、「設定」(①)タブを開いて「WindowsにサインインしたときにOneDriveを自動的に開始する」(②)のチェックを外し、OKで閉じます。ここでアカウントにサインインし直し、通知領域に雲マークが無いことを確認しましょう。</t>
+    <rPh sb="8" eb="10">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="60" eb="63">
+      <t>ジドウテキ</t>
+    </rPh>
+    <rPh sb="64" eb="66">
+      <t>カイシ</t>
+    </rPh>
+    <rPh sb="78" eb="79">
+      <t>ハズ</t>
+    </rPh>
+    <rPh sb="84" eb="85">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="104" eb="105">
+      <t>ナオ</t>
+    </rPh>
+    <rPh sb="107" eb="109">
+      <t>ツウチ</t>
+    </rPh>
+    <rPh sb="109" eb="111">
+      <t>リョウイキ</t>
+    </rPh>
+    <rPh sb="112" eb="113">
+      <t>クモ</t>
+    </rPh>
+    <rPh sb="117" eb="118">
+      <t>ナ</t>
+    </rPh>
+    <rPh sb="122" eb="124">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h3 id="block_autostart_2022"&gt;自動起動の抑止&lt;/h3&gt;</t>
     <rPh sb="30" eb="32">
-      <t>カクニン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&lt;h3 id="link_2022"&gt;OneDriveの状況確認（バージョン2022）&lt;/h3&gt;</t>
-    <rPh sb="28" eb="30">
-      <t>ジョウキョウ</t>
-    </rPh>
-    <rPh sb="30" eb="32">
-      <t>カクニン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&lt;h3 id="check_status_2022"&gt;OneDriveの状況確認（バージョン2022）&lt;/h3&gt;</t>
-    <rPh sb="36" eb="38">
-      <t>ジョウキョウ</t>
-    </rPh>
-    <rPh sb="38" eb="40">
-      <t>カクニン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&lt;h3 id="check_status_2024"&gt;OneDriveの状況確認（バージョン2024）&lt;/h3&gt;</t>
-    <rPh sb="36" eb="38">
-      <t>ジョウキョウ</t>
-    </rPh>
-    <rPh sb="38" eb="40">
-      <t>カクニン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>OneDriveサービスを使うためのOneDriveアプリは2023年中に変更があり、2022年からの古いものと、2024年に切り替わる予定の新しいもので画面構成が異なります。概念的には同じですが、それぞれのスクリーンショットを示しながら解説します。</t>
-    <rPh sb="13" eb="14">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="34" eb="35">
-      <t>ネン</t>
-    </rPh>
-    <rPh sb="35" eb="36">
-      <t>チュウ</t>
-    </rPh>
-    <rPh sb="37" eb="39">
-      <t>ヘンコウ</t>
-    </rPh>
-    <rPh sb="47" eb="48">
-      <t>ネン</t>
-    </rPh>
-    <rPh sb="51" eb="52">
-      <t>フル</t>
-    </rPh>
-    <rPh sb="61" eb="62">
-      <t>ネン</t>
-    </rPh>
-    <rPh sb="63" eb="64">
-      <t>キ</t>
-    </rPh>
-    <rPh sb="65" eb="66">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="68" eb="70">
-      <t>ヨテイ</t>
-    </rPh>
-    <rPh sb="71" eb="72">
-      <t>アタラ</t>
-    </rPh>
-    <rPh sb="77" eb="79">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="79" eb="81">
-      <t>コウセイ</t>
-    </rPh>
-    <rPh sb="82" eb="83">
-      <t>コト</t>
-    </rPh>
-    <rPh sb="88" eb="91">
-      <t>ガイネンテキ</t>
-    </rPh>
-    <rPh sb="93" eb="94">
-      <t>オナ</t>
-    </rPh>
-    <rPh sb="114" eb="115">
-      <t>シメ</t>
-    </rPh>
-    <rPh sb="119" eb="121">
-      <t>カイセツ</t>
+      <t>ジドウ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>キドウ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>ヨクシ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>雲アイコンを右クリックしてOneDriveアプリのウィンドウを開き、歯車アイコン(①)をクリックして「設定」メニュー(②)に進みましょう。「お使いのPCのアップデート状況により、アプリの画面が微妙に異なります。
-以降では状況確認、リンク解除、リンク設定の3つの手順について、現状最も多いと思われる2022年版での手順を先に示し、2024年版での手順をその後に示します。</t>
+以降では状態確認、リンク解除、自動起動抑止、リンク設定の3つの手順について、現状最も多いと思われる2022年版での手順を先に示し、2024年版での手順をその後に示します。</t>
     <rPh sb="0" eb="1">
       <t>クモ</t>
     </rPh>
@@ -7074,7 +7386,7 @@
       <t>イコウ</t>
     </rPh>
     <rPh sb="110" eb="112">
-      <t>ジョウキョウ</t>
+      <t>ジョウタイ</t>
     </rPh>
     <rPh sb="112" eb="114">
       <t>カクニン</t>
@@ -7082,362 +7394,320 @@
     <rPh sb="118" eb="120">
       <t>カイジョ</t>
     </rPh>
-    <rPh sb="124" eb="126">
+    <rPh sb="121" eb="123">
+      <t>ジドウ</t>
+    </rPh>
+    <rPh sb="123" eb="125">
+      <t>キドウ</t>
+    </rPh>
+    <rPh sb="125" eb="127">
+      <t>ヨクシ</t>
+    </rPh>
+    <rPh sb="131" eb="133">
       <t>セッテイ</t>
     </rPh>
-    <rPh sb="130" eb="132">
+    <rPh sb="137" eb="139">
       <t>テジュン</t>
     </rPh>
-    <rPh sb="137" eb="139">
+    <rPh sb="144" eb="146">
       <t>ゲンジョウ</t>
     </rPh>
-    <rPh sb="139" eb="140">
+    <rPh sb="146" eb="147">
       <t>モット</t>
     </rPh>
-    <rPh sb="141" eb="142">
+    <rPh sb="148" eb="149">
       <t>オオ</t>
     </rPh>
-    <rPh sb="144" eb="145">
+    <rPh sb="151" eb="152">
       <t>オモ</t>
     </rPh>
-    <rPh sb="152" eb="154">
+    <rPh sb="159" eb="161">
       <t>ネンバン</t>
     </rPh>
-    <rPh sb="156" eb="158">
+    <rPh sb="163" eb="165">
       <t>テジュン</t>
     </rPh>
-    <rPh sb="159" eb="160">
+    <rPh sb="166" eb="167">
       <t>サキ</t>
     </rPh>
-    <rPh sb="161" eb="162">
+    <rPh sb="168" eb="169">
       <t>シメ</t>
     </rPh>
-    <rPh sb="168" eb="170">
+    <rPh sb="175" eb="177">
       <t>ネンバン</t>
     </rPh>
-    <rPh sb="172" eb="174">
+    <rPh sb="179" eb="181">
       <t>テジュン</t>
     </rPh>
-    <rPh sb="177" eb="178">
+    <rPh sb="184" eb="185">
       <t>アト</t>
     </rPh>
-    <rPh sb="179" eb="180">
+    <rPh sb="186" eb="187">
       <t>シメ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>まずOneDriveアプリのウィンドウを開き、「ヘルプと設定」(①)をクリックして、コンテキストメニューの「設定」(②)に進みます。</t>
-    <rPh sb="20" eb="21">
+    <t>&lt;h2 id="version2022"&gt;バージョン2022での手順&lt;/h2&gt;</t>
+    <rPh sb="32" eb="34">
+      <t>テジュン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h3 id="check_status_2022"&gt;状態確認&lt;/h3&gt;</t>
+    <rPh sb="27" eb="29">
+      <t>ジョウタイ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h3 id="unlink_2022"&gt;リンク解除&lt;/h3&gt;</t>
+    <rPh sb="24" eb="26">
+      <t>カイジョ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2 id="link"&gt;バージョン2024&lt;/h2&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h3 id="block_autostart_2022"&gt;OneDriveへのIMCアカウントの追加&lt;/h3&gt;</t>
+    <rPh sb="49" eb="51">
+      <t>ツイカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「設定」アプリから「アカウント」(①)メニューを開き、「OneDrive」アイコンをクリックします。</t>
+    <rPh sb="1" eb="3">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
       <t>ヒラ</t>
     </rPh>
-    <rPh sb="28" eb="30">
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MSアカウントを入力するウィンドウが開きます。IMCアカウント(@hiroshima-u.ac.jpを付加すること)とパスワードでサインインします。「すべてのアプリにサインインしたままにする」で「OK」を押さないよう注意してください。</t>
+    <rPh sb="8" eb="10">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>フカ</t>
+    </rPh>
+    <rPh sb="102" eb="103">
+      <t>オ</t>
+    </rPh>
+    <rPh sb="108" eb="110">
+      <t>チュウイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>この手順は初期設定の中では必須ではありません。必要な方だけ実施してください。一度設定すると再インストールしない限り元に戻せない部分があるので注意してください。</t>
+    <rPh sb="2" eb="4">
+      <t>テジュン</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ショキ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
       <t>セッテイ</t>
     </rPh>
-    <rPh sb="54" eb="56">
+    <rPh sb="10" eb="11">
+      <t>ナカ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ヒッス</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>カタ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>ジッシ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>イチド</t>
+    </rPh>
+    <rPh sb="40" eb="42">
       <t>セッテイ</t>
     </rPh>
-    <rPh sb="61" eb="62">
-      <t>スス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11ja-odrv22-open-setting.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11ja-odrv22-withaccount.png</t>
-  </si>
-  <si>
-    <t>win11ja-odrv22-noaccount.png</t>
-  </si>
-  <si>
-    <t>OneDrive設定のウィンドウが開きます。「アカウント」(①)タブを確認します。メールアドレスが表示されていれば連携済みです。</t>
-    <rPh sb="8" eb="10">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="17" eb="18">
-      <t>ヒラ</t>
-    </rPh>
-    <rPh sb="35" eb="37">
+    <rPh sb="45" eb="46">
+      <t>サイ</t>
+    </rPh>
+    <rPh sb="55" eb="56">
+      <t>カギ</t>
+    </rPh>
+    <rPh sb="57" eb="58">
+      <t>モト</t>
+    </rPh>
+    <rPh sb="59" eb="60">
+      <t>モド</t>
+    </rPh>
+    <rPh sb="63" eb="65">
+      <t>ブブン</t>
+    </rPh>
+    <rPh sb="70" eb="72">
+      <t>チュウイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-odrv-add-acct.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OneDriveフォルダーに「- Hiroshima University」がついていることを確認しましょう。</t>
+    <rPh sb="47" eb="49">
       <t>カクニン</t>
     </rPh>
-    <rPh sb="49" eb="51">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="57" eb="59">
-      <t>レンケイ</t>
-    </rPh>
-    <rPh sb="59" eb="60">
-      <t>ズ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「連携されているアカウントがありません」と表示された場合は、&lt;a href="block_autostart"&gt;OneDriveアプリの自動起動の抑止&lt;/a&gt;に進んでください。</t>
-    <rPh sb="1" eb="3">
-      <t>レンケイ</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="68" eb="70">
-      <t>ジドウ</t>
-    </rPh>
-    <rPh sb="70" eb="72">
-      <t>キドウ</t>
-    </rPh>
-    <rPh sb="73" eb="75">
-      <t>ヨクシ</t>
-    </rPh>
-    <rPh sb="80" eb="81">
-      <t>スス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>連携されている場合は「バックアップ」(②)タブを表示し、「バックアップを管理」(②)ボタンを押します。</t>
-    <rPh sb="0" eb="2">
-      <t>レンケイ</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="36" eb="38">
-      <t>カンリ</t>
-    </rPh>
-    <rPh sb="46" eb="47">
-      <t>オ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11ja-odrv22-backup.png</t>
-  </si>
-  <si>
-    <t>win11ja-odrv22-backup-mgr.png</t>
-  </si>
-  <si>
-    <t>バックアップ対象のフォルダを選ぶウィンドウが表示されます。全ての「バックアップを停止」を実行します。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-odrv22-dir-selector.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>バックアップ対象のフォルダを選ぶ画面になります。ここでは&lt;strong&gt;必ずデスクトップを除外してください&lt;/strong&gt;。さもないと貴方が普通に作るデータは全てOneDrive管理下となるため、同期の異常が起きたり、一部の授業で使うOneDrive管理下で動かないアプリを使うことができなくなります。</t>
     <rPh sb="6" eb="8">
       <t>タイショウ</t>
     </rPh>
     <rPh sb="14" eb="15">
       <t>エラ</t>
     </rPh>
-    <rPh sb="22" eb="24">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="29" eb="30">
+    <rPh sb="16" eb="18">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>カナラ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>ジョガイ</t>
+    </rPh>
+    <rPh sb="68" eb="70">
+      <t>アナタ</t>
+    </rPh>
+    <rPh sb="71" eb="73">
+      <t>フツウ</t>
+    </rPh>
+    <rPh sb="74" eb="75">
+      <t>ツク</t>
+    </rPh>
+    <rPh sb="80" eb="81">
       <t>スベ</t>
     </rPh>
-    <rPh sb="40" eb="42">
-      <t>テイシ</t>
-    </rPh>
-    <rPh sb="44" eb="46">
-      <t>ジッコウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>1つのフォルダの「バックアップを停止」をクリックするとこのような警告が出ますが、「バックアップを停止」で進めます。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ドキュメントと写真は選択してもしなくても構いません。終わったら「続ける」で進めます。</t>
+  </si>
+  <si>
+    <t>win11ja-odrv22-exclude-desktop.png</t>
+  </si>
+  <si>
+    <t>win11ja-odrv-backup-ready.png</t>
+  </si>
+  <si>
+    <t>指示に沿ってすすめていくと準備が完了します。「OneDriveフォルダを開く」をクリックします。</t>
+    <rPh sb="0" eb="2">
+      <t>シジ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ソ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ジュンビ</t>
+    </rPh>
     <rPh sb="16" eb="18">
-      <t>テイシ</t>
-    </rPh>
-    <rPh sb="32" eb="34">
-      <t>ケイコク</t>
-    </rPh>
-    <rPh sb="35" eb="36">
+      <t>カンリョウ</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>ヒラ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OneDriveフォルダに「デスクトップ」というフォルダができている場合があります。このデスクトップはOneDrive側にあるフォルダに単に「デスクトップ」という名前がつけてあるだけで、皆さんのPCのデスクトップのことを指している保証はありません。</t>
+    <rPh sb="34" eb="36">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="59" eb="60">
+      <t>ガワ</t>
+    </rPh>
+    <rPh sb="68" eb="69">
+      <t>タン</t>
+    </rPh>
+    <rPh sb="81" eb="83">
+      <t>ナマエ</t>
+    </rPh>
+    <rPh sb="93" eb="94">
+      <t>ミナ</t>
+    </rPh>
+    <rPh sb="110" eb="111">
+      <t>サ</t>
+    </rPh>
+    <rPh sb="115" eb="117">
+      <t>ホショウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11ja-odrv-explorer-home.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>エクスプローラの左サイドメニューの「ホーム」(①)をクリックし、クイックアクセスに出ているフォルダの状況を見てみましょう。少なくとも「デスクトップ」(②)には雲マークがついていないことを確認してください。ついていた場合は、&lt;a href="unlink_2022"&gt;リンク解除&lt;/a&gt;の手順を実施してからあらためてリンク設定を試してください。</t>
+    <rPh sb="8" eb="9">
+      <t>ヒダリ</t>
+    </rPh>
+    <rPh sb="41" eb="42">
       <t>デ</t>
     </rPh>
-    <rPh sb="48" eb="50">
-      <t>テイシ</t>
-    </rPh>
-    <rPh sb="52" eb="53">
-      <t>スス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11ja-odrv22-backup-stopwarn1.png</t>
-  </si>
-  <si>
-    <t>win11ja-odrv22-backup-stopwarn2.png</t>
-  </si>
-  <si>
-    <t>さらにこのようなメッセージが出ます。「閉じる」で進めます。</t>
-    <rPh sb="14" eb="15">
-      <t>デ</t>
-    </rPh>
-    <rPh sb="19" eb="20">
-      <t>ト</t>
-    </rPh>
-    <rPh sb="24" eb="25">
-      <t>スス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>全てのフォルダのバックアップを停止すると、改めてバックアップを開始する状態になっています。各フォルダアイコンの右上のチェックを外し、全てバックアップ対象から除外します。</t>
-    <rPh sb="0" eb="1">
-      <t>スベ</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>テイシ</t>
-    </rPh>
-    <rPh sb="21" eb="22">
-      <t>アラタ</t>
-    </rPh>
-    <rPh sb="31" eb="33">
-      <t>カイシ</t>
-    </rPh>
-    <rPh sb="35" eb="37">
-      <t>ジョウタイ</t>
-    </rPh>
-    <rPh sb="45" eb="46">
-      <t>カク</t>
-    </rPh>
-    <rPh sb="55" eb="57">
-      <t>ミギウエ</t>
-    </rPh>
-    <rPh sb="63" eb="64">
-      <t>ハズ</t>
-    </rPh>
-    <rPh sb="66" eb="67">
-      <t>スベ</t>
-    </rPh>
-    <rPh sb="74" eb="76">
-      <t>タイショウ</t>
-    </rPh>
-    <rPh sb="78" eb="80">
-      <t>ジョガイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11ja-odrv22-backup-select.png</t>
-  </si>
-  <si>
-    <t>全てのフォルダのバックアップの予定を解除すると「バックアップの開始」はグレーアウトします。右上の「X」ボタンでこのウィンドウを閉じます。</t>
-    <rPh sb="0" eb="1">
-      <t>スベ</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>ヨテイ</t>
-    </rPh>
-    <rPh sb="18" eb="20">
+    <rPh sb="50" eb="52">
+      <t>ジョウキョウ</t>
+    </rPh>
+    <rPh sb="53" eb="54">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="61" eb="62">
+      <t>スク</t>
+    </rPh>
+    <rPh sb="79" eb="80">
+      <t>クモ</t>
+    </rPh>
+    <rPh sb="93" eb="95">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="107" eb="109">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="136" eb="138">
       <t>カイジョ</t>
     </rPh>
-    <rPh sb="31" eb="33">
-      <t>カイシ</t>
-    </rPh>
-    <rPh sb="45" eb="47">
-      <t>ミギウエ</t>
-    </rPh>
-    <rPh sb="63" eb="64">
-      <t>ト</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11ja-odrv22-backup-unselect.png</t>
-  </si>
-  <si>
-    <t>再び「アカウント」(①)タブを表示し、「このPCのリンクを解除」(②)をクリックします。</t>
-    <rPh sb="0" eb="1">
-      <t>フタタ</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="29" eb="31">
-      <t>カイジョ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11ja-odrv22-unlink-pc.png</t>
-  </si>
-  <si>
-    <t>win11ja-odrv-close-signin.png</t>
-  </si>
-  <si>
-    <t>設定ウィンドウが閉じ、サインインを促すウィンドウが開くので、右上の「X」ボタンで閉じます。</t>
-    <rPh sb="0" eb="2">
+    <rPh sb="143" eb="145">
+      <t>テジュン</t>
+    </rPh>
+    <rPh sb="146" eb="148">
+      <t>ジッシ</t>
+    </rPh>
+    <rPh sb="160" eb="162">
       <t>セッテイ</t>
     </rPh>
-    <rPh sb="8" eb="9">
-      <t>ト</t>
-    </rPh>
-    <rPh sb="17" eb="18">
-      <t>ウナガ</t>
-    </rPh>
-    <rPh sb="25" eb="26">
-      <t>ヒラ</t>
-    </rPh>
-    <rPh sb="30" eb="32">
-      <t>ミギウエ</t>
-    </rPh>
-    <rPh sb="40" eb="41">
-      <t>ト</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>あらためてOneDrive設定ウィンドウを開き、「設定」(①)タブを開いて「WindowsにサインインしたときにOneDriveを自動的に開始する」(②)のチェックを外し、OKで閉じます。ここでアカウントにサインインし直し、通知領域に雲マークが無いことを確認しましょう。</t>
-    <rPh sb="13" eb="15">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="21" eb="22">
-      <t>ヒラ</t>
-    </rPh>
-    <rPh sb="25" eb="27">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="34" eb="35">
-      <t>ヒラ</t>
-    </rPh>
-    <rPh sb="65" eb="68">
-      <t>ジドウテキ</t>
-    </rPh>
-    <rPh sb="69" eb="71">
-      <t>カイシ</t>
-    </rPh>
-    <rPh sb="83" eb="84">
-      <t>ハズ</t>
-    </rPh>
-    <rPh sb="89" eb="90">
-      <t>ト</t>
-    </rPh>
-    <rPh sb="109" eb="110">
-      <t>ナオ</t>
-    </rPh>
-    <rPh sb="112" eb="114">
-      <t>ツウチ</t>
-    </rPh>
-    <rPh sb="114" eb="116">
-      <t>リョウイキ</t>
-    </rPh>
-    <rPh sb="117" eb="118">
-      <t>クモ</t>
-    </rPh>
-    <rPh sb="122" eb="123">
-      <t>ナ</t>
-    </rPh>
-    <rPh sb="127" eb="129">
-      <t>カクニン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11ja-odrv22-uncheck-autostart.png</t>
+    <rPh sb="163" eb="164">
+      <t>タメ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -7934,10 +8204,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3BA29DB-AD8A-49B1-A518-6FE0E420BFD4}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -7953,7 +8223,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7977,17 +8247,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="264" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>406</v>
+        <v>433</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -7997,7 +8267,7 @@
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8009,162 +8279,234 @@
         <v>268</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>417</v>
+        <v>439</v>
       </c>
       <c r="C13" ph="1"/>
-      <c r="D13" t="s" ph="1">
-        <v>269</v>
+      <c r="D13" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>414</v>
+        <v>441</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="D16" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>422</v>
+        <v>434</v>
       </c>
       <c r="D17" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>423</v>
+        <v>435</v>
       </c>
       <c r="D18" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="D19" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="D20" t="s">
-        <v>426</v>
+        <v>442</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D21" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="D22" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="D23" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D24" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="D25" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="D26" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="D27" t="s">
         <v>428</v>
       </c>
-      <c r="D21" t="s">
+    </row>
+    <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="D28" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="1" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="D32" t="s">
         <v>431</v>
       </c>
-      <c r="D22" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B23" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="D23" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="D24" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="D25" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="D36" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="D37" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B38" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="D38" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B39" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="D39" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="D26" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B27" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="D27" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B33" s="1" t="s">
+      <c r="B40" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="D40" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="D41" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="D42" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B43" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="D43" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B45" s="1" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B36" s="1" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B49" s="1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B52" s="1" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B39" s="1" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B43" s="1" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B55" s="1" t="s">
         <v>409</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B46" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B49" s="1" t="s">
-        <v>412</v>
       </c>
     </row>
   </sheetData>
@@ -8292,7 +8634,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>7</v>
@@ -8592,7 +8934,7 @@
     </row>
     <row r="38" spans="2:5" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C38" t="s" ph="1">
         <v>7</v>
@@ -10237,7 +10579,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -10390,7 +10732,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -10403,12 +10745,12 @@
     </row>
     <row r="29" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="4" customFormat="1" ht="39.6" x14ac:dyDescent="0.2">
@@ -10420,7 +10762,7 @@
       </c>
       <c r="C31" s="4" ph="1"/>
       <c r="D31" s="4" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -10428,7 +10770,7 @@
         <v>385</v>
       </c>
       <c r="D32" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
@@ -10436,20 +10778,20 @@
         <v>324</v>
       </c>
       <c r="D33" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D34" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D35" t="s">
         <v>325</v>
@@ -10457,18 +10799,18 @@
     </row>
     <row r="36" spans="2:4" x14a